<commit_message>
Ajout de l'activité de la journée sur le journal d'activité
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E5EFFA-8208-433E-B717-68AD553644A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E6E368-826E-4C8B-842C-17E406351BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28170" windowHeight="15360" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Constantin Minos</t>
+  </si>
+  <si>
+    <t>Travail sur un tutoriel de la configuratrion IP fixe pour la société 13ème Porte (Ajout d'une partie pour réserver des adresses IP dans le DHCP de la Box internet de la société 13ème Porte</t>
+  </si>
+  <si>
+    <t>Jour OFF (Entretien avec une école d'ingénieurs)</t>
   </si>
 </sst>
 </file>
@@ -361,7 +367,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -441,30 +447,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -486,16 +504,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -819,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +860,7 @@
       <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="40" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="22" t="s">
@@ -860,50 +869,50 @@
       <c r="F1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="38"/>
+      <c r="G1" s="42"/>
       <c r="H1" s="12" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="40"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
-      <c r="M1" s="27"/>
+      <c r="M1" s="37"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>43844</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="41"/>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
-      <c r="G2" s="39"/>
+      <c r="G2" s="43"/>
       <c r="H2" s="13"/>
       <c r="I2" s="15"/>
-      <c r="J2" s="41"/>
+      <c r="J2" s="45"/>
       <c r="K2" s="13"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="28"/>
+      <c r="M2" s="38"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>43845</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="17">
         <v>43845</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="30"/>
+      <c r="F3" s="32"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="K3" s="3"/>
@@ -913,25 +922,25 @@
       <c r="A4" s="17">
         <v>43846</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="17">
         <v>43846</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>43847</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="17">
         <v>43847</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="32"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="34"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1"/>
       <c r="K5" s="3"/>
@@ -941,49 +950,49 @@
       <c r="A6" s="17">
         <v>43848</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="17">
         <v>43848</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>43849</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="17">
         <v>43849</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>43850</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="17">
         <v>43850</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>43851</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="17">
         <v>43851</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="34"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
       <c r="K9" s="3"/>
@@ -993,13 +1002,13 @@
       <c r="A10" s="17">
         <v>43852</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="17">
         <v>43852</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="34"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
       <c r="K10" s="3"/>
@@ -1009,73 +1018,73 @@
       <c r="A11" s="17">
         <v>43853</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="17">
         <v>43853</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>43854</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="17">
         <v>43854</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>43855</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="17">
         <v>43855</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>43856</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="17">
         <v>43856</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>43857</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="17">
         <v>43857</v>
       </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>43858</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="17">
         <v>43858</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="34"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
       <c r="K16" s="3"/>
@@ -1085,13 +1094,13 @@
       <c r="A17" s="17">
         <v>43859</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="17">
         <v>43859</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="34"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
       <c r="K17" s="3"/>
@@ -1101,25 +1110,25 @@
       <c r="A18" s="17">
         <v>43860</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="17">
         <v>43860</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="34"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>43861</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="32"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="17">
         <v>43861</v>
       </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="34"/>
       <c r="I19" s="1"/>
       <c r="L19" s="1"/>
     </row>
@@ -1127,49 +1136,49 @@
       <c r="A20" s="17">
         <v>43862</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="32"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="17">
         <v>43862</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="34"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>43863</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="32"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="34"/>
       <c r="D21" s="17">
         <v>43863</v>
       </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="34"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>43864</v>
       </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="32"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="17">
         <v>43864</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="34"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>43865</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="32"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="17">
         <v>43865</v>
       </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="34"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
       <c r="K23" s="3"/>
@@ -1179,13 +1188,13 @@
       <c r="A24" s="17">
         <v>43866</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="32"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="34"/>
       <c r="D24" s="17">
         <v>43866</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="34"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
       <c r="K24" s="3"/>
@@ -1195,25 +1204,25 @@
       <c r="A25" s="17">
         <v>43867</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="32"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="17">
         <v>43867</v>
       </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="32"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>43868</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="32"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="34"/>
       <c r="D26" s="17">
         <v>43868</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="34"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
       <c r="K26" s="3"/>
@@ -1223,49 +1232,49 @@
       <c r="A27" s="17">
         <v>43869</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="32"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="17">
         <v>43869</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="34"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>43870</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="17">
         <v>43870</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>43871</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34"/>
       <c r="D29" s="17">
         <v>43871</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="34"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>43872</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="32"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="17">
         <v>43872</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="32"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
       <c r="H30" s="3"/>
       <c r="I30" s="1"/>
       <c r="K30" s="3"/>
@@ -1275,13 +1284,13 @@
       <c r="A31" s="17">
         <v>43873</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="32"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="34"/>
       <c r="D31" s="17">
         <v>43873</v>
       </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="32"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
       <c r="K31" s="3"/>
@@ -1291,25 +1300,25 @@
       <c r="A32" s="17">
         <v>43874</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="32"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="34"/>
       <c r="D32" s="17">
         <v>43874</v>
       </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="32"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="34"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>43875</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="32"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="34"/>
       <c r="D33" s="17">
         <v>43875</v>
       </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="32"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="34"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
       <c r="K33" s="3"/>
@@ -1319,145 +1328,145 @@
       <c r="A34" s="17">
         <v>43876</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="34"/>
       <c r="D34" s="17">
         <v>43876</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="34"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>43877</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="32"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="34"/>
       <c r="D35" s="17">
         <v>43877</v>
       </c>
-      <c r="E35" s="31"/>
-      <c r="F35" s="32"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="34"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>43878</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="32"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="34"/>
       <c r="D36" s="17">
         <v>43878</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="32"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="34"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>43879</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="32"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="34"/>
       <c r="D37" s="17">
         <v>43879</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="32"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="34"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>43880</v>
       </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="32"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="34"/>
       <c r="D38" s="17">
         <v>43880</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="32"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="34"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>43881</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="32"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="34"/>
       <c r="D39" s="17">
         <v>43881</v>
       </c>
-      <c r="E39" s="31"/>
-      <c r="F39" s="32"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="34"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>43882</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="32"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="34"/>
       <c r="D40" s="17">
         <v>43882</v>
       </c>
-      <c r="E40" s="31"/>
-      <c r="F40" s="32"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="34"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>43883</v>
       </c>
-      <c r="B41" s="31"/>
-      <c r="C41" s="32"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="34"/>
       <c r="D41" s="17">
         <v>43883</v>
       </c>
-      <c r="E41" s="31"/>
-      <c r="F41" s="32"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="34"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>43884</v>
       </c>
-      <c r="B42" s="31"/>
-      <c r="C42" s="32"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="34"/>
       <c r="D42" s="17">
         <v>43884</v>
       </c>
-      <c r="E42" s="31"/>
-      <c r="F42" s="32"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="34"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>43885</v>
       </c>
-      <c r="B43" s="31"/>
-      <c r="C43" s="32"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="34"/>
       <c r="D43" s="17">
         <v>43885</v>
       </c>
-      <c r="E43" s="31"/>
-      <c r="F43" s="32"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="34"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>43886</v>
       </c>
-      <c r="B44" s="31"/>
-      <c r="C44" s="32"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="34"/>
       <c r="D44" s="17">
         <v>43886</v>
       </c>
-      <c r="E44" s="31"/>
-      <c r="F44" s="32"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="34"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>43887</v>
       </c>
-      <c r="B45" s="31"/>
-      <c r="C45" s="32"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="34"/>
       <c r="D45" s="17">
         <v>43887</v>
       </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="32"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="34"/>
       <c r="H45" s="4"/>
       <c r="K45" s="4"/>
     </row>
@@ -1465,73 +1474,73 @@
       <c r="A46" s="17">
         <v>43888</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="32"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="34"/>
       <c r="D46" s="17">
         <v>43888</v>
       </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="32"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="34"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>43889</v>
       </c>
-      <c r="B47" s="31"/>
-      <c r="C47" s="32"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="34"/>
       <c r="D47" s="17">
         <v>43889</v>
       </c>
-      <c r="E47" s="31"/>
-      <c r="F47" s="32"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="34"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>43890</v>
       </c>
-      <c r="B48" s="31"/>
-      <c r="C48" s="32"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="34"/>
       <c r="D48" s="17">
         <v>43890</v>
       </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="32"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="34"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>43891</v>
       </c>
-      <c r="B49" s="31"/>
-      <c r="C49" s="32"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="34"/>
       <c r="D49" s="17">
         <v>43891</v>
       </c>
-      <c r="E49" s="31"/>
-      <c r="F49" s="32"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="34"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>43892</v>
       </c>
-      <c r="B50" s="31"/>
-      <c r="C50" s="32"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="34"/>
       <c r="D50" s="17">
         <v>43892</v>
       </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="32"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="34"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>43893</v>
       </c>
-      <c r="B51" s="31"/>
-      <c r="C51" s="32"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="34"/>
       <c r="D51" s="17">
         <v>43893</v>
       </c>
-      <c r="E51" s="31"/>
-      <c r="F51" s="32"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="34"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
       <c r="K51" s="4"/>
@@ -1541,13 +1550,13 @@
       <c r="A52" s="17">
         <v>43894</v>
       </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="32"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="34"/>
       <c r="D52" s="17">
         <v>43894</v>
       </c>
-      <c r="E52" s="31"/>
-      <c r="F52" s="32"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="34"/>
       <c r="H52" s="4"/>
       <c r="I52" s="1"/>
       <c r="K52" s="4"/>
@@ -1557,25 +1566,25 @@
       <c r="A53" s="17">
         <v>43895</v>
       </c>
-      <c r="B53" s="31"/>
-      <c r="C53" s="32"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="34"/>
       <c r="D53" s="17">
         <v>43895</v>
       </c>
-      <c r="E53" s="31"/>
-      <c r="F53" s="32"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="34"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>43896</v>
       </c>
-      <c r="B54" s="31"/>
-      <c r="C54" s="32"/>
+      <c r="B54" s="33"/>
+      <c r="C54" s="34"/>
       <c r="D54" s="17">
         <v>43896</v>
       </c>
-      <c r="E54" s="31"/>
-      <c r="F54" s="32"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="34"/>
       <c r="H54" s="4"/>
       <c r="I54" s="1"/>
       <c r="K54" s="4"/>
@@ -1585,49 +1594,49 @@
       <c r="A55" s="17">
         <v>43897</v>
       </c>
-      <c r="B55" s="31"/>
-      <c r="C55" s="32"/>
+      <c r="B55" s="33"/>
+      <c r="C55" s="34"/>
       <c r="D55" s="17">
         <v>43897</v>
       </c>
-      <c r="E55" s="31"/>
-      <c r="F55" s="32"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="34"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>43898</v>
       </c>
-      <c r="B56" s="31"/>
-      <c r="C56" s="32"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="34"/>
       <c r="D56" s="17">
         <v>43898</v>
       </c>
-      <c r="E56" s="31"/>
-      <c r="F56" s="32"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="34"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>43899</v>
       </c>
-      <c r="B57" s="31"/>
-      <c r="C57" s="32"/>
+      <c r="B57" s="33"/>
+      <c r="C57" s="34"/>
       <c r="D57" s="17">
         <v>43899</v>
       </c>
-      <c r="E57" s="31"/>
-      <c r="F57" s="32"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="34"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>43900</v>
       </c>
-      <c r="B58" s="31"/>
-      <c r="C58" s="32"/>
+      <c r="B58" s="33"/>
+      <c r="C58" s="34"/>
       <c r="D58" s="17">
         <v>43900</v>
       </c>
-      <c r="E58" s="31"/>
-      <c r="F58" s="32"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="34"/>
       <c r="H58" s="4"/>
       <c r="I58" s="1"/>
       <c r="K58" s="4"/>
@@ -1637,13 +1646,13 @@
       <c r="A59" s="17">
         <v>43901</v>
       </c>
-      <c r="B59" s="31"/>
-      <c r="C59" s="32"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="34"/>
       <c r="D59" s="17">
         <v>43901</v>
       </c>
-      <c r="E59" s="31"/>
-      <c r="F59" s="32"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="34"/>
       <c r="H59" s="4"/>
       <c r="I59" s="1"/>
       <c r="K59" s="4"/>
@@ -1653,25 +1662,25 @@
       <c r="A60" s="17">
         <v>43902</v>
       </c>
-      <c r="B60" s="31"/>
-      <c r="C60" s="32"/>
+      <c r="B60" s="33"/>
+      <c r="C60" s="34"/>
       <c r="D60" s="17">
         <v>43902</v>
       </c>
-      <c r="E60" s="31"/>
-      <c r="F60" s="32"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="34"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>43903</v>
       </c>
-      <c r="B61" s="31"/>
-      <c r="C61" s="32"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="34"/>
       <c r="D61" s="17">
         <v>43903</v>
       </c>
-      <c r="E61" s="31"/>
-      <c r="F61" s="32"/>
+      <c r="E61" s="33"/>
+      <c r="F61" s="34"/>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
       <c r="K61" s="4"/>
@@ -1681,25 +1690,25 @@
       <c r="A62" s="17">
         <v>43904</v>
       </c>
-      <c r="B62" s="31"/>
-      <c r="C62" s="32"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="34"/>
       <c r="D62" s="17">
         <v>43904</v>
       </c>
-      <c r="E62" s="31"/>
-      <c r="F62" s="32"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="34"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <v>43905</v>
       </c>
-      <c r="B63" s="31"/>
-      <c r="C63" s="32"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="34"/>
       <c r="D63" s="17">
         <v>43905</v>
       </c>
-      <c r="E63" s="31"/>
-      <c r="F63" s="32"/>
+      <c r="E63" s="33"/>
+      <c r="F63" s="34"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
@@ -1729,25 +1738,25 @@
       <c r="A65" s="17">
         <v>43907</v>
       </c>
-      <c r="B65" s="33" t="s">
+      <c r="B65" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="34">
+      <c r="C65" s="36">
         <v>10</v>
       </c>
       <c r="D65" s="17">
         <v>43907</v>
       </c>
-      <c r="E65" s="33" t="s">
+      <c r="E65" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="34">
+      <c r="F65" s="36">
         <v>13</v>
       </c>
-      <c r="H65" s="42" t="s">
+      <c r="H65" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I65" s="44"/>
+      <c r="I65" s="46"/>
       <c r="K65" s="4"/>
       <c r="L65" s="1"/>
     </row>
@@ -1755,15 +1764,15 @@
       <c r="A66" s="17">
         <v>43908</v>
       </c>
-      <c r="B66" s="33"/>
-      <c r="C66" s="34"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="36"/>
       <c r="D66" s="17">
         <v>43908</v>
       </c>
-      <c r="E66" s="33"/>
-      <c r="F66" s="34"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="44"/>
+      <c r="E66" s="35"/>
+      <c r="F66" s="36"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="46"/>
       <c r="K66" s="4"/>
       <c r="L66" s="1"/>
     </row>
@@ -1771,15 +1780,15 @@
       <c r="A67" s="17">
         <v>43909</v>
       </c>
-      <c r="B67" s="33"/>
-      <c r="C67" s="34"/>
+      <c r="B67" s="35"/>
+      <c r="C67" s="36"/>
       <c r="D67" s="17">
         <v>43909</v>
       </c>
-      <c r="E67" s="33"/>
-      <c r="F67" s="34"/>
-      <c r="H67" s="42"/>
-      <c r="I67" s="44"/>
+      <c r="E67" s="35"/>
+      <c r="F67" s="36"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="46"/>
       <c r="K67" s="4"/>
       <c r="L67" s="1"/>
     </row>
@@ -1787,51 +1796,51 @@
       <c r="A68" s="17">
         <v>43910</v>
       </c>
-      <c r="B68" s="33"/>
-      <c r="C68" s="34"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="36"/>
       <c r="D68" s="17">
         <v>43910</v>
       </c>
-      <c r="E68" s="33"/>
-      <c r="F68" s="34"/>
-      <c r="H68" s="42"/>
-      <c r="I68" s="44"/>
+      <c r="E68" s="35"/>
+      <c r="F68" s="36"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="46"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <v>43911</v>
       </c>
-      <c r="B69" s="33" t="s">
+      <c r="B69" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="35">
+      <c r="C69" s="39">
         <v>4</v>
       </c>
       <c r="D69" s="17">
         <v>43911</v>
       </c>
-      <c r="E69" s="33" t="s">
+      <c r="E69" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="43">
+      <c r="F69" s="30">
         <v>8</v>
       </c>
-      <c r="H69" s="42"/>
-      <c r="I69" s="44"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="46"/>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <v>43912</v>
       </c>
-      <c r="B70" s="33"/>
-      <c r="C70" s="35"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="39"/>
       <c r="D70" s="17">
         <v>43912</v>
       </c>
-      <c r="E70" s="33"/>
-      <c r="F70" s="43"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="44"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="30"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="46"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
@@ -1846,14 +1855,14 @@
       <c r="D71" s="17">
         <v>43913</v>
       </c>
-      <c r="E71" s="42" t="s">
+      <c r="E71" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F71" s="43">
+      <c r="F71" s="30">
         <v>6</v>
       </c>
-      <c r="H71" s="42"/>
-      <c r="I71" s="44"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="46"/>
     </row>
     <row r="72" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
@@ -1868,8 +1877,8 @@
       <c r="D72" s="17">
         <v>43914</v>
       </c>
-      <c r="E72" s="42"/>
-      <c r="F72" s="43"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="30"/>
       <c r="H72" s="2" t="s">
         <v>18</v>
       </c>
@@ -1903,18 +1912,24 @@
       <c r="A74" s="17">
         <v>43916</v>
       </c>
-      <c r="B74" s="21"/>
-      <c r="C74" s="20"/>
+      <c r="B74" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C74" s="30"/>
       <c r="D74" s="17">
         <v>43916</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="17">
         <v>43917</v>
       </c>
-      <c r="B75" s="21"/>
-      <c r="C75" s="20"/>
+      <c r="B75" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" s="20">
+        <v>2</v>
+      </c>
       <c r="D75" s="17">
         <v>43917</v>
       </c>
@@ -2737,7 +2752,7 @@
       </c>
       <c r="C159" s="11">
         <f>SUM(C64:C155)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D159" s="9" t="s">
         <v>2</v>
@@ -2746,7 +2761,7 @@
         <f>SUM(F64:F156)</f>
         <v>29</v>
       </c>
-      <c r="I159" s="45">
+      <c r="I159" s="28">
         <f>SUM(I2:I155)</f>
         <v>10</v>
       </c>
@@ -2760,14 +2775,8 @@
     </row>
     <row r="161" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="E3:F63"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
+  <mergeCells count="19">
+    <mergeCell ref="B74:C74"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="B2:C63"/>
     <mergeCell ref="B65:B68"/>
@@ -2779,6 +2788,13 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="H65:H71"/>
     <mergeCell ref="I65:I71"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="E3:F63"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mise à jour du journal d'activité
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E6E368-826E-4C8B-842C-17E406351BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81BFECF-FFA7-49EA-A3B5-A77A06B88692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28170" windowHeight="15360" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Jour OFF (Entretien avec une école d'ingénieurs)</t>
+  </si>
+  <si>
+    <t>Rédaction d'un document commun au groupe SFL5</t>
   </si>
 </sst>
 </file>
@@ -453,56 +456,56 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -828,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +863,7 @@
       <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="22" t="s">
@@ -869,50 +872,50 @@
       <c r="F1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="42"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="12" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="44"/>
+      <c r="J1" s="43"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
-      <c r="M1" s="37"/>
+      <c r="M1" s="31"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>43844</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="41"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
-      <c r="G2" s="43"/>
+      <c r="G2" s="42"/>
       <c r="H2" s="13"/>
       <c r="I2" s="15"/>
-      <c r="J2" s="45"/>
+      <c r="J2" s="44"/>
       <c r="K2" s="13"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="38"/>
+      <c r="M2" s="32"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>43845</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="17">
         <v>43845</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="32"/>
+      <c r="F3" s="34"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="K3" s="3"/>
@@ -922,25 +925,25 @@
       <c r="A4" s="17">
         <v>43846</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="17">
         <v>43846</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>43847</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="17">
         <v>43847</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="34"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1"/>
       <c r="K5" s="3"/>
@@ -950,49 +953,49 @@
       <c r="A6" s="17">
         <v>43848</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="17">
         <v>43848</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>43849</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="17">
         <v>43849</v>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>43850</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="17">
         <v>43850</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>43851</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="17">
         <v>43851</v>
       </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="36"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
       <c r="K9" s="3"/>
@@ -1002,13 +1005,13 @@
       <c r="A10" s="17">
         <v>43852</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="17">
         <v>43852</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
       <c r="K10" s="3"/>
@@ -1018,73 +1021,73 @@
       <c r="A11" s="17">
         <v>43853</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="17">
         <v>43853</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>43854</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="17">
         <v>43854</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="34"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>43855</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="17">
         <v>43855</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>43856</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="34"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="17">
         <v>43856</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="34"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>43857</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="17">
         <v>43857</v>
       </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="34"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>43858</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="17">
         <v>43858</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="36"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
       <c r="K16" s="3"/>
@@ -1094,13 +1097,13 @@
       <c r="A17" s="17">
         <v>43859</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="17">
         <v>43859</v>
       </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="34"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
       <c r="K17" s="3"/>
@@ -1110,25 +1113,25 @@
       <c r="A18" s="17">
         <v>43860</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
       <c r="D18" s="17">
         <v>43860</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>43861</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="17">
         <v>43861</v>
       </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="34"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="36"/>
       <c r="I19" s="1"/>
       <c r="L19" s="1"/>
     </row>
@@ -1136,49 +1139,49 @@
       <c r="A20" s="17">
         <v>43862</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="17">
         <v>43862</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>43863</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="17">
         <v>43863</v>
       </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="34"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>43864</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="17">
         <v>43864</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>43865</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="17">
         <v>43865</v>
       </c>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="36"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
       <c r="K23" s="3"/>
@@ -1188,13 +1191,13 @@
       <c r="A24" s="17">
         <v>43866</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="17">
         <v>43866</v>
       </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="36"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
       <c r="K24" s="3"/>
@@ -1204,25 +1207,25 @@
       <c r="A25" s="17">
         <v>43867</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="36"/>
       <c r="D25" s="17">
         <v>43867</v>
       </c>
-      <c r="E25" s="33"/>
-      <c r="F25" s="34"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>43868</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="17">
         <v>43868</v>
       </c>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
       <c r="K26" s="3"/>
@@ -1232,49 +1235,49 @@
       <c r="A27" s="17">
         <v>43869</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="36"/>
       <c r="D27" s="17">
         <v>43869</v>
       </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="34"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>43870</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="36"/>
       <c r="D28" s="17">
         <v>43870</v>
       </c>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>43871</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="34"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="36"/>
       <c r="D29" s="17">
         <v>43871</v>
       </c>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="36"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>43872</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="34"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="36"/>
       <c r="D30" s="17">
         <v>43872</v>
       </c>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="36"/>
       <c r="H30" s="3"/>
       <c r="I30" s="1"/>
       <c r="K30" s="3"/>
@@ -1284,13 +1287,13 @@
       <c r="A31" s="17">
         <v>43873</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="34"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="17">
         <v>43873</v>
       </c>
-      <c r="E31" s="33"/>
-      <c r="F31" s="34"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="36"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
       <c r="K31" s="3"/>
@@ -1300,25 +1303,25 @@
       <c r="A32" s="17">
         <v>43874</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="34"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="36"/>
       <c r="D32" s="17">
         <v>43874</v>
       </c>
-      <c r="E32" s="33"/>
-      <c r="F32" s="34"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="36"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>43875</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="34"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="17">
         <v>43875</v>
       </c>
-      <c r="E33" s="33"/>
-      <c r="F33" s="34"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="36"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
       <c r="K33" s="3"/>
@@ -1328,145 +1331,145 @@
       <c r="A34" s="17">
         <v>43876</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="34"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="36"/>
       <c r="D34" s="17">
         <v>43876</v>
       </c>
-      <c r="E34" s="33"/>
-      <c r="F34" s="34"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="36"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>43877</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="34"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="36"/>
       <c r="D35" s="17">
         <v>43877</v>
       </c>
-      <c r="E35" s="33"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="36"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>43878</v>
       </c>
-      <c r="B36" s="33"/>
-      <c r="C36" s="34"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="17">
         <v>43878</v>
       </c>
-      <c r="E36" s="33"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="36"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>43879</v>
       </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="34"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="36"/>
       <c r="D37" s="17">
         <v>43879</v>
       </c>
-      <c r="E37" s="33"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="36"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>43880</v>
       </c>
-      <c r="B38" s="33"/>
-      <c r="C38" s="34"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="36"/>
       <c r="D38" s="17">
         <v>43880</v>
       </c>
-      <c r="E38" s="33"/>
-      <c r="F38" s="34"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="36"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>43881</v>
       </c>
-      <c r="B39" s="33"/>
-      <c r="C39" s="34"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="36"/>
       <c r="D39" s="17">
         <v>43881</v>
       </c>
-      <c r="E39" s="33"/>
-      <c r="F39" s="34"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="36"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>43882</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="34"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="36"/>
       <c r="D40" s="17">
         <v>43882</v>
       </c>
-      <c r="E40" s="33"/>
-      <c r="F40" s="34"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="36"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>43883</v>
       </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="36"/>
       <c r="D41" s="17">
         <v>43883</v>
       </c>
-      <c r="E41" s="33"/>
-      <c r="F41" s="34"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="36"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>43884</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="34"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="36"/>
       <c r="D42" s="17">
         <v>43884</v>
       </c>
-      <c r="E42" s="33"/>
-      <c r="F42" s="34"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="36"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>43885</v>
       </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="34"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="36"/>
       <c r="D43" s="17">
         <v>43885</v>
       </c>
-      <c r="E43" s="33"/>
-      <c r="F43" s="34"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="36"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>43886</v>
       </c>
-      <c r="B44" s="33"/>
-      <c r="C44" s="34"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="36"/>
       <c r="D44" s="17">
         <v>43886</v>
       </c>
-      <c r="E44" s="33"/>
-      <c r="F44" s="34"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="36"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>43887</v>
       </c>
-      <c r="B45" s="33"/>
-      <c r="C45" s="34"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="36"/>
       <c r="D45" s="17">
         <v>43887</v>
       </c>
-      <c r="E45" s="33"/>
-      <c r="F45" s="34"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="36"/>
       <c r="H45" s="4"/>
       <c r="K45" s="4"/>
     </row>
@@ -1474,73 +1477,73 @@
       <c r="A46" s="17">
         <v>43888</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="34"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="36"/>
       <c r="D46" s="17">
         <v>43888</v>
       </c>
-      <c r="E46" s="33"/>
-      <c r="F46" s="34"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="36"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>43889</v>
       </c>
-      <c r="B47" s="33"/>
-      <c r="C47" s="34"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="36"/>
       <c r="D47" s="17">
         <v>43889</v>
       </c>
-      <c r="E47" s="33"/>
-      <c r="F47" s="34"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="36"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>43890</v>
       </c>
-      <c r="B48" s="33"/>
-      <c r="C48" s="34"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="36"/>
       <c r="D48" s="17">
         <v>43890</v>
       </c>
-      <c r="E48" s="33"/>
-      <c r="F48" s="34"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="36"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>43891</v>
       </c>
-      <c r="B49" s="33"/>
-      <c r="C49" s="34"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="36"/>
       <c r="D49" s="17">
         <v>43891</v>
       </c>
-      <c r="E49" s="33"/>
-      <c r="F49" s="34"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="36"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>43892</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="C50" s="34"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="36"/>
       <c r="D50" s="17">
         <v>43892</v>
       </c>
-      <c r="E50" s="33"/>
-      <c r="F50" s="34"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="36"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>43893</v>
       </c>
-      <c r="B51" s="33"/>
-      <c r="C51" s="34"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="36"/>
       <c r="D51" s="17">
         <v>43893</v>
       </c>
-      <c r="E51" s="33"/>
-      <c r="F51" s="34"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="36"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
       <c r="K51" s="4"/>
@@ -1550,13 +1553,13 @@
       <c r="A52" s="17">
         <v>43894</v>
       </c>
-      <c r="B52" s="33"/>
-      <c r="C52" s="34"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="36"/>
       <c r="D52" s="17">
         <v>43894</v>
       </c>
-      <c r="E52" s="33"/>
-      <c r="F52" s="34"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="36"/>
       <c r="H52" s="4"/>
       <c r="I52" s="1"/>
       <c r="K52" s="4"/>
@@ -1566,25 +1569,25 @@
       <c r="A53" s="17">
         <v>43895</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="34"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="36"/>
       <c r="D53" s="17">
         <v>43895</v>
       </c>
-      <c r="E53" s="33"/>
-      <c r="F53" s="34"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="36"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>43896</v>
       </c>
-      <c r="B54" s="33"/>
-      <c r="C54" s="34"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="36"/>
       <c r="D54" s="17">
         <v>43896</v>
       </c>
-      <c r="E54" s="33"/>
-      <c r="F54" s="34"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="36"/>
       <c r="H54" s="4"/>
       <c r="I54" s="1"/>
       <c r="K54" s="4"/>
@@ -1594,49 +1597,49 @@
       <c r="A55" s="17">
         <v>43897</v>
       </c>
-      <c r="B55" s="33"/>
-      <c r="C55" s="34"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="36"/>
       <c r="D55" s="17">
         <v>43897</v>
       </c>
-      <c r="E55" s="33"/>
-      <c r="F55" s="34"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="36"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>43898</v>
       </c>
-      <c r="B56" s="33"/>
-      <c r="C56" s="34"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="36"/>
       <c r="D56" s="17">
         <v>43898</v>
       </c>
-      <c r="E56" s="33"/>
-      <c r="F56" s="34"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="36"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>43899</v>
       </c>
-      <c r="B57" s="33"/>
-      <c r="C57" s="34"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="36"/>
       <c r="D57" s="17">
         <v>43899</v>
       </c>
-      <c r="E57" s="33"/>
-      <c r="F57" s="34"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="36"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>43900</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="34"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="36"/>
       <c r="D58" s="17">
         <v>43900</v>
       </c>
-      <c r="E58" s="33"/>
-      <c r="F58" s="34"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="36"/>
       <c r="H58" s="4"/>
       <c r="I58" s="1"/>
       <c r="K58" s="4"/>
@@ -1646,13 +1649,13 @@
       <c r="A59" s="17">
         <v>43901</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="34"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="36"/>
       <c r="D59" s="17">
         <v>43901</v>
       </c>
-      <c r="E59" s="33"/>
-      <c r="F59" s="34"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="36"/>
       <c r="H59" s="4"/>
       <c r="I59" s="1"/>
       <c r="K59" s="4"/>
@@ -1662,25 +1665,25 @@
       <c r="A60" s="17">
         <v>43902</v>
       </c>
-      <c r="B60" s="33"/>
-      <c r="C60" s="34"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="36"/>
       <c r="D60" s="17">
         <v>43902</v>
       </c>
-      <c r="E60" s="33"/>
-      <c r="F60" s="34"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="36"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>43903</v>
       </c>
-      <c r="B61" s="33"/>
-      <c r="C61" s="34"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="36"/>
       <c r="D61" s="17">
         <v>43903</v>
       </c>
-      <c r="E61" s="33"/>
-      <c r="F61" s="34"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="36"/>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
       <c r="K61" s="4"/>
@@ -1690,25 +1693,25 @@
       <c r="A62" s="17">
         <v>43904</v>
       </c>
-      <c r="B62" s="33"/>
-      <c r="C62" s="34"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="36"/>
       <c r="D62" s="17">
         <v>43904</v>
       </c>
-      <c r="E62" s="33"/>
-      <c r="F62" s="34"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="36"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <v>43905</v>
       </c>
-      <c r="B63" s="33"/>
-      <c r="C63" s="34"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="36"/>
       <c r="D63" s="17">
         <v>43905</v>
       </c>
-      <c r="E63" s="33"/>
-      <c r="F63" s="34"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="36"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
@@ -1738,22 +1741,22 @@
       <c r="A65" s="17">
         <v>43907</v>
       </c>
-      <c r="B65" s="35" t="s">
+      <c r="B65" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="36">
+      <c r="C65" s="37">
         <v>10</v>
       </c>
       <c r="D65" s="17">
         <v>43907</v>
       </c>
-      <c r="E65" s="35" t="s">
+      <c r="E65" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="36">
+      <c r="F65" s="37">
         <v>13</v>
       </c>
-      <c r="H65" s="29" t="s">
+      <c r="H65" s="45" t="s">
         <v>17</v>
       </c>
       <c r="I65" s="46"/>
@@ -1764,14 +1767,14 @@
       <c r="A66" s="17">
         <v>43908</v>
       </c>
-      <c r="B66" s="35"/>
-      <c r="C66" s="36"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="37"/>
       <c r="D66" s="17">
         <v>43908</v>
       </c>
-      <c r="E66" s="35"/>
-      <c r="F66" s="36"/>
-      <c r="H66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="37"/>
+      <c r="H66" s="45"/>
       <c r="I66" s="46"/>
       <c r="K66" s="4"/>
       <c r="L66" s="1"/>
@@ -1780,14 +1783,14 @@
       <c r="A67" s="17">
         <v>43909</v>
       </c>
-      <c r="B67" s="35"/>
-      <c r="C67" s="36"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="37"/>
       <c r="D67" s="17">
         <v>43909</v>
       </c>
-      <c r="E67" s="35"/>
-      <c r="F67" s="36"/>
-      <c r="H67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="37"/>
+      <c r="H67" s="45"/>
       <c r="I67" s="46"/>
       <c r="K67" s="4"/>
       <c r="L67" s="1"/>
@@ -1796,50 +1799,50 @@
       <c r="A68" s="17">
         <v>43910</v>
       </c>
-      <c r="B68" s="35"/>
-      <c r="C68" s="36"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="17">
         <v>43910</v>
       </c>
-      <c r="E68" s="35"/>
-      <c r="F68" s="36"/>
-      <c r="H68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="37"/>
+      <c r="H68" s="45"/>
       <c r="I68" s="46"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <v>43911</v>
       </c>
-      <c r="B69" s="35" t="s">
+      <c r="B69" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="39">
+      <c r="C69" s="38">
         <v>4</v>
       </c>
       <c r="D69" s="17">
         <v>43911</v>
       </c>
-      <c r="E69" s="35" t="s">
+      <c r="E69" s="29" t="s">
         <v>14</v>
       </c>
       <c r="F69" s="30">
         <v>8</v>
       </c>
-      <c r="H69" s="29"/>
+      <c r="H69" s="45"/>
       <c r="I69" s="46"/>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <v>43912</v>
       </c>
-      <c r="B70" s="35"/>
-      <c r="C70" s="39"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="38"/>
       <c r="D70" s="17">
         <v>43912</v>
       </c>
-      <c r="E70" s="35"/>
+      <c r="E70" s="29"/>
       <c r="F70" s="30"/>
-      <c r="H70" s="29"/>
+      <c r="H70" s="45"/>
       <c r="I70" s="46"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -1855,13 +1858,13 @@
       <c r="D71" s="17">
         <v>43913</v>
       </c>
-      <c r="E71" s="29" t="s">
+      <c r="E71" s="45" t="s">
         <v>15</v>
       </c>
       <c r="F71" s="30">
         <v>6</v>
       </c>
-      <c r="H71" s="29"/>
+      <c r="H71" s="45"/>
       <c r="I71" s="46"/>
     </row>
     <row r="72" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1877,7 +1880,7 @@
       <c r="D72" s="17">
         <v>43914</v>
       </c>
-      <c r="E72" s="29"/>
+      <c r="E72" s="45"/>
       <c r="F72" s="30"/>
       <c r="H72" s="2" t="s">
         <v>18</v>
@@ -1912,7 +1915,7 @@
       <c r="A74" s="17">
         <v>43916</v>
       </c>
-      <c r="B74" s="35" t="s">
+      <c r="B74" s="29" t="s">
         <v>22</v>
       </c>
       <c r="C74" s="30"/>
@@ -1938,8 +1941,12 @@
       <c r="A76" s="17">
         <v>43918</v>
       </c>
-      <c r="B76" s="21"/>
-      <c r="C76" s="20"/>
+      <c r="B76" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="20">
+        <v>3</v>
+      </c>
       <c r="D76" s="17">
         <v>43918</v>
       </c>
@@ -2752,7 +2759,7 @@
       </c>
       <c r="C159" s="11">
         <f>SUM(C64:C155)</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D159" s="9" t="s">
         <v>2</v>
@@ -2776,6 +2783,9 @@
     <row r="161" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="B2:C63"/>
@@ -2792,9 +2802,6 @@
     <mergeCell ref="F71:F72"/>
     <mergeCell ref="E3:F63"/>
     <mergeCell ref="E65:E68"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modification Journal d'activité et arduino
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81BFECF-FFA7-49EA-A3B5-A77A06B88692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E98204-7686-4DDA-B98E-BE0ACCF29196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -98,13 +98,13 @@
     <t>Constantin Minos</t>
   </si>
   <si>
-    <t>Travail sur un tutoriel de la configuratrion IP fixe pour la société 13ème Porte (Ajout d'une partie pour réserver des adresses IP dans le DHCP de la Box internet de la société 13ème Porte</t>
-  </si>
-  <si>
     <t>Jour OFF (Entretien avec une école d'ingénieurs)</t>
   </si>
   <si>
     <t>Rédaction d'un document commun au groupe SFL5</t>
+  </si>
+  <si>
+    <t>Travail sur un tutoriel de la configurarion IP fixe pour la société 13ème Porte (Ajout d'une partie pour réserver des adresses IP dans le DHCP de la Box internet de la société 13ème Porte</t>
   </si>
 </sst>
 </file>
@@ -456,6 +456,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -479,9 +482,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,16 +882,16 @@
       <c r="J1" s="43"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
-      <c r="M1" s="31"/>
+      <c r="M1" s="32"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>43844</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="40"/>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
@@ -901,21 +901,21 @@
       <c r="J2" s="44"/>
       <c r="K2" s="13"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="32"/>
+      <c r="M2" s="33"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>43845</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="17">
         <v>43845</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="34"/>
+      <c r="F3" s="35"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="K3" s="3"/>
@@ -925,25 +925,25 @@
       <c r="A4" s="17">
         <v>43846</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="17">
         <v>43846</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>43847</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="17">
         <v>43847</v>
       </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1"/>
       <c r="K5" s="3"/>
@@ -953,49 +953,49 @@
       <c r="A6" s="17">
         <v>43848</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="17">
         <v>43848</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>43849</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="17">
         <v>43849</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>43850</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="17">
         <v>43850</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>43851</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="17">
         <v>43851</v>
       </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
       <c r="K9" s="3"/>
@@ -1005,13 +1005,13 @@
       <c r="A10" s="17">
         <v>43852</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="17">
         <v>43852</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
       <c r="K10" s="3"/>
@@ -1021,73 +1021,73 @@
       <c r="A11" s="17">
         <v>43853</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="17">
         <v>43853</v>
       </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>43854</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="17">
         <v>43854</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>43855</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="17">
         <v>43855</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>43856</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="17">
         <v>43856</v>
       </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>43857</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="17">
         <v>43857</v>
       </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>43858</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="17">
         <v>43858</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
       <c r="K16" s="3"/>
@@ -1097,13 +1097,13 @@
       <c r="A17" s="17">
         <v>43859</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="17">
         <v>43859</v>
       </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
       <c r="K17" s="3"/>
@@ -1113,25 +1113,25 @@
       <c r="A18" s="17">
         <v>43860</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="17">
         <v>43860</v>
       </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>43861</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="17">
         <v>43861</v>
       </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
       <c r="I19" s="1"/>
       <c r="L19" s="1"/>
     </row>
@@ -1139,49 +1139,49 @@
       <c r="A20" s="17">
         <v>43862</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="17">
         <v>43862</v>
       </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>43863</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="17">
         <v>43863</v>
       </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>43864</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="17">
         <v>43864</v>
       </c>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>43865</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="17">
         <v>43865</v>
       </c>
-      <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="37"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
       <c r="K23" s="3"/>
@@ -1191,13 +1191,13 @@
       <c r="A24" s="17">
         <v>43866</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="17">
         <v>43866</v>
       </c>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
       <c r="K24" s="3"/>
@@ -1207,25 +1207,25 @@
       <c r="A25" s="17">
         <v>43867</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="17">
         <v>43867</v>
       </c>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>43868</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="17">
         <v>43868</v>
       </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
       <c r="K26" s="3"/>
@@ -1235,49 +1235,49 @@
       <c r="A27" s="17">
         <v>43869</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="36"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="17">
         <v>43869</v>
       </c>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>43870</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="36"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="17">
         <v>43870</v>
       </c>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>43871</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="36"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="17">
         <v>43871</v>
       </c>
-      <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="37"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>43872</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="36"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="17">
         <v>43872</v>
       </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="37"/>
       <c r="H30" s="3"/>
       <c r="I30" s="1"/>
       <c r="K30" s="3"/>
@@ -1287,13 +1287,13 @@
       <c r="A31" s="17">
         <v>43873</v>
       </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="17">
         <v>43873</v>
       </c>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="37"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
       <c r="K31" s="3"/>
@@ -1303,25 +1303,25 @@
       <c r="A32" s="17">
         <v>43874</v>
       </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="17">
         <v>43874</v>
       </c>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="37"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>43875</v>
       </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="36"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="17">
         <v>43875</v>
       </c>
-      <c r="E33" s="35"/>
-      <c r="F33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="37"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
       <c r="K33" s="3"/>
@@ -1331,145 +1331,145 @@
       <c r="A34" s="17">
         <v>43876</v>
       </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="36"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="17">
         <v>43876</v>
       </c>
-      <c r="E34" s="35"/>
-      <c r="F34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="37"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>43877</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="36"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="17">
         <v>43877</v>
       </c>
-      <c r="E35" s="35"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="37"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>43878</v>
       </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="36"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="37"/>
       <c r="D36" s="17">
         <v>43878</v>
       </c>
-      <c r="E36" s="35"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="37"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>43879</v>
       </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="36"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="17">
         <v>43879</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="37"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>43880</v>
       </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="36"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="37"/>
       <c r="D38" s="17">
         <v>43880</v>
       </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="37"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>43881</v>
       </c>
-      <c r="B39" s="35"/>
-      <c r="C39" s="36"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="37"/>
       <c r="D39" s="17">
         <v>43881</v>
       </c>
-      <c r="E39" s="35"/>
-      <c r="F39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="37"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>43882</v>
       </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="36"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="37"/>
       <c r="D40" s="17">
         <v>43882</v>
       </c>
-      <c r="E40" s="35"/>
-      <c r="F40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>43883</v>
       </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="36"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="17">
         <v>43883</v>
       </c>
-      <c r="E41" s="35"/>
-      <c r="F41" s="36"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="37"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>43884</v>
       </c>
-      <c r="B42" s="35"/>
-      <c r="C42" s="36"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="37"/>
       <c r="D42" s="17">
         <v>43884</v>
       </c>
-      <c r="E42" s="35"/>
-      <c r="F42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="37"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>43885</v>
       </c>
-      <c r="B43" s="35"/>
-      <c r="C43" s="36"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="37"/>
       <c r="D43" s="17">
         <v>43885</v>
       </c>
-      <c r="E43" s="35"/>
-      <c r="F43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="37"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>43886</v>
       </c>
-      <c r="B44" s="35"/>
-      <c r="C44" s="36"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="37"/>
       <c r="D44" s="17">
         <v>43886</v>
       </c>
-      <c r="E44" s="35"/>
-      <c r="F44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="37"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>43887</v>
       </c>
-      <c r="B45" s="35"/>
-      <c r="C45" s="36"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="37"/>
       <c r="D45" s="17">
         <v>43887</v>
       </c>
-      <c r="E45" s="35"/>
-      <c r="F45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="37"/>
       <c r="H45" s="4"/>
       <c r="K45" s="4"/>
     </row>
@@ -1477,73 +1477,73 @@
       <c r="A46" s="17">
         <v>43888</v>
       </c>
-      <c r="B46" s="35"/>
-      <c r="C46" s="36"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="37"/>
       <c r="D46" s="17">
         <v>43888</v>
       </c>
-      <c r="E46" s="35"/>
-      <c r="F46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="37"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>43889</v>
       </c>
-      <c r="B47" s="35"/>
-      <c r="C47" s="36"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="37"/>
       <c r="D47" s="17">
         <v>43889</v>
       </c>
-      <c r="E47" s="35"/>
-      <c r="F47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="37"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>43890</v>
       </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="36"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="37"/>
       <c r="D48" s="17">
         <v>43890</v>
       </c>
-      <c r="E48" s="35"/>
-      <c r="F48" s="36"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="37"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>43891</v>
       </c>
-      <c r="B49" s="35"/>
-      <c r="C49" s="36"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="37"/>
       <c r="D49" s="17">
         <v>43891</v>
       </c>
-      <c r="E49" s="35"/>
-      <c r="F49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="37"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>43892</v>
       </c>
-      <c r="B50" s="35"/>
-      <c r="C50" s="36"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="37"/>
       <c r="D50" s="17">
         <v>43892</v>
       </c>
-      <c r="E50" s="35"/>
-      <c r="F50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="37"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>43893</v>
       </c>
-      <c r="B51" s="35"/>
-      <c r="C51" s="36"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="37"/>
       <c r="D51" s="17">
         <v>43893</v>
       </c>
-      <c r="E51" s="35"/>
-      <c r="F51" s="36"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="37"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
       <c r="K51" s="4"/>
@@ -1553,13 +1553,13 @@
       <c r="A52" s="17">
         <v>43894</v>
       </c>
-      <c r="B52" s="35"/>
-      <c r="C52" s="36"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="37"/>
       <c r="D52" s="17">
         <v>43894</v>
       </c>
-      <c r="E52" s="35"/>
-      <c r="F52" s="36"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="37"/>
       <c r="H52" s="4"/>
       <c r="I52" s="1"/>
       <c r="K52" s="4"/>
@@ -1569,25 +1569,25 @@
       <c r="A53" s="17">
         <v>43895</v>
       </c>
-      <c r="B53" s="35"/>
-      <c r="C53" s="36"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="17">
         <v>43895</v>
       </c>
-      <c r="E53" s="35"/>
-      <c r="F53" s="36"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="37"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>43896</v>
       </c>
-      <c r="B54" s="35"/>
-      <c r="C54" s="36"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="37"/>
       <c r="D54" s="17">
         <v>43896</v>
       </c>
-      <c r="E54" s="35"/>
-      <c r="F54" s="36"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="37"/>
       <c r="H54" s="4"/>
       <c r="I54" s="1"/>
       <c r="K54" s="4"/>
@@ -1597,49 +1597,49 @@
       <c r="A55" s="17">
         <v>43897</v>
       </c>
-      <c r="B55" s="35"/>
-      <c r="C55" s="36"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="17">
         <v>43897</v>
       </c>
-      <c r="E55" s="35"/>
-      <c r="F55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="37"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>43898</v>
       </c>
-      <c r="B56" s="35"/>
-      <c r="C56" s="36"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="37"/>
       <c r="D56" s="17">
         <v>43898</v>
       </c>
-      <c r="E56" s="35"/>
-      <c r="F56" s="36"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="37"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>43899</v>
       </c>
-      <c r="B57" s="35"/>
-      <c r="C57" s="36"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="37"/>
       <c r="D57" s="17">
         <v>43899</v>
       </c>
-      <c r="E57" s="35"/>
-      <c r="F57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="37"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>43900</v>
       </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="36"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="37"/>
       <c r="D58" s="17">
         <v>43900</v>
       </c>
-      <c r="E58" s="35"/>
-      <c r="F58" s="36"/>
+      <c r="E58" s="36"/>
+      <c r="F58" s="37"/>
       <c r="H58" s="4"/>
       <c r="I58" s="1"/>
       <c r="K58" s="4"/>
@@ -1649,13 +1649,13 @@
       <c r="A59" s="17">
         <v>43901</v>
       </c>
-      <c r="B59" s="35"/>
-      <c r="C59" s="36"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="37"/>
       <c r="D59" s="17">
         <v>43901</v>
       </c>
-      <c r="E59" s="35"/>
-      <c r="F59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="37"/>
       <c r="H59" s="4"/>
       <c r="I59" s="1"/>
       <c r="K59" s="4"/>
@@ -1665,25 +1665,25 @@
       <c r="A60" s="17">
         <v>43902</v>
       </c>
-      <c r="B60" s="35"/>
-      <c r="C60" s="36"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="37"/>
       <c r="D60" s="17">
         <v>43902</v>
       </c>
-      <c r="E60" s="35"/>
-      <c r="F60" s="36"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="37"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>43903</v>
       </c>
-      <c r="B61" s="35"/>
-      <c r="C61" s="36"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="37"/>
       <c r="D61" s="17">
         <v>43903</v>
       </c>
-      <c r="E61" s="35"/>
-      <c r="F61" s="36"/>
+      <c r="E61" s="36"/>
+      <c r="F61" s="37"/>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
       <c r="K61" s="4"/>
@@ -1693,25 +1693,25 @@
       <c r="A62" s="17">
         <v>43904</v>
       </c>
-      <c r="B62" s="35"/>
-      <c r="C62" s="36"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="37"/>
       <c r="D62" s="17">
         <v>43904</v>
       </c>
-      <c r="E62" s="35"/>
-      <c r="F62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="37"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <v>43905</v>
       </c>
-      <c r="B63" s="35"/>
-      <c r="C63" s="36"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="37"/>
       <c r="D63" s="17">
         <v>43905</v>
       </c>
-      <c r="E63" s="35"/>
-      <c r="F63" s="36"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="37"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
@@ -1741,19 +1741,19 @@
       <c r="A65" s="17">
         <v>43907</v>
       </c>
-      <c r="B65" s="29" t="s">
+      <c r="B65" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="37">
+      <c r="C65" s="29">
         <v>10</v>
       </c>
       <c r="D65" s="17">
         <v>43907</v>
       </c>
-      <c r="E65" s="29" t="s">
+      <c r="E65" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="37">
+      <c r="F65" s="29">
         <v>13</v>
       </c>
       <c r="H65" s="45" t="s">
@@ -1767,13 +1767,13 @@
       <c r="A66" s="17">
         <v>43908</v>
       </c>
-      <c r="B66" s="29"/>
-      <c r="C66" s="37"/>
+      <c r="B66" s="30"/>
+      <c r="C66" s="29"/>
       <c r="D66" s="17">
         <v>43908</v>
       </c>
-      <c r="E66" s="29"/>
-      <c r="F66" s="37"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="29"/>
       <c r="H66" s="45"/>
       <c r="I66" s="46"/>
       <c r="K66" s="4"/>
@@ -1783,13 +1783,13 @@
       <c r="A67" s="17">
         <v>43909</v>
       </c>
-      <c r="B67" s="29"/>
-      <c r="C67" s="37"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="29"/>
       <c r="D67" s="17">
         <v>43909</v>
       </c>
-      <c r="E67" s="29"/>
-      <c r="F67" s="37"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="29"/>
       <c r="H67" s="45"/>
       <c r="I67" s="46"/>
       <c r="K67" s="4"/>
@@ -1799,13 +1799,13 @@
       <c r="A68" s="17">
         <v>43910</v>
       </c>
-      <c r="B68" s="29"/>
-      <c r="C68" s="37"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="29"/>
       <c r="D68" s="17">
         <v>43910</v>
       </c>
-      <c r="E68" s="29"/>
-      <c r="F68" s="37"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="29"/>
       <c r="H68" s="45"/>
       <c r="I68" s="46"/>
     </row>
@@ -1813,7 +1813,7 @@
       <c r="A69" s="17">
         <v>43911</v>
       </c>
-      <c r="B69" s="29" t="s">
+      <c r="B69" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C69" s="38">
@@ -1822,10 +1822,10 @@
       <c r="D69" s="17">
         <v>43911</v>
       </c>
-      <c r="E69" s="29" t="s">
+      <c r="E69" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="30">
+      <c r="F69" s="31">
         <v>8</v>
       </c>
       <c r="H69" s="45"/>
@@ -1835,13 +1835,13 @@
       <c r="A70" s="17">
         <v>43912</v>
       </c>
-      <c r="B70" s="29"/>
+      <c r="B70" s="30"/>
       <c r="C70" s="38"/>
       <c r="D70" s="17">
         <v>43912</v>
       </c>
-      <c r="E70" s="29"/>
-      <c r="F70" s="30"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="31"/>
       <c r="H70" s="45"/>
       <c r="I70" s="46"/>
     </row>
@@ -1861,7 +1861,7 @@
       <c r="E71" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F71" s="30">
+      <c r="F71" s="31">
         <v>6</v>
       </c>
       <c r="H71" s="45"/>
@@ -1881,7 +1881,7 @@
         <v>43914</v>
       </c>
       <c r="E72" s="45"/>
-      <c r="F72" s="30"/>
+      <c r="F72" s="31"/>
       <c r="H72" s="2" t="s">
         <v>18</v>
       </c>
@@ -1915,10 +1915,10 @@
       <c r="A74" s="17">
         <v>43916</v>
       </c>
-      <c r="B74" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C74" s="30"/>
+      <c r="B74" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C74" s="31"/>
       <c r="D74" s="17">
         <v>43916</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>43917</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C75" s="20">
         <v>2</v>
@@ -1942,7 +1942,7 @@
         <v>43918</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C76" s="20">
         <v>3</v>
@@ -1955,8 +1955,7 @@
       <c r="A77" s="17">
         <v>43919</v>
       </c>
-      <c r="B77" s="21"/>
-      <c r="C77" s="20"/>
+      <c r="C77" s="21"/>
       <c r="D77" s="17">
         <v>43919</v>
       </c>
@@ -2783,6 +2782,9 @@
     <row r="161" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="E3:F63"/>
+    <mergeCell ref="E65:E68"/>
     <mergeCell ref="F65:F68"/>
     <mergeCell ref="E69:E70"/>
     <mergeCell ref="F69:F70"/>
@@ -2799,9 +2801,6 @@
     <mergeCell ref="H65:H71"/>
     <mergeCell ref="I65:I71"/>
     <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="E3:F63"/>
-    <mergeCell ref="E65:E68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Journal d'activité + ajout de connexion.php
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E98204-7686-4DDA-B98E-BE0ACCF29196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9FC05E-69F8-4B76-9B83-AEEF2E9AEFD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Travail sur un tutoriel de la configurarion IP fixe pour la société 13ème Porte (Ajout d'une partie pour réserver des adresses IP dans le DHCP de la Box internet de la société 13ème Porte</t>
+  </si>
+  <si>
+    <t>Création du fichier connexion.php, intégration à la l'appli Web + téléchargement de Wamp &amp; PhpMyAdmin</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -456,32 +459,38 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -831,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +872,7 @@
       <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="41" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="22" t="s">
@@ -872,50 +881,50 @@
       <c r="F1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="41"/>
+      <c r="G1" s="43"/>
       <c r="H1" s="12" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="43"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
-      <c r="M1" s="32"/>
+      <c r="M1" s="38"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>43844</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
-      <c r="G2" s="42"/>
+      <c r="G2" s="44"/>
       <c r="H2" s="13"/>
       <c r="I2" s="15"/>
-      <c r="J2" s="44"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="13"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="33"/>
+      <c r="M2" s="39"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>43845</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="17">
         <v>43845</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="35"/>
+      <c r="F3" s="33"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="K3" s="3"/>
@@ -925,25 +934,25 @@
       <c r="A4" s="17">
         <v>43846</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="17">
         <v>43846</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>43847</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="17">
         <v>43847</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="35"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1"/>
       <c r="K5" s="3"/>
@@ -953,49 +962,49 @@
       <c r="A6" s="17">
         <v>43848</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="17">
         <v>43848</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>43849</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="17">
         <v>43849</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>43850</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="17">
         <v>43850</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>43851</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="17">
         <v>43851</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
       <c r="K9" s="3"/>
@@ -1005,13 +1014,13 @@
       <c r="A10" s="17">
         <v>43852</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="17">
         <v>43852</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
       <c r="K10" s="3"/>
@@ -1021,73 +1030,73 @@
       <c r="A11" s="17">
         <v>43853</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="17">
         <v>43853</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>43854</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="17">
         <v>43854</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>43855</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="17">
         <v>43855</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>43856</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="17">
         <v>43856</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>43857</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="17">
         <v>43857</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>43858</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="17">
         <v>43858</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
       <c r="K16" s="3"/>
@@ -1097,13 +1106,13 @@
       <c r="A17" s="17">
         <v>43859</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="17">
         <v>43859</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="37"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
       <c r="K17" s="3"/>
@@ -1113,25 +1122,25 @@
       <c r="A18" s="17">
         <v>43860</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="17">
         <v>43860</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="37"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>43861</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="17">
         <v>43861</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="37"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
       <c r="I19" s="1"/>
       <c r="L19" s="1"/>
     </row>
@@ -1139,49 +1148,49 @@
       <c r="A20" s="17">
         <v>43862</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="17">
         <v>43862</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>43863</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="17">
         <v>43863</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="37"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>43864</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="17">
         <v>43864</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="37"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>43865</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="17">
         <v>43865</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="37"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="35"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
       <c r="K23" s="3"/>
@@ -1191,13 +1200,13 @@
       <c r="A24" s="17">
         <v>43866</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
       <c r="D24" s="17">
         <v>43866</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="37"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="35"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
       <c r="K24" s="3"/>
@@ -1207,25 +1216,25 @@
       <c r="A25" s="17">
         <v>43867</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="37"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="17">
         <v>43867</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="37"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>43868</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="17">
         <v>43868</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
       <c r="K26" s="3"/>
@@ -1235,49 +1244,49 @@
       <c r="A27" s="17">
         <v>43869</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="37"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
       <c r="D27" s="17">
         <v>43869</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>43870</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="37"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="35"/>
       <c r="D28" s="17">
         <v>43870</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="37"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>43871</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="37"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
       <c r="D29" s="17">
         <v>43871</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="37"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>43872</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="37"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
       <c r="D30" s="17">
         <v>43872</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="37"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="35"/>
       <c r="H30" s="3"/>
       <c r="I30" s="1"/>
       <c r="K30" s="3"/>
@@ -1287,13 +1296,13 @@
       <c r="A31" s="17">
         <v>43873</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="37"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
       <c r="D31" s="17">
         <v>43873</v>
       </c>
-      <c r="E31" s="36"/>
-      <c r="F31" s="37"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="35"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
       <c r="K31" s="3"/>
@@ -1303,25 +1312,25 @@
       <c r="A32" s="17">
         <v>43874</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="37"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="35"/>
       <c r="D32" s="17">
         <v>43874</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="37"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="35"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>43875</v>
       </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="37"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="35"/>
       <c r="D33" s="17">
         <v>43875</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="37"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="35"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
       <c r="K33" s="3"/>
@@ -1331,145 +1340,145 @@
       <c r="A34" s="17">
         <v>43876</v>
       </c>
-      <c r="B34" s="36"/>
-      <c r="C34" s="37"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
       <c r="D34" s="17">
         <v>43876</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="37"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="35"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>43877</v>
       </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="37"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="35"/>
       <c r="D35" s="17">
         <v>43877</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="37"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="35"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>43878</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="37"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="35"/>
       <c r="D36" s="17">
         <v>43878</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="37"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="35"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>43879</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="37"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="35"/>
       <c r="D37" s="17">
         <v>43879</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="37"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="35"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>43880</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="37"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
       <c r="D38" s="17">
         <v>43880</v>
       </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="37"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="35"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>43881</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="37"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="35"/>
       <c r="D39" s="17">
         <v>43881</v>
       </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="37"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="35"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>43882</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="37"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="35"/>
       <c r="D40" s="17">
         <v>43882</v>
       </c>
-      <c r="E40" s="36"/>
-      <c r="F40" s="37"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="35"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>43883</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="37"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="35"/>
       <c r="D41" s="17">
         <v>43883</v>
       </c>
-      <c r="E41" s="36"/>
-      <c r="F41" s="37"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="35"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>43884</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="37"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="35"/>
       <c r="D42" s="17">
         <v>43884</v>
       </c>
-      <c r="E42" s="36"/>
-      <c r="F42" s="37"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="35"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>43885</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="37"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="35"/>
       <c r="D43" s="17">
         <v>43885</v>
       </c>
-      <c r="E43" s="36"/>
-      <c r="F43" s="37"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="35"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>43886</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="37"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="35"/>
       <c r="D44" s="17">
         <v>43886</v>
       </c>
-      <c r="E44" s="36"/>
-      <c r="F44" s="37"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="35"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>43887</v>
       </c>
-      <c r="B45" s="36"/>
-      <c r="C45" s="37"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="35"/>
       <c r="D45" s="17">
         <v>43887</v>
       </c>
-      <c r="E45" s="36"/>
-      <c r="F45" s="37"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="35"/>
       <c r="H45" s="4"/>
       <c r="K45" s="4"/>
     </row>
@@ -1477,73 +1486,73 @@
       <c r="A46" s="17">
         <v>43888</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="37"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="35"/>
       <c r="D46" s="17">
         <v>43888</v>
       </c>
-      <c r="E46" s="36"/>
-      <c r="F46" s="37"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="35"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>43889</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="37"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="35"/>
       <c r="D47" s="17">
         <v>43889</v>
       </c>
-      <c r="E47" s="36"/>
-      <c r="F47" s="37"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="35"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>43890</v>
       </c>
-      <c r="B48" s="36"/>
-      <c r="C48" s="37"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="35"/>
       <c r="D48" s="17">
         <v>43890</v>
       </c>
-      <c r="E48" s="36"/>
-      <c r="F48" s="37"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="35"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>43891</v>
       </c>
-      <c r="B49" s="36"/>
-      <c r="C49" s="37"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="35"/>
       <c r="D49" s="17">
         <v>43891</v>
       </c>
-      <c r="E49" s="36"/>
-      <c r="F49" s="37"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="35"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>43892</v>
       </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="37"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="35"/>
       <c r="D50" s="17">
         <v>43892</v>
       </c>
-      <c r="E50" s="36"/>
-      <c r="F50" s="37"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="35"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>43893</v>
       </c>
-      <c r="B51" s="36"/>
-      <c r="C51" s="37"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="35"/>
       <c r="D51" s="17">
         <v>43893</v>
       </c>
-      <c r="E51" s="36"/>
-      <c r="F51" s="37"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="35"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
       <c r="K51" s="4"/>
@@ -1553,13 +1562,13 @@
       <c r="A52" s="17">
         <v>43894</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="37"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="35"/>
       <c r="D52" s="17">
         <v>43894</v>
       </c>
-      <c r="E52" s="36"/>
-      <c r="F52" s="37"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="35"/>
       <c r="H52" s="4"/>
       <c r="I52" s="1"/>
       <c r="K52" s="4"/>
@@ -1569,25 +1578,25 @@
       <c r="A53" s="17">
         <v>43895</v>
       </c>
-      <c r="B53" s="36"/>
-      <c r="C53" s="37"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="35"/>
       <c r="D53" s="17">
         <v>43895</v>
       </c>
-      <c r="E53" s="36"/>
-      <c r="F53" s="37"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="35"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>43896</v>
       </c>
-      <c r="B54" s="36"/>
-      <c r="C54" s="37"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="35"/>
       <c r="D54" s="17">
         <v>43896</v>
       </c>
-      <c r="E54" s="36"/>
-      <c r="F54" s="37"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="35"/>
       <c r="H54" s="4"/>
       <c r="I54" s="1"/>
       <c r="K54" s="4"/>
@@ -1597,49 +1606,49 @@
       <c r="A55" s="17">
         <v>43897</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="37"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="35"/>
       <c r="D55" s="17">
         <v>43897</v>
       </c>
-      <c r="E55" s="36"/>
-      <c r="F55" s="37"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="35"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>43898</v>
       </c>
-      <c r="B56" s="36"/>
-      <c r="C56" s="37"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="35"/>
       <c r="D56" s="17">
         <v>43898</v>
       </c>
-      <c r="E56" s="36"/>
-      <c r="F56" s="37"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="35"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>43899</v>
       </c>
-      <c r="B57" s="36"/>
-      <c r="C57" s="37"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="35"/>
       <c r="D57" s="17">
         <v>43899</v>
       </c>
-      <c r="E57" s="36"/>
-      <c r="F57" s="37"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="35"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>43900</v>
       </c>
-      <c r="B58" s="36"/>
-      <c r="C58" s="37"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="35"/>
       <c r="D58" s="17">
         <v>43900</v>
       </c>
-      <c r="E58" s="36"/>
-      <c r="F58" s="37"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="35"/>
       <c r="H58" s="4"/>
       <c r="I58" s="1"/>
       <c r="K58" s="4"/>
@@ -1649,13 +1658,13 @@
       <c r="A59" s="17">
         <v>43901</v>
       </c>
-      <c r="B59" s="36"/>
-      <c r="C59" s="37"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="35"/>
       <c r="D59" s="17">
         <v>43901</v>
       </c>
-      <c r="E59" s="36"/>
-      <c r="F59" s="37"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="35"/>
       <c r="H59" s="4"/>
       <c r="I59" s="1"/>
       <c r="K59" s="4"/>
@@ -1665,25 +1674,25 @@
       <c r="A60" s="17">
         <v>43902</v>
       </c>
-      <c r="B60" s="36"/>
-      <c r="C60" s="37"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="35"/>
       <c r="D60" s="17">
         <v>43902</v>
       </c>
-      <c r="E60" s="36"/>
-      <c r="F60" s="37"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="35"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>43903</v>
       </c>
-      <c r="B61" s="36"/>
-      <c r="C61" s="37"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="35"/>
       <c r="D61" s="17">
         <v>43903</v>
       </c>
-      <c r="E61" s="36"/>
-      <c r="F61" s="37"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="35"/>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
       <c r="K61" s="4"/>
@@ -1693,25 +1702,25 @@
       <c r="A62" s="17">
         <v>43904</v>
       </c>
-      <c r="B62" s="36"/>
-      <c r="C62" s="37"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="35"/>
       <c r="D62" s="17">
         <v>43904</v>
       </c>
-      <c r="E62" s="36"/>
-      <c r="F62" s="37"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="35"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <v>43905</v>
       </c>
-      <c r="B63" s="36"/>
-      <c r="C63" s="37"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="35"/>
       <c r="D63" s="17">
         <v>43905</v>
       </c>
-      <c r="E63" s="36"/>
-      <c r="F63" s="37"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="35"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
@@ -1741,25 +1750,25 @@
       <c r="A65" s="17">
         <v>43907</v>
       </c>
-      <c r="B65" s="30" t="s">
+      <c r="B65" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="29">
+      <c r="C65" s="37">
         <v>10</v>
       </c>
       <c r="D65" s="17">
         <v>43907</v>
       </c>
-      <c r="E65" s="30" t="s">
+      <c r="E65" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="29">
+      <c r="F65" s="37">
         <v>13</v>
       </c>
-      <c r="H65" s="45" t="s">
+      <c r="H65" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="I65" s="46"/>
+      <c r="I65" s="48"/>
       <c r="K65" s="4"/>
       <c r="L65" s="1"/>
     </row>
@@ -1767,15 +1776,15 @@
       <c r="A66" s="17">
         <v>43908</v>
       </c>
-      <c r="B66" s="30"/>
-      <c r="C66" s="29"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="37"/>
       <c r="D66" s="17">
         <v>43908</v>
       </c>
-      <c r="E66" s="30"/>
-      <c r="F66" s="29"/>
-      <c r="H66" s="45"/>
-      <c r="I66" s="46"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="37"/>
+      <c r="H66" s="47"/>
+      <c r="I66" s="48"/>
       <c r="K66" s="4"/>
       <c r="L66" s="1"/>
     </row>
@@ -1783,15 +1792,15 @@
       <c r="A67" s="17">
         <v>43909</v>
       </c>
-      <c r="B67" s="30"/>
-      <c r="C67" s="29"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="37"/>
       <c r="D67" s="17">
         <v>43909</v>
       </c>
-      <c r="E67" s="30"/>
-      <c r="F67" s="29"/>
-      <c r="H67" s="45"/>
-      <c r="I67" s="46"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="37"/>
+      <c r="H67" s="47"/>
+      <c r="I67" s="48"/>
       <c r="K67" s="4"/>
       <c r="L67" s="1"/>
     </row>
@@ -1799,51 +1808,51 @@
       <c r="A68" s="17">
         <v>43910</v>
       </c>
-      <c r="B68" s="30"/>
-      <c r="C68" s="29"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="17">
         <v>43910</v>
       </c>
-      <c r="E68" s="30"/>
-      <c r="F68" s="29"/>
-      <c r="H68" s="45"/>
-      <c r="I68" s="46"/>
+      <c r="E68" s="36"/>
+      <c r="F68" s="37"/>
+      <c r="H68" s="47"/>
+      <c r="I68" s="48"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <v>43911</v>
       </c>
-      <c r="B69" s="30" t="s">
+      <c r="B69" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="38">
+      <c r="C69" s="40">
         <v>4</v>
       </c>
       <c r="D69" s="17">
         <v>43911</v>
       </c>
-      <c r="E69" s="30" t="s">
+      <c r="E69" s="36" t="s">
         <v>14</v>
       </c>
       <c r="F69" s="31">
         <v>8</v>
       </c>
-      <c r="H69" s="45"/>
-      <c r="I69" s="46"/>
+      <c r="H69" s="47"/>
+      <c r="I69" s="48"/>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <v>43912</v>
       </c>
-      <c r="B70" s="30"/>
-      <c r="C70" s="38"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="40"/>
       <c r="D70" s="17">
         <v>43912</v>
       </c>
-      <c r="E70" s="30"/>
+      <c r="E70" s="36"/>
       <c r="F70" s="31"/>
-      <c r="H70" s="45"/>
-      <c r="I70" s="46"/>
+      <c r="H70" s="47"/>
+      <c r="I70" s="48"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
@@ -1858,14 +1867,14 @@
       <c r="D71" s="17">
         <v>43913</v>
       </c>
-      <c r="E71" s="45" t="s">
+      <c r="E71" s="47" t="s">
         <v>15</v>
       </c>
       <c r="F71" s="31">
         <v>6</v>
       </c>
-      <c r="H71" s="45"/>
-      <c r="I71" s="46"/>
+      <c r="H71" s="47"/>
+      <c r="I71" s="48"/>
     </row>
     <row r="72" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
@@ -1880,7 +1889,7 @@
       <c r="D72" s="17">
         <v>43914</v>
       </c>
-      <c r="E72" s="45"/>
+      <c r="E72" s="47"/>
       <c r="F72" s="31"/>
       <c r="H72" s="2" t="s">
         <v>18</v>
@@ -1915,7 +1924,7 @@
       <c r="A74" s="17">
         <v>43916</v>
       </c>
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="36" t="s">
         <v>21</v>
       </c>
       <c r="C74" s="31"/>
@@ -1955,17 +1964,22 @@
       <c r="A77" s="17">
         <v>43919</v>
       </c>
-      <c r="C77" s="21"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
       <c r="D77" s="17">
         <v>43919</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="17">
         <v>43920</v>
       </c>
-      <c r="B78" s="21"/>
-      <c r="C78" s="20"/>
+      <c r="B78" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C78" s="21">
+        <v>2</v>
+      </c>
       <c r="D78" s="17">
         <v>43920</v>
       </c>
@@ -1974,8 +1988,8 @@
       <c r="A79" s="17">
         <v>43921</v>
       </c>
-      <c r="B79" s="21"/>
-      <c r="C79" s="20"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="30"/>
       <c r="D79" s="17">
         <v>43921</v>
       </c>
@@ -1984,8 +1998,8 @@
       <c r="A80" s="17">
         <v>43922</v>
       </c>
-      <c r="B80" s="21"/>
-      <c r="C80" s="20"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="30"/>
       <c r="D80" s="17">
         <v>43922</v>
       </c>
@@ -1994,8 +2008,8 @@
       <c r="A81" s="17">
         <v>43923</v>
       </c>
-      <c r="B81" s="21"/>
-      <c r="C81" s="20"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="30"/>
       <c r="D81" s="17">
         <v>43923</v>
       </c>
@@ -2004,8 +2018,8 @@
       <c r="A82" s="17">
         <v>43924</v>
       </c>
-      <c r="B82" s="21"/>
-      <c r="C82" s="20"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="30"/>
       <c r="D82" s="17">
         <v>43924</v>
       </c>
@@ -2014,8 +2028,8 @@
       <c r="A83" s="17">
         <v>43925</v>
       </c>
-      <c r="B83" s="21"/>
-      <c r="C83" s="20"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="30"/>
       <c r="D83" s="17">
         <v>43925</v>
       </c>
@@ -2024,8 +2038,8 @@
       <c r="A84" s="17">
         <v>43926</v>
       </c>
-      <c r="B84" s="21"/>
-      <c r="C84" s="20"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="30"/>
       <c r="D84" s="17">
         <v>43926</v>
       </c>
@@ -2034,8 +2048,8 @@
       <c r="A85" s="17">
         <v>43927</v>
       </c>
-      <c r="B85" s="21"/>
-      <c r="C85" s="20"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="30"/>
       <c r="D85" s="17">
         <v>43927</v>
       </c>
@@ -2044,8 +2058,8 @@
       <c r="A86" s="17">
         <v>43928</v>
       </c>
-      <c r="B86" s="21"/>
-      <c r="C86" s="20"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="30"/>
       <c r="D86" s="17">
         <v>43928</v>
       </c>
@@ -2054,8 +2068,8 @@
       <c r="A87" s="17">
         <v>43929</v>
       </c>
-      <c r="B87" s="21"/>
-      <c r="C87" s="20"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="30"/>
       <c r="D87" s="17">
         <v>43929</v>
       </c>
@@ -2064,8 +2078,8 @@
       <c r="A88" s="17">
         <v>43930</v>
       </c>
-      <c r="B88" s="21"/>
-      <c r="C88" s="20"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="30"/>
       <c r="D88" s="17">
         <v>43930</v>
       </c>
@@ -2074,8 +2088,8 @@
       <c r="A89" s="17">
         <v>43931</v>
       </c>
-      <c r="B89" s="21"/>
-      <c r="C89" s="20"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="30"/>
       <c r="D89" s="17">
         <v>43931</v>
       </c>
@@ -2084,8 +2098,8 @@
       <c r="A90" s="17">
         <v>43932</v>
       </c>
-      <c r="B90" s="21"/>
-      <c r="C90" s="20"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="30"/>
       <c r="D90" s="17">
         <v>43932</v>
       </c>
@@ -2094,8 +2108,8 @@
       <c r="A91" s="17">
         <v>43933</v>
       </c>
-      <c r="B91" s="21"/>
-      <c r="C91" s="20"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="30"/>
       <c r="D91" s="17">
         <v>43933</v>
       </c>
@@ -2104,8 +2118,8 @@
       <c r="A92" s="17">
         <v>43934</v>
       </c>
-      <c r="B92" s="21"/>
-      <c r="C92" s="20"/>
+      <c r="B92" s="29"/>
+      <c r="C92" s="30"/>
       <c r="D92" s="17">
         <v>43934</v>
       </c>
@@ -2114,8 +2128,8 @@
       <c r="A93" s="17">
         <v>43935</v>
       </c>
-      <c r="B93" s="21"/>
-      <c r="C93" s="20"/>
+      <c r="B93" s="29"/>
+      <c r="C93" s="30"/>
       <c r="D93" s="17">
         <v>43935</v>
       </c>
@@ -2124,8 +2138,8 @@
       <c r="A94" s="17">
         <v>43936</v>
       </c>
-      <c r="B94" s="21"/>
-      <c r="C94" s="20"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="30"/>
       <c r="D94" s="17">
         <v>43936</v>
       </c>
@@ -2134,8 +2148,8 @@
       <c r="A95" s="17">
         <v>43937</v>
       </c>
-      <c r="B95" s="21"/>
-      <c r="C95" s="20"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="30"/>
       <c r="D95" s="17">
         <v>43937</v>
       </c>
@@ -2144,8 +2158,8 @@
       <c r="A96" s="17">
         <v>43938</v>
       </c>
-      <c r="B96" s="21"/>
-      <c r="C96" s="20"/>
+      <c r="B96" s="29"/>
+      <c r="C96" s="30"/>
       <c r="D96" s="17">
         <v>43938</v>
       </c>
@@ -2154,8 +2168,8 @@
       <c r="A97" s="17">
         <v>43939</v>
       </c>
-      <c r="B97" s="21"/>
-      <c r="C97" s="20"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="30"/>
       <c r="D97" s="17">
         <v>43939</v>
       </c>
@@ -2164,8 +2178,8 @@
       <c r="A98" s="17">
         <v>43940</v>
       </c>
-      <c r="B98" s="21"/>
-      <c r="C98" s="20"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="30"/>
       <c r="D98" s="17">
         <v>43940</v>
       </c>
@@ -2174,8 +2188,8 @@
       <c r="A99" s="17">
         <v>43941</v>
       </c>
-      <c r="B99" s="21"/>
-      <c r="C99" s="20"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="30"/>
       <c r="D99" s="17">
         <v>43941</v>
       </c>
@@ -2184,8 +2198,8 @@
       <c r="A100" s="17">
         <v>43942</v>
       </c>
-      <c r="B100" s="21"/>
-      <c r="C100" s="20"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="30"/>
       <c r="D100" s="17">
         <v>43942</v>
       </c>
@@ -2194,8 +2208,8 @@
       <c r="A101" s="17">
         <v>43943</v>
       </c>
-      <c r="B101" s="21"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="29"/>
+      <c r="C101" s="30"/>
       <c r="D101" s="17">
         <v>43943</v>
       </c>
@@ -2204,8 +2218,8 @@
       <c r="A102" s="17">
         <v>43944</v>
       </c>
-      <c r="B102" s="21"/>
-      <c r="C102" s="20"/>
+      <c r="B102" s="29"/>
+      <c r="C102" s="30"/>
       <c r="D102" s="17">
         <v>43944</v>
       </c>
@@ -2214,8 +2228,8 @@
       <c r="A103" s="17">
         <v>43945</v>
       </c>
-      <c r="B103" s="21"/>
-      <c r="C103" s="20"/>
+      <c r="B103" s="29"/>
+      <c r="C103" s="30"/>
       <c r="D103" s="17">
         <v>43945</v>
       </c>
@@ -2224,8 +2238,8 @@
       <c r="A104" s="17">
         <v>43946</v>
       </c>
-      <c r="B104" s="21"/>
-      <c r="C104" s="20"/>
+      <c r="B104" s="29"/>
+      <c r="C104" s="30"/>
       <c r="D104" s="17">
         <v>43946</v>
       </c>
@@ -2234,8 +2248,8 @@
       <c r="A105" s="17">
         <v>43947</v>
       </c>
-      <c r="B105" s="21"/>
-      <c r="C105" s="20"/>
+      <c r="B105" s="29"/>
+      <c r="C105" s="30"/>
       <c r="D105" s="17">
         <v>43947</v>
       </c>
@@ -2244,8 +2258,8 @@
       <c r="A106" s="17">
         <v>43948</v>
       </c>
-      <c r="B106" s="21"/>
-      <c r="C106" s="20"/>
+      <c r="B106" s="29"/>
+      <c r="C106" s="30"/>
       <c r="D106" s="17">
         <v>43948</v>
       </c>
@@ -2254,8 +2268,8 @@
       <c r="A107" s="17">
         <v>43949</v>
       </c>
-      <c r="B107" s="21"/>
-      <c r="C107" s="20"/>
+      <c r="B107" s="29"/>
+      <c r="C107" s="30"/>
       <c r="D107" s="17">
         <v>43949</v>
       </c>
@@ -2264,8 +2278,8 @@
       <c r="A108" s="17">
         <v>43950</v>
       </c>
-      <c r="B108" s="21"/>
-      <c r="C108" s="20"/>
+      <c r="B108" s="29"/>
+      <c r="C108" s="30"/>
       <c r="D108" s="17">
         <v>43950</v>
       </c>
@@ -2274,8 +2288,8 @@
       <c r="A109" s="17">
         <v>43951</v>
       </c>
-      <c r="B109" s="21"/>
-      <c r="C109" s="20"/>
+      <c r="B109" s="29"/>
+      <c r="C109" s="30"/>
       <c r="D109" s="17">
         <v>43951</v>
       </c>
@@ -2284,8 +2298,8 @@
       <c r="A110" s="17">
         <v>43952</v>
       </c>
-      <c r="B110" s="21"/>
-      <c r="C110" s="20"/>
+      <c r="B110" s="29"/>
+      <c r="C110" s="30"/>
       <c r="D110" s="17">
         <v>43952</v>
       </c>
@@ -2294,8 +2308,8 @@
       <c r="A111" s="17">
         <v>43953</v>
       </c>
-      <c r="B111" s="21"/>
-      <c r="C111" s="20"/>
+      <c r="B111" s="29"/>
+      <c r="C111" s="30"/>
       <c r="D111" s="17">
         <v>43953</v>
       </c>
@@ -2304,8 +2318,8 @@
       <c r="A112" s="17">
         <v>43954</v>
       </c>
-      <c r="B112" s="21"/>
-      <c r="C112" s="20"/>
+      <c r="B112" s="29"/>
+      <c r="C112" s="30"/>
       <c r="D112" s="17">
         <v>43954</v>
       </c>
@@ -2314,8 +2328,8 @@
       <c r="A113" s="17">
         <v>43955</v>
       </c>
-      <c r="B113" s="21"/>
-      <c r="C113" s="20"/>
+      <c r="B113" s="29"/>
+      <c r="C113" s="30"/>
       <c r="D113" s="17">
         <v>43955</v>
       </c>
@@ -2324,8 +2338,8 @@
       <c r="A114" s="17">
         <v>43956</v>
       </c>
-      <c r="B114" s="21"/>
-      <c r="C114" s="20"/>
+      <c r="B114" s="29"/>
+      <c r="C114" s="30"/>
       <c r="D114" s="17">
         <v>43956</v>
       </c>
@@ -2334,8 +2348,8 @@
       <c r="A115" s="17">
         <v>43957</v>
       </c>
-      <c r="B115" s="21"/>
-      <c r="C115" s="20"/>
+      <c r="B115" s="29"/>
+      <c r="C115" s="30"/>
       <c r="D115" s="17">
         <v>43957</v>
       </c>
@@ -2344,8 +2358,8 @@
       <c r="A116" s="17">
         <v>43958</v>
       </c>
-      <c r="B116" s="21"/>
-      <c r="C116" s="20"/>
+      <c r="B116" s="29"/>
+      <c r="C116" s="30"/>
       <c r="D116" s="17">
         <v>43958</v>
       </c>
@@ -2354,8 +2368,8 @@
       <c r="A117" s="17">
         <v>43959</v>
       </c>
-      <c r="B117" s="21"/>
-      <c r="C117" s="20"/>
+      <c r="B117" s="29"/>
+      <c r="C117" s="30"/>
       <c r="D117" s="17">
         <v>43959</v>
       </c>
@@ -2364,8 +2378,8 @@
       <c r="A118" s="17">
         <v>43960</v>
       </c>
-      <c r="B118" s="21"/>
-      <c r="C118" s="20"/>
+      <c r="B118" s="29"/>
+      <c r="C118" s="30"/>
       <c r="D118" s="17">
         <v>43960</v>
       </c>
@@ -2374,8 +2388,8 @@
       <c r="A119" s="17">
         <v>43961</v>
       </c>
-      <c r="B119" s="21"/>
-      <c r="C119" s="20"/>
+      <c r="B119" s="29"/>
+      <c r="C119" s="30"/>
       <c r="D119" s="17">
         <v>43961</v>
       </c>
@@ -2384,8 +2398,8 @@
       <c r="A120" s="17">
         <v>43962</v>
       </c>
-      <c r="B120" s="21"/>
-      <c r="C120" s="20"/>
+      <c r="B120" s="29"/>
+      <c r="C120" s="30"/>
       <c r="D120" s="17">
         <v>43962</v>
       </c>
@@ -2394,8 +2408,8 @@
       <c r="A121" s="17">
         <v>43963</v>
       </c>
-      <c r="B121" s="21"/>
-      <c r="C121" s="20"/>
+      <c r="B121" s="29"/>
+      <c r="C121" s="30"/>
       <c r="D121" s="17">
         <v>43963</v>
       </c>
@@ -2404,8 +2418,8 @@
       <c r="A122" s="17">
         <v>43964</v>
       </c>
-      <c r="B122" s="21"/>
-      <c r="C122" s="20"/>
+      <c r="B122" s="29"/>
+      <c r="C122" s="30"/>
       <c r="D122" s="17">
         <v>43964</v>
       </c>
@@ -2414,8 +2428,8 @@
       <c r="A123" s="17">
         <v>43965</v>
       </c>
-      <c r="B123" s="21"/>
-      <c r="C123" s="20"/>
+      <c r="B123" s="29"/>
+      <c r="C123" s="30"/>
       <c r="D123" s="17">
         <v>43965</v>
       </c>
@@ -2424,8 +2438,8 @@
       <c r="A124" s="17">
         <v>43966</v>
       </c>
-      <c r="B124" s="21"/>
-      <c r="C124" s="20"/>
+      <c r="B124" s="29"/>
+      <c r="C124" s="30"/>
       <c r="D124" s="17">
         <v>43966</v>
       </c>
@@ -2434,8 +2448,8 @@
       <c r="A125" s="17">
         <v>43967</v>
       </c>
-      <c r="B125" s="21"/>
-      <c r="C125" s="20"/>
+      <c r="B125" s="29"/>
+      <c r="C125" s="30"/>
       <c r="D125" s="17">
         <v>43967</v>
       </c>
@@ -2444,8 +2458,8 @@
       <c r="A126" s="17">
         <v>43968</v>
       </c>
-      <c r="B126" s="21"/>
-      <c r="C126" s="20"/>
+      <c r="B126" s="29"/>
+      <c r="C126" s="30"/>
       <c r="D126" s="17">
         <v>43968</v>
       </c>
@@ -2454,8 +2468,8 @@
       <c r="A127" s="17">
         <v>43969</v>
       </c>
-      <c r="B127" s="21"/>
-      <c r="C127" s="20"/>
+      <c r="B127" s="29"/>
+      <c r="C127" s="30"/>
       <c r="D127" s="17">
         <v>43969</v>
       </c>
@@ -2464,8 +2478,8 @@
       <c r="A128" s="17">
         <v>43970</v>
       </c>
-      <c r="B128" s="21"/>
-      <c r="C128" s="20"/>
+      <c r="B128" s="29"/>
+      <c r="C128" s="30"/>
       <c r="D128" s="17">
         <v>43970</v>
       </c>
@@ -2474,8 +2488,8 @@
       <c r="A129" s="17">
         <v>43971</v>
       </c>
-      <c r="B129" s="21"/>
-      <c r="C129" s="20"/>
+      <c r="B129" s="29"/>
+      <c r="C129" s="30"/>
       <c r="D129" s="17">
         <v>43971</v>
       </c>
@@ -2484,8 +2498,8 @@
       <c r="A130" s="17">
         <v>43972</v>
       </c>
-      <c r="B130" s="21"/>
-      <c r="C130" s="20"/>
+      <c r="B130" s="29"/>
+      <c r="C130" s="30"/>
       <c r="D130" s="17">
         <v>43972</v>
       </c>
@@ -2494,8 +2508,8 @@
       <c r="A131" s="17">
         <v>43973</v>
       </c>
-      <c r="B131" s="21"/>
-      <c r="C131" s="20"/>
+      <c r="B131" s="29"/>
+      <c r="C131" s="30"/>
       <c r="D131" s="17">
         <v>43973</v>
       </c>
@@ -2504,8 +2518,8 @@
       <c r="A132" s="17">
         <v>43974</v>
       </c>
-      <c r="B132" s="21"/>
-      <c r="C132" s="20"/>
+      <c r="B132" s="29"/>
+      <c r="C132" s="30"/>
       <c r="D132" s="17">
         <v>43974</v>
       </c>
@@ -2514,8 +2528,8 @@
       <c r="A133" s="17">
         <v>43975</v>
       </c>
-      <c r="B133" s="21"/>
-      <c r="C133" s="20"/>
+      <c r="B133" s="29"/>
+      <c r="C133" s="30"/>
       <c r="D133" s="17">
         <v>43975</v>
       </c>
@@ -2524,8 +2538,8 @@
       <c r="A134" s="17">
         <v>43976</v>
       </c>
-      <c r="B134" s="21"/>
-      <c r="C134" s="20"/>
+      <c r="B134" s="29"/>
+      <c r="C134" s="30"/>
       <c r="D134" s="17">
         <v>43976</v>
       </c>
@@ -2534,8 +2548,8 @@
       <c r="A135" s="17">
         <v>43977</v>
       </c>
-      <c r="B135" s="21"/>
-      <c r="C135" s="20"/>
+      <c r="B135" s="29"/>
+      <c r="C135" s="30"/>
       <c r="D135" s="17">
         <v>43977</v>
       </c>
@@ -2544,8 +2558,8 @@
       <c r="A136" s="17">
         <v>43978</v>
       </c>
-      <c r="B136" s="21"/>
-      <c r="C136" s="20"/>
+      <c r="B136" s="29"/>
+      <c r="C136" s="30"/>
       <c r="D136" s="17">
         <v>43978</v>
       </c>
@@ -2554,8 +2568,8 @@
       <c r="A137" s="17">
         <v>43979</v>
       </c>
-      <c r="B137" s="21"/>
-      <c r="C137" s="20"/>
+      <c r="B137" s="29"/>
+      <c r="C137" s="30"/>
       <c r="D137" s="17">
         <v>43979</v>
       </c>
@@ -2564,8 +2578,8 @@
       <c r="A138" s="17">
         <v>43980</v>
       </c>
-      <c r="B138" s="21"/>
-      <c r="C138" s="20"/>
+      <c r="B138" s="29"/>
+      <c r="C138" s="30"/>
       <c r="D138" s="17">
         <v>43980</v>
       </c>
@@ -2574,8 +2588,8 @@
       <c r="A139" s="17">
         <v>43981</v>
       </c>
-      <c r="B139" s="21"/>
-      <c r="C139" s="20"/>
+      <c r="B139" s="29"/>
+      <c r="C139" s="30"/>
       <c r="D139" s="17">
         <v>43981</v>
       </c>
@@ -2584,8 +2598,8 @@
       <c r="A140" s="17">
         <v>43982</v>
       </c>
-      <c r="B140" s="21"/>
-      <c r="C140" s="20"/>
+      <c r="B140" s="29"/>
+      <c r="C140" s="30"/>
       <c r="D140" s="17">
         <v>43982</v>
       </c>
@@ -2594,8 +2608,8 @@
       <c r="A141" s="17">
         <v>43983</v>
       </c>
-      <c r="B141" s="21"/>
-      <c r="C141" s="20"/>
+      <c r="B141" s="29"/>
+      <c r="C141" s="30"/>
       <c r="D141" s="17">
         <v>43983</v>
       </c>
@@ -2604,8 +2618,8 @@
       <c r="A142" s="17">
         <v>43984</v>
       </c>
-      <c r="B142" s="21"/>
-      <c r="C142" s="20"/>
+      <c r="B142" s="29"/>
+      <c r="C142" s="30"/>
       <c r="D142" s="17">
         <v>43984</v>
       </c>
@@ -2614,8 +2628,8 @@
       <c r="A143" s="17">
         <v>43985</v>
       </c>
-      <c r="B143" s="21"/>
-      <c r="C143" s="20"/>
+      <c r="B143" s="29"/>
+      <c r="C143" s="30"/>
       <c r="D143" s="17">
         <v>43985</v>
       </c>
@@ -2624,8 +2638,8 @@
       <c r="A144" s="17">
         <v>43986</v>
       </c>
-      <c r="B144" s="21"/>
-      <c r="C144" s="20"/>
+      <c r="B144" s="29"/>
+      <c r="C144" s="30"/>
       <c r="D144" s="17">
         <v>43986</v>
       </c>
@@ -2634,8 +2648,8 @@
       <c r="A145" s="17">
         <v>43987</v>
       </c>
-      <c r="B145" s="21"/>
-      <c r="C145" s="20"/>
+      <c r="B145" s="29"/>
+      <c r="C145" s="30"/>
       <c r="D145" s="17">
         <v>43987</v>
       </c>
@@ -2644,8 +2658,8 @@
       <c r="A146" s="17">
         <v>43988</v>
       </c>
-      <c r="B146" s="21"/>
-      <c r="C146" s="20"/>
+      <c r="B146" s="29"/>
+      <c r="C146" s="30"/>
       <c r="D146" s="17">
         <v>43988</v>
       </c>
@@ -2654,8 +2668,8 @@
       <c r="A147" s="17">
         <v>43989</v>
       </c>
-      <c r="B147" s="21"/>
-      <c r="C147" s="20"/>
+      <c r="B147" s="29"/>
+      <c r="C147" s="30"/>
       <c r="D147" s="17">
         <v>43989</v>
       </c>
@@ -2664,8 +2678,8 @@
       <c r="A148" s="17">
         <v>43990</v>
       </c>
-      <c r="B148" s="21"/>
-      <c r="C148" s="20"/>
+      <c r="B148" s="29"/>
+      <c r="C148" s="30"/>
       <c r="D148" s="17">
         <v>43990</v>
       </c>
@@ -2674,8 +2688,8 @@
       <c r="A149" s="17">
         <v>43991</v>
       </c>
-      <c r="B149" s="21"/>
-      <c r="C149" s="20"/>
+      <c r="B149" s="29"/>
+      <c r="C149" s="30"/>
       <c r="D149" s="17">
         <v>43991</v>
       </c>
@@ -2684,8 +2698,8 @@
       <c r="A150" s="17">
         <v>43992</v>
       </c>
-      <c r="B150" s="21"/>
-      <c r="C150" s="20"/>
+      <c r="B150" s="29"/>
+      <c r="C150" s="30"/>
       <c r="D150" s="17">
         <v>43992</v>
       </c>
@@ -2694,8 +2708,8 @@
       <c r="A151" s="17">
         <v>43993</v>
       </c>
-      <c r="B151" s="21"/>
-      <c r="C151" s="20"/>
+      <c r="B151" s="29"/>
+      <c r="C151" s="30"/>
       <c r="D151" s="17">
         <v>43993</v>
       </c>
@@ -2704,8 +2718,8 @@
       <c r="A152" s="17">
         <v>43994</v>
       </c>
-      <c r="B152" s="21"/>
-      <c r="C152" s="20"/>
+      <c r="B152" s="29"/>
+      <c r="C152" s="30"/>
       <c r="D152" s="17">
         <v>43994</v>
       </c>
@@ -2714,8 +2728,8 @@
       <c r="A153" s="17">
         <v>43995</v>
       </c>
-      <c r="B153" s="21"/>
-      <c r="C153" s="20"/>
+      <c r="B153" s="29"/>
+      <c r="C153" s="30"/>
       <c r="D153" s="17">
         <v>43995</v>
       </c>
@@ -2724,8 +2738,8 @@
       <c r="A154" s="17">
         <v>43996</v>
       </c>
-      <c r="B154" s="21"/>
-      <c r="C154" s="20"/>
+      <c r="B154" s="29"/>
+      <c r="C154" s="30"/>
       <c r="D154" s="17">
         <v>43996</v>
       </c>
@@ -2734,8 +2748,8 @@
       <c r="A155" s="17">
         <v>43997</v>
       </c>
-      <c r="B155" s="21"/>
-      <c r="C155" s="20"/>
+      <c r="B155" s="29"/>
+      <c r="C155" s="30"/>
       <c r="D155" s="17">
         <v>43997</v>
       </c>
@@ -2758,7 +2772,7 @@
       </c>
       <c r="C159" s="11">
         <f>SUM(C64:C155)</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D159" s="9" t="s">
         <v>2</v>
@@ -2782,12 +2796,6 @@
     <row r="161" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="E3:F63"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="B2:C63"/>
@@ -2801,6 +2809,12 @@
     <mergeCell ref="H65:H71"/>
     <mergeCell ref="I65:I71"/>
     <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="E3:F63"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Travail sur le php et journal d'activité
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\totok\Documents\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B96514F-431A-4175-ADE8-904016ED4AD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3320DC5F-28A4-4600-8FC1-9E839CCB5D57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28170" windowHeight="15360" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Programmation du Mécanisme Eau : Recherche de l'enregistrement des valeurs du capteurs dans la BDD. Commencement de la programmation avec des fonctions.</t>
+  </si>
+  <si>
+    <t>Travail sur la partie php permettant de récupérer l'état des capteurs et des actionneurs pour l'afficher dans l'appli WEB</t>
   </si>
 </sst>
 </file>
@@ -523,10 +526,46 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -534,21 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -567,29 +591,8 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -913,7 +916,7 @@
   <dimension ref="A1:M161"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,7 +947,7 @@
       <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="49" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="21" t="s">
@@ -953,934 +956,934 @@
       <c r="F1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="44"/>
+      <c r="G1" s="51"/>
       <c r="H1" s="11" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="46"/>
+      <c r="J1" s="53"/>
       <c r="K1" s="21" t="s">
         <v>23</v>
       </c>
       <c r="L1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="35"/>
+      <c r="M1" s="47"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>43844</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="50"/>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="45"/>
+      <c r="G2" s="52"/>
       <c r="H2" s="12"/>
       <c r="I2" s="14"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="36"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="48"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>43845</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="16">
         <v>43845</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="38"/>
+      <c r="F3" s="35"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="54"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="44"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>43846</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="16">
         <v>43846</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="54"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="44"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>43847</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="16">
         <v>43847</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="40"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="54"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="44"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>43848</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="16">
         <v>43848</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="54"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="44"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>43849</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="16">
         <v>43849</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="54"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="44"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>43850</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="40"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="16">
         <v>43850</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="54"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="44"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>43851</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="40"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="16">
         <v>43851</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="54"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="44"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>43852</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="16">
         <v>43852</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="54"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>43853</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="16">
         <v>43853</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="54"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="44"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>43854</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="16">
         <v>43854</v>
       </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="54"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="44"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>43855</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="16">
         <v>43855</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="54"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="44"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>43856</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="16">
         <v>43856</v>
       </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="54"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="44"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>43857</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="16">
         <v>43857</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="54"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="44"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>43858</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="16">
         <v>43858</v>
       </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="40"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="54"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="44"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>43859</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="16">
         <v>43859</v>
       </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="54"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="44"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>43860</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="16">
         <v>43860</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="40"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="54"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="44"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>43861</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="16">
         <v>43861</v>
       </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
       <c r="I19" s="1"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="54"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="44"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>43862</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="16">
         <v>43862</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="54"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="44"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>43863</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="16">
         <v>43863</v>
       </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="54"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="44"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>43864</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="16">
         <v>43864</v>
       </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="40"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="54"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="37"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="44"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>43865</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="16">
         <v>43865</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="37"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="54"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="44"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>43866</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="16">
         <v>43866</v>
       </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="40"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="54"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="44"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>43867</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="40"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="16">
         <v>43867</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="54"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="37"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="44"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>43868</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="40"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="16">
         <v>43868</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="40"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="54"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="44"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>43869</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="40"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="16">
         <v>43869</v>
       </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="40"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="54"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="44"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>43870</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="16">
         <v>43870</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="40"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="54"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="37"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="44"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>43871</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="16">
         <v>43871</v>
       </c>
-      <c r="E29" s="39"/>
-      <c r="F29" s="40"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="54"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="37"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="44"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>43872</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="40"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="16">
         <v>43872</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="40"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="37"/>
       <c r="H30" s="3"/>
       <c r="I30" s="1"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="54"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="44"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>43873</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="40"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="16">
         <v>43873</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="40"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="37"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="54"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="44"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>43874</v>
       </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="16">
         <v>43874</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="40"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="54"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="37"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="44"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>43875</v>
       </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="40"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="16">
         <v>43875</v>
       </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="40"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="37"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="54"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="44"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>43876</v>
       </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="40"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="16">
         <v>43876</v>
       </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="40"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="54"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="37"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="44"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>43877</v>
       </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="16">
         <v>43877</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="40"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="54"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="37"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="44"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
         <v>43878</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="37"/>
       <c r="D36" s="16">
         <v>43878</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="40"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="54"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="37"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="44"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>43879</v>
       </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="40"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="16">
         <v>43879</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="40"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="54"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="37"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="44"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
         <v>43880</v>
       </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="40"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="37"/>
       <c r="D38" s="16">
         <v>43880</v>
       </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="40"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="54"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="37"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="44"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
         <v>43881</v>
       </c>
-      <c r="B39" s="39"/>
-      <c r="C39" s="40"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="37"/>
       <c r="D39" s="16">
         <v>43881</v>
       </c>
-      <c r="E39" s="39"/>
-      <c r="F39" s="40"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="54"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="37"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="44"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <v>43882</v>
       </c>
-      <c r="B40" s="39"/>
-      <c r="C40" s="40"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="37"/>
       <c r="D40" s="16">
         <v>43882</v>
       </c>
-      <c r="E40" s="39"/>
-      <c r="F40" s="40"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="54"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="44"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>43883</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="40"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="16">
         <v>43883</v>
       </c>
-      <c r="E41" s="39"/>
-      <c r="F41" s="40"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="54"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="37"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="44"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
         <v>43884</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="40"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="37"/>
       <c r="D42" s="16">
         <v>43884</v>
       </c>
-      <c r="E42" s="39"/>
-      <c r="F42" s="40"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="54"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="37"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="44"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
         <v>43885</v>
       </c>
-      <c r="B43" s="39"/>
-      <c r="C43" s="40"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="37"/>
       <c r="D43" s="16">
         <v>43885</v>
       </c>
-      <c r="E43" s="39"/>
-      <c r="F43" s="40"/>
-      <c r="K43" s="53"/>
-      <c r="L43" s="54"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="37"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="44"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
         <v>43886</v>
       </c>
-      <c r="B44" s="39"/>
-      <c r="C44" s="40"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="37"/>
       <c r="D44" s="16">
         <v>43886</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="F44" s="40"/>
-      <c r="K44" s="53"/>
-      <c r="L44" s="54"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="37"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="44"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
         <v>43887</v>
       </c>
-      <c r="B45" s="39"/>
-      <c r="C45" s="40"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="37"/>
       <c r="D45" s="16">
         <v>43887</v>
       </c>
-      <c r="E45" s="39"/>
-      <c r="F45" s="40"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="37"/>
       <c r="H45" s="4"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="54"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="44"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>43888</v>
       </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="40"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="37"/>
       <c r="D46" s="16">
         <v>43888</v>
       </c>
-      <c r="E46" s="39"/>
-      <c r="F46" s="40"/>
-      <c r="K46" s="53"/>
-      <c r="L46" s="54"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="37"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="44"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
         <v>43889</v>
       </c>
-      <c r="B47" s="39"/>
-      <c r="C47" s="40"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="37"/>
       <c r="D47" s="16">
         <v>43889</v>
       </c>
-      <c r="E47" s="39"/>
-      <c r="F47" s="40"/>
-      <c r="K47" s="53"/>
-      <c r="L47" s="54"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="37"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="44"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
         <v>43890</v>
       </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="40"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="37"/>
       <c r="D48" s="16">
         <v>43890</v>
       </c>
-      <c r="E48" s="39"/>
-      <c r="F48" s="40"/>
-      <c r="K48" s="53"/>
-      <c r="L48" s="54"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="37"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="44"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
         <v>43891</v>
       </c>
-      <c r="B49" s="39"/>
-      <c r="C49" s="40"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="37"/>
       <c r="D49" s="16">
         <v>43891</v>
       </c>
-      <c r="E49" s="39"/>
-      <c r="F49" s="40"/>
-      <c r="K49" s="53"/>
-      <c r="L49" s="54"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="37"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="44"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>43892</v>
       </c>
-      <c r="B50" s="39"/>
-      <c r="C50" s="40"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="37"/>
       <c r="D50" s="16">
         <v>43892</v>
       </c>
-      <c r="E50" s="39"/>
-      <c r="F50" s="40"/>
-      <c r="K50" s="53"/>
-      <c r="L50" s="54"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="37"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="44"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>43893</v>
       </c>
-      <c r="B51" s="39"/>
-      <c r="C51" s="40"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="37"/>
       <c r="D51" s="16">
         <v>43893</v>
       </c>
-      <c r="E51" s="39"/>
-      <c r="F51" s="40"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="37"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
-      <c r="K51" s="53"/>
-      <c r="L51" s="54"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="44"/>
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>43894</v>
       </c>
-      <c r="B52" s="39"/>
-      <c r="C52" s="40"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="37"/>
       <c r="D52" s="16">
         <v>43894</v>
       </c>
-      <c r="E52" s="39"/>
-      <c r="F52" s="40"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="37"/>
       <c r="H52" s="4"/>
       <c r="I52" s="1"/>
-      <c r="K52" s="53"/>
-      <c r="L52" s="54"/>
+      <c r="K52" s="43"/>
+      <c r="L52" s="44"/>
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>43895</v>
       </c>
-      <c r="B53" s="39"/>
-      <c r="C53" s="40"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="16">
         <v>43895</v>
       </c>
-      <c r="E53" s="39"/>
-      <c r="F53" s="40"/>
-      <c r="K53" s="53"/>
-      <c r="L53" s="54"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="37"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="44"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>43896</v>
       </c>
-      <c r="B54" s="39"/>
-      <c r="C54" s="40"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="37"/>
       <c r="D54" s="16">
         <v>43896</v>
       </c>
-      <c r="E54" s="39"/>
-      <c r="F54" s="40"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="37"/>
       <c r="H54" s="4"/>
       <c r="I54" s="1"/>
-      <c r="K54" s="53"/>
-      <c r="L54" s="54"/>
+      <c r="K54" s="43"/>
+      <c r="L54" s="44"/>
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
         <v>43897</v>
       </c>
-      <c r="B55" s="39"/>
-      <c r="C55" s="40"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="16">
         <v>43897</v>
       </c>
-      <c r="E55" s="39"/>
-      <c r="F55" s="40"/>
-      <c r="K55" s="53"/>
-      <c r="L55" s="54"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="37"/>
+      <c r="K55" s="43"/>
+      <c r="L55" s="44"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
         <v>43898</v>
       </c>
-      <c r="B56" s="39"/>
-      <c r="C56" s="40"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="37"/>
       <c r="D56" s="16">
         <v>43898</v>
       </c>
-      <c r="E56" s="39"/>
-      <c r="F56" s="40"/>
-      <c r="K56" s="53"/>
-      <c r="L56" s="54"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="37"/>
+      <c r="K56" s="43"/>
+      <c r="L56" s="44"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
         <v>43899</v>
       </c>
-      <c r="B57" s="39"/>
-      <c r="C57" s="40"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="37"/>
       <c r="D57" s="16">
         <v>43899</v>
       </c>
-      <c r="E57" s="39"/>
-      <c r="F57" s="40"/>
-      <c r="K57" s="53"/>
-      <c r="L57" s="54"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="37"/>
+      <c r="K57" s="43"/>
+      <c r="L57" s="44"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="16">
         <v>43900</v>
       </c>
-      <c r="B58" s="39"/>
-      <c r="C58" s="40"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="37"/>
       <c r="D58" s="16">
         <v>43900</v>
       </c>
-      <c r="E58" s="39"/>
-      <c r="F58" s="40"/>
+      <c r="E58" s="36"/>
+      <c r="F58" s="37"/>
       <c r="H58" s="4"/>
       <c r="I58" s="1"/>
-      <c r="K58" s="53"/>
-      <c r="L58" s="54"/>
+      <c r="K58" s="43"/>
+      <c r="L58" s="44"/>
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16">
         <v>43901</v>
       </c>
-      <c r="B59" s="39"/>
-      <c r="C59" s="40"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="37"/>
       <c r="D59" s="16">
         <v>43901</v>
       </c>
-      <c r="E59" s="39"/>
-      <c r="F59" s="40"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="37"/>
       <c r="H59" s="4"/>
       <c r="I59" s="1"/>
-      <c r="K59" s="53"/>
-      <c r="L59" s="54"/>
+      <c r="K59" s="43"/>
+      <c r="L59" s="44"/>
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
         <v>43902</v>
       </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="40"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="37"/>
       <c r="D60" s="16">
         <v>43902</v>
       </c>
-      <c r="E60" s="39"/>
-      <c r="F60" s="40"/>
-      <c r="K60" s="53"/>
-      <c r="L60" s="54"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="37"/>
+      <c r="K60" s="43"/>
+      <c r="L60" s="44"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
         <v>43903</v>
       </c>
-      <c r="B61" s="39"/>
-      <c r="C61" s="40"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="37"/>
       <c r="D61" s="16">
         <v>43903</v>
       </c>
-      <c r="E61" s="39"/>
-      <c r="F61" s="40"/>
+      <c r="E61" s="36"/>
+      <c r="F61" s="37"/>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
-      <c r="K61" s="53"/>
-      <c r="L61" s="54"/>
+      <c r="K61" s="43"/>
+      <c r="L61" s="44"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16">
         <v>43904</v>
       </c>
-      <c r="B62" s="39"/>
-      <c r="C62" s="40"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="37"/>
       <c r="D62" s="16">
         <v>43904</v>
       </c>
-      <c r="E62" s="39"/>
-      <c r="F62" s="40"/>
-      <c r="K62" s="53"/>
-      <c r="L62" s="54"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="37"/>
+      <c r="K62" s="43"/>
+      <c r="L62" s="44"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
         <v>43905</v>
       </c>
-      <c r="B63" s="39"/>
-      <c r="C63" s="40"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="37"/>
       <c r="D63" s="16">
         <v>43905</v>
       </c>
-      <c r="E63" s="39"/>
-      <c r="F63" s="40"/>
-      <c r="K63" s="53"/>
-      <c r="L63" s="54"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="37"/>
+      <c r="K63" s="43"/>
+      <c r="L63" s="44"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
@@ -1917,7 +1920,7 @@
       <c r="B65" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="41">
+      <c r="C65" s="40">
         <v>10</v>
       </c>
       <c r="D65" s="16">
@@ -1926,17 +1929,17 @@
       <c r="E65" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="41">
+      <c r="F65" s="40">
         <v>12</v>
       </c>
-      <c r="H65" s="48" t="s">
+      <c r="H65" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="I65" s="49"/>
+      <c r="I65" s="55"/>
       <c r="K65" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="L65" s="55" t="s">
+      <c r="L65" s="45" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1945,48 +1948,48 @@
         <v>43908</v>
       </c>
       <c r="B66" s="32"/>
-      <c r="C66" s="41"/>
+      <c r="C66" s="40"/>
       <c r="D66" s="16">
         <v>43908</v>
       </c>
       <c r="E66" s="32"/>
-      <c r="F66" s="41"/>
-      <c r="H66" s="48"/>
-      <c r="I66" s="49"/>
+      <c r="F66" s="40"/>
+      <c r="H66" s="39"/>
+      <c r="I66" s="55"/>
       <c r="K66" s="32"/>
-      <c r="L66" s="55"/>
+      <c r="L66" s="45"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="16">
         <v>43909</v>
       </c>
       <c r="B67" s="32"/>
-      <c r="C67" s="41"/>
+      <c r="C67" s="40"/>
       <c r="D67" s="16">
         <v>43909</v>
       </c>
       <c r="E67" s="32"/>
-      <c r="F67" s="41"/>
-      <c r="H67" s="48"/>
-      <c r="I67" s="49"/>
+      <c r="F67" s="40"/>
+      <c r="H67" s="39"/>
+      <c r="I67" s="55"/>
       <c r="K67" s="32"/>
-      <c r="L67" s="55"/>
+      <c r="L67" s="45"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="16">
         <v>43910</v>
       </c>
       <c r="B68" s="32"/>
-      <c r="C68" s="41"/>
+      <c r="C68" s="40"/>
       <c r="D68" s="16">
         <v>43910</v>
       </c>
       <c r="E68" s="32"/>
-      <c r="F68" s="41"/>
-      <c r="H68" s="48"/>
-      <c r="I68" s="49"/>
+      <c r="F68" s="40"/>
+      <c r="H68" s="39"/>
+      <c r="I68" s="55"/>
       <c r="K68" s="32"/>
-      <c r="L68" s="55"/>
+      <c r="L68" s="45"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="16">
@@ -1995,7 +1998,7 @@
       <c r="B69" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="33">
+      <c r="C69" s="46">
         <v>4</v>
       </c>
       <c r="D69" s="16">
@@ -2004,31 +2007,31 @@
       <c r="E69" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="34">
+      <c r="F69" s="33">
         <v>6</v>
       </c>
-      <c r="H69" s="48"/>
-      <c r="I69" s="49"/>
+      <c r="H69" s="39"/>
+      <c r="I69" s="55"/>
       <c r="K69" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="L69" s="34"/>
+      <c r="L69" s="33"/>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16">
         <v>43912</v>
       </c>
       <c r="B70" s="32"/>
-      <c r="C70" s="33"/>
+      <c r="C70" s="46"/>
       <c r="D70" s="16">
         <v>43912</v>
       </c>
       <c r="E70" s="32"/>
-      <c r="F70" s="34"/>
-      <c r="H70" s="48"/>
-      <c r="I70" s="49"/>
+      <c r="F70" s="33"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="55"/>
       <c r="K70" s="32"/>
-      <c r="L70" s="34"/>
+      <c r="L70" s="33"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="16">
@@ -2046,11 +2049,11 @@
       <c r="E71" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F71" s="34">
+      <c r="F71" s="33">
         <v>4</v>
       </c>
-      <c r="H71" s="48"/>
-      <c r="I71" s="49"/>
+      <c r="H71" s="39"/>
+      <c r="I71" s="55"/>
       <c r="K71" s="26" t="s">
         <v>30</v>
       </c>
@@ -2072,7 +2075,7 @@
         <v>43914</v>
       </c>
       <c r="E72" s="32"/>
-      <c r="F72" s="34"/>
+      <c r="F72" s="33"/>
       <c r="H72" s="2" t="s">
         <v>18</v>
       </c>
@@ -2102,7 +2105,7 @@
       <c r="E73" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F73" s="34">
+      <c r="F73" s="33">
         <v>6</v>
       </c>
       <c r="H73" s="4" t="s">
@@ -2125,12 +2128,12 @@
       <c r="B74" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C74" s="34"/>
+      <c r="C74" s="33"/>
       <c r="D74" s="16">
         <v>43916</v>
       </c>
       <c r="E74" s="32"/>
-      <c r="F74" s="34"/>
+      <c r="F74" s="33"/>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
     </row>
@@ -2148,7 +2151,7 @@
         <v>43917</v>
       </c>
       <c r="E75" s="32"/>
-      <c r="F75" s="34"/>
+      <c r="F75" s="33"/>
       <c r="K75" s="26" t="s">
         <v>35</v>
       </c>
@@ -2168,11 +2171,11 @@
         <v>43918</v>
       </c>
       <c r="E76" s="32"/>
-      <c r="F76" s="34"/>
+      <c r="F76" s="33"/>
       <c r="K76" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="L76" s="50"/>
+      <c r="L76" s="38"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="16">
@@ -2185,8 +2188,8 @@
       </c>
       <c r="E77" s="30"/>
       <c r="F77" s="31"/>
-      <c r="K77" s="48"/>
-      <c r="L77" s="50"/>
+      <c r="K77" s="39"/>
+      <c r="L77" s="38"/>
     </row>
     <row r="78" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="16">
@@ -2204,7 +2207,7 @@
       <c r="E78" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="F78" s="34">
+      <c r="F78" s="33">
         <v>4</v>
       </c>
       <c r="K78" s="26" t="s">
@@ -2221,14 +2224,14 @@
       <c r="B79" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C79" s="33">
+      <c r="C79" s="46">
         <v>4</v>
       </c>
       <c r="D79" s="16">
         <v>43921</v>
       </c>
       <c r="E79" s="32"/>
-      <c r="F79" s="34"/>
+      <c r="F79" s="33"/>
       <c r="K79" s="26" t="s">
         <v>38</v>
       </c>
@@ -2241,31 +2244,35 @@
         <v>43922</v>
       </c>
       <c r="B80" s="32"/>
-      <c r="C80" s="33"/>
+      <c r="C80" s="46"/>
       <c r="D80" s="16">
         <v>43922</v>
       </c>
       <c r="E80" s="32"/>
-      <c r="F80" s="34"/>
+      <c r="F80" s="33"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="16">
         <v>43923</v>
       </c>
       <c r="B81" s="32"/>
-      <c r="C81" s="33"/>
+      <c r="C81" s="46"/>
       <c r="D81" s="16">
         <v>43923</v>
       </c>
       <c r="E81" s="32"/>
-      <c r="F81" s="34"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F81" s="33"/>
+    </row>
+    <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="16">
         <v>43924</v>
       </c>
-      <c r="B82" s="20"/>
-      <c r="C82" s="19"/>
+      <c r="B82" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C82" s="19">
+        <v>3</v>
+      </c>
       <c r="D82" s="16">
         <v>43924</v>
       </c>
@@ -3038,7 +3045,7 @@
       </c>
       <c r="C159" s="10">
         <f>SUM(C64:C155)</f>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D159" s="8" t="s">
         <v>2</v>
@@ -3062,20 +3069,6 @@
     <row r="161" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="F73:F76"/>
-    <mergeCell ref="F78:F81"/>
-    <mergeCell ref="E3:F63"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="K76:L77"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="K2:L63"/>
-    <mergeCell ref="K65:K68"/>
-    <mergeCell ref="L65:L68"/>
-    <mergeCell ref="K69:L70"/>
-    <mergeCell ref="E73:E76"/>
     <mergeCell ref="B79:B81"/>
     <mergeCell ref="C79:C81"/>
     <mergeCell ref="B74:C74"/>
@@ -3092,6 +3085,20 @@
     <mergeCell ref="I65:I71"/>
     <mergeCell ref="E71:E72"/>
     <mergeCell ref="F71:F72"/>
+    <mergeCell ref="K76:L77"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="K2:L63"/>
+    <mergeCell ref="K65:K68"/>
+    <mergeCell ref="L65:L68"/>
+    <mergeCell ref="K69:L70"/>
+    <mergeCell ref="E73:E76"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="F73:F76"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="E3:F63"/>
+    <mergeCell ref="E65:E68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finition de la partie intégration à la BDD et modificaiton du journal d'activité
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CORENTIN1\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D85EBEA-6884-4820-919C-1E5DA2B61659}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C190597B-00CF-4E93-86B6-2126BFD7EE18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -558,34 +558,85 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -603,65 +654,8 @@
     <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -984,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K87" sqref="K87"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85:B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1010,7 @@
       <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="51" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="21" t="s">
@@ -1025,934 +1019,934 @@
       <c r="F1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="59"/>
+      <c r="G1" s="53"/>
       <c r="H1" s="11" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="61"/>
+      <c r="J1" s="55"/>
       <c r="K1" s="21" t="s">
         <v>23</v>
       </c>
       <c r="L1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="54"/>
+      <c r="M1" s="44"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>43844</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="58"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="52"/>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="60"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="12"/>
       <c r="I2" s="14"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="55"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="45"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>43845</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="53"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="16">
         <v>43845</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="51"/>
+      <c r="F3" s="47"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="48"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="65"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>43846</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="53"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="16">
         <v>43846</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="53"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="49"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="65"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>43847</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="53"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="16">
         <v>43847</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="53"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="48"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="65"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>43848</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="16">
         <v>43848</v>
       </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="53"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="49"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="65"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>43849</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="16">
         <v>43849</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="53"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="49"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="65"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>43850</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="53"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
       <c r="D8" s="16">
         <v>43850</v>
       </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="53"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="49"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="65"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>43851</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="53"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="16">
         <v>43851</v>
       </c>
-      <c r="E9" s="52"/>
-      <c r="F9" s="53"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="49"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="48"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="65"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>43852</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="16">
         <v>43852</v>
       </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="49"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="48"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>43853</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="53"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="16">
         <v>43853</v>
       </c>
-      <c r="E11" s="52"/>
-      <c r="F11" s="53"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="49"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="65"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>43854</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="53"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="16">
         <v>43854</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="49"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="65"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>43855</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="53"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="16">
         <v>43855</v>
       </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="53"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="49"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="65"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>43856</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="53"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="16">
         <v>43856</v>
       </c>
-      <c r="E14" s="52"/>
-      <c r="F14" s="53"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="65"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>43857</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="53"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="16">
         <v>43857</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="53"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="65"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>43858</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="53"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="16">
         <v>43858</v>
       </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="48"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="65"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>43859</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="53"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="16">
         <v>43859</v>
       </c>
-      <c r="E17" s="52"/>
-      <c r="F17" s="53"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="48"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="65"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>43860</v>
       </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="16">
         <v>43860</v>
       </c>
-      <c r="E18" s="52"/>
-      <c r="F18" s="53"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="65"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>43861</v>
       </c>
-      <c r="B19" s="52"/>
-      <c r="C19" s="53"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="16">
         <v>43861</v>
       </c>
-      <c r="E19" s="52"/>
-      <c r="F19" s="53"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="49"/>
       <c r="I19" s="1"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="48"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="65"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>43862</v>
       </c>
-      <c r="B20" s="52"/>
-      <c r="C20" s="53"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="16">
         <v>43862</v>
       </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="53"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="49"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="65"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>43863</v>
       </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="53"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="16">
         <v>43863</v>
       </c>
-      <c r="E21" s="52"/>
-      <c r="F21" s="53"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="49"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="65"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>43864</v>
       </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="53"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="16">
         <v>43864</v>
       </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="53"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="49"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="65"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>43865</v>
       </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="53"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="16">
         <v>43865</v>
       </c>
-      <c r="E23" s="52"/>
-      <c r="F23" s="53"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="49"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="48"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="65"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>43866</v>
       </c>
-      <c r="B24" s="52"/>
-      <c r="C24" s="53"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="16">
         <v>43866</v>
       </c>
-      <c r="E24" s="52"/>
-      <c r="F24" s="53"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="49"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="48"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="65"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>43867</v>
       </c>
-      <c r="B25" s="52"/>
-      <c r="C25" s="53"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="16">
         <v>43867</v>
       </c>
-      <c r="E25" s="52"/>
-      <c r="F25" s="53"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="49"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="65"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>43868</v>
       </c>
-      <c r="B26" s="52"/>
-      <c r="C26" s="53"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="16">
         <v>43868</v>
       </c>
-      <c r="E26" s="52"/>
-      <c r="F26" s="53"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="49"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="48"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="65"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>43869</v>
       </c>
-      <c r="B27" s="52"/>
-      <c r="C27" s="53"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="16">
         <v>43869</v>
       </c>
-      <c r="E27" s="52"/>
-      <c r="F27" s="53"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="49"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="65"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>43870</v>
       </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="53"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="16">
         <v>43870</v>
       </c>
-      <c r="E28" s="52"/>
-      <c r="F28" s="53"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="49"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="65"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>43871</v>
       </c>
-      <c r="B29" s="52"/>
-      <c r="C29" s="53"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="16">
         <v>43871</v>
       </c>
-      <c r="E29" s="52"/>
-      <c r="F29" s="53"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="49"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="65"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>43872</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="53"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
       <c r="D30" s="16">
         <v>43872</v>
       </c>
-      <c r="E30" s="52"/>
-      <c r="F30" s="53"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="49"/>
       <c r="H30" s="3"/>
       <c r="I30" s="1"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="48"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="65"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>43873</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="53"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="49"/>
       <c r="D31" s="16">
         <v>43873</v>
       </c>
-      <c r="E31" s="52"/>
-      <c r="F31" s="53"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="49"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="48"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="65"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>43874</v>
       </c>
-      <c r="B32" s="52"/>
-      <c r="C32" s="53"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
       <c r="D32" s="16">
         <v>43874</v>
       </c>
-      <c r="E32" s="52"/>
-      <c r="F32" s="53"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="49"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="65"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>43875</v>
       </c>
-      <c r="B33" s="52"/>
-      <c r="C33" s="53"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
       <c r="D33" s="16">
         <v>43875</v>
       </c>
-      <c r="E33" s="52"/>
-      <c r="F33" s="53"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="49"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="48"/>
+      <c r="K33" s="64"/>
+      <c r="L33" s="65"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>43876</v>
       </c>
-      <c r="B34" s="52"/>
-      <c r="C34" s="53"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="49"/>
       <c r="D34" s="16">
         <v>43876</v>
       </c>
-      <c r="E34" s="52"/>
-      <c r="F34" s="53"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="49"/>
+      <c r="K34" s="64"/>
+      <c r="L34" s="65"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>43877</v>
       </c>
-      <c r="B35" s="52"/>
-      <c r="C35" s="53"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="16">
         <v>43877</v>
       </c>
-      <c r="E35" s="52"/>
-      <c r="F35" s="53"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="49"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="65"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
         <v>43878</v>
       </c>
-      <c r="B36" s="52"/>
-      <c r="C36" s="53"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="16">
         <v>43878</v>
       </c>
-      <c r="E36" s="52"/>
-      <c r="F36" s="53"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="48"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="49"/>
+      <c r="K36" s="64"/>
+      <c r="L36" s="65"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>43879</v>
       </c>
-      <c r="B37" s="52"/>
-      <c r="C37" s="53"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="49"/>
       <c r="D37" s="16">
         <v>43879</v>
       </c>
-      <c r="E37" s="52"/>
-      <c r="F37" s="53"/>
-      <c r="K37" s="47"/>
-      <c r="L37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="49"/>
+      <c r="K37" s="64"/>
+      <c r="L37" s="65"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
         <v>43880</v>
       </c>
-      <c r="B38" s="52"/>
-      <c r="C38" s="53"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="49"/>
       <c r="D38" s="16">
         <v>43880</v>
       </c>
-      <c r="E38" s="52"/>
-      <c r="F38" s="53"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="49"/>
+      <c r="K38" s="64"/>
+      <c r="L38" s="65"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
         <v>43881</v>
       </c>
-      <c r="B39" s="52"/>
-      <c r="C39" s="53"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="49"/>
       <c r="D39" s="16">
         <v>43881</v>
       </c>
-      <c r="E39" s="52"/>
-      <c r="F39" s="53"/>
-      <c r="K39" s="47"/>
-      <c r="L39" s="48"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="49"/>
+      <c r="K39" s="64"/>
+      <c r="L39" s="65"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <v>43882</v>
       </c>
-      <c r="B40" s="52"/>
-      <c r="C40" s="53"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
       <c r="D40" s="16">
         <v>43882</v>
       </c>
-      <c r="E40" s="52"/>
-      <c r="F40" s="53"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="48"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="49"/>
+      <c r="K40" s="64"/>
+      <c r="L40" s="65"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>43883</v>
       </c>
-      <c r="B41" s="52"/>
-      <c r="C41" s="53"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="49"/>
       <c r="D41" s="16">
         <v>43883</v>
       </c>
-      <c r="E41" s="52"/>
-      <c r="F41" s="53"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="49"/>
+      <c r="K41" s="64"/>
+      <c r="L41" s="65"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
         <v>43884</v>
       </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="53"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="49"/>
       <c r="D42" s="16">
         <v>43884</v>
       </c>
-      <c r="E42" s="52"/>
-      <c r="F42" s="53"/>
-      <c r="K42" s="47"/>
-      <c r="L42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="49"/>
+      <c r="K42" s="64"/>
+      <c r="L42" s="65"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
         <v>43885</v>
       </c>
-      <c r="B43" s="52"/>
-      <c r="C43" s="53"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="16">
         <v>43885</v>
       </c>
-      <c r="E43" s="52"/>
-      <c r="F43" s="53"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="49"/>
+      <c r="K43" s="64"/>
+      <c r="L43" s="65"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
         <v>43886</v>
       </c>
-      <c r="B44" s="52"/>
-      <c r="C44" s="53"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="49"/>
       <c r="D44" s="16">
         <v>43886</v>
       </c>
-      <c r="E44" s="52"/>
-      <c r="F44" s="53"/>
-      <c r="K44" s="47"/>
-      <c r="L44" s="48"/>
+      <c r="E44" s="48"/>
+      <c r="F44" s="49"/>
+      <c r="K44" s="64"/>
+      <c r="L44" s="65"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
         <v>43887</v>
       </c>
-      <c r="B45" s="52"/>
-      <c r="C45" s="53"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="49"/>
       <c r="D45" s="16">
         <v>43887</v>
       </c>
-      <c r="E45" s="52"/>
-      <c r="F45" s="53"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="49"/>
       <c r="H45" s="4"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="48"/>
+      <c r="K45" s="64"/>
+      <c r="L45" s="65"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>43888</v>
       </c>
-      <c r="B46" s="52"/>
-      <c r="C46" s="53"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="49"/>
       <c r="D46" s="16">
         <v>43888</v>
       </c>
-      <c r="E46" s="52"/>
-      <c r="F46" s="53"/>
-      <c r="K46" s="47"/>
-      <c r="L46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="49"/>
+      <c r="K46" s="64"/>
+      <c r="L46" s="65"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
         <v>43889</v>
       </c>
-      <c r="B47" s="52"/>
-      <c r="C47" s="53"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="49"/>
       <c r="D47" s="16">
         <v>43889</v>
       </c>
-      <c r="E47" s="52"/>
-      <c r="F47" s="53"/>
-      <c r="K47" s="47"/>
-      <c r="L47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="49"/>
+      <c r="K47" s="64"/>
+      <c r="L47" s="65"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
         <v>43890</v>
       </c>
-      <c r="B48" s="52"/>
-      <c r="C48" s="53"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="49"/>
       <c r="D48" s="16">
         <v>43890</v>
       </c>
-      <c r="E48" s="52"/>
-      <c r="F48" s="53"/>
-      <c r="K48" s="47"/>
-      <c r="L48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="49"/>
+      <c r="K48" s="64"/>
+      <c r="L48" s="65"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
         <v>43891</v>
       </c>
-      <c r="B49" s="52"/>
-      <c r="C49" s="53"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="49"/>
       <c r="D49" s="16">
         <v>43891</v>
       </c>
-      <c r="E49" s="52"/>
-      <c r="F49" s="53"/>
-      <c r="K49" s="47"/>
-      <c r="L49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="49"/>
+      <c r="K49" s="64"/>
+      <c r="L49" s="65"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>43892</v>
       </c>
-      <c r="B50" s="52"/>
-      <c r="C50" s="53"/>
+      <c r="B50" s="48"/>
+      <c r="C50" s="49"/>
       <c r="D50" s="16">
         <v>43892</v>
       </c>
-      <c r="E50" s="52"/>
-      <c r="F50" s="53"/>
-      <c r="K50" s="47"/>
-      <c r="L50" s="48"/>
+      <c r="E50" s="48"/>
+      <c r="F50" s="49"/>
+      <c r="K50" s="64"/>
+      <c r="L50" s="65"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>43893</v>
       </c>
-      <c r="B51" s="52"/>
-      <c r="C51" s="53"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="49"/>
       <c r="D51" s="16">
         <v>43893</v>
       </c>
-      <c r="E51" s="52"/>
-      <c r="F51" s="53"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="49"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
-      <c r="K51" s="47"/>
-      <c r="L51" s="48"/>
+      <c r="K51" s="64"/>
+      <c r="L51" s="65"/>
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>43894</v>
       </c>
-      <c r="B52" s="52"/>
-      <c r="C52" s="53"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="49"/>
       <c r="D52" s="16">
         <v>43894</v>
       </c>
-      <c r="E52" s="52"/>
-      <c r="F52" s="53"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="49"/>
       <c r="H52" s="4"/>
       <c r="I52" s="1"/>
-      <c r="K52" s="47"/>
-      <c r="L52" s="48"/>
+      <c r="K52" s="64"/>
+      <c r="L52" s="65"/>
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>43895</v>
       </c>
-      <c r="B53" s="52"/>
-      <c r="C53" s="53"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="49"/>
       <c r="D53" s="16">
         <v>43895</v>
       </c>
-      <c r="E53" s="52"/>
-      <c r="F53" s="53"/>
-      <c r="K53" s="47"/>
-      <c r="L53" s="48"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="49"/>
+      <c r="K53" s="64"/>
+      <c r="L53" s="65"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>43896</v>
       </c>
-      <c r="B54" s="52"/>
-      <c r="C54" s="53"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="49"/>
       <c r="D54" s="16">
         <v>43896</v>
       </c>
-      <c r="E54" s="52"/>
-      <c r="F54" s="53"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="49"/>
       <c r="H54" s="4"/>
       <c r="I54" s="1"/>
-      <c r="K54" s="47"/>
-      <c r="L54" s="48"/>
+      <c r="K54" s="64"/>
+      <c r="L54" s="65"/>
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
         <v>43897</v>
       </c>
-      <c r="B55" s="52"/>
-      <c r="C55" s="53"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="49"/>
       <c r="D55" s="16">
         <v>43897</v>
       </c>
-      <c r="E55" s="52"/>
-      <c r="F55" s="53"/>
-      <c r="K55" s="47"/>
-      <c r="L55" s="48"/>
+      <c r="E55" s="48"/>
+      <c r="F55" s="49"/>
+      <c r="K55" s="64"/>
+      <c r="L55" s="65"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
         <v>43898</v>
       </c>
-      <c r="B56" s="52"/>
-      <c r="C56" s="53"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="49"/>
       <c r="D56" s="16">
         <v>43898</v>
       </c>
-      <c r="E56" s="52"/>
-      <c r="F56" s="53"/>
-      <c r="K56" s="47"/>
-      <c r="L56" s="48"/>
+      <c r="E56" s="48"/>
+      <c r="F56" s="49"/>
+      <c r="K56" s="64"/>
+      <c r="L56" s="65"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
         <v>43899</v>
       </c>
-      <c r="B57" s="52"/>
-      <c r="C57" s="53"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="49"/>
       <c r="D57" s="16">
         <v>43899</v>
       </c>
-      <c r="E57" s="52"/>
-      <c r="F57" s="53"/>
-      <c r="K57" s="47"/>
-      <c r="L57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="49"/>
+      <c r="K57" s="64"/>
+      <c r="L57" s="65"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="16">
         <v>43900</v>
       </c>
-      <c r="B58" s="52"/>
-      <c r="C58" s="53"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="49"/>
       <c r="D58" s="16">
         <v>43900</v>
       </c>
-      <c r="E58" s="52"/>
-      <c r="F58" s="53"/>
+      <c r="E58" s="48"/>
+      <c r="F58" s="49"/>
       <c r="H58" s="4"/>
       <c r="I58" s="1"/>
-      <c r="K58" s="47"/>
-      <c r="L58" s="48"/>
+      <c r="K58" s="64"/>
+      <c r="L58" s="65"/>
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16">
         <v>43901</v>
       </c>
-      <c r="B59" s="52"/>
-      <c r="C59" s="53"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="49"/>
       <c r="D59" s="16">
         <v>43901</v>
       </c>
-      <c r="E59" s="52"/>
-      <c r="F59" s="53"/>
+      <c r="E59" s="48"/>
+      <c r="F59" s="49"/>
       <c r="H59" s="4"/>
       <c r="I59" s="1"/>
-      <c r="K59" s="47"/>
-      <c r="L59" s="48"/>
+      <c r="K59" s="64"/>
+      <c r="L59" s="65"/>
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
         <v>43902</v>
       </c>
-      <c r="B60" s="52"/>
-      <c r="C60" s="53"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="49"/>
       <c r="D60" s="16">
         <v>43902</v>
       </c>
-      <c r="E60" s="52"/>
-      <c r="F60" s="53"/>
-      <c r="K60" s="47"/>
-      <c r="L60" s="48"/>
+      <c r="E60" s="48"/>
+      <c r="F60" s="49"/>
+      <c r="K60" s="64"/>
+      <c r="L60" s="65"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
         <v>43903</v>
       </c>
-      <c r="B61" s="52"/>
-      <c r="C61" s="53"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="49"/>
       <c r="D61" s="16">
         <v>43903</v>
       </c>
-      <c r="E61" s="52"/>
-      <c r="F61" s="53"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="49"/>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
-      <c r="K61" s="47"/>
-      <c r="L61" s="48"/>
+      <c r="K61" s="64"/>
+      <c r="L61" s="65"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16">
         <v>43904</v>
       </c>
-      <c r="B62" s="52"/>
-      <c r="C62" s="53"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="49"/>
       <c r="D62" s="16">
         <v>43904</v>
       </c>
-      <c r="E62" s="52"/>
-      <c r="F62" s="53"/>
-      <c r="K62" s="47"/>
-      <c r="L62" s="48"/>
+      <c r="E62" s="48"/>
+      <c r="F62" s="49"/>
+      <c r="K62" s="64"/>
+      <c r="L62" s="65"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
         <v>43905</v>
       </c>
-      <c r="B63" s="52"/>
-      <c r="C63" s="53"/>
+      <c r="B63" s="48"/>
+      <c r="C63" s="49"/>
       <c r="D63" s="16">
         <v>43905</v>
       </c>
-      <c r="E63" s="52"/>
-      <c r="F63" s="53"/>
-      <c r="K63" s="47"/>
-      <c r="L63" s="48"/>
+      <c r="E63" s="48"/>
+      <c r="F63" s="49"/>
+      <c r="K63" s="64"/>
+      <c r="L63" s="65"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
@@ -1975,7 +1969,7 @@
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="1"/>
-      <c r="J64" s="69">
+      <c r="J64" s="39">
         <v>43906</v>
       </c>
       <c r="K64" s="26" t="s">
@@ -1989,33 +1983,33 @@
       <c r="A65" s="16">
         <v>43907</v>
       </c>
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="43">
+      <c r="C65" s="50">
         <v>10</v>
       </c>
       <c r="D65" s="16">
         <v>43907</v>
       </c>
-      <c r="E65" s="41" t="s">
+      <c r="E65" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="43">
+      <c r="F65" s="50">
         <v>12</v>
       </c>
-      <c r="H65" s="42" t="s">
+      <c r="H65" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="I65" s="63"/>
-      <c r="J65" s="69">
+      <c r="I65" s="58"/>
+      <c r="J65" s="39">
         <f>J64+1</f>
         <v>43907</v>
       </c>
-      <c r="K65" s="41" t="s">
+      <c r="K65" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="L65" s="49" t="s">
+      <c r="L65" s="66" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2023,88 +2017,88 @@
       <c r="A66" s="16">
         <v>43908</v>
       </c>
-      <c r="B66" s="41"/>
-      <c r="C66" s="43"/>
+      <c r="B66" s="42"/>
+      <c r="C66" s="50"/>
       <c r="D66" s="16">
         <v>43908</v>
       </c>
-      <c r="E66" s="41"/>
-      <c r="F66" s="43"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="63"/>
-      <c r="J66" s="69">
+      <c r="E66" s="42"/>
+      <c r="F66" s="50"/>
+      <c r="H66" s="57"/>
+      <c r="I66" s="58"/>
+      <c r="J66" s="39">
         <f t="shared" ref="J66:J129" si="0">J65+1</f>
         <v>43908</v>
       </c>
-      <c r="K66" s="41"/>
-      <c r="L66" s="49"/>
+      <c r="K66" s="42"/>
+      <c r="L66" s="66"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="16">
         <v>43909</v>
       </c>
-      <c r="B67" s="41"/>
-      <c r="C67" s="43"/>
+      <c r="B67" s="42"/>
+      <c r="C67" s="50"/>
       <c r="D67" s="16">
         <v>43909</v>
       </c>
-      <c r="E67" s="41"/>
-      <c r="F67" s="43"/>
-      <c r="H67" s="42"/>
-      <c r="I67" s="63"/>
-      <c r="J67" s="69">
+      <c r="E67" s="42"/>
+      <c r="F67" s="50"/>
+      <c r="H67" s="57"/>
+      <c r="I67" s="58"/>
+      <c r="J67" s="39">
         <f t="shared" si="0"/>
         <v>43909</v>
       </c>
-      <c r="K67" s="41"/>
-      <c r="L67" s="49"/>
+      <c r="K67" s="42"/>
+      <c r="L67" s="66"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="16">
         <v>43910</v>
       </c>
-      <c r="B68" s="41"/>
-      <c r="C68" s="43"/>
+      <c r="B68" s="42"/>
+      <c r="C68" s="50"/>
       <c r="D68" s="16">
         <v>43910</v>
       </c>
-      <c r="E68" s="41"/>
-      <c r="F68" s="43"/>
-      <c r="H68" s="42"/>
-      <c r="I68" s="63"/>
-      <c r="J68" s="69">
+      <c r="E68" s="42"/>
+      <c r="F68" s="50"/>
+      <c r="H68" s="57"/>
+      <c r="I68" s="58"/>
+      <c r="J68" s="39">
         <f t="shared" si="0"/>
         <v>43910</v>
       </c>
-      <c r="K68" s="41"/>
-      <c r="L68" s="49"/>
+      <c r="K68" s="42"/>
+      <c r="L68" s="66"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="16">
         <v>43911</v>
       </c>
-      <c r="B69" s="41" t="s">
+      <c r="B69" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="56">
+      <c r="C69" s="40">
         <v>4</v>
       </c>
       <c r="D69" s="16">
         <v>43911</v>
       </c>
-      <c r="E69" s="41" t="s">
+      <c r="E69" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="44">
+      <c r="F69" s="43">
         <v>6</v>
       </c>
-      <c r="H69" s="42"/>
-      <c r="I69" s="63"/>
-      <c r="J69" s="69">
+      <c r="H69" s="57"/>
+      <c r="I69" s="58"/>
+      <c r="J69" s="39">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="K69" s="64" t="s">
+      <c r="K69" s="59" t="s">
         <v>29</v>
       </c>
       <c r="L69" s="67"/>
@@ -2113,20 +2107,20 @@
       <c r="A70" s="16">
         <v>43912</v>
       </c>
-      <c r="B70" s="41"/>
-      <c r="C70" s="56"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="40"/>
       <c r="D70" s="16">
         <v>43912</v>
       </c>
-      <c r="E70" s="41"/>
-      <c r="F70" s="44"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="63"/>
-      <c r="J70" s="69">
+      <c r="E70" s="42"/>
+      <c r="F70" s="43"/>
+      <c r="H70" s="57"/>
+      <c r="I70" s="58"/>
+      <c r="J70" s="39">
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
-      <c r="K70" s="64"/>
+      <c r="K70" s="59"/>
       <c r="L70" s="67"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -2142,15 +2136,15 @@
       <c r="D71" s="16">
         <v>43913</v>
       </c>
-      <c r="E71" s="41" t="s">
+      <c r="E71" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F71" s="44">
+      <c r="F71" s="43">
         <v>4</v>
       </c>
-      <c r="H71" s="42"/>
-      <c r="I71" s="63"/>
-      <c r="J71" s="69">
+      <c r="H71" s="57"/>
+      <c r="I71" s="58"/>
+      <c r="J71" s="39">
         <f t="shared" si="0"/>
         <v>43913</v>
       </c>
@@ -2174,15 +2168,15 @@
       <c r="D72" s="16">
         <v>43914</v>
       </c>
-      <c r="E72" s="41"/>
-      <c r="F72" s="44"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="43"/>
       <c r="H72" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I72" s="2">
         <v>6</v>
       </c>
-      <c r="J72" s="69">
+      <c r="J72" s="39">
         <f t="shared" si="0"/>
         <v>43914</v>
       </c>
@@ -2206,10 +2200,10 @@
       <c r="D73" s="16">
         <v>43915</v>
       </c>
-      <c r="E73" s="41" t="s">
+      <c r="E73" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F73" s="44">
+      <c r="F73" s="43">
         <v>6</v>
       </c>
       <c r="H73" s="4" t="s">
@@ -2218,7 +2212,7 @@
       <c r="I73" s="2">
         <v>4</v>
       </c>
-      <c r="J73" s="69">
+      <c r="J73" s="39">
         <f t="shared" si="0"/>
         <v>43915</v>
       </c>
@@ -2233,16 +2227,16 @@
       <c r="A74" s="16">
         <v>43916</v>
       </c>
-      <c r="B74" s="41" t="s">
+      <c r="B74" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C74" s="44"/>
+      <c r="C74" s="43"/>
       <c r="D74" s="16">
         <v>43916</v>
       </c>
-      <c r="E74" s="41"/>
-      <c r="F74" s="44"/>
-      <c r="J74" s="69">
+      <c r="E74" s="42"/>
+      <c r="F74" s="43"/>
+      <c r="J74" s="39">
         <f t="shared" si="0"/>
         <v>43916</v>
       </c>
@@ -2262,9 +2256,9 @@
       <c r="D75" s="16">
         <v>43917</v>
       </c>
-      <c r="E75" s="41"/>
-      <c r="F75" s="44"/>
-      <c r="J75" s="69">
+      <c r="E75" s="42"/>
+      <c r="F75" s="43"/>
+      <c r="J75" s="39">
         <f t="shared" si="0"/>
         <v>43917</v>
       </c>
@@ -2286,16 +2280,16 @@
       <c r="D76" s="16">
         <v>43918</v>
       </c>
-      <c r="E76" s="41"/>
-      <c r="F76" s="44"/>
-      <c r="J76" s="69">
+      <c r="E76" s="42"/>
+      <c r="F76" s="43"/>
+      <c r="J76" s="39">
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
-      <c r="K76" s="64" t="s">
+      <c r="K76" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="L76" s="65"/>
+      <c r="L76" s="60"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="16">
@@ -2308,12 +2302,12 @@
       </c>
       <c r="E77" s="30"/>
       <c r="F77" s="31"/>
-      <c r="J77" s="69">
+      <c r="J77" s="39">
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="K77" s="66"/>
-      <c r="L77" s="65"/>
+      <c r="K77" s="61"/>
+      <c r="L77" s="60"/>
     </row>
     <row r="78" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="16">
@@ -2328,13 +2322,13 @@
       <c r="D78" s="16">
         <v>43920</v>
       </c>
-      <c r="E78" s="41" t="s">
+      <c r="E78" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="F78" s="44">
+      <c r="F78" s="43">
         <v>4</v>
       </c>
-      <c r="J78" s="69">
+      <c r="J78" s="39">
         <f t="shared" si="0"/>
         <v>43920</v>
       </c>
@@ -2349,18 +2343,18 @@
       <c r="A79" s="16">
         <v>43921</v>
       </c>
-      <c r="B79" s="41" t="s">
+      <c r="B79" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C79" s="56">
+      <c r="C79" s="40">
         <v>4</v>
       </c>
       <c r="D79" s="16">
         <v>43921</v>
       </c>
-      <c r="E79" s="41"/>
-      <c r="F79" s="44"/>
-      <c r="J79" s="69">
+      <c r="E79" s="42"/>
+      <c r="F79" s="43"/>
+      <c r="J79" s="39">
         <f t="shared" si="0"/>
         <v>43921</v>
       </c>
@@ -2375,14 +2369,14 @@
       <c r="A80" s="16">
         <v>43922</v>
       </c>
-      <c r="B80" s="41"/>
-      <c r="C80" s="56"/>
+      <c r="B80" s="42"/>
+      <c r="C80" s="40"/>
       <c r="D80" s="16">
         <v>43922</v>
       </c>
-      <c r="E80" s="41"/>
-      <c r="F80" s="44"/>
-      <c r="J80" s="69">
+      <c r="E80" s="42"/>
+      <c r="F80" s="43"/>
+      <c r="J80" s="39">
         <f t="shared" si="0"/>
         <v>43922</v>
       </c>
@@ -2394,21 +2388,21 @@
       <c r="A81" s="16">
         <v>43923</v>
       </c>
-      <c r="B81" s="41"/>
-      <c r="C81" s="56"/>
+      <c r="B81" s="42"/>
+      <c r="C81" s="40"/>
       <c r="D81" s="16">
         <v>43923</v>
       </c>
-      <c r="E81" s="41"/>
-      <c r="F81" s="44"/>
-      <c r="J81" s="69">
+      <c r="E81" s="42"/>
+      <c r="F81" s="43"/>
+      <c r="J81" s="39">
         <f t="shared" si="0"/>
         <v>43923</v>
       </c>
-      <c r="K81" s="56" t="s">
+      <c r="K81" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="L81" s="56" t="s">
+      <c r="L81" s="40" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2425,18 +2419,18 @@
       <c r="D82" s="16">
         <v>43924</v>
       </c>
-      <c r="E82" s="41" t="s">
+      <c r="E82" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="F82" s="44">
+      <c r="F82" s="43">
         <v>3</v>
       </c>
-      <c r="J82" s="69">
+      <c r="J82" s="39">
         <f t="shared" si="0"/>
         <v>43924</v>
       </c>
-      <c r="K82" s="56"/>
-      <c r="L82" s="56"/>
+      <c r="K82" s="40"/>
+      <c r="L82" s="40"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="16">
@@ -2447,16 +2441,16 @@
       <c r="D83" s="16">
         <v>43925</v>
       </c>
-      <c r="E83" s="41"/>
-      <c r="F83" s="44"/>
-      <c r="J83" s="69">
+      <c r="E83" s="42"/>
+      <c r="F83" s="43"/>
+      <c r="J83" s="39">
         <f t="shared" si="0"/>
         <v>43925</v>
       </c>
-      <c r="K83" s="68" t="s">
+      <c r="K83" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="L83" s="68"/>
+      <c r="L83" s="41"/>
     </row>
     <row r="84" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="16">
@@ -2465,7 +2459,7 @@
       <c r="B84" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C84" s="37">
+      <c r="C84" s="35">
         <v>2</v>
       </c>
       <c r="D84" s="16">
@@ -2473,36 +2467,36 @@
       </c>
       <c r="E84" s="30"/>
       <c r="F84" s="31"/>
-      <c r="J84" s="69">
+      <c r="J84" s="39">
         <f t="shared" si="0"/>
         <v>43926</v>
       </c>
-      <c r="K84" s="68"/>
-      <c r="L84" s="68"/>
+      <c r="K84" s="41"/>
+      <c r="L84" s="41"/>
     </row>
     <row r="85" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16">
         <v>43927</v>
       </c>
-      <c r="B85" s="33" t="s">
+      <c r="B85" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C85" s="34">
-        <v>4</v>
+      <c r="C85" s="40">
+        <v>6</v>
       </c>
       <c r="D85" s="16">
         <v>43927</v>
       </c>
       <c r="E85" s="29"/>
       <c r="F85" s="29"/>
-      <c r="J85" s="69">
+      <c r="J85" s="39">
         <f t="shared" si="0"/>
         <v>43927</v>
       </c>
-      <c r="K85" s="35" t="s">
+      <c r="K85" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="L85" s="36" t="s">
+      <c r="L85" s="34" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2510,21 +2504,21 @@
       <c r="A86" s="16">
         <v>43928</v>
       </c>
-      <c r="B86" s="20"/>
-      <c r="C86" s="19"/>
+      <c r="B86" s="42"/>
+      <c r="C86" s="40"/>
       <c r="D86" s="16">
         <v>43928</v>
       </c>
       <c r="E86" s="29"/>
       <c r="F86" s="29"/>
-      <c r="J86" s="69">
+      <c r="J86" s="39">
         <f>J85+1</f>
         <v>43928</v>
       </c>
-      <c r="K86" s="35" t="s">
+      <c r="K86" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="L86" s="36" t="s">
+      <c r="L86" s="34" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2539,55 +2533,55 @@
       </c>
       <c r="E87" s="29"/>
       <c r="F87" s="29"/>
-      <c r="J87" s="69">
+      <c r="J87" s="39">
         <f t="shared" si="0"/>
         <v>43929</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" s="38">
+      <c r="A88" s="36">
         <v>43930</v>
       </c>
-      <c r="B88" s="39"/>
+      <c r="B88" s="37"/>
       <c r="C88" s="19"/>
       <c r="D88" s="16">
         <v>43930</v>
       </c>
       <c r="E88" s="29"/>
       <c r="F88" s="29"/>
-      <c r="J88" s="69">
+      <c r="J88" s="39">
         <f t="shared" si="0"/>
         <v>43930</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="38">
+      <c r="A89" s="36">
         <v>43931</v>
       </c>
-      <c r="B89" s="39"/>
-      <c r="C89" s="40"/>
+      <c r="B89" s="37"/>
+      <c r="C89" s="38"/>
       <c r="D89" s="16">
         <v>43931</v>
       </c>
       <c r="E89" s="29"/>
       <c r="F89" s="29"/>
-      <c r="J89" s="69">
+      <c r="J89" s="39">
         <f t="shared" si="0"/>
         <v>43931</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="38">
+      <c r="A90" s="36">
         <v>43932</v>
       </c>
-      <c r="B90" s="39"/>
-      <c r="C90" s="40"/>
+      <c r="B90" s="37"/>
+      <c r="C90" s="38"/>
       <c r="D90" s="16">
         <v>43932</v>
       </c>
       <c r="E90" s="29"/>
       <c r="F90" s="29"/>
-      <c r="J90" s="69">
+      <c r="J90" s="39">
         <f t="shared" si="0"/>
         <v>43932</v>
       </c>
@@ -2603,7 +2597,7 @@
       </c>
       <c r="E91" s="30"/>
       <c r="F91" s="31"/>
-      <c r="J91" s="69">
+      <c r="J91" s="39">
         <f t="shared" si="0"/>
         <v>43933</v>
       </c>
@@ -2617,7 +2611,7 @@
       <c r="D92" s="16">
         <v>43934</v>
       </c>
-      <c r="J92" s="69">
+      <c r="J92" s="39">
         <f t="shared" si="0"/>
         <v>43934</v>
       </c>
@@ -2631,7 +2625,7 @@
       <c r="D93" s="16">
         <v>43935</v>
       </c>
-      <c r="J93" s="69">
+      <c r="J93" s="39">
         <f t="shared" si="0"/>
         <v>43935</v>
       </c>
@@ -2645,7 +2639,7 @@
       <c r="D94" s="16">
         <v>43936</v>
       </c>
-      <c r="J94" s="69">
+      <c r="J94" s="39">
         <f t="shared" si="0"/>
         <v>43936</v>
       </c>
@@ -2659,7 +2653,7 @@
       <c r="D95" s="16">
         <v>43937</v>
       </c>
-      <c r="J95" s="69">
+      <c r="J95" s="39">
         <f t="shared" si="0"/>
         <v>43937</v>
       </c>
@@ -2673,7 +2667,7 @@
       <c r="D96" s="16">
         <v>43938</v>
       </c>
-      <c r="J96" s="69">
+      <c r="J96" s="39">
         <f t="shared" si="0"/>
         <v>43938</v>
       </c>
@@ -2687,7 +2681,7 @@
       <c r="D97" s="16">
         <v>43939</v>
       </c>
-      <c r="J97" s="69">
+      <c r="J97" s="39">
         <f t="shared" si="0"/>
         <v>43939</v>
       </c>
@@ -2701,7 +2695,7 @@
       <c r="D98" s="16">
         <v>43940</v>
       </c>
-      <c r="J98" s="69">
+      <c r="J98" s="39">
         <f t="shared" si="0"/>
         <v>43940</v>
       </c>
@@ -2715,7 +2709,7 @@
       <c r="D99" s="16">
         <v>43941</v>
       </c>
-      <c r="J99" s="69">
+      <c r="J99" s="39">
         <f t="shared" si="0"/>
         <v>43941</v>
       </c>
@@ -2729,7 +2723,7 @@
       <c r="D100" s="16">
         <v>43942</v>
       </c>
-      <c r="J100" s="69">
+      <c r="J100" s="39">
         <f t="shared" si="0"/>
         <v>43942</v>
       </c>
@@ -2743,7 +2737,7 @@
       <c r="D101" s="16">
         <v>43943</v>
       </c>
-      <c r="J101" s="69">
+      <c r="J101" s="39">
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
@@ -2757,7 +2751,7 @@
       <c r="D102" s="16">
         <v>43944</v>
       </c>
-      <c r="J102" s="69">
+      <c r="J102" s="39">
         <f t="shared" si="0"/>
         <v>43944</v>
       </c>
@@ -2771,7 +2765,7 @@
       <c r="D103" s="16">
         <v>43945</v>
       </c>
-      <c r="J103" s="69">
+      <c r="J103" s="39">
         <f t="shared" si="0"/>
         <v>43945</v>
       </c>
@@ -2785,7 +2779,7 @@
       <c r="D104" s="16">
         <v>43946</v>
       </c>
-      <c r="J104" s="69">
+      <c r="J104" s="39">
         <f t="shared" si="0"/>
         <v>43946</v>
       </c>
@@ -2799,7 +2793,7 @@
       <c r="D105" s="16">
         <v>43947</v>
       </c>
-      <c r="J105" s="69">
+      <c r="J105" s="39">
         <f t="shared" si="0"/>
         <v>43947</v>
       </c>
@@ -2813,7 +2807,7 @@
       <c r="D106" s="16">
         <v>43948</v>
       </c>
-      <c r="J106" s="69">
+      <c r="J106" s="39">
         <f t="shared" si="0"/>
         <v>43948</v>
       </c>
@@ -2827,7 +2821,7 @@
       <c r="D107" s="16">
         <v>43949</v>
       </c>
-      <c r="J107" s="69">
+      <c r="J107" s="39">
         <f t="shared" si="0"/>
         <v>43949</v>
       </c>
@@ -2841,7 +2835,7 @@
       <c r="D108" s="16">
         <v>43950</v>
       </c>
-      <c r="J108" s="69">
+      <c r="J108" s="39">
         <f t="shared" si="0"/>
         <v>43950</v>
       </c>
@@ -2855,7 +2849,7 @@
       <c r="D109" s="16">
         <v>43951</v>
       </c>
-      <c r="J109" s="69">
+      <c r="J109" s="39">
         <f t="shared" si="0"/>
         <v>43951</v>
       </c>
@@ -2869,7 +2863,7 @@
       <c r="D110" s="16">
         <v>43952</v>
       </c>
-      <c r="J110" s="69">
+      <c r="J110" s="39">
         <f t="shared" si="0"/>
         <v>43952</v>
       </c>
@@ -2883,7 +2877,7 @@
       <c r="D111" s="16">
         <v>43953</v>
       </c>
-      <c r="J111" s="69">
+      <c r="J111" s="39">
         <f t="shared" si="0"/>
         <v>43953</v>
       </c>
@@ -2897,7 +2891,7 @@
       <c r="D112" s="16">
         <v>43954</v>
       </c>
-      <c r="J112" s="69">
+      <c r="J112" s="39">
         <f t="shared" si="0"/>
         <v>43954</v>
       </c>
@@ -2911,7 +2905,7 @@
       <c r="D113" s="16">
         <v>43955</v>
       </c>
-      <c r="J113" s="69">
+      <c r="J113" s="39">
         <f t="shared" si="0"/>
         <v>43955</v>
       </c>
@@ -2925,7 +2919,7 @@
       <c r="D114" s="16">
         <v>43956</v>
       </c>
-      <c r="J114" s="69">
+      <c r="J114" s="39">
         <f t="shared" si="0"/>
         <v>43956</v>
       </c>
@@ -2939,7 +2933,7 @@
       <c r="D115" s="16">
         <v>43957</v>
       </c>
-      <c r="J115" s="69">
+      <c r="J115" s="39">
         <f>J114+1</f>
         <v>43957</v>
       </c>
@@ -2953,7 +2947,7 @@
       <c r="D116" s="16">
         <v>43958</v>
       </c>
-      <c r="J116" s="69">
+      <c r="J116" s="39">
         <f t="shared" si="0"/>
         <v>43958</v>
       </c>
@@ -2967,7 +2961,7 @@
       <c r="D117" s="16">
         <v>43959</v>
       </c>
-      <c r="J117" s="69">
+      <c r="J117" s="39">
         <f t="shared" si="0"/>
         <v>43959</v>
       </c>
@@ -2981,7 +2975,7 @@
       <c r="D118" s="16">
         <v>43960</v>
       </c>
-      <c r="J118" s="69">
+      <c r="J118" s="39">
         <f t="shared" si="0"/>
         <v>43960</v>
       </c>
@@ -2995,7 +2989,7 @@
       <c r="D119" s="16">
         <v>43961</v>
       </c>
-      <c r="J119" s="69">
+      <c r="J119" s="39">
         <f t="shared" si="0"/>
         <v>43961</v>
       </c>
@@ -3009,7 +3003,7 @@
       <c r="D120" s="16">
         <v>43962</v>
       </c>
-      <c r="J120" s="69">
+      <c r="J120" s="39">
         <f t="shared" si="0"/>
         <v>43962</v>
       </c>
@@ -3023,7 +3017,7 @@
       <c r="D121" s="16">
         <v>43963</v>
       </c>
-      <c r="J121" s="69">
+      <c r="J121" s="39">
         <f t="shared" si="0"/>
         <v>43963</v>
       </c>
@@ -3037,7 +3031,7 @@
       <c r="D122" s="16">
         <v>43964</v>
       </c>
-      <c r="J122" s="69">
+      <c r="J122" s="39">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
@@ -3051,7 +3045,7 @@
       <c r="D123" s="16">
         <v>43965</v>
       </c>
-      <c r="J123" s="69">
+      <c r="J123" s="39">
         <f>J122+1</f>
         <v>43965</v>
       </c>
@@ -3065,7 +3059,7 @@
       <c r="D124" s="16">
         <v>43966</v>
       </c>
-      <c r="J124" s="69">
+      <c r="J124" s="39">
         <f t="shared" si="0"/>
         <v>43966</v>
       </c>
@@ -3079,7 +3073,7 @@
       <c r="D125" s="16">
         <v>43967</v>
       </c>
-      <c r="J125" s="69">
+      <c r="J125" s="39">
         <f t="shared" si="0"/>
         <v>43967</v>
       </c>
@@ -3093,7 +3087,7 @@
       <c r="D126" s="16">
         <v>43968</v>
       </c>
-      <c r="J126" s="69">
+      <c r="J126" s="39">
         <f t="shared" si="0"/>
         <v>43968</v>
       </c>
@@ -3107,7 +3101,7 @@
       <c r="D127" s="16">
         <v>43969</v>
       </c>
-      <c r="J127" s="69">
+      <c r="J127" s="39">
         <f t="shared" si="0"/>
         <v>43969</v>
       </c>
@@ -3121,7 +3115,7 @@
       <c r="D128" s="16">
         <v>43970</v>
       </c>
-      <c r="J128" s="69">
+      <c r="J128" s="39">
         <f t="shared" si="0"/>
         <v>43970</v>
       </c>
@@ -3135,7 +3129,7 @@
       <c r="D129" s="16">
         <v>43971</v>
       </c>
-      <c r="J129" s="69">
+      <c r="J129" s="39">
         <f t="shared" si="0"/>
         <v>43971</v>
       </c>
@@ -3149,7 +3143,7 @@
       <c r="D130" s="16">
         <v>43972</v>
       </c>
-      <c r="J130" s="69">
+      <c r="J130" s="39">
         <f t="shared" ref="J130:J160" si="1">J129+1</f>
         <v>43972</v>
       </c>
@@ -3163,7 +3157,7 @@
       <c r="D131" s="16">
         <v>43973</v>
       </c>
-      <c r="J131" s="69">
+      <c r="J131" s="39">
         <f t="shared" si="1"/>
         <v>43973</v>
       </c>
@@ -3177,7 +3171,7 @@
       <c r="D132" s="16">
         <v>43974</v>
       </c>
-      <c r="J132" s="69">
+      <c r="J132" s="39">
         <f t="shared" si="1"/>
         <v>43974</v>
       </c>
@@ -3191,7 +3185,7 @@
       <c r="D133" s="16">
         <v>43975</v>
       </c>
-      <c r="J133" s="69">
+      <c r="J133" s="39">
         <f t="shared" si="1"/>
         <v>43975</v>
       </c>
@@ -3205,7 +3199,7 @@
       <c r="D134" s="16">
         <v>43976</v>
       </c>
-      <c r="J134" s="69">
+      <c r="J134" s="39">
         <f t="shared" si="1"/>
         <v>43976</v>
       </c>
@@ -3219,7 +3213,7 @@
       <c r="D135" s="16">
         <v>43977</v>
       </c>
-      <c r="J135" s="69">
+      <c r="J135" s="39">
         <f t="shared" si="1"/>
         <v>43977</v>
       </c>
@@ -3233,7 +3227,7 @@
       <c r="D136" s="16">
         <v>43978</v>
       </c>
-      <c r="J136" s="69">
+      <c r="J136" s="39">
         <f t="shared" si="1"/>
         <v>43978</v>
       </c>
@@ -3247,7 +3241,7 @@
       <c r="D137" s="16">
         <v>43979</v>
       </c>
-      <c r="J137" s="69">
+      <c r="J137" s="39">
         <f t="shared" si="1"/>
         <v>43979</v>
       </c>
@@ -3261,7 +3255,7 @@
       <c r="D138" s="16">
         <v>43980</v>
       </c>
-      <c r="J138" s="69">
+      <c r="J138" s="39">
         <f t="shared" si="1"/>
         <v>43980</v>
       </c>
@@ -3275,7 +3269,7 @@
       <c r="D139" s="16">
         <v>43981</v>
       </c>
-      <c r="J139" s="69">
+      <c r="J139" s="39">
         <f t="shared" si="1"/>
         <v>43981</v>
       </c>
@@ -3289,7 +3283,7 @@
       <c r="D140" s="16">
         <v>43982</v>
       </c>
-      <c r="J140" s="69">
+      <c r="J140" s="39">
         <f t="shared" si="1"/>
         <v>43982</v>
       </c>
@@ -3303,7 +3297,7 @@
       <c r="D141" s="16">
         <v>43983</v>
       </c>
-      <c r="J141" s="69">
+      <c r="J141" s="39">
         <f t="shared" si="1"/>
         <v>43983</v>
       </c>
@@ -3317,7 +3311,7 @@
       <c r="D142" s="16">
         <v>43984</v>
       </c>
-      <c r="J142" s="69">
+      <c r="J142" s="39">
         <f t="shared" si="1"/>
         <v>43984</v>
       </c>
@@ -3331,7 +3325,7 @@
       <c r="D143" s="16">
         <v>43985</v>
       </c>
-      <c r="J143" s="69">
+      <c r="J143" s="39">
         <f t="shared" si="1"/>
         <v>43985</v>
       </c>
@@ -3345,7 +3339,7 @@
       <c r="D144" s="16">
         <v>43986</v>
       </c>
-      <c r="J144" s="69">
+      <c r="J144" s="39">
         <f t="shared" si="1"/>
         <v>43986</v>
       </c>
@@ -3359,7 +3353,7 @@
       <c r="D145" s="16">
         <v>43987</v>
       </c>
-      <c r="J145" s="69">
+      <c r="J145" s="39">
         <f t="shared" si="1"/>
         <v>43987</v>
       </c>
@@ -3373,7 +3367,7 @@
       <c r="D146" s="16">
         <v>43988</v>
       </c>
-      <c r="J146" s="69">
+      <c r="J146" s="39">
         <f t="shared" si="1"/>
         <v>43988</v>
       </c>
@@ -3387,7 +3381,7 @@
       <c r="D147" s="16">
         <v>43989</v>
       </c>
-      <c r="J147" s="69">
+      <c r="J147" s="39">
         <f t="shared" si="1"/>
         <v>43989</v>
       </c>
@@ -3401,7 +3395,7 @@
       <c r="D148" s="16">
         <v>43990</v>
       </c>
-      <c r="J148" s="69">
+      <c r="J148" s="39">
         <f t="shared" si="1"/>
         <v>43990</v>
       </c>
@@ -3415,7 +3409,7 @@
       <c r="D149" s="16">
         <v>43991</v>
       </c>
-      <c r="J149" s="69">
+      <c r="J149" s="39">
         <f t="shared" si="1"/>
         <v>43991</v>
       </c>
@@ -3429,7 +3423,7 @@
       <c r="D150" s="16">
         <v>43992</v>
       </c>
-      <c r="J150" s="69">
+      <c r="J150" s="39">
         <f t="shared" si="1"/>
         <v>43992</v>
       </c>
@@ -3443,7 +3437,7 @@
       <c r="D151" s="16">
         <v>43993</v>
       </c>
-      <c r="J151" s="69">
+      <c r="J151" s="39">
         <f t="shared" si="1"/>
         <v>43993</v>
       </c>
@@ -3457,7 +3451,7 @@
       <c r="D152" s="16">
         <v>43994</v>
       </c>
-      <c r="J152" s="69">
+      <c r="J152" s="39">
         <f t="shared" si="1"/>
         <v>43994</v>
       </c>
@@ -3471,7 +3465,7 @@
       <c r="D153" s="16">
         <v>43995</v>
       </c>
-      <c r="J153" s="69">
+      <c r="J153" s="39">
         <f t="shared" si="1"/>
         <v>43995</v>
       </c>
@@ -3485,7 +3479,7 @@
       <c r="D154" s="16">
         <v>43996</v>
       </c>
-      <c r="J154" s="69">
+      <c r="J154" s="39">
         <f t="shared" si="1"/>
         <v>43996</v>
       </c>
@@ -3499,7 +3493,7 @@
       <c r="D155" s="16">
         <v>43997</v>
       </c>
-      <c r="J155" s="69">
+      <c r="J155" s="39">
         <f t="shared" si="1"/>
         <v>43997</v>
       </c>
@@ -3507,7 +3501,7 @@
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="17"/>
       <c r="D156" s="16"/>
-      <c r="J156" s="69">
+      <c r="J156" s="39">
         <f t="shared" si="1"/>
         <v>43998</v>
       </c>
@@ -3515,7 +3509,7 @@
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="17"/>
       <c r="D157" s="17"/>
-      <c r="J157" s="69">
+      <c r="J157" s="39">
         <f t="shared" si="1"/>
         <v>43999</v>
       </c>
@@ -3523,7 +3517,7 @@
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="17"/>
       <c r="D158" s="17"/>
-      <c r="J158" s="69">
+      <c r="J158" s="39">
         <f t="shared" si="1"/>
         <v>44000</v>
       </c>
@@ -3534,7 +3528,7 @@
       </c>
       <c r="C159" s="10">
         <f>SUM(C64:C155)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D159" s="8" t="s">
         <v>2</v>
@@ -3547,7 +3541,7 @@
         <f>SUM(I2:I155)</f>
         <v>10</v>
       </c>
-      <c r="J159" s="69">
+      <c r="J159" s="39">
         <f t="shared" si="1"/>
         <v>44001</v>
       </c>
@@ -3558,107 +3552,111 @@
     </row>
     <row r="160" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D160" s="8"/>
-      <c r="J160" s="69">
+      <c r="J160" s="39">
         <f t="shared" si="1"/>
         <v>44002</v>
       </c>
     </row>
     <row r="161" spans="10:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="J161" s="69">
+      <c r="J161" s="39">
         <f>J160+1</f>
         <v>44003</v>
       </c>
     </row>
     <row r="162" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J162" s="69">
+      <c r="J162" s="39">
         <f t="shared" ref="J162:J168" si="2">J161+1</f>
         <v>44004</v>
       </c>
     </row>
     <row r="163" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J163" s="69">
+      <c r="J163" s="39">
         <f t="shared" si="2"/>
         <v>44005</v>
       </c>
     </row>
     <row r="164" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J164" s="69">
+      <c r="J164" s="39">
         <f t="shared" si="2"/>
         <v>44006</v>
       </c>
     </row>
     <row r="165" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J165" s="69">
+      <c r="J165" s="39">
         <f t="shared" si="2"/>
         <v>44007</v>
       </c>
     </row>
     <row r="166" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J166" s="69">
+      <c r="J166" s="39">
         <f t="shared" si="2"/>
         <v>44008</v>
       </c>
     </row>
     <row r="167" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J167" s="69">
+      <c r="J167" s="39">
         <f t="shared" si="2"/>
         <v>44009</v>
       </c>
     </row>
     <row r="168" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J168" s="69">
+      <c r="J168" s="39">
         <f t="shared" si="2"/>
         <v>44010</v>
       </c>
     </row>
     <row r="169" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J169" s="69">
+      <c r="J169" s="39">
         <f>J168+1</f>
         <v>44011</v>
       </c>
     </row>
     <row r="170" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J170" s="69">
+      <c r="J170" s="39">
         <f t="shared" ref="J170:J171" si="3">J169+1</f>
         <v>44012</v>
       </c>
     </row>
     <row r="171" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J171" s="69">
+      <c r="J171" s="39">
         <f t="shared" si="3"/>
         <v>44013</v>
       </c>
     </row>
     <row r="172" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J172" s="69">
+      <c r="J172" s="39">
         <f>J171+1</f>
         <v>44014</v>
       </c>
     </row>
     <row r="173" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J173" s="69">
+      <c r="J173" s="39">
         <f t="shared" ref="J173:J174" si="4">J172+1</f>
         <v>44015</v>
       </c>
     </row>
     <row r="174" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J174" s="69">
+      <c r="J174" s="39">
         <f t="shared" si="4"/>
         <v>44016</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="K81:K82"/>
-    <mergeCell ref="K83:L84"/>
-    <mergeCell ref="L81:L82"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="F78:F81"/>
+  <mergeCells count="37">
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="K76:L77"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="K2:L63"/>
+    <mergeCell ref="K65:K68"/>
+    <mergeCell ref="L65:L68"/>
+    <mergeCell ref="K69:L70"/>
+    <mergeCell ref="E73:E76"/>
+    <mergeCell ref="F73:F76"/>
+    <mergeCell ref="E3:F63"/>
+    <mergeCell ref="E65:E68"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="B2:C63"/>
     <mergeCell ref="B65:B68"/>
@@ -3672,18 +3670,16 @@
     <mergeCell ref="I65:I71"/>
     <mergeCell ref="E71:E72"/>
     <mergeCell ref="F71:F72"/>
-    <mergeCell ref="K76:L77"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="K2:L63"/>
-    <mergeCell ref="K65:K68"/>
-    <mergeCell ref="L65:L68"/>
-    <mergeCell ref="K69:L70"/>
-    <mergeCell ref="E73:E76"/>
-    <mergeCell ref="F73:F76"/>
-    <mergeCell ref="E3:F63"/>
-    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="K81:K82"/>
+    <mergeCell ref="K83:L84"/>
+    <mergeCell ref="L81:L82"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F82:F83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Màj du journal d'activité
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CORENTIN1\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB646DB1-5669-4EFB-870D-ED2D75E4D652}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2F3A8B-CC27-4C12-B871-C0BDDC5C2F42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -585,88 +585,88 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L88" sqref="L88"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1022,7 @@
       <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="51" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="21" t="s">
@@ -1031,21 +1031,21 @@
       <c r="F1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="60"/>
+      <c r="G1" s="53"/>
       <c r="H1" s="11" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="62"/>
+      <c r="J1" s="55"/>
       <c r="K1" s="21" t="s">
         <v>23</v>
       </c>
       <c r="L1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="56"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
@@ -1055,16 +1055,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="45"/>
-      <c r="D2" s="59"/>
+      <c r="D2" s="52"/>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="61"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="12"/>
       <c r="I2" s="14"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="57"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="43"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
@@ -1081,8 +1081,8 @@
       <c r="F3" s="45"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="69"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="63"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
@@ -1095,8 +1095,8 @@
       </c>
       <c r="E4" s="46"/>
       <c r="F4" s="47"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="69"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="63"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
@@ -1111,8 +1111,8 @@
       <c r="F5" s="47"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="69"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="63"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
@@ -1125,8 +1125,8 @@
       </c>
       <c r="E6" s="46"/>
       <c r="F6" s="47"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="69"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="63"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
@@ -1139,8 +1139,8 @@
       </c>
       <c r="E7" s="46"/>
       <c r="F7" s="47"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="69"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="63"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
@@ -1153,8 +1153,8 @@
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="47"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="69"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="63"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
@@ -1169,8 +1169,8 @@
       <c r="F9" s="47"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="69"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="63"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
@@ -1185,8 +1185,8 @@
       <c r="F10" s="47"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="69"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="63"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
@@ -1199,8 +1199,8 @@
       </c>
       <c r="E11" s="46"/>
       <c r="F11" s="47"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="69"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="63"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -1213,8 +1213,8 @@
       </c>
       <c r="E12" s="46"/>
       <c r="F12" s="47"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="69"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="63"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
@@ -1227,8 +1227,8 @@
       </c>
       <c r="E13" s="46"/>
       <c r="F13" s="47"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="69"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="63"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
@@ -1241,8 +1241,8 @@
       </c>
       <c r="E14" s="46"/>
       <c r="F14" s="47"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="69"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="63"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
@@ -1255,8 +1255,8 @@
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="47"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="69"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="63"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
@@ -1271,8 +1271,8 @@
       <c r="F16" s="47"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="69"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="63"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
@@ -1287,8 +1287,8 @@
       <c r="F17" s="47"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="69"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="63"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
@@ -1301,8 +1301,8 @@
       </c>
       <c r="E18" s="46"/>
       <c r="F18" s="47"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="69"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="63"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
@@ -1316,8 +1316,8 @@
       <c r="E19" s="46"/>
       <c r="F19" s="47"/>
       <c r="I19" s="1"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="69"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="63"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
@@ -1330,8 +1330,8 @@
       </c>
       <c r="E20" s="46"/>
       <c r="F20" s="47"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="69"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="63"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
@@ -1344,8 +1344,8 @@
       </c>
       <c r="E21" s="46"/>
       <c r="F21" s="47"/>
-      <c r="K21" s="68"/>
-      <c r="L21" s="69"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="63"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
@@ -1358,8 +1358,8 @@
       </c>
       <c r="E22" s="46"/>
       <c r="F22" s="47"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="69"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="63"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
@@ -1374,8 +1374,8 @@
       <c r="F23" s="47"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
-      <c r="K23" s="68"/>
-      <c r="L23" s="69"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="63"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
@@ -1390,8 +1390,8 @@
       <c r="F24" s="47"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="69"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="63"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
@@ -1404,8 +1404,8 @@
       </c>
       <c r="E25" s="46"/>
       <c r="F25" s="47"/>
-      <c r="K25" s="68"/>
-      <c r="L25" s="69"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="63"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
@@ -1420,8 +1420,8 @@
       <c r="F26" s="47"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="69"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="63"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
@@ -1434,8 +1434,8 @@
       </c>
       <c r="E27" s="46"/>
       <c r="F27" s="47"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="69"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="63"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
@@ -1448,8 +1448,8 @@
       </c>
       <c r="E28" s="46"/>
       <c r="F28" s="47"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="69"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="63"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
@@ -1462,8 +1462,8 @@
       </c>
       <c r="E29" s="46"/>
       <c r="F29" s="47"/>
-      <c r="K29" s="68"/>
-      <c r="L29" s="69"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="63"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
@@ -1478,8 +1478,8 @@
       <c r="F30" s="47"/>
       <c r="H30" s="3"/>
       <c r="I30" s="1"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="69"/>
+      <c r="K30" s="62"/>
+      <c r="L30" s="63"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
@@ -1494,8 +1494,8 @@
       <c r="F31" s="47"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
-      <c r="K31" s="68"/>
-      <c r="L31" s="69"/>
+      <c r="K31" s="62"/>
+      <c r="L31" s="63"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
@@ -1508,8 +1508,8 @@
       </c>
       <c r="E32" s="46"/>
       <c r="F32" s="47"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="69"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="63"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
@@ -1524,8 +1524,8 @@
       <c r="F33" s="47"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
-      <c r="K33" s="68"/>
-      <c r="L33" s="69"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="63"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
@@ -1538,8 +1538,8 @@
       </c>
       <c r="E34" s="46"/>
       <c r="F34" s="47"/>
-      <c r="K34" s="68"/>
-      <c r="L34" s="69"/>
+      <c r="K34" s="62"/>
+      <c r="L34" s="63"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
@@ -1552,8 +1552,8 @@
       </c>
       <c r="E35" s="46"/>
       <c r="F35" s="47"/>
-      <c r="K35" s="68"/>
-      <c r="L35" s="69"/>
+      <c r="K35" s="62"/>
+      <c r="L35" s="63"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
@@ -1566,8 +1566,8 @@
       </c>
       <c r="E36" s="46"/>
       <c r="F36" s="47"/>
-      <c r="K36" s="68"/>
-      <c r="L36" s="69"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="63"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
@@ -1580,8 +1580,8 @@
       </c>
       <c r="E37" s="46"/>
       <c r="F37" s="47"/>
-      <c r="K37" s="68"/>
-      <c r="L37" s="69"/>
+      <c r="K37" s="62"/>
+      <c r="L37" s="63"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
@@ -1594,8 +1594,8 @@
       </c>
       <c r="E38" s="46"/>
       <c r="F38" s="47"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="69"/>
+      <c r="K38" s="62"/>
+      <c r="L38" s="63"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
@@ -1608,8 +1608,8 @@
       </c>
       <c r="E39" s="46"/>
       <c r="F39" s="47"/>
-      <c r="K39" s="68"/>
-      <c r="L39" s="69"/>
+      <c r="K39" s="62"/>
+      <c r="L39" s="63"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
@@ -1622,8 +1622,8 @@
       </c>
       <c r="E40" s="46"/>
       <c r="F40" s="47"/>
-      <c r="K40" s="68"/>
-      <c r="L40" s="69"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="63"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
@@ -1636,8 +1636,8 @@
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="47"/>
-      <c r="K41" s="68"/>
-      <c r="L41" s="69"/>
+      <c r="K41" s="62"/>
+      <c r="L41" s="63"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
@@ -1650,8 +1650,8 @@
       </c>
       <c r="E42" s="46"/>
       <c r="F42" s="47"/>
-      <c r="K42" s="68"/>
-      <c r="L42" s="69"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="63"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
@@ -1664,8 +1664,8 @@
       </c>
       <c r="E43" s="46"/>
       <c r="F43" s="47"/>
-      <c r="K43" s="68"/>
-      <c r="L43" s="69"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="63"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
@@ -1678,8 +1678,8 @@
       </c>
       <c r="E44" s="46"/>
       <c r="F44" s="47"/>
-      <c r="K44" s="68"/>
-      <c r="L44" s="69"/>
+      <c r="K44" s="62"/>
+      <c r="L44" s="63"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
@@ -1693,8 +1693,8 @@
       <c r="E45" s="46"/>
       <c r="F45" s="47"/>
       <c r="H45" s="4"/>
-      <c r="K45" s="68"/>
-      <c r="L45" s="69"/>
+      <c r="K45" s="62"/>
+      <c r="L45" s="63"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
@@ -1707,8 +1707,8 @@
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="47"/>
-      <c r="K46" s="68"/>
-      <c r="L46" s="69"/>
+      <c r="K46" s="62"/>
+      <c r="L46" s="63"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
@@ -1721,8 +1721,8 @@
       </c>
       <c r="E47" s="46"/>
       <c r="F47" s="47"/>
-      <c r="K47" s="68"/>
-      <c r="L47" s="69"/>
+      <c r="K47" s="62"/>
+      <c r="L47" s="63"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
@@ -1735,8 +1735,8 @@
       </c>
       <c r="E48" s="46"/>
       <c r="F48" s="47"/>
-      <c r="K48" s="68"/>
-      <c r="L48" s="69"/>
+      <c r="K48" s="62"/>
+      <c r="L48" s="63"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
@@ -1749,8 +1749,8 @@
       </c>
       <c r="E49" s="46"/>
       <c r="F49" s="47"/>
-      <c r="K49" s="68"/>
-      <c r="L49" s="69"/>
+      <c r="K49" s="62"/>
+      <c r="L49" s="63"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
@@ -1763,8 +1763,8 @@
       </c>
       <c r="E50" s="46"/>
       <c r="F50" s="47"/>
-      <c r="K50" s="68"/>
-      <c r="L50" s="69"/>
+      <c r="K50" s="62"/>
+      <c r="L50" s="63"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
@@ -1779,8 +1779,8 @@
       <c r="F51" s="47"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
-      <c r="K51" s="68"/>
-      <c r="L51" s="69"/>
+      <c r="K51" s="62"/>
+      <c r="L51" s="63"/>
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
@@ -1795,8 +1795,8 @@
       <c r="F52" s="47"/>
       <c r="H52" s="4"/>
       <c r="I52" s="1"/>
-      <c r="K52" s="68"/>
-      <c r="L52" s="69"/>
+      <c r="K52" s="62"/>
+      <c r="L52" s="63"/>
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
@@ -1809,8 +1809,8 @@
       </c>
       <c r="E53" s="46"/>
       <c r="F53" s="47"/>
-      <c r="K53" s="68"/>
-      <c r="L53" s="69"/>
+      <c r="K53" s="62"/>
+      <c r="L53" s="63"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
@@ -1825,8 +1825,8 @@
       <c r="F54" s="47"/>
       <c r="H54" s="4"/>
       <c r="I54" s="1"/>
-      <c r="K54" s="68"/>
-      <c r="L54" s="69"/>
+      <c r="K54" s="62"/>
+      <c r="L54" s="63"/>
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
@@ -1839,8 +1839,8 @@
       </c>
       <c r="E55" s="46"/>
       <c r="F55" s="47"/>
-      <c r="K55" s="68"/>
-      <c r="L55" s="69"/>
+      <c r="K55" s="62"/>
+      <c r="L55" s="63"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
@@ -1853,8 +1853,8 @@
       </c>
       <c r="E56" s="46"/>
       <c r="F56" s="47"/>
-      <c r="K56" s="68"/>
-      <c r="L56" s="69"/>
+      <c r="K56" s="62"/>
+      <c r="L56" s="63"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
@@ -1867,8 +1867,8 @@
       </c>
       <c r="E57" s="46"/>
       <c r="F57" s="47"/>
-      <c r="K57" s="68"/>
-      <c r="L57" s="69"/>
+      <c r="K57" s="62"/>
+      <c r="L57" s="63"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="16">
@@ -1883,8 +1883,8 @@
       <c r="F58" s="47"/>
       <c r="H58" s="4"/>
       <c r="I58" s="1"/>
-      <c r="K58" s="68"/>
-      <c r="L58" s="69"/>
+      <c r="K58" s="62"/>
+      <c r="L58" s="63"/>
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16">
@@ -1899,8 +1899,8 @@
       <c r="F59" s="47"/>
       <c r="H59" s="4"/>
       <c r="I59" s="1"/>
-      <c r="K59" s="68"/>
-      <c r="L59" s="69"/>
+      <c r="K59" s="62"/>
+      <c r="L59" s="63"/>
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
@@ -1913,8 +1913,8 @@
       </c>
       <c r="E60" s="46"/>
       <c r="F60" s="47"/>
-      <c r="K60" s="68"/>
-      <c r="L60" s="69"/>
+      <c r="K60" s="62"/>
+      <c r="L60" s="63"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
@@ -1929,8 +1929,8 @@
       <c r="F61" s="47"/>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
-      <c r="K61" s="68"/>
-      <c r="L61" s="69"/>
+      <c r="K61" s="62"/>
+      <c r="L61" s="63"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16">
@@ -1943,8 +1943,8 @@
       </c>
       <c r="E62" s="46"/>
       <c r="F62" s="47"/>
-      <c r="K62" s="68"/>
-      <c r="L62" s="69"/>
+      <c r="K62" s="62"/>
+      <c r="L62" s="63"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
@@ -1957,8 +1957,8 @@
       </c>
       <c r="E63" s="46"/>
       <c r="F63" s="47"/>
-      <c r="K63" s="68"/>
-      <c r="L63" s="69"/>
+      <c r="K63" s="62"/>
+      <c r="L63" s="63"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
@@ -1995,33 +1995,33 @@
       <c r="A65" s="16">
         <v>43907</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="52">
+      <c r="C65" s="49">
         <v>10</v>
       </c>
       <c r="D65" s="16">
         <v>43907</v>
       </c>
-      <c r="E65" s="42" t="s">
+      <c r="E65" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="52">
+      <c r="F65" s="49">
         <v>12</v>
       </c>
-      <c r="H65" s="64" t="s">
+      <c r="H65" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="I65" s="65"/>
+      <c r="I65" s="58"/>
       <c r="J65" s="39">
         <f>J64+1</f>
         <v>43907</v>
       </c>
-      <c r="K65" s="42" t="s">
+      <c r="K65" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="L65" s="54" t="s">
+      <c r="L65" s="65" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2029,111 +2029,111 @@
       <c r="A66" s="16">
         <v>43908</v>
       </c>
-      <c r="B66" s="42"/>
-      <c r="C66" s="52"/>
+      <c r="B66" s="48"/>
+      <c r="C66" s="49"/>
       <c r="D66" s="16">
         <v>43908</v>
       </c>
-      <c r="E66" s="42"/>
-      <c r="F66" s="52"/>
-      <c r="H66" s="64"/>
-      <c r="I66" s="65"/>
+      <c r="E66" s="48"/>
+      <c r="F66" s="49"/>
+      <c r="H66" s="57"/>
+      <c r="I66" s="58"/>
       <c r="J66" s="39">
         <f t="shared" ref="J66:J129" si="0">J65+1</f>
         <v>43908</v>
       </c>
-      <c r="K66" s="42"/>
-      <c r="L66" s="54"/>
+      <c r="K66" s="48"/>
+      <c r="L66" s="65"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="16">
         <v>43909</v>
       </c>
-      <c r="B67" s="42"/>
-      <c r="C67" s="52"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="49"/>
       <c r="D67" s="16">
         <v>43909</v>
       </c>
-      <c r="E67" s="42"/>
-      <c r="F67" s="52"/>
-      <c r="H67" s="64"/>
-      <c r="I67" s="65"/>
+      <c r="E67" s="48"/>
+      <c r="F67" s="49"/>
+      <c r="H67" s="57"/>
+      <c r="I67" s="58"/>
       <c r="J67" s="39">
         <f t="shared" si="0"/>
         <v>43909</v>
       </c>
-      <c r="K67" s="42"/>
-      <c r="L67" s="54"/>
+      <c r="K67" s="48"/>
+      <c r="L67" s="65"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="16">
         <v>43910</v>
       </c>
-      <c r="B68" s="42"/>
-      <c r="C68" s="52"/>
+      <c r="B68" s="48"/>
+      <c r="C68" s="49"/>
       <c r="D68" s="16">
         <v>43910</v>
       </c>
-      <c r="E68" s="42"/>
-      <c r="F68" s="52"/>
-      <c r="H68" s="64"/>
-      <c r="I68" s="65"/>
+      <c r="E68" s="48"/>
+      <c r="F68" s="49"/>
+      <c r="H68" s="57"/>
+      <c r="I68" s="58"/>
       <c r="J68" s="39">
         <f t="shared" si="0"/>
         <v>43910</v>
       </c>
-      <c r="K68" s="42"/>
-      <c r="L68" s="54"/>
+      <c r="K68" s="48"/>
+      <c r="L68" s="65"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="16">
         <v>43911</v>
       </c>
-      <c r="B69" s="42" t="s">
+      <c r="B69" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="48">
+      <c r="C69" s="50">
         <v>4</v>
       </c>
       <c r="D69" s="16">
         <v>43911</v>
       </c>
-      <c r="E69" s="42" t="s">
+      <c r="E69" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="43">
+      <c r="F69" s="59">
         <v>6</v>
       </c>
-      <c r="H69" s="64"/>
-      <c r="I69" s="65"/>
+      <c r="H69" s="57"/>
+      <c r="I69" s="58"/>
       <c r="J69" s="39">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="K69" s="49" t="s">
+      <c r="K69" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="L69" s="55"/>
+      <c r="L69" s="67"/>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16">
         <v>43912</v>
       </c>
-      <c r="B70" s="42"/>
-      <c r="C70" s="48"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="50"/>
       <c r="D70" s="16">
         <v>43912</v>
       </c>
-      <c r="E70" s="42"/>
-      <c r="F70" s="43"/>
-      <c r="H70" s="64"/>
-      <c r="I70" s="65"/>
+      <c r="E70" s="48"/>
+      <c r="F70" s="59"/>
+      <c r="H70" s="57"/>
+      <c r="I70" s="58"/>
       <c r="J70" s="39">
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
-      <c r="K70" s="49"/>
-      <c r="L70" s="55"/>
+      <c r="K70" s="66"/>
+      <c r="L70" s="67"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="16">
@@ -2148,14 +2148,14 @@
       <c r="D71" s="16">
         <v>43913</v>
       </c>
-      <c r="E71" s="42" t="s">
+      <c r="E71" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F71" s="43">
+      <c r="F71" s="59">
         <v>4</v>
       </c>
-      <c r="H71" s="64"/>
-      <c r="I71" s="65"/>
+      <c r="H71" s="57"/>
+      <c r="I71" s="58"/>
       <c r="J71" s="39">
         <f t="shared" si="0"/>
         <v>43913</v>
@@ -2180,8 +2180,8 @@
       <c r="D72" s="16">
         <v>43914</v>
       </c>
-      <c r="E72" s="42"/>
-      <c r="F72" s="43"/>
+      <c r="E72" s="48"/>
+      <c r="F72" s="59"/>
       <c r="H72" s="2" t="s">
         <v>18</v>
       </c>
@@ -2212,10 +2212,10 @@
       <c r="D73" s="16">
         <v>43915</v>
       </c>
-      <c r="E73" s="42" t="s">
+      <c r="E73" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="F73" s="43">
+      <c r="F73" s="59">
         <v>6</v>
       </c>
       <c r="H73" s="4" t="s">
@@ -2239,15 +2239,15 @@
       <c r="A74" s="16">
         <v>43916</v>
       </c>
-      <c r="B74" s="42" t="s">
+      <c r="B74" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C74" s="43"/>
+      <c r="C74" s="59"/>
       <c r="D74" s="16">
         <v>43916</v>
       </c>
-      <c r="E74" s="42"/>
-      <c r="F74" s="43"/>
+      <c r="E74" s="48"/>
+      <c r="F74" s="59"/>
       <c r="J74" s="39">
         <f t="shared" si="0"/>
         <v>43916</v>
@@ -2268,8 +2268,8 @@
       <c r="D75" s="16">
         <v>43917</v>
       </c>
-      <c r="E75" s="42"/>
-      <c r="F75" s="43"/>
+      <c r="E75" s="48"/>
+      <c r="F75" s="59"/>
       <c r="J75" s="39">
         <f t="shared" si="0"/>
         <v>43917</v>
@@ -2292,16 +2292,16 @@
       <c r="D76" s="16">
         <v>43918</v>
       </c>
-      <c r="E76" s="42"/>
-      <c r="F76" s="43"/>
+      <c r="E76" s="48"/>
+      <c r="F76" s="59"/>
       <c r="J76" s="39">
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
-      <c r="K76" s="49" t="s">
+      <c r="K76" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="L76" s="50"/>
+      <c r="L76" s="68"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="16">
@@ -2318,8 +2318,8 @@
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="K77" s="51"/>
-      <c r="L77" s="50"/>
+      <c r="K77" s="69"/>
+      <c r="L77" s="68"/>
     </row>
     <row r="78" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="16">
@@ -2334,10 +2334,10 @@
       <c r="D78" s="16">
         <v>43920</v>
       </c>
-      <c r="E78" s="42" t="s">
+      <c r="E78" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="F78" s="43">
+      <c r="F78" s="59">
         <v>4</v>
       </c>
       <c r="J78" s="39">
@@ -2355,17 +2355,17 @@
       <c r="A79" s="16">
         <v>43921</v>
       </c>
-      <c r="B79" s="42" t="s">
+      <c r="B79" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C79" s="48">
+      <c r="C79" s="50">
         <v>4</v>
       </c>
       <c r="D79" s="16">
         <v>43921</v>
       </c>
-      <c r="E79" s="42"/>
-      <c r="F79" s="43"/>
+      <c r="E79" s="48"/>
+      <c r="F79" s="59"/>
       <c r="J79" s="39">
         <f t="shared" si="0"/>
         <v>43921</v>
@@ -2381,13 +2381,13 @@
       <c r="A80" s="16">
         <v>43922</v>
       </c>
-      <c r="B80" s="42"/>
-      <c r="C80" s="48"/>
+      <c r="B80" s="48"/>
+      <c r="C80" s="50"/>
       <c r="D80" s="16">
         <v>43922</v>
       </c>
-      <c r="E80" s="42"/>
-      <c r="F80" s="43"/>
+      <c r="E80" s="48"/>
+      <c r="F80" s="59"/>
       <c r="J80" s="39">
         <f t="shared" si="0"/>
         <v>43922</v>
@@ -2400,21 +2400,21 @@
       <c r="A81" s="16">
         <v>43923</v>
       </c>
-      <c r="B81" s="42"/>
-      <c r="C81" s="48"/>
+      <c r="B81" s="48"/>
+      <c r="C81" s="50"/>
       <c r="D81" s="16">
         <v>43923</v>
       </c>
-      <c r="E81" s="42"/>
-      <c r="F81" s="43"/>
+      <c r="E81" s="48"/>
+      <c r="F81" s="59"/>
       <c r="J81" s="39">
         <f t="shared" si="0"/>
         <v>43923</v>
       </c>
-      <c r="K81" s="48" t="s">
+      <c r="K81" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="L81" s="48" t="s">
+      <c r="L81" s="50" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2431,18 +2431,18 @@
       <c r="D82" s="16">
         <v>43924</v>
       </c>
-      <c r="E82" s="42" t="s">
+      <c r="E82" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="F82" s="43">
+      <c r="F82" s="59">
         <v>3</v>
       </c>
       <c r="J82" s="39">
         <f t="shared" si="0"/>
         <v>43924</v>
       </c>
-      <c r="K82" s="48"/>
-      <c r="L82" s="48"/>
+      <c r="K82" s="50"/>
+      <c r="L82" s="50"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="16">
@@ -2453,16 +2453,16 @@
       <c r="D83" s="16">
         <v>43925</v>
       </c>
-      <c r="E83" s="42"/>
-      <c r="F83" s="43"/>
+      <c r="E83" s="48"/>
+      <c r="F83" s="59"/>
       <c r="J83" s="39">
         <f t="shared" si="0"/>
         <v>43925</v>
       </c>
-      <c r="K83" s="53" t="s">
+      <c r="K83" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="L83" s="53"/>
+      <c r="L83" s="64"/>
     </row>
     <row r="84" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="16">
@@ -2483,26 +2483,26 @@
         <f t="shared" si="0"/>
         <v>43926</v>
       </c>
-      <c r="K84" s="53"/>
-      <c r="L84" s="53"/>
+      <c r="K84" s="64"/>
+      <c r="L84" s="64"/>
     </row>
     <row r="85" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16">
         <v>43927</v>
       </c>
-      <c r="B85" s="42" t="s">
+      <c r="B85" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C85" s="48">
-        <v>6</v>
+      <c r="C85" s="50">
+        <v>10</v>
       </c>
       <c r="D85" s="16">
         <v>43927</v>
       </c>
-      <c r="E85" s="42" t="s">
+      <c r="E85" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="F85" s="43">
+      <c r="F85" s="59">
         <v>6</v>
       </c>
       <c r="J85" s="39">
@@ -2520,13 +2520,13 @@
       <c r="A86" s="16">
         <v>43928</v>
       </c>
-      <c r="B86" s="42"/>
-      <c r="C86" s="48"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="50"/>
       <c r="D86" s="16">
         <v>43928</v>
       </c>
-      <c r="E86" s="42"/>
-      <c r="F86" s="43"/>
+      <c r="E86" s="48"/>
+      <c r="F86" s="59"/>
       <c r="J86" s="39">
         <f>J85+1</f>
         <v>43928</v>
@@ -2542,13 +2542,13 @@
       <c r="A87" s="16">
         <v>43929</v>
       </c>
-      <c r="B87" s="20"/>
-      <c r="C87" s="19"/>
+      <c r="B87" s="48"/>
+      <c r="C87" s="50"/>
       <c r="D87" s="16">
         <v>43929</v>
       </c>
-      <c r="E87" s="42"/>
-      <c r="F87" s="43"/>
+      <c r="E87" s="48"/>
+      <c r="F87" s="59"/>
       <c r="J87" s="39">
         <f t="shared" si="0"/>
         <v>43929</v>
@@ -2564,8 +2564,8 @@
       <c r="A88" s="36">
         <v>43930</v>
       </c>
-      <c r="B88" s="37"/>
-      <c r="C88" s="19"/>
+      <c r="B88" s="48"/>
+      <c r="C88" s="50"/>
       <c r="D88" s="16">
         <v>43930</v>
       </c>
@@ -3550,7 +3550,7 @@
       </c>
       <c r="C159" s="10">
         <f>SUM(C64:C155)</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D159" s="8" t="s">
         <v>2</v>
@@ -3665,6 +3665,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B85:B88"/>
+    <mergeCell ref="C85:C88"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E3:F63"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="F85:F87"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="E73:E76"/>
+    <mergeCell ref="F73:F76"/>
+    <mergeCell ref="K83:L84"/>
+    <mergeCell ref="L81:L82"/>
+    <mergeCell ref="K65:K68"/>
+    <mergeCell ref="L65:L68"/>
+    <mergeCell ref="K69:L70"/>
+    <mergeCell ref="K76:L77"/>
+    <mergeCell ref="K81:K82"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="B2:C63"/>
     <mergeCell ref="B65:B68"/>
@@ -3679,31 +3702,8 @@
     <mergeCell ref="E71:E72"/>
     <mergeCell ref="F71:F72"/>
     <mergeCell ref="K2:L63"/>
-    <mergeCell ref="K83:L84"/>
-    <mergeCell ref="L81:L82"/>
-    <mergeCell ref="K65:K68"/>
-    <mergeCell ref="L65:L68"/>
-    <mergeCell ref="K69:L70"/>
-    <mergeCell ref="K76:L77"/>
     <mergeCell ref="F65:F68"/>
     <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="F78:F81"/>
-    <mergeCell ref="K81:K82"/>
-    <mergeCell ref="E73:E76"/>
-    <mergeCell ref="F73:F76"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E3:F63"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="F85:F87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Travail sur le document commun et mise à jour du journal d'activité
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96042A76-B6AA-44F0-A21E-F0B5310F127E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7428A8-B67F-4243-B550-C38917A7D536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -607,10 +607,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -627,6 +630,45 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -643,48 +685,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:M174"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1040,7 @@
       <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="53" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="21" t="s">
@@ -1049,934 +1049,934 @@
       <c r="F1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="61"/>
+      <c r="G1" s="55"/>
       <c r="H1" s="11" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="63"/>
+      <c r="J1" s="57"/>
       <c r="K1" s="21" t="s">
         <v>23</v>
       </c>
       <c r="L1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="57"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>43844</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="60"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="62"/>
+      <c r="G2" s="56"/>
       <c r="H2" s="12"/>
       <c r="I2" s="14"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>43845</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="16">
         <v>43845</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="47"/>
+      <c r="F3" s="48"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="70"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="64"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>43846</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="16">
         <v>43846</v>
       </c>
-      <c r="E4" s="48"/>
-      <c r="F4" s="49"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="70"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="64"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>43847</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="16">
         <v>43847</v>
       </c>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="70"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="64"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>43848</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="16">
         <v>43848</v>
       </c>
-      <c r="E6" s="48"/>
-      <c r="F6" s="49"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="70"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="64"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>43849</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="16">
         <v>43849</v>
       </c>
-      <c r="E7" s="48"/>
-      <c r="F7" s="49"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="70"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="64"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>43850</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="16">
         <v>43850</v>
       </c>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="70"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="64"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>43851</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="16">
         <v>43851</v>
       </c>
-      <c r="E9" s="48"/>
-      <c r="F9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="50"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="70"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="64"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>43852</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="16">
         <v>43852</v>
       </c>
-      <c r="E10" s="48"/>
-      <c r="F10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="50"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="70"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="64"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>43853</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="16">
         <v>43853</v>
       </c>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="70"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="64"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>43854</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="49"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="16">
         <v>43854</v>
       </c>
-      <c r="E12" s="48"/>
-      <c r="F12" s="49"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="70"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="64"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>43855</v>
       </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="16">
         <v>43855</v>
       </c>
-      <c r="E13" s="48"/>
-      <c r="F13" s="49"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="70"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="64"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>43856</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="16">
         <v>43856</v>
       </c>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="70"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="64"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>43857</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="49"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="16">
         <v>43857</v>
       </c>
-      <c r="E15" s="48"/>
-      <c r="F15" s="49"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="70"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="50"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="64"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>43858</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="49"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="16">
         <v>43858</v>
       </c>
-      <c r="E16" s="48"/>
-      <c r="F16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="50"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="70"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="64"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>43859</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="16">
         <v>43859</v>
       </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="50"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="70"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="64"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>43860</v>
       </c>
-      <c r="B18" s="48"/>
-      <c r="C18" s="49"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="16">
         <v>43860</v>
       </c>
-      <c r="E18" s="48"/>
-      <c r="F18" s="49"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="70"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="50"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="64"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>43861</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="16">
         <v>43861</v>
       </c>
-      <c r="E19" s="48"/>
-      <c r="F19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="50"/>
       <c r="I19" s="1"/>
-      <c r="K19" s="69"/>
-      <c r="L19" s="70"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="64"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>43862</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="16">
         <v>43862</v>
       </c>
-      <c r="E20" s="48"/>
-      <c r="F20" s="49"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="70"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="64"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>43863</v>
       </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="49"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
       <c r="D21" s="16">
         <v>43863</v>
       </c>
-      <c r="E21" s="48"/>
-      <c r="F21" s="49"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="70"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="64"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>43864</v>
       </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="16">
         <v>43864</v>
       </c>
-      <c r="E22" s="48"/>
-      <c r="F22" s="49"/>
-      <c r="K22" s="69"/>
-      <c r="L22" s="70"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="50"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="64"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>43865</v>
       </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="49"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="16">
         <v>43865</v>
       </c>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
-      <c r="K23" s="69"/>
-      <c r="L23" s="70"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="64"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>43866</v>
       </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="49"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="16">
         <v>43866</v>
       </c>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="50"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
-      <c r="K24" s="69"/>
-      <c r="L24" s="70"/>
+      <c r="K24" s="63"/>
+      <c r="L24" s="64"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>43867</v>
       </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="16">
         <v>43867</v>
       </c>
-      <c r="E25" s="48"/>
-      <c r="F25" s="49"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="70"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="64"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>43868</v>
       </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="16">
         <v>43868</v>
       </c>
-      <c r="E26" s="48"/>
-      <c r="F26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="50"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="70"/>
+      <c r="K26" s="63"/>
+      <c r="L26" s="64"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>43869</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="49"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="16">
         <v>43869</v>
       </c>
-      <c r="E27" s="48"/>
-      <c r="F27" s="49"/>
-      <c r="K27" s="69"/>
-      <c r="L27" s="70"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="64"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>43870</v>
       </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="49"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="16">
         <v>43870</v>
       </c>
-      <c r="E28" s="48"/>
-      <c r="F28" s="49"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="70"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="64"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>43871</v>
       </c>
-      <c r="B29" s="48"/>
-      <c r="C29" s="49"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="50"/>
       <c r="D29" s="16">
         <v>43871</v>
       </c>
-      <c r="E29" s="48"/>
-      <c r="F29" s="49"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="70"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="50"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="64"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>43872</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="49"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="16">
         <v>43872</v>
       </c>
-      <c r="E30" s="48"/>
-      <c r="F30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="50"/>
       <c r="H30" s="3"/>
       <c r="I30" s="1"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="70"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="64"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>43873</v>
       </c>
-      <c r="B31" s="48"/>
-      <c r="C31" s="49"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
       <c r="D31" s="16">
         <v>43873</v>
       </c>
-      <c r="E31" s="48"/>
-      <c r="F31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="50"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="70"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="64"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>43874</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="49"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="50"/>
       <c r="D32" s="16">
         <v>43874</v>
       </c>
-      <c r="E32" s="48"/>
-      <c r="F32" s="49"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="70"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="50"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="64"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>43875</v>
       </c>
-      <c r="B33" s="48"/>
-      <c r="C33" s="49"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="50"/>
       <c r="D33" s="16">
         <v>43875</v>
       </c>
-      <c r="E33" s="48"/>
-      <c r="F33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="50"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="70"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="64"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>43876</v>
       </c>
-      <c r="B34" s="48"/>
-      <c r="C34" s="49"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="50"/>
       <c r="D34" s="16">
         <v>43876</v>
       </c>
-      <c r="E34" s="48"/>
-      <c r="F34" s="49"/>
-      <c r="K34" s="69"/>
-      <c r="L34" s="70"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="50"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="64"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>43877</v>
       </c>
-      <c r="B35" s="48"/>
-      <c r="C35" s="49"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="16">
         <v>43877</v>
       </c>
-      <c r="E35" s="48"/>
-      <c r="F35" s="49"/>
-      <c r="K35" s="69"/>
-      <c r="L35" s="70"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="50"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="64"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
         <v>43878</v>
       </c>
-      <c r="B36" s="48"/>
-      <c r="C36" s="49"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
       <c r="D36" s="16">
         <v>43878</v>
       </c>
-      <c r="E36" s="48"/>
-      <c r="F36" s="49"/>
-      <c r="K36" s="69"/>
-      <c r="L36" s="70"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="50"/>
+      <c r="K36" s="63"/>
+      <c r="L36" s="64"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>43879</v>
       </c>
-      <c r="B37" s="48"/>
-      <c r="C37" s="49"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
       <c r="D37" s="16">
         <v>43879</v>
       </c>
-      <c r="E37" s="48"/>
-      <c r="F37" s="49"/>
-      <c r="K37" s="69"/>
-      <c r="L37" s="70"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="50"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="64"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
         <v>43880</v>
       </c>
-      <c r="B38" s="48"/>
-      <c r="C38" s="49"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
       <c r="D38" s="16">
         <v>43880</v>
       </c>
-      <c r="E38" s="48"/>
-      <c r="F38" s="49"/>
-      <c r="K38" s="69"/>
-      <c r="L38" s="70"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="50"/>
+      <c r="K38" s="63"/>
+      <c r="L38" s="64"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
         <v>43881</v>
       </c>
-      <c r="B39" s="48"/>
-      <c r="C39" s="49"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
       <c r="D39" s="16">
         <v>43881</v>
       </c>
-      <c r="E39" s="48"/>
-      <c r="F39" s="49"/>
-      <c r="K39" s="69"/>
-      <c r="L39" s="70"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="50"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="64"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <v>43882</v>
       </c>
-      <c r="B40" s="48"/>
-      <c r="C40" s="49"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="50"/>
       <c r="D40" s="16">
         <v>43882</v>
       </c>
-      <c r="E40" s="48"/>
-      <c r="F40" s="49"/>
-      <c r="K40" s="69"/>
-      <c r="L40" s="70"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="50"/>
+      <c r="K40" s="63"/>
+      <c r="L40" s="64"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>43883</v>
       </c>
-      <c r="B41" s="48"/>
-      <c r="C41" s="49"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="50"/>
       <c r="D41" s="16">
         <v>43883</v>
       </c>
-      <c r="E41" s="48"/>
-      <c r="F41" s="49"/>
-      <c r="K41" s="69"/>
-      <c r="L41" s="70"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="50"/>
+      <c r="K41" s="63"/>
+      <c r="L41" s="64"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
         <v>43884</v>
       </c>
-      <c r="B42" s="48"/>
-      <c r="C42" s="49"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="50"/>
       <c r="D42" s="16">
         <v>43884</v>
       </c>
-      <c r="E42" s="48"/>
-      <c r="F42" s="49"/>
-      <c r="K42" s="69"/>
-      <c r="L42" s="70"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="50"/>
+      <c r="K42" s="63"/>
+      <c r="L42" s="64"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
         <v>43885</v>
       </c>
-      <c r="B43" s="48"/>
-      <c r="C43" s="49"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="50"/>
       <c r="D43" s="16">
         <v>43885</v>
       </c>
-      <c r="E43" s="48"/>
-      <c r="F43" s="49"/>
-      <c r="K43" s="69"/>
-      <c r="L43" s="70"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="50"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="64"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
         <v>43886</v>
       </c>
-      <c r="B44" s="48"/>
-      <c r="C44" s="49"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="50"/>
       <c r="D44" s="16">
         <v>43886</v>
       </c>
-      <c r="E44" s="48"/>
-      <c r="F44" s="49"/>
-      <c r="K44" s="69"/>
-      <c r="L44" s="70"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="50"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="64"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
         <v>43887</v>
       </c>
-      <c r="B45" s="48"/>
-      <c r="C45" s="49"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="50"/>
       <c r="D45" s="16">
         <v>43887</v>
       </c>
-      <c r="E45" s="48"/>
-      <c r="F45" s="49"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="50"/>
       <c r="H45" s="4"/>
-      <c r="K45" s="69"/>
-      <c r="L45" s="70"/>
+      <c r="K45" s="63"/>
+      <c r="L45" s="64"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>43888</v>
       </c>
-      <c r="B46" s="48"/>
-      <c r="C46" s="49"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="50"/>
       <c r="D46" s="16">
         <v>43888</v>
       </c>
-      <c r="E46" s="48"/>
-      <c r="F46" s="49"/>
-      <c r="K46" s="69"/>
-      <c r="L46" s="70"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="50"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="64"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
         <v>43889</v>
       </c>
-      <c r="B47" s="48"/>
-      <c r="C47" s="49"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="50"/>
       <c r="D47" s="16">
         <v>43889</v>
       </c>
-      <c r="E47" s="48"/>
-      <c r="F47" s="49"/>
-      <c r="K47" s="69"/>
-      <c r="L47" s="70"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="50"/>
+      <c r="K47" s="63"/>
+      <c r="L47" s="64"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
         <v>43890</v>
       </c>
-      <c r="B48" s="48"/>
-      <c r="C48" s="49"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="16">
         <v>43890</v>
       </c>
-      <c r="E48" s="48"/>
-      <c r="F48" s="49"/>
-      <c r="K48" s="69"/>
-      <c r="L48" s="70"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="50"/>
+      <c r="K48" s="63"/>
+      <c r="L48" s="64"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
         <v>43891</v>
       </c>
-      <c r="B49" s="48"/>
-      <c r="C49" s="49"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="50"/>
       <c r="D49" s="16">
         <v>43891</v>
       </c>
-      <c r="E49" s="48"/>
-      <c r="F49" s="49"/>
-      <c r="K49" s="69"/>
-      <c r="L49" s="70"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="50"/>
+      <c r="K49" s="63"/>
+      <c r="L49" s="64"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>43892</v>
       </c>
-      <c r="B50" s="48"/>
-      <c r="C50" s="49"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="50"/>
       <c r="D50" s="16">
         <v>43892</v>
       </c>
-      <c r="E50" s="48"/>
-      <c r="F50" s="49"/>
-      <c r="K50" s="69"/>
-      <c r="L50" s="70"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="50"/>
+      <c r="K50" s="63"/>
+      <c r="L50" s="64"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>43893</v>
       </c>
-      <c r="B51" s="48"/>
-      <c r="C51" s="49"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="50"/>
       <c r="D51" s="16">
         <v>43893</v>
       </c>
-      <c r="E51" s="48"/>
-      <c r="F51" s="49"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="50"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
-      <c r="K51" s="69"/>
-      <c r="L51" s="70"/>
+      <c r="K51" s="63"/>
+      <c r="L51" s="64"/>
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>43894</v>
       </c>
-      <c r="B52" s="48"/>
-      <c r="C52" s="49"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="50"/>
       <c r="D52" s="16">
         <v>43894</v>
       </c>
-      <c r="E52" s="48"/>
-      <c r="F52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="50"/>
       <c r="H52" s="4"/>
       <c r="I52" s="1"/>
-      <c r="K52" s="69"/>
-      <c r="L52" s="70"/>
+      <c r="K52" s="63"/>
+      <c r="L52" s="64"/>
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>43895</v>
       </c>
-      <c r="B53" s="48"/>
-      <c r="C53" s="49"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="50"/>
       <c r="D53" s="16">
         <v>43895</v>
       </c>
-      <c r="E53" s="48"/>
-      <c r="F53" s="49"/>
-      <c r="K53" s="69"/>
-      <c r="L53" s="70"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="50"/>
+      <c r="K53" s="63"/>
+      <c r="L53" s="64"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>43896</v>
       </c>
-      <c r="B54" s="48"/>
-      <c r="C54" s="49"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="50"/>
       <c r="D54" s="16">
         <v>43896</v>
       </c>
-      <c r="E54" s="48"/>
-      <c r="F54" s="49"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="50"/>
       <c r="H54" s="4"/>
       <c r="I54" s="1"/>
-      <c r="K54" s="69"/>
-      <c r="L54" s="70"/>
+      <c r="K54" s="63"/>
+      <c r="L54" s="64"/>
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
         <v>43897</v>
       </c>
-      <c r="B55" s="48"/>
-      <c r="C55" s="49"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="50"/>
       <c r="D55" s="16">
         <v>43897</v>
       </c>
-      <c r="E55" s="48"/>
-      <c r="F55" s="49"/>
-      <c r="K55" s="69"/>
-      <c r="L55" s="70"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="50"/>
+      <c r="K55" s="63"/>
+      <c r="L55" s="64"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
         <v>43898</v>
       </c>
-      <c r="B56" s="48"/>
-      <c r="C56" s="49"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="50"/>
       <c r="D56" s="16">
         <v>43898</v>
       </c>
-      <c r="E56" s="48"/>
-      <c r="F56" s="49"/>
-      <c r="K56" s="69"/>
-      <c r="L56" s="70"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="50"/>
+      <c r="K56" s="63"/>
+      <c r="L56" s="64"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
         <v>43899</v>
       </c>
-      <c r="B57" s="48"/>
-      <c r="C57" s="49"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="50"/>
       <c r="D57" s="16">
         <v>43899</v>
       </c>
-      <c r="E57" s="48"/>
-      <c r="F57" s="49"/>
-      <c r="K57" s="69"/>
-      <c r="L57" s="70"/>
+      <c r="E57" s="49"/>
+      <c r="F57" s="50"/>
+      <c r="K57" s="63"/>
+      <c r="L57" s="64"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="16">
         <v>43900</v>
       </c>
-      <c r="B58" s="48"/>
-      <c r="C58" s="49"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="50"/>
       <c r="D58" s="16">
         <v>43900</v>
       </c>
-      <c r="E58" s="48"/>
-      <c r="F58" s="49"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="50"/>
       <c r="H58" s="4"/>
       <c r="I58" s="1"/>
-      <c r="K58" s="69"/>
-      <c r="L58" s="70"/>
+      <c r="K58" s="63"/>
+      <c r="L58" s="64"/>
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16">
         <v>43901</v>
       </c>
-      <c r="B59" s="48"/>
-      <c r="C59" s="49"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="50"/>
       <c r="D59" s="16">
         <v>43901</v>
       </c>
-      <c r="E59" s="48"/>
-      <c r="F59" s="49"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="50"/>
       <c r="H59" s="4"/>
       <c r="I59" s="1"/>
-      <c r="K59" s="69"/>
-      <c r="L59" s="70"/>
+      <c r="K59" s="63"/>
+      <c r="L59" s="64"/>
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
         <v>43902</v>
       </c>
-      <c r="B60" s="48"/>
-      <c r="C60" s="49"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="50"/>
       <c r="D60" s="16">
         <v>43902</v>
       </c>
-      <c r="E60" s="48"/>
-      <c r="F60" s="49"/>
-      <c r="K60" s="69"/>
-      <c r="L60" s="70"/>
+      <c r="E60" s="49"/>
+      <c r="F60" s="50"/>
+      <c r="K60" s="63"/>
+      <c r="L60" s="64"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
         <v>43903</v>
       </c>
-      <c r="B61" s="48"/>
-      <c r="C61" s="49"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="50"/>
       <c r="D61" s="16">
         <v>43903</v>
       </c>
-      <c r="E61" s="48"/>
-      <c r="F61" s="49"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="50"/>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
-      <c r="K61" s="69"/>
-      <c r="L61" s="70"/>
+      <c r="K61" s="63"/>
+      <c r="L61" s="64"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16">
         <v>43904</v>
       </c>
-      <c r="B62" s="48"/>
-      <c r="C62" s="49"/>
+      <c r="B62" s="49"/>
+      <c r="C62" s="50"/>
       <c r="D62" s="16">
         <v>43904</v>
       </c>
-      <c r="E62" s="48"/>
-      <c r="F62" s="49"/>
-      <c r="K62" s="69"/>
-      <c r="L62" s="70"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="50"/>
+      <c r="K62" s="63"/>
+      <c r="L62" s="64"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
         <v>43905</v>
       </c>
-      <c r="B63" s="48"/>
-      <c r="C63" s="49"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="50"/>
       <c r="D63" s="16">
         <v>43905</v>
       </c>
-      <c r="E63" s="48"/>
-      <c r="F63" s="49"/>
-      <c r="K63" s="69"/>
-      <c r="L63" s="70"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="50"/>
+      <c r="K63" s="63"/>
+      <c r="L63" s="64"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
@@ -2016,7 +2016,7 @@
       <c r="B65" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="50">
+      <c r="C65" s="51">
         <v>10</v>
       </c>
       <c r="D65" s="16">
@@ -2025,13 +2025,13 @@
       <c r="E65" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="50">
+      <c r="F65" s="51">
         <v>12</v>
       </c>
-      <c r="H65" s="65" t="s">
+      <c r="H65" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="I65" s="66"/>
+      <c r="I65" s="60"/>
       <c r="J65" s="38">
         <f>J64+1</f>
         <v>43907</v>
@@ -2039,7 +2039,7 @@
       <c r="K65" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="L65" s="52" t="s">
+      <c r="L65" s="66" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2048,60 +2048,60 @@
         <v>43908</v>
       </c>
       <c r="B66" s="43"/>
-      <c r="C66" s="50"/>
+      <c r="C66" s="51"/>
       <c r="D66" s="16">
         <v>43908</v>
       </c>
       <c r="E66" s="43"/>
-      <c r="F66" s="50"/>
-      <c r="H66" s="65"/>
-      <c r="I66" s="66"/>
+      <c r="F66" s="51"/>
+      <c r="H66" s="59"/>
+      <c r="I66" s="60"/>
       <c r="J66" s="38">
         <f t="shared" ref="J66:J129" si="0">J65+1</f>
         <v>43908</v>
       </c>
       <c r="K66" s="43"/>
-      <c r="L66" s="52"/>
+      <c r="L66" s="66"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="16">
         <v>43909</v>
       </c>
       <c r="B67" s="43"/>
-      <c r="C67" s="50"/>
+      <c r="C67" s="51"/>
       <c r="D67" s="16">
         <v>43909</v>
       </c>
       <c r="E67" s="43"/>
-      <c r="F67" s="50"/>
-      <c r="H67" s="65"/>
-      <c r="I67" s="66"/>
+      <c r="F67" s="51"/>
+      <c r="H67" s="59"/>
+      <c r="I67" s="60"/>
       <c r="J67" s="38">
         <f t="shared" si="0"/>
         <v>43909</v>
       </c>
       <c r="K67" s="43"/>
-      <c r="L67" s="52"/>
+      <c r="L67" s="66"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="16">
         <v>43910</v>
       </c>
       <c r="B68" s="43"/>
-      <c r="C68" s="50"/>
+      <c r="C68" s="51"/>
       <c r="D68" s="16">
         <v>43910</v>
       </c>
       <c r="E68" s="43"/>
-      <c r="F68" s="50"/>
-      <c r="H68" s="65"/>
-      <c r="I68" s="66"/>
+      <c r="F68" s="51"/>
+      <c r="H68" s="59"/>
+      <c r="I68" s="60"/>
       <c r="J68" s="38">
         <f t="shared" si="0"/>
         <v>43910</v>
       </c>
       <c r="K68" s="43"/>
-      <c r="L68" s="52"/>
+      <c r="L68" s="66"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="16">
@@ -2110,7 +2110,7 @@
       <c r="B69" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="44">
+      <c r="C69" s="52">
         <v>4</v>
       </c>
       <c r="D69" s="16">
@@ -2119,39 +2119,39 @@
       <c r="E69" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="45">
+      <c r="F69" s="44">
         <v>6</v>
       </c>
-      <c r="H69" s="65"/>
-      <c r="I69" s="66"/>
+      <c r="H69" s="59"/>
+      <c r="I69" s="60"/>
       <c r="J69" s="38">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="K69" s="53" t="s">
+      <c r="K69" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="L69" s="54"/>
+      <c r="L69" s="68"/>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16">
         <v>43912</v>
       </c>
       <c r="B70" s="43"/>
-      <c r="C70" s="44"/>
+      <c r="C70" s="52"/>
       <c r="D70" s="16">
         <v>43912</v>
       </c>
       <c r="E70" s="43"/>
-      <c r="F70" s="45"/>
-      <c r="H70" s="65"/>
-      <c r="I70" s="66"/>
+      <c r="F70" s="44"/>
+      <c r="H70" s="59"/>
+      <c r="I70" s="60"/>
       <c r="J70" s="38">
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
-      <c r="K70" s="53"/>
-      <c r="L70" s="54"/>
+      <c r="K70" s="67"/>
+      <c r="L70" s="68"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="16">
@@ -2169,11 +2169,11 @@
       <c r="E71" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="F71" s="45">
+      <c r="F71" s="44">
         <v>4</v>
       </c>
-      <c r="H71" s="65"/>
-      <c r="I71" s="66"/>
+      <c r="H71" s="59"/>
+      <c r="I71" s="60"/>
       <c r="J71" s="38">
         <f t="shared" si="0"/>
         <v>43913</v>
@@ -2199,7 +2199,7 @@
         <v>43914</v>
       </c>
       <c r="E72" s="43"/>
-      <c r="F72" s="45"/>
+      <c r="F72" s="44"/>
       <c r="H72" s="2" t="s">
         <v>18</v>
       </c>
@@ -2233,7 +2233,7 @@
       <c r="E73" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F73" s="45">
+      <c r="F73" s="44">
         <v>6</v>
       </c>
       <c r="H73" s="4" t="s">
@@ -2260,12 +2260,12 @@
       <c r="B74" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C74" s="45"/>
+      <c r="C74" s="44"/>
       <c r="D74" s="16">
         <v>43916</v>
       </c>
       <c r="E74" s="43"/>
-      <c r="F74" s="45"/>
+      <c r="F74" s="44"/>
       <c r="J74" s="38">
         <f t="shared" si="0"/>
         <v>43916</v>
@@ -2287,7 +2287,7 @@
         <v>43917</v>
       </c>
       <c r="E75" s="43"/>
-      <c r="F75" s="45"/>
+      <c r="F75" s="44"/>
       <c r="J75" s="38">
         <f t="shared" si="0"/>
         <v>43917</v>
@@ -2311,15 +2311,15 @@
         <v>43918</v>
       </c>
       <c r="E76" s="43"/>
-      <c r="F76" s="45"/>
+      <c r="F76" s="44"/>
       <c r="J76" s="38">
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
-      <c r="K76" s="53" t="s">
+      <c r="K76" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="L76" s="55"/>
+      <c r="L76" s="69"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="16">
@@ -2336,8 +2336,8 @@
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="K77" s="56"/>
-      <c r="L77" s="55"/>
+      <c r="K77" s="70"/>
+      <c r="L77" s="69"/>
     </row>
     <row r="78" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="16">
@@ -2355,7 +2355,7 @@
       <c r="E78" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="F78" s="45">
+      <c r="F78" s="44">
         <v>4</v>
       </c>
       <c r="J78" s="38">
@@ -2376,14 +2376,14 @@
       <c r="B79" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C79" s="44">
+      <c r="C79" s="52">
         <v>4</v>
       </c>
       <c r="D79" s="16">
         <v>43921</v>
       </c>
       <c r="E79" s="43"/>
-      <c r="F79" s="45"/>
+      <c r="F79" s="44"/>
       <c r="J79" s="38">
         <f t="shared" si="0"/>
         <v>43921</v>
@@ -2400,12 +2400,12 @@
         <v>43922</v>
       </c>
       <c r="B80" s="43"/>
-      <c r="C80" s="44"/>
+      <c r="C80" s="52"/>
       <c r="D80" s="16">
         <v>43922</v>
       </c>
       <c r="E80" s="43"/>
-      <c r="F80" s="45"/>
+      <c r="F80" s="44"/>
       <c r="J80" s="38">
         <f t="shared" si="0"/>
         <v>43922</v>
@@ -2419,20 +2419,20 @@
         <v>43923</v>
       </c>
       <c r="B81" s="43"/>
-      <c r="C81" s="44"/>
+      <c r="C81" s="52"/>
       <c r="D81" s="16">
         <v>43923</v>
       </c>
       <c r="E81" s="43"/>
-      <c r="F81" s="45"/>
+      <c r="F81" s="44"/>
       <c r="J81" s="38">
         <f t="shared" si="0"/>
         <v>43923</v>
       </c>
-      <c r="K81" s="44" t="s">
+      <c r="K81" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="L81" s="44" t="s">
+      <c r="L81" s="52" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2452,15 +2452,15 @@
       <c r="E82" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F82" s="45">
+      <c r="F82" s="44">
         <v>3</v>
       </c>
       <c r="J82" s="38">
         <f t="shared" si="0"/>
         <v>43924</v>
       </c>
-      <c r="K82" s="44"/>
-      <c r="L82" s="44"/>
+      <c r="K82" s="52"/>
+      <c r="L82" s="52"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="16">
@@ -2472,15 +2472,15 @@
         <v>43925</v>
       </c>
       <c r="E83" s="43"/>
-      <c r="F83" s="45"/>
+      <c r="F83" s="44"/>
       <c r="J83" s="38">
         <f t="shared" si="0"/>
         <v>43925</v>
       </c>
-      <c r="K83" s="51" t="s">
+      <c r="K83" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="L83" s="51"/>
+      <c r="L83" s="65"/>
     </row>
     <row r="84" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="16">
@@ -2501,8 +2501,8 @@
         <f t="shared" si="0"/>
         <v>43926</v>
       </c>
-      <c r="K84" s="51"/>
-      <c r="L84" s="51"/>
+      <c r="K84" s="65"/>
+      <c r="L84" s="65"/>
     </row>
     <row r="85" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16">
@@ -2511,7 +2511,7 @@
       <c r="B85" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C85" s="44">
+      <c r="C85" s="52">
         <v>10</v>
       </c>
       <c r="D85" s="16">
@@ -2520,7 +2520,7 @@
       <c r="E85" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="F85" s="45">
+      <c r="F85" s="44">
         <v>6</v>
       </c>
       <c r="J85" s="38">
@@ -2539,12 +2539,12 @@
         <v>43928</v>
       </c>
       <c r="B86" s="43"/>
-      <c r="C86" s="44"/>
+      <c r="C86" s="52"/>
       <c r="D86" s="16">
         <v>43928</v>
       </c>
       <c r="E86" s="43"/>
-      <c r="F86" s="45"/>
+      <c r="F86" s="44"/>
       <c r="J86" s="38">
         <f>J85+1</f>
         <v>43928</v>
@@ -2561,12 +2561,12 @@
         <v>43929</v>
       </c>
       <c r="B87" s="43"/>
-      <c r="C87" s="44"/>
+      <c r="C87" s="52"/>
       <c r="D87" s="16">
         <v>43929</v>
       </c>
       <c r="E87" s="43"/>
-      <c r="F87" s="45"/>
+      <c r="F87" s="44"/>
       <c r="J87" s="38">
         <f t="shared" si="0"/>
         <v>43929</v>
@@ -2583,14 +2583,14 @@
         <v>43930</v>
       </c>
       <c r="B88" s="43"/>
-      <c r="C88" s="44"/>
+      <c r="C88" s="52"/>
       <c r="D88" s="16">
         <v>43930</v>
       </c>
       <c r="E88" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="F88" s="45">
+      <c r="F88" s="44">
         <v>4</v>
       </c>
       <c r="J88" s="38">
@@ -2614,7 +2614,7 @@
         <v>43931</v>
       </c>
       <c r="E89" s="43"/>
-      <c r="F89" s="45"/>
+      <c r="F89" s="44"/>
       <c r="J89" s="38">
         <f t="shared" si="0"/>
         <v>43931</v>
@@ -2633,7 +2633,7 @@
         <v>43932</v>
       </c>
       <c r="E90" s="43"/>
-      <c r="F90" s="45"/>
+      <c r="F90" s="44"/>
       <c r="J90" s="38">
         <f t="shared" si="0"/>
         <v>43932</v>
@@ -2767,15 +2767,15 @@
         <v>43941</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="16">
         <v>43942</v>
       </c>
-      <c r="B100" s="20" t="s">
+      <c r="B100" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C100" s="19">
-        <v>2</v>
+      <c r="C100" s="52">
+        <v>3</v>
       </c>
       <c r="D100" s="16">
         <v>43942</v>
@@ -2789,8 +2789,8 @@
       <c r="A101" s="16">
         <v>43943</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="43"/>
+      <c r="C101" s="52"/>
       <c r="D101" s="16">
         <v>43943</v>
       </c>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="C159" s="10">
         <f>SUM(C64:C155)</f>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D159" s="8" t="s">
         <v>2</v>
@@ -3699,7 +3699,34 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="43">
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="B85:B88"/>
+    <mergeCell ref="C85:C88"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E3:F63"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="F85:F87"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="E73:E76"/>
+    <mergeCell ref="F73:F76"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="K83:L84"/>
+    <mergeCell ref="L81:L82"/>
+    <mergeCell ref="K65:K68"/>
+    <mergeCell ref="L65:L68"/>
+    <mergeCell ref="K69:L70"/>
+    <mergeCell ref="K76:L77"/>
+    <mergeCell ref="K81:K82"/>
     <mergeCell ref="E88:E90"/>
     <mergeCell ref="F88:F90"/>
     <mergeCell ref="M1:M2"/>
@@ -3716,31 +3743,6 @@
     <mergeCell ref="E71:E72"/>
     <mergeCell ref="F71:F72"/>
     <mergeCell ref="K2:L63"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="K83:L84"/>
-    <mergeCell ref="L81:L82"/>
-    <mergeCell ref="K65:K68"/>
-    <mergeCell ref="L65:L68"/>
-    <mergeCell ref="K69:L70"/>
-    <mergeCell ref="K76:L77"/>
-    <mergeCell ref="K81:K82"/>
-    <mergeCell ref="B85:B88"/>
-    <mergeCell ref="C85:C88"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E3:F63"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="F78:F81"/>
-    <mergeCell ref="E73:E76"/>
-    <mergeCell ref="F73:F76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Journal et Méca EAU
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minos\OneDrive\Bureau\PROJET\PROJET\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\totok\Documents\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B035BD1-27E2-4D27-ABEB-F4EA0040EB4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDA4914-848D-4B3C-9867-703904F79D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -273,6 +273,21 @@
   </si>
   <si>
     <t>Fin rapport partie perso</t>
+  </si>
+  <si>
+    <t>Commencer Rapport Partie Perso : Ajout des différents diagrammes pour Mécanisme Eau, et présentation du Mécanisme.</t>
+  </si>
+  <si>
+    <t>Rapport : Explication du Code du mécanisme EAU.</t>
+  </si>
+  <si>
+    <t>Rapport : Ajout des différents diagrammes pour Mécanisme 4 éléments, et présentation du mécanisme.</t>
+  </si>
+  <si>
+    <t>Rapport : explication du Code du mécanisme 4 éléments. Prgrammation : Création des fonctions execute() et setupMecanism().</t>
+  </si>
+  <si>
+    <t>Rapport : Commencer rédaction Partie Web.</t>
   </si>
 </sst>
 </file>
@@ -558,7 +573,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -650,98 +665,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1064,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H115" sqref="H115"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1114,7 @@
       <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
@@ -1105,1020 +1123,1020 @@
       <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="57"/>
+      <c r="G1" s="43"/>
       <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="59"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="42"/>
+      <c r="M1" s="48"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>43844</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="56"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="27"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="58"/>
+      <c r="G2" s="44"/>
       <c r="H2" s="27"/>
       <c r="I2" s="11"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="43"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="49"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>43845</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="13">
         <v>43845</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="H3" s="37" t="s">
+      <c r="F3" s="36"/>
+      <c r="H3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="47"/>
+      <c r="I3" s="36"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="53"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>43846</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="13">
         <v>43846</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="40"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="47"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="38"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="53"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>43847</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="13">
         <v>43847</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="40"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="40"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="47"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="38"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="38"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="53"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>43848</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="13">
         <v>43848</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="47"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="38"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>43849</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="13">
         <v>43849</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="40"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="47"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="38"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="53"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>43850</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="40"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="13">
         <v>43850</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="40"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="47"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="53"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>43851</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="40"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="38"/>
       <c r="D9" s="13">
         <v>43851</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="40"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="47"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="38"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="53"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>43852</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="13">
         <v>43852</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="40"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="47"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="53"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>43853</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
       <c r="D11" s="13">
         <v>43853</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="47"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="38"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="53"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>43854</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="13">
         <v>43854</v>
       </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="40"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="47"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="38"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="38"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="53"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>43855</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="13">
         <v>43855</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="40"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="47"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="53"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>43856</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="13">
         <v>43856</v>
       </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="40"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="47"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="53"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>43857</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="13">
         <v>43857</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="40"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="47"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="38"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="53"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>43858</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="13">
         <v>43858</v>
       </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="40"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="40"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="47"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="38"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="38"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="53"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>43859</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
       <c r="D17" s="13">
         <v>43859</v>
       </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="47"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="38"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="38"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="53"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>43860</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="13">
         <v>43860</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="40"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="40"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="47"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="38"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="38"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="53"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>43861</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
       <c r="D19" s="13">
         <v>43861</v>
       </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="47"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="38"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="53"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>43862</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="13">
         <v>43862</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="40"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="47"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="53"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>43863</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
       <c r="D21" s="13">
         <v>43863</v>
       </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="40"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="47"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="38"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="53"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>43864</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="38"/>
       <c r="D22" s="13">
         <v>43864</v>
       </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="40"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="47"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="38"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="38"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="53"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>43865</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="38"/>
       <c r="D23" s="13">
         <v>43865</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="40"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="47"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="38"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="53"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>43866</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="13">
         <v>43866</v>
       </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="40"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="40"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="47"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="38"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="38"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="53"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>43867</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="40"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="38"/>
       <c r="D25" s="13">
         <v>43867</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="40"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="47"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="38"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="38"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="53"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>43868</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="40"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="38"/>
       <c r="D26" s="13">
         <v>43868</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="40"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="40"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="47"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="38"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="38"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="53"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>43869</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="40"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
       <c r="D27" s="13">
         <v>43869</v>
       </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="40"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="40"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="47"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="38"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="38"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="53"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>43870</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="38"/>
       <c r="D28" s="13">
         <v>43870</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="40"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
-      <c r="K28" s="46"/>
-      <c r="L28" s="47"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="38"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="38"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="53"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>43871</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="38"/>
       <c r="D29" s="13">
         <v>43871</v>
       </c>
-      <c r="E29" s="39"/>
-      <c r="F29" s="40"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="47"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="38"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="38"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="53"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>43872</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="40"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
       <c r="D30" s="13">
         <v>43872</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="40"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="40"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="47"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="38"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="38"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="53"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>43873</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="40"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="38"/>
       <c r="D31" s="13">
         <v>43873</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="40"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="40"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="47"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="38"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="38"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="53"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>43874</v>
       </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="40"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="38"/>
       <c r="D32" s="13">
         <v>43874</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="40"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="40"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="47"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="38"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="38"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="53"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>43875</v>
       </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="40"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="38"/>
       <c r="D33" s="13">
         <v>43875</v>
       </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="40"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="40"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="47"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="38"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="38"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="53"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>43876</v>
       </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="40"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="38"/>
       <c r="D34" s="13">
         <v>43876</v>
       </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="40"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="40"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="47"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="38"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="38"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="53"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>43877</v>
       </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="38"/>
       <c r="D35" s="13">
         <v>43877</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="40"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="40"/>
-      <c r="K35" s="46"/>
-      <c r="L35" s="47"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="38"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="38"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="53"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>43878</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="38"/>
       <c r="D36" s="13">
         <v>43878</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="40"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="40"/>
-      <c r="K36" s="46"/>
-      <c r="L36" s="47"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="38"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="38"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="53"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>43879</v>
       </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="40"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="38"/>
       <c r="D37" s="13">
         <v>43879</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="40"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="40"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="47"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="38"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="38"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="53"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>43880</v>
       </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="40"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="38"/>
       <c r="D38" s="13">
         <v>43880</v>
       </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="40"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="40"/>
-      <c r="K38" s="46"/>
-      <c r="L38" s="47"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="38"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="38"/>
+      <c r="K38" s="52"/>
+      <c r="L38" s="53"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>43881</v>
       </c>
-      <c r="B39" s="39"/>
-      <c r="C39" s="40"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="38"/>
       <c r="D39" s="13">
         <v>43881</v>
       </c>
-      <c r="E39" s="39"/>
-      <c r="F39" s="40"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="40"/>
-      <c r="K39" s="46"/>
-      <c r="L39" s="47"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="38"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="38"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="53"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>43882</v>
       </c>
-      <c r="B40" s="39"/>
-      <c r="C40" s="40"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="38"/>
       <c r="D40" s="13">
         <v>43882</v>
       </c>
-      <c r="E40" s="39"/>
-      <c r="F40" s="40"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="40"/>
-      <c r="K40" s="46"/>
-      <c r="L40" s="47"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="38"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="38"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="53"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>43883</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="40"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="38"/>
       <c r="D41" s="13">
         <v>43883</v>
       </c>
-      <c r="E41" s="39"/>
-      <c r="F41" s="40"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="40"/>
-      <c r="K41" s="46"/>
-      <c r="L41" s="47"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="38"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="38"/>
+      <c r="K41" s="52"/>
+      <c r="L41" s="53"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>43884</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="40"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="38"/>
       <c r="D42" s="13">
         <v>43884</v>
       </c>
-      <c r="E42" s="39"/>
-      <c r="F42" s="40"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="40"/>
-      <c r="K42" s="46"/>
-      <c r="L42" s="47"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="38"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="38"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="53"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>43885</v>
       </c>
-      <c r="B43" s="39"/>
-      <c r="C43" s="40"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="38"/>
       <c r="D43" s="13">
         <v>43885</v>
       </c>
-      <c r="E43" s="39"/>
-      <c r="F43" s="40"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="40"/>
-      <c r="K43" s="46"/>
-      <c r="L43" s="47"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="38"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="38"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="53"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>43886</v>
       </c>
-      <c r="B44" s="39"/>
-      <c r="C44" s="40"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="38"/>
       <c r="D44" s="13">
         <v>43886</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="F44" s="40"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="40"/>
-      <c r="K44" s="46"/>
-      <c r="L44" s="47"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="38"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="38"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="53"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>43887</v>
       </c>
-      <c r="B45" s="39"/>
-      <c r="C45" s="40"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="38"/>
       <c r="D45" s="13">
         <v>43887</v>
       </c>
-      <c r="E45" s="39"/>
-      <c r="F45" s="40"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="40"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="47"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="38"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="38"/>
+      <c r="K45" s="52"/>
+      <c r="L45" s="53"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>43888</v>
       </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="40"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="38"/>
       <c r="D46" s="13">
         <v>43888</v>
       </c>
-      <c r="E46" s="39"/>
-      <c r="F46" s="40"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="40"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="47"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="38"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="38"/>
+      <c r="K46" s="52"/>
+      <c r="L46" s="53"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>43889</v>
       </c>
-      <c r="B47" s="39"/>
-      <c r="C47" s="40"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="38"/>
       <c r="D47" s="13">
         <v>43889</v>
       </c>
-      <c r="E47" s="39"/>
-      <c r="F47" s="40"/>
-      <c r="H47" s="39"/>
-      <c r="I47" s="40"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="47"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="38"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="38"/>
+      <c r="K47" s="52"/>
+      <c r="L47" s="53"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>43890</v>
       </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="40"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="38"/>
       <c r="D48" s="13">
         <v>43890</v>
       </c>
-      <c r="E48" s="39"/>
-      <c r="F48" s="40"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="40"/>
-      <c r="K48" s="46"/>
-      <c r="L48" s="47"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="38"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="38"/>
+      <c r="K48" s="52"/>
+      <c r="L48" s="53"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>43891</v>
       </c>
-      <c r="B49" s="39"/>
-      <c r="C49" s="40"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="38"/>
       <c r="D49" s="13">
         <v>43891</v>
       </c>
-      <c r="E49" s="39"/>
-      <c r="F49" s="40"/>
-      <c r="H49" s="39"/>
-      <c r="I49" s="40"/>
-      <c r="K49" s="46"/>
-      <c r="L49" s="47"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="38"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="38"/>
+      <c r="K49" s="52"/>
+      <c r="L49" s="53"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>43892</v>
       </c>
-      <c r="B50" s="39"/>
-      <c r="C50" s="40"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="38"/>
       <c r="D50" s="13">
         <v>43892</v>
       </c>
-      <c r="E50" s="39"/>
-      <c r="F50" s="40"/>
-      <c r="H50" s="39"/>
-      <c r="I50" s="40"/>
-      <c r="K50" s="46"/>
-      <c r="L50" s="47"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="38"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="38"/>
+      <c r="K50" s="52"/>
+      <c r="L50" s="53"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>43893</v>
       </c>
-      <c r="B51" s="39"/>
-      <c r="C51" s="40"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="38"/>
       <c r="D51" s="13">
         <v>43893</v>
       </c>
-      <c r="E51" s="39"/>
-      <c r="F51" s="40"/>
-      <c r="H51" s="39"/>
-      <c r="I51" s="40"/>
-      <c r="K51" s="46"/>
-      <c r="L51" s="47"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="38"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="38"/>
+      <c r="K51" s="52"/>
+      <c r="L51" s="53"/>
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>43894</v>
       </c>
-      <c r="B52" s="39"/>
-      <c r="C52" s="40"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="38"/>
       <c r="D52" s="13">
         <v>43894</v>
       </c>
-      <c r="E52" s="39"/>
-      <c r="F52" s="40"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="40"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="47"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="38"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="38"/>
+      <c r="K52" s="52"/>
+      <c r="L52" s="53"/>
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
         <v>43895</v>
       </c>
-      <c r="B53" s="39"/>
-      <c r="C53" s="40"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="38"/>
       <c r="D53" s="13">
         <v>43895</v>
       </c>
-      <c r="E53" s="39"/>
-      <c r="F53" s="40"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="40"/>
-      <c r="K53" s="46"/>
-      <c r="L53" s="47"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="38"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="38"/>
+      <c r="K53" s="52"/>
+      <c r="L53" s="53"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>43896</v>
       </c>
-      <c r="B54" s="39"/>
-      <c r="C54" s="40"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="38"/>
       <c r="D54" s="13">
         <v>43896</v>
       </c>
-      <c r="E54" s="39"/>
-      <c r="F54" s="40"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="40"/>
-      <c r="K54" s="46"/>
-      <c r="L54" s="47"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="38"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="38"/>
+      <c r="K54" s="52"/>
+      <c r="L54" s="53"/>
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>43897</v>
       </c>
-      <c r="B55" s="39"/>
-      <c r="C55" s="40"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="38"/>
       <c r="D55" s="13">
         <v>43897</v>
       </c>
-      <c r="E55" s="39"/>
-      <c r="F55" s="40"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="40"/>
-      <c r="K55" s="46"/>
-      <c r="L55" s="47"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="38"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="38"/>
+      <c r="K55" s="52"/>
+      <c r="L55" s="53"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>43898</v>
       </c>
-      <c r="B56" s="39"/>
-      <c r="C56" s="40"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="38"/>
       <c r="D56" s="13">
         <v>43898</v>
       </c>
-      <c r="E56" s="39"/>
-      <c r="F56" s="40"/>
-      <c r="H56" s="39"/>
-      <c r="I56" s="40"/>
-      <c r="K56" s="46"/>
-      <c r="L56" s="47"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="38"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="38"/>
+      <c r="K56" s="52"/>
+      <c r="L56" s="53"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>43899</v>
       </c>
-      <c r="B57" s="39"/>
-      <c r="C57" s="40"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="38"/>
       <c r="D57" s="13">
         <v>43899</v>
       </c>
-      <c r="E57" s="39"/>
-      <c r="F57" s="40"/>
-      <c r="H57" s="39"/>
-      <c r="I57" s="40"/>
-      <c r="K57" s="46"/>
-      <c r="L57" s="47"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="38"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="38"/>
+      <c r="K57" s="52"/>
+      <c r="L57" s="53"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>43900</v>
       </c>
-      <c r="B58" s="39"/>
-      <c r="C58" s="40"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="38"/>
       <c r="D58" s="13">
         <v>43900</v>
       </c>
-      <c r="E58" s="39"/>
-      <c r="F58" s="40"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="40"/>
-      <c r="K58" s="46"/>
-      <c r="L58" s="47"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="38"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="38"/>
+      <c r="K58" s="52"/>
+      <c r="L58" s="53"/>
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>43901</v>
       </c>
-      <c r="B59" s="39"/>
-      <c r="C59" s="40"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="38"/>
       <c r="D59" s="13">
         <v>43901</v>
       </c>
-      <c r="E59" s="39"/>
-      <c r="F59" s="40"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="40"/>
-      <c r="K59" s="46"/>
-      <c r="L59" s="47"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="38"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="38"/>
+      <c r="K59" s="52"/>
+      <c r="L59" s="53"/>
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>43902</v>
       </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="40"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="38"/>
       <c r="D60" s="13">
         <v>43902</v>
       </c>
-      <c r="E60" s="39"/>
-      <c r="F60" s="40"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="40"/>
-      <c r="K60" s="46"/>
-      <c r="L60" s="47"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="38"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="38"/>
+      <c r="K60" s="52"/>
+      <c r="L60" s="53"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>43903</v>
       </c>
-      <c r="B61" s="39"/>
-      <c r="C61" s="40"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="38"/>
       <c r="D61" s="13">
         <v>43903</v>
       </c>
-      <c r="E61" s="39"/>
-      <c r="F61" s="40"/>
-      <c r="H61" s="39"/>
-      <c r="I61" s="40"/>
-      <c r="K61" s="46"/>
-      <c r="L61" s="47"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="38"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="38"/>
+      <c r="K61" s="52"/>
+      <c r="L61" s="53"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>43904</v>
       </c>
-      <c r="B62" s="39"/>
-      <c r="C62" s="40"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="38"/>
       <c r="D62" s="13">
         <v>43904</v>
       </c>
-      <c r="E62" s="39"/>
-      <c r="F62" s="40"/>
-      <c r="H62" s="39"/>
-      <c r="I62" s="40"/>
-      <c r="K62" s="46"/>
-      <c r="L62" s="47"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="38"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="38"/>
+      <c r="K62" s="52"/>
+      <c r="L62" s="53"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>43905</v>
       </c>
-      <c r="B63" s="39"/>
-      <c r="C63" s="40"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="38"/>
       <c r="D63" s="13">
         <v>43905</v>
       </c>
-      <c r="E63" s="39"/>
-      <c r="F63" s="40"/>
-      <c r="H63" s="39"/>
-      <c r="I63" s="40"/>
-      <c r="K63" s="46"/>
-      <c r="L63" s="47"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="38"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="38"/>
+      <c r="K63" s="52"/>
+      <c r="L63" s="53"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
@@ -2139,8 +2157,8 @@
       <c r="F64" s="26">
         <v>2</v>
       </c>
-      <c r="H64" s="39"/>
-      <c r="I64" s="40"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="38"/>
       <c r="J64" s="22">
         <v>43906</v>
       </c>
@@ -2155,33 +2173,33 @@
       <c r="A65" s="13">
         <v>43907</v>
       </c>
-      <c r="B65" s="34" t="s">
+      <c r="B65" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="41">
+      <c r="C65" s="40">
         <v>10</v>
       </c>
       <c r="D65" s="13">
         <v>43907</v>
       </c>
-      <c r="E65" s="34" t="s">
+      <c r="E65" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="41">
+      <c r="F65" s="40">
         <v>12</v>
       </c>
-      <c r="H65" s="34" t="s">
+      <c r="H65" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="I65" s="61"/>
+      <c r="I65" s="47"/>
       <c r="J65" s="22">
         <f>J64+1</f>
         <v>43907</v>
       </c>
-      <c r="K65" s="34" t="s">
+      <c r="K65" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="L65" s="48" t="s">
+      <c r="L65" s="54" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2189,67 +2207,67 @@
       <c r="A66" s="13">
         <v>43908</v>
       </c>
-      <c r="B66" s="34"/>
-      <c r="C66" s="41"/>
+      <c r="B66" s="32"/>
+      <c r="C66" s="40"/>
       <c r="D66" s="13">
         <v>43908</v>
       </c>
-      <c r="E66" s="34"/>
-      <c r="F66" s="41"/>
-      <c r="H66" s="34"/>
-      <c r="I66" s="61"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="40"/>
+      <c r="H66" s="32"/>
+      <c r="I66" s="47"/>
       <c r="J66" s="22">
         <f t="shared" ref="J66:J129" si="0">J65+1</f>
         <v>43908</v>
       </c>
-      <c r="K66" s="34"/>
-      <c r="L66" s="48"/>
+      <c r="K66" s="32"/>
+      <c r="L66" s="54"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
         <v>43909</v>
       </c>
-      <c r="B67" s="34"/>
-      <c r="C67" s="41"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="40"/>
       <c r="D67" s="13">
         <v>43909</v>
       </c>
-      <c r="E67" s="34"/>
-      <c r="F67" s="41"/>
-      <c r="H67" s="34"/>
-      <c r="I67" s="61"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="40"/>
+      <c r="H67" s="32"/>
+      <c r="I67" s="47"/>
       <c r="J67" s="22">
         <f t="shared" si="0"/>
         <v>43909</v>
       </c>
-      <c r="K67" s="34"/>
-      <c r="L67" s="48"/>
+      <c r="K67" s="32"/>
+      <c r="L67" s="54"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
         <v>43910</v>
       </c>
-      <c r="B68" s="34"/>
-      <c r="C68" s="41"/>
+      <c r="B68" s="32"/>
+      <c r="C68" s="40"/>
       <c r="D68" s="13">
         <v>43910</v>
       </c>
-      <c r="E68" s="34"/>
-      <c r="F68" s="41"/>
-      <c r="H68" s="34"/>
-      <c r="I68" s="61"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="40"/>
+      <c r="H68" s="32"/>
+      <c r="I68" s="47"/>
       <c r="J68" s="22">
         <f t="shared" si="0"/>
         <v>43910</v>
       </c>
-      <c r="K68" s="34"/>
-      <c r="L68" s="48"/>
+      <c r="K68" s="32"/>
+      <c r="L68" s="54"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
         <v>43911</v>
       </c>
-      <c r="B69" s="34" t="s">
+      <c r="B69" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C69" s="33">
@@ -2258,42 +2276,42 @@
       <c r="D69" s="13">
         <v>43911</v>
       </c>
-      <c r="E69" s="34" t="s">
+      <c r="E69" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F69" s="32">
+      <c r="F69" s="60">
         <v>6</v>
       </c>
-      <c r="H69" s="34"/>
-      <c r="I69" s="61"/>
+      <c r="H69" s="32"/>
+      <c r="I69" s="47"/>
       <c r="J69" s="22">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="K69" s="49" t="s">
+      <c r="K69" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="L69" s="50"/>
+      <c r="L69" s="56"/>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
         <v>43912</v>
       </c>
-      <c r="B70" s="34"/>
+      <c r="B70" s="32"/>
       <c r="C70" s="33"/>
       <c r="D70" s="13">
         <v>43912</v>
       </c>
-      <c r="E70" s="34"/>
-      <c r="F70" s="32"/>
-      <c r="H70" s="34"/>
-      <c r="I70" s="61"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="60"/>
+      <c r="H70" s="32"/>
+      <c r="I70" s="47"/>
       <c r="J70" s="22">
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
-      <c r="K70" s="49"/>
-      <c r="L70" s="50"/>
+      <c r="K70" s="55"/>
+      <c r="L70" s="56"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
@@ -2308,14 +2326,14 @@
       <c r="D71" s="13">
         <v>43913</v>
       </c>
-      <c r="E71" s="34" t="s">
+      <c r="E71" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F71" s="32">
+      <c r="F71" s="60">
         <v>4</v>
       </c>
-      <c r="H71" s="34"/>
-      <c r="I71" s="61"/>
+      <c r="H71" s="32"/>
+      <c r="I71" s="47"/>
       <c r="J71" s="22">
         <f t="shared" si="0"/>
         <v>43913</v>
@@ -2340,8 +2358,8 @@
       <c r="D72" s="13">
         <v>43914</v>
       </c>
-      <c r="E72" s="34"/>
-      <c r="F72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="60"/>
       <c r="G72" s="13">
         <v>43913</v>
       </c>
@@ -2375,19 +2393,19 @@
       <c r="D73" s="13">
         <v>43915</v>
       </c>
-      <c r="E73" s="34" t="s">
+      <c r="E73" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F73" s="32">
+      <c r="F73" s="60">
         <v>6</v>
       </c>
       <c r="G73" s="13">
         <v>43914</v>
       </c>
-      <c r="H73" s="34" t="s">
+      <c r="H73" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="I73" s="54"/>
+      <c r="I73" s="39"/>
       <c r="J73" s="22">
         <f t="shared" si="0"/>
         <v>43915</v>
@@ -2403,17 +2421,17 @@
       <c r="A74" s="13">
         <v>43916</v>
       </c>
-      <c r="B74" s="34" t="s">
+      <c r="B74" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="32"/>
+      <c r="C74" s="60"/>
       <c r="D74" s="13">
         <v>43916</v>
       </c>
-      <c r="E74" s="34"/>
-      <c r="F74" s="32"/>
-      <c r="H74" s="34"/>
-      <c r="I74" s="54"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="60"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="39"/>
       <c r="J74" s="22">
         <f t="shared" si="0"/>
         <v>43916</v>
@@ -2434,8 +2452,8 @@
       <c r="D75" s="13">
         <v>43917</v>
       </c>
-      <c r="E75" s="34"/>
-      <c r="F75" s="32"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="60"/>
       <c r="G75" s="13">
         <v>43915</v>
       </c>
@@ -2467,8 +2485,8 @@
       <c r="D76" s="13">
         <v>43918</v>
       </c>
-      <c r="E76" s="34"/>
-      <c r="F76" s="32"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="60"/>
       <c r="G76" s="13">
         <v>43916</v>
       </c>
@@ -2482,10 +2500,10 @@
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
-      <c r="K76" s="49" t="s">
+      <c r="K76" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="L76" s="51"/>
+      <c r="L76" s="57"/>
     </row>
     <row r="77" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="13">
@@ -2511,8 +2529,8 @@
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="K77" s="52"/>
-      <c r="L77" s="51"/>
+      <c r="K77" s="58"/>
+      <c r="L77" s="57"/>
     </row>
     <row r="78" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="13">
@@ -2527,10 +2545,10 @@
       <c r="D78" s="13">
         <v>43920</v>
       </c>
-      <c r="E78" s="34" t="s">
+      <c r="E78" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F78" s="32">
+      <c r="F78" s="60">
         <v>4</v>
       </c>
       <c r="G78" s="13">
@@ -2557,7 +2575,7 @@
       <c r="A79" s="13">
         <v>43921</v>
       </c>
-      <c r="B79" s="34" t="s">
+      <c r="B79" s="32" t="s">
         <v>44</v>
       </c>
       <c r="C79" s="33">
@@ -2566,8 +2584,8 @@
       <c r="D79" s="13">
         <v>43921</v>
       </c>
-      <c r="E79" s="34"/>
-      <c r="F79" s="32"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="60"/>
       <c r="G79" s="13">
         <v>43919</v>
       </c>
@@ -2592,13 +2610,13 @@
       <c r="A80" s="13">
         <v>43922</v>
       </c>
-      <c r="B80" s="34"/>
+      <c r="B80" s="32"/>
       <c r="C80" s="33"/>
       <c r="D80" s="13">
         <v>43922</v>
       </c>
-      <c r="E80" s="34"/>
-      <c r="F80" s="32"/>
+      <c r="E80" s="32"/>
+      <c r="F80" s="60"/>
       <c r="G80" s="13">
         <v>43920</v>
       </c>
@@ -2621,13 +2639,13 @@
       <c r="A81" s="13">
         <v>43923</v>
       </c>
-      <c r="B81" s="34"/>
+      <c r="B81" s="32"/>
       <c r="C81" s="33"/>
       <c r="D81" s="13">
         <v>43923</v>
       </c>
-      <c r="E81" s="34"/>
-      <c r="F81" s="32"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="60"/>
       <c r="H81" s="20"/>
       <c r="I81" s="20"/>
       <c r="J81" s="22">
@@ -2654,10 +2672,10 @@
       <c r="D82" s="13">
         <v>43924</v>
       </c>
-      <c r="E82" s="34" t="s">
+      <c r="E82" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="F82" s="32">
+      <c r="F82" s="60">
         <v>3</v>
       </c>
       <c r="H82" s="20"/>
@@ -2678,18 +2696,18 @@
       <c r="D83" s="13">
         <v>43925</v>
       </c>
-      <c r="E83" s="34"/>
-      <c r="F83" s="32"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="60"/>
       <c r="H83" s="20"/>
       <c r="I83" s="20"/>
       <c r="J83" s="22">
         <f t="shared" si="0"/>
         <v>43925</v>
       </c>
-      <c r="K83" s="53" t="s">
+      <c r="K83" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="L83" s="53"/>
+      <c r="L83" s="34"/>
     </row>
     <row r="84" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13">
@@ -2712,14 +2730,14 @@
         <f t="shared" si="0"/>
         <v>43926</v>
       </c>
-      <c r="K84" s="53"/>
-      <c r="L84" s="53"/>
+      <c r="K84" s="34"/>
+      <c r="L84" s="34"/>
     </row>
     <row r="85" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13">
         <v>43927</v>
       </c>
-      <c r="B85" s="36" t="s">
+      <c r="B85" s="59" t="s">
         <v>53</v>
       </c>
       <c r="C85" s="33">
@@ -2728,10 +2746,10 @@
       <c r="D85" s="13">
         <v>43927</v>
       </c>
-      <c r="E85" s="34" t="s">
+      <c r="E85" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="F85" s="32">
+      <c r="F85" s="60">
         <v>6</v>
       </c>
       <c r="H85" s="20"/>
@@ -2751,13 +2769,13 @@
       <c r="A86" s="13">
         <v>43928</v>
       </c>
-      <c r="B86" s="36"/>
+      <c r="B86" s="59"/>
       <c r="C86" s="33"/>
       <c r="D86" s="13">
         <v>43928</v>
       </c>
-      <c r="E86" s="34"/>
-      <c r="F86" s="32"/>
+      <c r="E86" s="32"/>
+      <c r="F86" s="60"/>
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
       <c r="J86" s="22">
@@ -2775,13 +2793,13 @@
       <c r="A87" s="13">
         <v>43929</v>
       </c>
-      <c r="B87" s="36"/>
+      <c r="B87" s="59"/>
       <c r="C87" s="33"/>
       <c r="D87" s="13">
         <v>43929</v>
       </c>
-      <c r="E87" s="34"/>
-      <c r="F87" s="32"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="60"/>
       <c r="H87" s="20"/>
       <c r="I87" s="20"/>
       <c r="J87" s="22">
@@ -2799,15 +2817,15 @@
       <c r="A88" s="21">
         <v>43930</v>
       </c>
-      <c r="B88" s="36"/>
+      <c r="B88" s="59"/>
       <c r="C88" s="33"/>
       <c r="D88" s="13">
         <v>43930</v>
       </c>
-      <c r="E88" s="34" t="s">
+      <c r="E88" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="F88" s="32">
+      <c r="F88" s="60">
         <v>4</v>
       </c>
       <c r="H88" s="20"/>
@@ -2827,13 +2845,13 @@
       <c r="A89" s="21">
         <v>43931</v>
       </c>
-      <c r="B89" s="36"/>
+      <c r="B89" s="59"/>
       <c r="C89" s="33"/>
       <c r="D89" s="13">
         <v>43931</v>
       </c>
-      <c r="E89" s="34"/>
-      <c r="F89" s="32"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="60"/>
       <c r="H89" s="20"/>
       <c r="I89" s="20"/>
       <c r="J89" s="22">
@@ -2851,13 +2869,13 @@
       <c r="A90" s="21">
         <v>43932</v>
       </c>
-      <c r="B90" s="36"/>
+      <c r="B90" s="59"/>
       <c r="C90" s="33"/>
       <c r="D90" s="13">
         <v>43932</v>
       </c>
-      <c r="E90" s="34"/>
-      <c r="F90" s="32"/>
+      <c r="E90" s="32"/>
+      <c r="F90" s="60"/>
       <c r="H90" s="20"/>
       <c r="I90" s="20"/>
       <c r="J90" s="22">
@@ -2888,16 +2906,16 @@
         <f t="shared" si="0"/>
         <v>43933</v>
       </c>
-      <c r="K91" s="31" t="s">
+      <c r="K91" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="L91" s="31"/>
+      <c r="L91" s="61"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="13">
         <v>43934</v>
       </c>
-      <c r="B92" s="34" t="s">
+      <c r="B92" s="32" t="s">
         <v>64</v>
       </c>
       <c r="C92" s="33">
@@ -2906,7 +2924,7 @@
       <c r="D92" s="13">
         <v>43934</v>
       </c>
-      <c r="E92" s="34" t="s">
+      <c r="E92" s="32" t="s">
         <v>65</v>
       </c>
       <c r="H92" s="20"/>
@@ -2915,84 +2933,84 @@
         <f t="shared" si="0"/>
         <v>43934</v>
       </c>
-      <c r="K92" s="31"/>
-      <c r="L92" s="31"/>
+      <c r="K92" s="61"/>
+      <c r="L92" s="61"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="13">
         <v>43935</v>
       </c>
-      <c r="B93" s="34"/>
+      <c r="B93" s="32"/>
       <c r="C93" s="33"/>
       <c r="D93" s="13">
         <v>43935</v>
       </c>
-      <c r="E93" s="35"/>
+      <c r="E93" s="62"/>
       <c r="H93" s="20"/>
       <c r="I93" s="20"/>
       <c r="J93" s="22">
         <f t="shared" si="0"/>
         <v>43935</v>
       </c>
-      <c r="K93" s="31"/>
-      <c r="L93" s="31"/>
+      <c r="K93" s="61"/>
+      <c r="L93" s="61"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="13">
         <v>43936</v>
       </c>
-      <c r="B94" s="34"/>
+      <c r="B94" s="32"/>
       <c r="C94" s="33"/>
       <c r="D94" s="13">
         <v>43936</v>
       </c>
-      <c r="E94" s="35"/>
+      <c r="E94" s="62"/>
       <c r="H94" s="20"/>
       <c r="I94" s="20"/>
       <c r="J94" s="22">
         <f t="shared" si="0"/>
         <v>43936</v>
       </c>
-      <c r="K94" s="31"/>
-      <c r="L94" s="31"/>
+      <c r="K94" s="61"/>
+      <c r="L94" s="61"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="13">
         <v>43937</v>
       </c>
-      <c r="B95" s="34"/>
+      <c r="B95" s="32"/>
       <c r="C95" s="33"/>
       <c r="D95" s="13">
         <v>43937</v>
       </c>
-      <c r="E95" s="35"/>
+      <c r="E95" s="62"/>
       <c r="H95" s="20"/>
       <c r="I95" s="20"/>
       <c r="J95" s="22">
         <f t="shared" si="0"/>
         <v>43937</v>
       </c>
-      <c r="K95" s="31"/>
-      <c r="L95" s="31"/>
+      <c r="K95" s="61"/>
+      <c r="L95" s="61"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="13">
         <v>43938</v>
       </c>
-      <c r="B96" s="34"/>
+      <c r="B96" s="32"/>
       <c r="C96" s="33"/>
       <c r="D96" s="13">
         <v>43938</v>
       </c>
-      <c r="E96" s="35"/>
+      <c r="E96" s="62"/>
       <c r="H96" s="20"/>
       <c r="I96" s="20"/>
       <c r="J96" s="22">
         <f t="shared" si="0"/>
         <v>43938</v>
       </c>
-      <c r="K96" s="31"/>
-      <c r="L96" s="31"/>
+      <c r="K96" s="61"/>
+      <c r="L96" s="61"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="13">
@@ -3003,15 +3021,15 @@
       <c r="D97" s="13">
         <v>43939</v>
       </c>
-      <c r="E97" s="35"/>
+      <c r="E97" s="62"/>
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
       <c r="J97" s="22">
         <f t="shared" si="0"/>
         <v>43939</v>
       </c>
-      <c r="K97" s="31"/>
-      <c r="L97" s="31"/>
+      <c r="K97" s="61"/>
+      <c r="L97" s="61"/>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="13">
@@ -3022,21 +3040,21 @@
       <c r="D98" s="13">
         <v>43940</v>
       </c>
-      <c r="E98" s="35"/>
+      <c r="E98" s="62"/>
       <c r="H98" s="20"/>
       <c r="I98" s="20"/>
       <c r="J98" s="22">
         <f t="shared" si="0"/>
         <v>43940</v>
       </c>
-      <c r="K98" s="31"/>
-      <c r="L98" s="31"/>
+      <c r="K98" s="61"/>
+      <c r="L98" s="61"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="13">
         <v>43941</v>
       </c>
-      <c r="B99" s="34" t="s">
+      <c r="B99" s="32" t="s">
         <v>66</v>
       </c>
       <c r="C99" s="33">
@@ -3045,44 +3063,50 @@
       <c r="D99" s="13">
         <v>43941</v>
       </c>
-      <c r="E99" s="35"/>
+      <c r="E99" s="62"/>
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
       <c r="J99" s="22">
         <f t="shared" si="0"/>
         <v>43941</v>
       </c>
-      <c r="K99" s="31"/>
-      <c r="L99" s="31"/>
+      <c r="K99" s="61"/>
+      <c r="L99" s="61"/>
     </row>
     <row r="100" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13">
         <v>43942</v>
       </c>
-      <c r="B100" s="34"/>
+      <c r="B100" s="32"/>
       <c r="C100" s="33"/>
       <c r="D100" s="13">
         <v>43942</v>
       </c>
-      <c r="E100" s="35"/>
+      <c r="E100" s="62"/>
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
       <c r="J100" s="22">
         <f t="shared" si="0"/>
         <v>43942</v>
       </c>
-      <c r="K100" s="31"/>
-      <c r="L100" s="31"/>
+      <c r="K100" s="61"/>
+      <c r="L100" s="61"/>
     </row>
     <row r="101" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13">
         <v>43943</v>
       </c>
-      <c r="B101" s="34"/>
+      <c r="B101" s="32"/>
       <c r="C101" s="33"/>
       <c r="D101" s="13">
         <v>43943</v>
       </c>
+      <c r="E101" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F101" s="60">
+        <v>3</v>
+      </c>
       <c r="G101" s="13">
         <v>43943</v>
       </c>
@@ -3094,14 +3118,14 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="K101" s="31"/>
-      <c r="L101" s="31"/>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K101" s="61"/>
+      <c r="L101" s="61"/>
+    </row>
+    <row r="102" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13">
         <v>43944</v>
       </c>
-      <c r="B102" s="34" t="s">
+      <c r="B102" s="32" t="s">
         <v>68</v>
       </c>
       <c r="C102" s="33">
@@ -3110,6 +3134,8 @@
       <c r="D102" s="13">
         <v>43944</v>
       </c>
+      <c r="E102" s="32"/>
+      <c r="F102" s="60"/>
       <c r="G102" s="13">
         <v>43944</v>
       </c>
@@ -3121,18 +3147,24 @@
         <f t="shared" si="0"/>
         <v>43944</v>
       </c>
-      <c r="K102" s="31"/>
-      <c r="L102" s="31"/>
-    </row>
-    <row r="103" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K102" s="61"/>
+      <c r="L102" s="61"/>
+    </row>
+    <row r="103" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13">
         <v>43945</v>
       </c>
-      <c r="B103" s="34"/>
+      <c r="B103" s="32"/>
       <c r="C103" s="33"/>
       <c r="D103" s="13">
         <v>43945</v>
       </c>
+      <c r="E103" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F103" s="31">
+        <v>2</v>
+      </c>
       <c r="G103" s="13">
         <v>43945</v>
       </c>
@@ -3144,8 +3176,8 @@
         <f t="shared" si="0"/>
         <v>43945</v>
       </c>
-      <c r="K103" s="31"/>
-      <c r="L103" s="31"/>
+      <c r="K103" s="61"/>
+      <c r="L103" s="61"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="13">
@@ -3167,8 +3199,8 @@
         <f t="shared" si="0"/>
         <v>43946</v>
       </c>
-      <c r="K104" s="31"/>
-      <c r="L104" s="31"/>
+      <c r="K104" s="61"/>
+      <c r="L104" s="61"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="13">
@@ -3190,7 +3222,7 @@
         <f t="shared" si="0"/>
         <v>43947</v>
       </c>
-      <c r="K105" s="32" t="s">
+      <c r="K105" s="60" t="s">
         <v>71</v>
       </c>
       <c r="L105" s="33" t="s">
@@ -3210,6 +3242,12 @@
       <c r="D106" s="13">
         <v>43948</v>
       </c>
+      <c r="E106" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F106" s="60">
+        <v>3</v>
+      </c>
       <c r="G106" s="13">
         <v>43948</v>
       </c>
@@ -3219,14 +3257,14 @@
         <f t="shared" si="0"/>
         <v>43948</v>
       </c>
-      <c r="K106" s="32"/>
+      <c r="K106" s="60"/>
       <c r="L106" s="33"/>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="13">
         <v>43949</v>
       </c>
-      <c r="B107" s="34" t="s">
+      <c r="B107" s="32" t="s">
         <v>73</v>
       </c>
       <c r="C107" s="33">
@@ -3235,6 +3273,8 @@
       <c r="D107" s="13">
         <v>43949</v>
       </c>
+      <c r="E107" s="32"/>
+      <c r="F107" s="60"/>
       <c r="G107" s="13">
         <v>43949</v>
       </c>
@@ -3255,10 +3295,16 @@
       <c r="A108" s="13">
         <v>43950</v>
       </c>
-      <c r="B108" s="34"/>
+      <c r="B108" s="32"/>
       <c r="C108" s="33"/>
       <c r="D108" s="13">
         <v>43950</v>
+      </c>
+      <c r="E108" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="F108" s="60">
+        <v>3</v>
       </c>
       <c r="G108" s="13">
         <v>43950</v>
@@ -3285,6 +3331,8 @@
       <c r="D109" s="13">
         <v>43951</v>
       </c>
+      <c r="E109" s="32"/>
+      <c r="F109" s="60"/>
       <c r="G109" s="13">
         <v>43951</v>
       </c>
@@ -3306,6 +3354,12 @@
       <c r="D110" s="13">
         <v>43952</v>
       </c>
+      <c r="E110" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="F110" s="60">
+        <v>2</v>
+      </c>
       <c r="G110" s="13">
         <v>43952</v>
       </c>
@@ -3327,6 +3381,8 @@
       <c r="D111" s="13">
         <v>43953</v>
       </c>
+      <c r="E111" s="32"/>
+      <c r="F111" s="60"/>
       <c r="G111" s="13">
         <v>43953</v>
       </c>
@@ -3352,6 +3408,8 @@
       <c r="D112" s="13">
         <v>43954</v>
       </c>
+      <c r="E112" s="19"/>
+      <c r="F112" s="20"/>
       <c r="G112" s="13">
         <v>43954</v>
       </c>
@@ -4261,7 +4319,7 @@
       </c>
       <c r="F159" s="8">
         <f>SUM(F64:F156)</f>
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="H159" s="28"/>
       <c r="I159" s="17">
@@ -4376,7 +4434,55 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="64">
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="E110:E111"/>
+    <mergeCell ref="F110:F111"/>
+    <mergeCell ref="K91:L104"/>
+    <mergeCell ref="K105:K106"/>
+    <mergeCell ref="L105:L106"/>
+    <mergeCell ref="C92:C96"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="E92:E100"/>
+    <mergeCell ref="F88:F90"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="F85:F87"/>
+    <mergeCell ref="E101:E102"/>
+    <mergeCell ref="F101:F102"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="B85:B90"/>
+    <mergeCell ref="C85:C90"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="E3:F63"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="E73:E76"/>
+    <mergeCell ref="F73:F76"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="K2:L63"/>
+    <mergeCell ref="L81:L82"/>
+    <mergeCell ref="K65:K68"/>
+    <mergeCell ref="L65:L68"/>
+    <mergeCell ref="K69:L70"/>
+    <mergeCell ref="K76:L77"/>
+    <mergeCell ref="K81:K82"/>
     <mergeCell ref="B107:B108"/>
     <mergeCell ref="C107:C108"/>
     <mergeCell ref="K83:L84"/>
@@ -4393,46 +4499,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="H65:H71"/>
     <mergeCell ref="I65:I71"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="K2:L63"/>
-    <mergeCell ref="L81:L82"/>
-    <mergeCell ref="K65:K68"/>
-    <mergeCell ref="L65:L68"/>
-    <mergeCell ref="K69:L70"/>
-    <mergeCell ref="K76:L77"/>
-    <mergeCell ref="K81:K82"/>
-    <mergeCell ref="B85:B90"/>
-    <mergeCell ref="C85:C90"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="E3:F63"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="F78:F81"/>
-    <mergeCell ref="E73:E76"/>
-    <mergeCell ref="F73:F76"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="K91:L104"/>
-    <mergeCell ref="K105:K106"/>
-    <mergeCell ref="L105:L106"/>
-    <mergeCell ref="C92:C96"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="E88:E90"/>
-    <mergeCell ref="E92:E100"/>
-    <mergeCell ref="F88:F90"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="F85:F87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
JA + up memoriser etat
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22904"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\totok\Documents\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDA4914-848D-4B3C-9867-703904F79D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C130FDB-ED4F-41DC-9D86-62B939951EA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="88">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -236,6 +236,9 @@
     <t>Ajout d'une partie de mon travail dans le document commun + Travail sur le CSS de l'application Web pour modifier les margin et les mettre en "%" de la page</t>
   </si>
   <si>
+    <t>Commencer Rapport Partie Perso : Ajout des différents diagrammes pour Mécanisme Eau, et présentation du Mécanisme.</t>
+  </si>
+  <si>
     <t>Rapport : Explication Programme Python global</t>
   </si>
   <si>
@@ -245,6 +248,9 @@
     <t>Rapport : Explication Liste Dictionnaire // Python</t>
   </si>
   <si>
+    <t>Rapport : Explication du Code du mécanisme EAU.</t>
+  </si>
+  <si>
     <t>Rapport : Explication Thread // Python</t>
   </si>
   <si>
@@ -254,47 +260,50 @@
     <t>Remise en forme du document commun au groupe + ajout d'une table des matières corrigée après entretien avec notre prof référent + Travail sur les mécanismes Echec et Lion basculant</t>
   </si>
   <si>
+    <t>Rapport : Ajout des différents diagrammes pour Mécanisme 4 éléments, et présentation du mécanisme.</t>
+  </si>
+  <si>
     <t>Travail sur les trois mécanismes, le code sur Arduino, modifications</t>
   </si>
   <si>
     <t>2h30</t>
   </si>
   <si>
+    <t>Rapport : explication du Code du mécanisme 4 éléments. Prgrammation : Création des fonctions execute() et setupMecanism().</t>
+  </si>
+  <si>
     <t>rapport + infos sur code+code memoriser etat</t>
   </si>
   <si>
     <t>3h30</t>
   </si>
   <si>
+    <t>WEEK END</t>
+  </si>
+  <si>
+    <t>Rapport : Commencer rédaction Partie Web.</t>
+  </si>
+  <si>
+    <t>Amélioration/Fin programme Python+Arduino</t>
+  </si>
+  <si>
+    <t>Fin rapport partie perso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rapport </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fusionner les rapports + physique </t>
+  </si>
+  <si>
     <t>Total heures</t>
-  </si>
-  <si>
-    <t>Amélioration/Fin programme Python+Arduino</t>
-  </si>
-  <si>
-    <t>Fin rapport partie perso</t>
-  </si>
-  <si>
-    <t>Commencer Rapport Partie Perso : Ajout des différents diagrammes pour Mécanisme Eau, et présentation du Mécanisme.</t>
-  </si>
-  <si>
-    <t>Rapport : Explication du Code du mécanisme EAU.</t>
-  </si>
-  <si>
-    <t>Rapport : Ajout des différents diagrammes pour Mécanisme 4 éléments, et présentation du mécanisme.</t>
-  </si>
-  <si>
-    <t>Rapport : explication du Code du mécanisme 4 éléments. Prgrammation : Création des fonctions execute() et setupMecanism().</t>
-  </si>
-  <si>
-    <t>Rapport : Commencer rédaction Partie Web.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +399,14 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -573,7 +590,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -648,53 +665,89 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -716,50 +769,8 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -784,7 +795,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1082,11 +1093,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView tabSelected="1" topLeftCell="E103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L114" sqref="L114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="15"/>
     <col min="2" max="2" width="49.7109375" style="1" customWidth="1"/>
@@ -1104,7 +1115,7 @@
     <col min="14" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="57.75" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1125,7 @@
       <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="53" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
@@ -1123,23 +1134,23 @@
       <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="43"/>
+      <c r="G1" s="55"/>
       <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="45"/>
+      <c r="J1" s="57"/>
       <c r="K1" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="48"/>
-    </row>
-    <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="40"/>
+    </row>
+    <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1">
       <c r="A2" s="13">
         <v>43844</v>
       </c>
@@ -1147,18 +1158,18 @@
         <v>9</v>
       </c>
       <c r="C2" s="36"/>
-      <c r="D2" s="42"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="27"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="44"/>
+      <c r="G2" s="56"/>
       <c r="H2" s="27"/>
       <c r="I2" s="11"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="49"/>
-    </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="58"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="41"/>
+    </row>
+    <row r="3" spans="1:13" ht="15" customHeight="1">
       <c r="A3" s="13">
         <v>43845</v>
       </c>
@@ -1175,10 +1186,10 @@
         <v>9</v>
       </c>
       <c r="I3" s="36"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="53"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="44"/>
+      <c r="L3" s="45"/>
+    </row>
+    <row r="4" spans="1:13" ht="15" customHeight="1">
       <c r="A4" s="13">
         <v>43846</v>
       </c>
@@ -1191,10 +1202,10 @@
       <c r="F4" s="38"/>
       <c r="H4" s="37"/>
       <c r="I4" s="38"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="53"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="44"/>
+      <c r="L4" s="45"/>
+    </row>
+    <row r="5" spans="1:13" ht="15" customHeight="1">
       <c r="A5" s="13">
         <v>43847</v>
       </c>
@@ -1207,10 +1218,10 @@
       <c r="F5" s="38"/>
       <c r="H5" s="37"/>
       <c r="I5" s="38"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="53"/>
-    </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="44"/>
+      <c r="L5" s="45"/>
+    </row>
+    <row r="6" spans="1:13" ht="15" customHeight="1">
       <c r="A6" s="13">
         <v>43848</v>
       </c>
@@ -1223,10 +1234,10 @@
       <c r="F6" s="38"/>
       <c r="H6" s="37"/>
       <c r="I6" s="38"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="44"/>
+      <c r="L6" s="45"/>
+    </row>
+    <row r="7" spans="1:13" ht="15" customHeight="1">
       <c r="A7" s="13">
         <v>43849</v>
       </c>
@@ -1239,10 +1250,10 @@
       <c r="F7" s="38"/>
       <c r="H7" s="37"/>
       <c r="I7" s="38"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="53"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="44"/>
+      <c r="L7" s="45"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1">
       <c r="A8" s="13">
         <v>43850</v>
       </c>
@@ -1255,10 +1266,10 @@
       <c r="F8" s="38"/>
       <c r="H8" s="37"/>
       <c r="I8" s="38"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="53"/>
-    </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="44"/>
+      <c r="L8" s="45"/>
+    </row>
+    <row r="9" spans="1:13" ht="15" customHeight="1">
       <c r="A9" s="13">
         <v>43851</v>
       </c>
@@ -1271,10 +1282,10 @@
       <c r="F9" s="38"/>
       <c r="H9" s="37"/>
       <c r="I9" s="38"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="53"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="44"/>
+      <c r="L9" s="45"/>
+    </row>
+    <row r="10" spans="1:13" ht="15" customHeight="1">
       <c r="A10" s="13">
         <v>43852</v>
       </c>
@@ -1287,10 +1298,10 @@
       <c r="F10" s="38"/>
       <c r="H10" s="37"/>
       <c r="I10" s="38"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="53"/>
-    </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
+    </row>
+    <row r="11" spans="1:13" ht="15" customHeight="1">
       <c r="A11" s="13">
         <v>43853</v>
       </c>
@@ -1303,10 +1314,10 @@
       <c r="F11" s="38"/>
       <c r="H11" s="37"/>
       <c r="I11" s="38"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="53"/>
-    </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="44"/>
+      <c r="L11" s="45"/>
+    </row>
+    <row r="12" spans="1:13" ht="15" customHeight="1">
       <c r="A12" s="13">
         <v>43854</v>
       </c>
@@ -1319,10 +1330,10 @@
       <c r="F12" s="38"/>
       <c r="H12" s="37"/>
       <c r="I12" s="38"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="53"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
+    </row>
+    <row r="13" spans="1:13" ht="15" customHeight="1">
       <c r="A13" s="13">
         <v>43855</v>
       </c>
@@ -1335,10 +1346,10 @@
       <c r="F13" s="38"/>
       <c r="H13" s="37"/>
       <c r="I13" s="38"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="53"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="44"/>
+      <c r="L13" s="45"/>
+    </row>
+    <row r="14" spans="1:13" ht="15" customHeight="1">
       <c r="A14" s="13">
         <v>43856</v>
       </c>
@@ -1351,10 +1362,10 @@
       <c r="F14" s="38"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="53"/>
-    </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="44"/>
+      <c r="L14" s="45"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1">
       <c r="A15" s="13">
         <v>43857</v>
       </c>
@@ -1367,10 +1378,10 @@
       <c r="F15" s="38"/>
       <c r="H15" s="37"/>
       <c r="I15" s="38"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="53"/>
-    </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="44"/>
+      <c r="L15" s="45"/>
+    </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1">
       <c r="A16" s="13">
         <v>43858</v>
       </c>
@@ -1383,10 +1394,10 @@
       <c r="F16" s="38"/>
       <c r="H16" s="37"/>
       <c r="I16" s="38"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="53"/>
-    </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="44"/>
+      <c r="L16" s="45"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" customHeight="1">
       <c r="A17" s="13">
         <v>43859</v>
       </c>
@@ -1399,10 +1410,10 @@
       <c r="F17" s="38"/>
       <c r="H17" s="37"/>
       <c r="I17" s="38"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="53"/>
-    </row>
-    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="44"/>
+      <c r="L17" s="45"/>
+    </row>
+    <row r="18" spans="1:12" ht="15" customHeight="1">
       <c r="A18" s="13">
         <v>43860</v>
       </c>
@@ -1415,10 +1426,10 @@
       <c r="F18" s="38"/>
       <c r="H18" s="37"/>
       <c r="I18" s="38"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="53"/>
-    </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="44"/>
+      <c r="L18" s="45"/>
+    </row>
+    <row r="19" spans="1:12" ht="15" customHeight="1">
       <c r="A19" s="13">
         <v>43861</v>
       </c>
@@ -1431,10 +1442,10 @@
       <c r="F19" s="38"/>
       <c r="H19" s="37"/>
       <c r="I19" s="38"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="53"/>
-    </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="44"/>
+      <c r="L19" s="45"/>
+    </row>
+    <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="A20" s="13">
         <v>43862</v>
       </c>
@@ -1447,10 +1458,10 @@
       <c r="F20" s="38"/>
       <c r="H20" s="37"/>
       <c r="I20" s="38"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="53"/>
-    </row>
-    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="44"/>
+      <c r="L20" s="45"/>
+    </row>
+    <row r="21" spans="1:12" ht="15" customHeight="1">
       <c r="A21" s="13">
         <v>43863</v>
       </c>
@@ -1463,10 +1474,10 @@
       <c r="F21" s="38"/>
       <c r="H21" s="37"/>
       <c r="I21" s="38"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="53"/>
-    </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="44"/>
+      <c r="L21" s="45"/>
+    </row>
+    <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="A22" s="13">
         <v>43864</v>
       </c>
@@ -1479,10 +1490,10 @@
       <c r="F22" s="38"/>
       <c r="H22" s="37"/>
       <c r="I22" s="38"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="53"/>
-    </row>
-    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="44"/>
+      <c r="L22" s="45"/>
+    </row>
+    <row r="23" spans="1:12" ht="15" customHeight="1">
       <c r="A23" s="13">
         <v>43865</v>
       </c>
@@ -1495,10 +1506,10 @@
       <c r="F23" s="38"/>
       <c r="H23" s="37"/>
       <c r="I23" s="38"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="53"/>
-    </row>
-    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="44"/>
+      <c r="L23" s="45"/>
+    </row>
+    <row r="24" spans="1:12" ht="15" customHeight="1">
       <c r="A24" s="13">
         <v>43866</v>
       </c>
@@ -1511,10 +1522,10 @@
       <c r="F24" s="38"/>
       <c r="H24" s="37"/>
       <c r="I24" s="38"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="53"/>
-    </row>
-    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="44"/>
+      <c r="L24" s="45"/>
+    </row>
+    <row r="25" spans="1:12" ht="15" customHeight="1">
       <c r="A25" s="13">
         <v>43867</v>
       </c>
@@ -1527,10 +1538,10 @@
       <c r="F25" s="38"/>
       <c r="H25" s="37"/>
       <c r="I25" s="38"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="53"/>
-    </row>
-    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="44"/>
+      <c r="L25" s="45"/>
+    </row>
+    <row r="26" spans="1:12" ht="15" customHeight="1">
       <c r="A26" s="13">
         <v>43868</v>
       </c>
@@ -1543,10 +1554,10 @@
       <c r="F26" s="38"/>
       <c r="H26" s="37"/>
       <c r="I26" s="38"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="53"/>
-    </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="44"/>
+      <c r="L26" s="45"/>
+    </row>
+    <row r="27" spans="1:12" ht="15" customHeight="1">
       <c r="A27" s="13">
         <v>43869</v>
       </c>
@@ -1559,10 +1570,10 @@
       <c r="F27" s="38"/>
       <c r="H27" s="37"/>
       <c r="I27" s="38"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="53"/>
-    </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="44"/>
+      <c r="L27" s="45"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" customHeight="1">
       <c r="A28" s="13">
         <v>43870</v>
       </c>
@@ -1575,10 +1586,10 @@
       <c r="F28" s="38"/>
       <c r="H28" s="37"/>
       <c r="I28" s="38"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="53"/>
-    </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="44"/>
+      <c r="L28" s="45"/>
+    </row>
+    <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="A29" s="13">
         <v>43871</v>
       </c>
@@ -1591,10 +1602,10 @@
       <c r="F29" s="38"/>
       <c r="H29" s="37"/>
       <c r="I29" s="38"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="53"/>
-    </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="44"/>
+      <c r="L29" s="45"/>
+    </row>
+    <row r="30" spans="1:12" ht="15" customHeight="1">
       <c r="A30" s="13">
         <v>43872</v>
       </c>
@@ -1607,10 +1618,10 @@
       <c r="F30" s="38"/>
       <c r="H30" s="37"/>
       <c r="I30" s="38"/>
-      <c r="K30" s="52"/>
-      <c r="L30" s="53"/>
-    </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="44"/>
+      <c r="L30" s="45"/>
+    </row>
+    <row r="31" spans="1:12" ht="15" customHeight="1">
       <c r="A31" s="13">
         <v>43873</v>
       </c>
@@ -1623,10 +1634,10 @@
       <c r="F31" s="38"/>
       <c r="H31" s="37"/>
       <c r="I31" s="38"/>
-      <c r="K31" s="52"/>
-      <c r="L31" s="53"/>
-    </row>
-    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K31" s="44"/>
+      <c r="L31" s="45"/>
+    </row>
+    <row r="32" spans="1:12" ht="15" customHeight="1">
       <c r="A32" s="13">
         <v>43874</v>
       </c>
@@ -1639,10 +1650,10 @@
       <c r="F32" s="38"/>
       <c r="H32" s="37"/>
       <c r="I32" s="38"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="53"/>
-    </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="44"/>
+      <c r="L32" s="45"/>
+    </row>
+    <row r="33" spans="1:12" ht="15" customHeight="1">
       <c r="A33" s="13">
         <v>43875</v>
       </c>
@@ -1655,10 +1666,10 @@
       <c r="F33" s="38"/>
       <c r="H33" s="37"/>
       <c r="I33" s="38"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="53"/>
-    </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K33" s="44"/>
+      <c r="L33" s="45"/>
+    </row>
+    <row r="34" spans="1:12" ht="15" customHeight="1">
       <c r="A34" s="13">
         <v>43876</v>
       </c>
@@ -1671,10 +1682,10 @@
       <c r="F34" s="38"/>
       <c r="H34" s="37"/>
       <c r="I34" s="38"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="53"/>
-    </row>
-    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="44"/>
+      <c r="L34" s="45"/>
+    </row>
+    <row r="35" spans="1:12" ht="15" customHeight="1">
       <c r="A35" s="13">
         <v>43877</v>
       </c>
@@ -1687,10 +1698,10 @@
       <c r="F35" s="38"/>
       <c r="H35" s="37"/>
       <c r="I35" s="38"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="53"/>
-    </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K35" s="44"/>
+      <c r="L35" s="45"/>
+    </row>
+    <row r="36" spans="1:12" ht="15" customHeight="1">
       <c r="A36" s="13">
         <v>43878</v>
       </c>
@@ -1703,10 +1714,10 @@
       <c r="F36" s="38"/>
       <c r="H36" s="37"/>
       <c r="I36" s="38"/>
-      <c r="K36" s="52"/>
-      <c r="L36" s="53"/>
-    </row>
-    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K36" s="44"/>
+      <c r="L36" s="45"/>
+    </row>
+    <row r="37" spans="1:12" ht="15" customHeight="1">
       <c r="A37" s="13">
         <v>43879</v>
       </c>
@@ -1719,10 +1730,10 @@
       <c r="F37" s="38"/>
       <c r="H37" s="37"/>
       <c r="I37" s="38"/>
-      <c r="K37" s="52"/>
-      <c r="L37" s="53"/>
-    </row>
-    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K37" s="44"/>
+      <c r="L37" s="45"/>
+    </row>
+    <row r="38" spans="1:12" ht="15" customHeight="1">
       <c r="A38" s="13">
         <v>43880</v>
       </c>
@@ -1735,10 +1746,10 @@
       <c r="F38" s="38"/>
       <c r="H38" s="37"/>
       <c r="I38" s="38"/>
-      <c r="K38" s="52"/>
-      <c r="L38" s="53"/>
-    </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="44"/>
+      <c r="L38" s="45"/>
+    </row>
+    <row r="39" spans="1:12" ht="15" customHeight="1">
       <c r="A39" s="13">
         <v>43881</v>
       </c>
@@ -1751,10 +1762,10 @@
       <c r="F39" s="38"/>
       <c r="H39" s="37"/>
       <c r="I39" s="38"/>
-      <c r="K39" s="52"/>
-      <c r="L39" s="53"/>
-    </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="44"/>
+      <c r="L39" s="45"/>
+    </row>
+    <row r="40" spans="1:12" ht="15" customHeight="1">
       <c r="A40" s="13">
         <v>43882</v>
       </c>
@@ -1767,10 +1778,10 @@
       <c r="F40" s="38"/>
       <c r="H40" s="37"/>
       <c r="I40" s="38"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="53"/>
-    </row>
-    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="44"/>
+      <c r="L40" s="45"/>
+    </row>
+    <row r="41" spans="1:12" ht="15" customHeight="1">
       <c r="A41" s="13">
         <v>43883</v>
       </c>
@@ -1783,10 +1794,10 @@
       <c r="F41" s="38"/>
       <c r="H41" s="37"/>
       <c r="I41" s="38"/>
-      <c r="K41" s="52"/>
-      <c r="L41" s="53"/>
-    </row>
-    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K41" s="44"/>
+      <c r="L41" s="45"/>
+    </row>
+    <row r="42" spans="1:12" ht="15" customHeight="1">
       <c r="A42" s="13">
         <v>43884</v>
       </c>
@@ -1799,10 +1810,10 @@
       <c r="F42" s="38"/>
       <c r="H42" s="37"/>
       <c r="I42" s="38"/>
-      <c r="K42" s="52"/>
-      <c r="L42" s="53"/>
-    </row>
-    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K42" s="44"/>
+      <c r="L42" s="45"/>
+    </row>
+    <row r="43" spans="1:12" ht="15" customHeight="1">
       <c r="A43" s="13">
         <v>43885</v>
       </c>
@@ -1815,10 +1826,10 @@
       <c r="F43" s="38"/>
       <c r="H43" s="37"/>
       <c r="I43" s="38"/>
-      <c r="K43" s="52"/>
-      <c r="L43" s="53"/>
-    </row>
-    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K43" s="44"/>
+      <c r="L43" s="45"/>
+    </row>
+    <row r="44" spans="1:12" ht="15" customHeight="1">
       <c r="A44" s="13">
         <v>43886</v>
       </c>
@@ -1831,10 +1842,10 @@
       <c r="F44" s="38"/>
       <c r="H44" s="37"/>
       <c r="I44" s="38"/>
-      <c r="K44" s="52"/>
-      <c r="L44" s="53"/>
-    </row>
-    <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="44"/>
+      <c r="L44" s="45"/>
+    </row>
+    <row r="45" spans="1:12" ht="15" customHeight="1">
       <c r="A45" s="13">
         <v>43887</v>
       </c>
@@ -1847,10 +1858,10 @@
       <c r="F45" s="38"/>
       <c r="H45" s="37"/>
       <c r="I45" s="38"/>
-      <c r="K45" s="52"/>
-      <c r="L45" s="53"/>
-    </row>
-    <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K45" s="44"/>
+      <c r="L45" s="45"/>
+    </row>
+    <row r="46" spans="1:12" ht="15" customHeight="1">
       <c r="A46" s="13">
         <v>43888</v>
       </c>
@@ -1863,10 +1874,10 @@
       <c r="F46" s="38"/>
       <c r="H46" s="37"/>
       <c r="I46" s="38"/>
-      <c r="K46" s="52"/>
-      <c r="L46" s="53"/>
-    </row>
-    <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K46" s="44"/>
+      <c r="L46" s="45"/>
+    </row>
+    <row r="47" spans="1:12" ht="15" customHeight="1">
       <c r="A47" s="13">
         <v>43889</v>
       </c>
@@ -1879,10 +1890,10 @@
       <c r="F47" s="38"/>
       <c r="H47" s="37"/>
       <c r="I47" s="38"/>
-      <c r="K47" s="52"/>
-      <c r="L47" s="53"/>
-    </row>
-    <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K47" s="44"/>
+      <c r="L47" s="45"/>
+    </row>
+    <row r="48" spans="1:12" ht="15" customHeight="1">
       <c r="A48" s="13">
         <v>43890</v>
       </c>
@@ -1895,10 +1906,10 @@
       <c r="F48" s="38"/>
       <c r="H48" s="37"/>
       <c r="I48" s="38"/>
-      <c r="K48" s="52"/>
-      <c r="L48" s="53"/>
-    </row>
-    <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K48" s="44"/>
+      <c r="L48" s="45"/>
+    </row>
+    <row r="49" spans="1:12" ht="15" customHeight="1">
       <c r="A49" s="13">
         <v>43891</v>
       </c>
@@ -1911,10 +1922,10 @@
       <c r="F49" s="38"/>
       <c r="H49" s="37"/>
       <c r="I49" s="38"/>
-      <c r="K49" s="52"/>
-      <c r="L49" s="53"/>
-    </row>
-    <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K49" s="44"/>
+      <c r="L49" s="45"/>
+    </row>
+    <row r="50" spans="1:12" ht="15" customHeight="1">
       <c r="A50" s="13">
         <v>43892</v>
       </c>
@@ -1927,10 +1938,10 @@
       <c r="F50" s="38"/>
       <c r="H50" s="37"/>
       <c r="I50" s="38"/>
-      <c r="K50" s="52"/>
-      <c r="L50" s="53"/>
-    </row>
-    <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K50" s="44"/>
+      <c r="L50" s="45"/>
+    </row>
+    <row r="51" spans="1:12" ht="15" customHeight="1">
       <c r="A51" s="13">
         <v>43893</v>
       </c>
@@ -1943,10 +1954,10 @@
       <c r="F51" s="38"/>
       <c r="H51" s="37"/>
       <c r="I51" s="38"/>
-      <c r="K51" s="52"/>
-      <c r="L51" s="53"/>
-    </row>
-    <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K51" s="44"/>
+      <c r="L51" s="45"/>
+    </row>
+    <row r="52" spans="1:12" ht="15" customHeight="1">
       <c r="A52" s="13">
         <v>43894</v>
       </c>
@@ -1959,10 +1970,10 @@
       <c r="F52" s="38"/>
       <c r="H52" s="37"/>
       <c r="I52" s="38"/>
-      <c r="K52" s="52"/>
-      <c r="L52" s="53"/>
-    </row>
-    <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K52" s="44"/>
+      <c r="L52" s="45"/>
+    </row>
+    <row r="53" spans="1:12" ht="15" customHeight="1">
       <c r="A53" s="13">
         <v>43895</v>
       </c>
@@ -1975,10 +1986,10 @@
       <c r="F53" s="38"/>
       <c r="H53" s="37"/>
       <c r="I53" s="38"/>
-      <c r="K53" s="52"/>
-      <c r="L53" s="53"/>
-    </row>
-    <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K53" s="44"/>
+      <c r="L53" s="45"/>
+    </row>
+    <row r="54" spans="1:12" ht="15" customHeight="1">
       <c r="A54" s="13">
         <v>43896</v>
       </c>
@@ -1991,10 +2002,10 @@
       <c r="F54" s="38"/>
       <c r="H54" s="37"/>
       <c r="I54" s="38"/>
-      <c r="K54" s="52"/>
-      <c r="L54" s="53"/>
-    </row>
-    <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K54" s="44"/>
+      <c r="L54" s="45"/>
+    </row>
+    <row r="55" spans="1:12" ht="15" customHeight="1">
       <c r="A55" s="13">
         <v>43897</v>
       </c>
@@ -2007,10 +2018,10 @@
       <c r="F55" s="38"/>
       <c r="H55" s="37"/>
       <c r="I55" s="38"/>
-      <c r="K55" s="52"/>
-      <c r="L55" s="53"/>
-    </row>
-    <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K55" s="44"/>
+      <c r="L55" s="45"/>
+    </row>
+    <row r="56" spans="1:12" ht="15" customHeight="1">
       <c r="A56" s="13">
         <v>43898</v>
       </c>
@@ -2023,10 +2034,10 @@
       <c r="F56" s="38"/>
       <c r="H56" s="37"/>
       <c r="I56" s="38"/>
-      <c r="K56" s="52"/>
-      <c r="L56" s="53"/>
-    </row>
-    <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K56" s="44"/>
+      <c r="L56" s="45"/>
+    </row>
+    <row r="57" spans="1:12" ht="15" customHeight="1">
       <c r="A57" s="13">
         <v>43899</v>
       </c>
@@ -2039,10 +2050,10 @@
       <c r="F57" s="38"/>
       <c r="H57" s="37"/>
       <c r="I57" s="38"/>
-      <c r="K57" s="52"/>
-      <c r="L57" s="53"/>
-    </row>
-    <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K57" s="44"/>
+      <c r="L57" s="45"/>
+    </row>
+    <row r="58" spans="1:12" ht="15" customHeight="1">
       <c r="A58" s="13">
         <v>43900</v>
       </c>
@@ -2055,10 +2066,10 @@
       <c r="F58" s="38"/>
       <c r="H58" s="37"/>
       <c r="I58" s="38"/>
-      <c r="K58" s="52"/>
-      <c r="L58" s="53"/>
-    </row>
-    <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K58" s="44"/>
+      <c r="L58" s="45"/>
+    </row>
+    <row r="59" spans="1:12" ht="15" customHeight="1">
       <c r="A59" s="13">
         <v>43901</v>
       </c>
@@ -2071,10 +2082,10 @@
       <c r="F59" s="38"/>
       <c r="H59" s="37"/>
       <c r="I59" s="38"/>
-      <c r="K59" s="52"/>
-      <c r="L59" s="53"/>
-    </row>
-    <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K59" s="44"/>
+      <c r="L59" s="45"/>
+    </row>
+    <row r="60" spans="1:12" ht="15" customHeight="1">
       <c r="A60" s="13">
         <v>43902</v>
       </c>
@@ -2087,10 +2098,10 @@
       <c r="F60" s="38"/>
       <c r="H60" s="37"/>
       <c r="I60" s="38"/>
-      <c r="K60" s="52"/>
-      <c r="L60" s="53"/>
-    </row>
-    <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K60" s="44"/>
+      <c r="L60" s="45"/>
+    </row>
+    <row r="61" spans="1:12" ht="15" customHeight="1">
       <c r="A61" s="13">
         <v>43903</v>
       </c>
@@ -2103,10 +2114,10 @@
       <c r="F61" s="38"/>
       <c r="H61" s="37"/>
       <c r="I61" s="38"/>
-      <c r="K61" s="52"/>
-      <c r="L61" s="53"/>
-    </row>
-    <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K61" s="44"/>
+      <c r="L61" s="45"/>
+    </row>
+    <row r="62" spans="1:12" ht="15" customHeight="1">
       <c r="A62" s="13">
         <v>43904</v>
       </c>
@@ -2119,10 +2130,10 @@
       <c r="F62" s="38"/>
       <c r="H62" s="37"/>
       <c r="I62" s="38"/>
-      <c r="K62" s="52"/>
-      <c r="L62" s="53"/>
-    </row>
-    <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K62" s="44"/>
+      <c r="L62" s="45"/>
+    </row>
+    <row r="63" spans="1:12" ht="15" customHeight="1">
       <c r="A63" s="13">
         <v>43905</v>
       </c>
@@ -2135,26 +2146,26 @@
       <c r="F63" s="38"/>
       <c r="H63" s="37"/>
       <c r="I63" s="38"/>
-      <c r="K63" s="52"/>
-      <c r="L63" s="53"/>
-    </row>
-    <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K63" s="44"/>
+      <c r="L63" s="45"/>
+    </row>
+    <row r="64" spans="1:12" ht="60" customHeight="1">
       <c r="A64" s="13">
         <v>43906</v>
       </c>
-      <c r="B64" s="25" t="s">
+      <c r="B64" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C64" s="26">
+      <c r="C64" s="25">
         <v>2</v>
       </c>
       <c r="D64" s="13">
         <v>43906</v>
       </c>
-      <c r="E64" s="25" t="s">
+      <c r="E64" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F64" s="26">
+      <c r="F64" s="25">
         <v>2</v>
       </c>
       <c r="H64" s="37"/>
@@ -2162,276 +2173,276 @@
       <c r="J64" s="22">
         <v>43906</v>
       </c>
-      <c r="K64" s="25" t="s">
+      <c r="K64" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L64" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="15" customHeight="1">
       <c r="A65" s="13">
         <v>43907</v>
       </c>
-      <c r="B65" s="32" t="s">
+      <c r="B65" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="40">
+      <c r="C65" s="39">
         <v>10</v>
       </c>
       <c r="D65" s="13">
         <v>43907</v>
       </c>
-      <c r="E65" s="32" t="s">
+      <c r="E65" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="40">
+      <c r="F65" s="39">
         <v>12</v>
       </c>
-      <c r="H65" s="32" t="s">
+      <c r="H65" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I65" s="47"/>
+      <c r="I65" s="59"/>
       <c r="J65" s="22">
         <f>J64+1</f>
         <v>43907</v>
       </c>
-      <c r="K65" s="32" t="s">
+      <c r="K65" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="L65" s="54" t="s">
+      <c r="L65" s="46" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="60" customHeight="1">
       <c r="A66" s="13">
         <v>43908</v>
       </c>
-      <c r="B66" s="32"/>
-      <c r="C66" s="40"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="39"/>
       <c r="D66" s="13">
         <v>43908</v>
       </c>
-      <c r="E66" s="32"/>
-      <c r="F66" s="40"/>
-      <c r="H66" s="32"/>
-      <c r="I66" s="47"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="39"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="59"/>
       <c r="J66" s="22">
         <f t="shared" ref="J66:J129" si="0">J65+1</f>
         <v>43908</v>
       </c>
-      <c r="K66" s="32"/>
-      <c r="L66" s="54"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K66" s="29"/>
+      <c r="L66" s="46"/>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" s="13">
         <v>43909</v>
       </c>
-      <c r="B67" s="32"/>
-      <c r="C67" s="40"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="39"/>
       <c r="D67" s="13">
         <v>43909</v>
       </c>
-      <c r="E67" s="32"/>
-      <c r="F67" s="40"/>
-      <c r="H67" s="32"/>
-      <c r="I67" s="47"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="39"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="59"/>
       <c r="J67" s="22">
         <f t="shared" si="0"/>
         <v>43909</v>
       </c>
-      <c r="K67" s="32"/>
-      <c r="L67" s="54"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K67" s="29"/>
+      <c r="L67" s="46"/>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" s="13">
         <v>43910</v>
       </c>
-      <c r="B68" s="32"/>
-      <c r="C68" s="40"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="39"/>
       <c r="D68" s="13">
         <v>43910</v>
       </c>
-      <c r="E68" s="32"/>
-      <c r="F68" s="40"/>
-      <c r="H68" s="32"/>
-      <c r="I68" s="47"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="39"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="59"/>
       <c r="J68" s="22">
         <f t="shared" si="0"/>
         <v>43910</v>
       </c>
-      <c r="K68" s="32"/>
-      <c r="L68" s="54"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K68" s="29"/>
+      <c r="L68" s="46"/>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" s="13">
         <v>43911</v>
       </c>
-      <c r="B69" s="32" t="s">
+      <c r="B69" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C69" s="33">
+      <c r="C69" s="32">
         <v>4</v>
       </c>
       <c r="D69" s="13">
         <v>43911</v>
       </c>
-      <c r="E69" s="32" t="s">
+      <c r="E69" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F69" s="60">
+      <c r="F69" s="30">
         <v>6</v>
       </c>
-      <c r="H69" s="32"/>
-      <c r="I69" s="47"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="59"/>
       <c r="J69" s="22">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="K69" s="55" t="s">
+      <c r="K69" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="L69" s="56"/>
-    </row>
-    <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L69" s="48"/>
+    </row>
+    <row r="70" spans="1:12" ht="45" customHeight="1">
       <c r="A70" s="13">
         <v>43912</v>
       </c>
-      <c r="B70" s="32"/>
-      <c r="C70" s="33"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="32"/>
       <c r="D70" s="13">
         <v>43912</v>
       </c>
-      <c r="E70" s="32"/>
-      <c r="F70" s="60"/>
-      <c r="H70" s="32"/>
-      <c r="I70" s="47"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="30"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="59"/>
       <c r="J70" s="22">
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
-      <c r="K70" s="55"/>
-      <c r="L70" s="56"/>
-    </row>
-    <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="K70" s="47"/>
+      <c r="L70" s="48"/>
+    </row>
+    <row r="71" spans="1:12" ht="60">
       <c r="A71" s="13">
         <v>43913</v>
       </c>
-      <c r="B71" s="25" t="s">
+      <c r="B71" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C71" s="26">
+      <c r="C71" s="25">
         <v>2</v>
       </c>
       <c r="D71" s="13">
         <v>43913</v>
       </c>
-      <c r="E71" s="32" t="s">
+      <c r="E71" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F71" s="60">
+      <c r="F71" s="30">
         <v>4</v>
       </c>
-      <c r="H71" s="32"/>
-      <c r="I71" s="47"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="59"/>
       <c r="J71" s="22">
         <f t="shared" si="0"/>
         <v>43913</v>
       </c>
-      <c r="K71" s="25" t="s">
+      <c r="K71" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="L71" s="25" t="s">
+      <c r="L71" s="28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="30" customHeight="1">
       <c r="A72" s="13">
         <v>43914</v>
       </c>
-      <c r="B72" s="25" t="s">
+      <c r="B72" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C72" s="26">
+      <c r="C72" s="25">
         <v>3</v>
       </c>
       <c r="D72" s="13">
         <v>43914</v>
       </c>
-      <c r="E72" s="32"/>
-      <c r="F72" s="60"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="30"/>
       <c r="G72" s="13">
         <v>43913</v>
       </c>
-      <c r="H72" s="25" t="s">
+      <c r="H72" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="I72" s="26">
+      <c r="I72" s="25">
         <v>6</v>
       </c>
       <c r="J72" s="22">
         <f t="shared" si="0"/>
         <v>43914</v>
       </c>
-      <c r="K72" s="25" t="s">
+      <c r="K72" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="L72" s="25" t="s">
+      <c r="L72" s="28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="45.75" customHeight="1">
       <c r="A73" s="13">
         <v>43915</v>
       </c>
-      <c r="B73" s="25" t="s">
+      <c r="B73" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C73" s="26">
+      <c r="C73" s="25">
         <v>2</v>
       </c>
       <c r="D73" s="13">
         <v>43915</v>
       </c>
-      <c r="E73" s="32" t="s">
+      <c r="E73" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F73" s="60">
+      <c r="F73" s="30">
         <v>6</v>
       </c>
       <c r="G73" s="13">
         <v>43914</v>
       </c>
-      <c r="H73" s="32" t="s">
+      <c r="H73" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="I73" s="39"/>
+      <c r="I73" s="52"/>
       <c r="J73" s="22">
         <f t="shared" si="0"/>
         <v>43915</v>
       </c>
-      <c r="K73" s="25" t="s">
+      <c r="K73" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="L73" s="25" t="s">
+      <c r="L73" s="28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12">
       <c r="A74" s="13">
         <v>43916</v>
       </c>
-      <c r="B74" s="32" t="s">
+      <c r="B74" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="60"/>
+      <c r="C74" s="30"/>
       <c r="D74" s="13">
         <v>43916</v>
       </c>
-      <c r="E74" s="32"/>
-      <c r="F74" s="60"/>
-      <c r="H74" s="32"/>
-      <c r="I74" s="39"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="30"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="52"/>
       <c r="J74" s="22">
         <f t="shared" si="0"/>
         <v>43916</v>
@@ -2439,73 +2450,73 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="60">
       <c r="A75" s="13">
         <v>43917</v>
       </c>
-      <c r="B75" s="25" t="s">
+      <c r="B75" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C75" s="26">
+      <c r="C75" s="25">
         <v>2</v>
       </c>
       <c r="D75" s="13">
         <v>43917</v>
       </c>
-      <c r="E75" s="32"/>
-      <c r="F75" s="60"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="30"/>
       <c r="G75" s="13">
         <v>43915</v>
       </c>
-      <c r="H75" s="25" t="s">
+      <c r="H75" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="I75" s="26">
+      <c r="I75" s="25">
         <v>3</v>
       </c>
       <c r="J75" s="22">
         <f t="shared" si="0"/>
         <v>43917</v>
       </c>
-      <c r="K75" s="25" t="s">
+      <c r="K75" s="28" t="s">
         <v>36</v>
       </c>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="90">
       <c r="A76" s="13">
         <v>43918</v>
       </c>
-      <c r="B76" s="25" t="s">
+      <c r="B76" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="26">
+      <c r="C76" s="25">
         <v>2</v>
       </c>
       <c r="D76" s="13">
         <v>43918</v>
       </c>
-      <c r="E76" s="32"/>
-      <c r="F76" s="60"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="30"/>
       <c r="G76" s="13">
         <v>43916</v>
       </c>
-      <c r="H76" s="25" t="s">
+      <c r="H76" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="I76" s="26">
+      <c r="I76" s="25">
         <v>8</v>
       </c>
       <c r="J76" s="22">
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
-      <c r="K76" s="55" t="s">
+      <c r="K76" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="L76" s="57"/>
-    </row>
-    <row r="77" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L76" s="49"/>
+    </row>
+    <row r="77" spans="1:12" ht="30">
       <c r="A77" s="13">
         <v>43919</v>
       </c>
@@ -2519,163 +2530,163 @@
       <c r="G77" s="13">
         <v>43917</v>
       </c>
-      <c r="H77" s="25" t="s">
+      <c r="H77" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="I77" s="26">
+      <c r="I77" s="25">
         <v>8</v>
       </c>
       <c r="J77" s="22">
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="K77" s="58"/>
-      <c r="L77" s="57"/>
-    </row>
-    <row r="78" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="K77" s="50"/>
+      <c r="L77" s="49"/>
+    </row>
+    <row r="78" spans="1:12" ht="30">
       <c r="A78" s="13">
         <v>43920</v>
       </c>
-      <c r="B78" s="25" t="s">
+      <c r="B78" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C78" s="26">
+      <c r="C78" s="25">
         <v>2</v>
       </c>
       <c r="D78" s="13">
         <v>43920</v>
       </c>
-      <c r="E78" s="32" t="s">
+      <c r="E78" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F78" s="60">
+      <c r="F78" s="30">
         <v>4</v>
       </c>
       <c r="G78" s="13">
         <v>43918</v>
       </c>
-      <c r="H78" s="25" t="s">
+      <c r="H78" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="I78" s="26">
+      <c r="I78" s="25">
         <v>8</v>
       </c>
       <c r="J78" s="22">
         <f t="shared" si="0"/>
         <v>43920</v>
       </c>
-      <c r="K78" s="25" t="s">
+      <c r="K78" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="L78" s="25" t="s">
+      <c r="L78" s="28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="30">
       <c r="A79" s="13">
         <v>43921</v>
       </c>
-      <c r="B79" s="32" t="s">
+      <c r="B79" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C79" s="33">
+      <c r="C79" s="32">
         <v>4</v>
       </c>
       <c r="D79" s="13">
         <v>43921</v>
       </c>
-      <c r="E79" s="32"/>
-      <c r="F79" s="60"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="30"/>
       <c r="G79" s="13">
         <v>43919</v>
       </c>
-      <c r="H79" s="25" t="s">
+      <c r="H79" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="I79" s="26">
+      <c r="I79" s="25">
         <v>8</v>
       </c>
       <c r="J79" s="22">
         <f t="shared" si="0"/>
         <v>43921</v>
       </c>
-      <c r="K79" s="25" t="s">
+      <c r="K79" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="L79" s="25" t="s">
+      <c r="L79" s="28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="30">
       <c r="A80" s="13">
         <v>43922</v>
       </c>
-      <c r="B80" s="32"/>
-      <c r="C80" s="33"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="32"/>
       <c r="D80" s="13">
         <v>43922</v>
       </c>
-      <c r="E80" s="32"/>
-      <c r="F80" s="60"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="30"/>
       <c r="G80" s="13">
         <v>43920</v>
       </c>
-      <c r="H80" s="25" t="s">
+      <c r="H80" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I80" s="26">
+      <c r="I80" s="25">
         <v>6</v>
       </c>
       <c r="J80" s="22">
         <f t="shared" si="0"/>
         <v>43922</v>
       </c>
-      <c r="K80" s="28" t="s">
+      <c r="K80" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="L80" s="28"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L80" s="26"/>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" s="13">
         <v>43923</v>
       </c>
-      <c r="B81" s="32"/>
-      <c r="C81" s="33"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="32"/>
       <c r="D81" s="13">
         <v>43923</v>
       </c>
-      <c r="E81" s="32"/>
-      <c r="F81" s="60"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="30"/>
       <c r="H81" s="20"/>
       <c r="I81" s="20"/>
       <c r="J81" s="22">
         <f t="shared" si="0"/>
         <v>43923</v>
       </c>
-      <c r="K81" s="33" t="s">
+      <c r="K81" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="L81" s="33" t="s">
+      <c r="L81" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="45">
       <c r="A82" s="13">
         <v>43924</v>
       </c>
-      <c r="B82" s="25" t="s">
+      <c r="B82" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C82" s="26">
+      <c r="C82" s="25">
         <v>3</v>
       </c>
       <c r="D82" s="13">
         <v>43924</v>
       </c>
-      <c r="E82" s="32" t="s">
+      <c r="E82" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F82" s="60">
+      <c r="F82" s="30">
         <v>3</v>
       </c>
       <c r="H82" s="20"/>
@@ -2684,10 +2695,10 @@
         <f t="shared" si="0"/>
         <v>43924</v>
       </c>
-      <c r="K82" s="33"/>
-      <c r="L82" s="33"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K82" s="32"/>
+      <c r="L82" s="32"/>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" s="13">
         <v>43925</v>
       </c>
@@ -2696,20 +2707,20 @@
       <c r="D83" s="13">
         <v>43925</v>
       </c>
-      <c r="E83" s="32"/>
-      <c r="F83" s="60"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="30"/>
       <c r="H83" s="20"/>
       <c r="I83" s="20"/>
       <c r="J83" s="22">
         <f t="shared" si="0"/>
         <v>43925</v>
       </c>
-      <c r="K83" s="34" t="s">
+      <c r="K83" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="L83" s="34"/>
-    </row>
-    <row r="84" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L83" s="51"/>
+    </row>
+    <row r="84" spans="1:12" ht="30" customHeight="1">
       <c r="A84" s="13">
         <v>43926</v>
       </c>
@@ -2730,26 +2741,26 @@
         <f t="shared" si="0"/>
         <v>43926</v>
       </c>
-      <c r="K84" s="34"/>
-      <c r="L84" s="34"/>
-    </row>
-    <row r="85" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K84" s="51"/>
+      <c r="L84" s="51"/>
+    </row>
+    <row r="85" spans="1:12" ht="53.25" customHeight="1">
       <c r="A85" s="13">
         <v>43927</v>
       </c>
-      <c r="B85" s="59" t="s">
+      <c r="B85" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C85" s="33">
+      <c r="C85" s="32">
         <v>12</v>
       </c>
       <c r="D85" s="13">
         <v>43927</v>
       </c>
-      <c r="E85" s="32" t="s">
+      <c r="E85" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F85" s="60">
+      <c r="F85" s="30">
         <v>6</v>
       </c>
       <c r="H85" s="20"/>
@@ -2758,74 +2769,74 @@
         <f t="shared" si="0"/>
         <v>43927</v>
       </c>
-      <c r="K85" s="25" t="s">
+      <c r="K85" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="L85" s="26" t="s">
+      <c r="L85" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="30">
       <c r="A86" s="13">
         <v>43928</v>
       </c>
-      <c r="B86" s="59"/>
-      <c r="C86" s="33"/>
+      <c r="B86" s="34"/>
+      <c r="C86" s="32"/>
       <c r="D86" s="13">
         <v>43928</v>
       </c>
-      <c r="E86" s="32"/>
-      <c r="F86" s="60"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="30"/>
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
       <c r="J86" s="22">
         <f>J85+1</f>
         <v>43928</v>
       </c>
-      <c r="K86" s="25" t="s">
+      <c r="K86" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="L86" s="26" t="s">
+      <c r="L86" s="25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="30">
       <c r="A87" s="13">
         <v>43929</v>
       </c>
-      <c r="B87" s="59"/>
-      <c r="C87" s="33"/>
+      <c r="B87" s="34"/>
+      <c r="C87" s="32"/>
       <c r="D87" s="13">
         <v>43929</v>
       </c>
-      <c r="E87" s="32"/>
-      <c r="F87" s="60"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="30"/>
       <c r="H87" s="20"/>
       <c r="I87" s="20"/>
       <c r="J87" s="22">
         <f t="shared" si="0"/>
         <v>43929</v>
       </c>
-      <c r="K87" s="25" t="s">
+      <c r="K87" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="L87" s="26" t="s">
+      <c r="L87" s="25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="45">
       <c r="A88" s="21">
         <v>43930</v>
       </c>
-      <c r="B88" s="59"/>
-      <c r="C88" s="33"/>
+      <c r="B88" s="34"/>
+      <c r="C88" s="32"/>
       <c r="D88" s="13">
         <v>43930</v>
       </c>
-      <c r="E88" s="32" t="s">
+      <c r="E88" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F88" s="60">
+      <c r="F88" s="30">
         <v>4</v>
       </c>
       <c r="H88" s="20"/>
@@ -2834,62 +2845,62 @@
         <f t="shared" si="0"/>
         <v>43930</v>
       </c>
-      <c r="K88" s="25" t="s">
+      <c r="K88" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="L88" s="26" t="s">
+      <c r="L88" s="25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12">
       <c r="A89" s="21">
         <v>43931</v>
       </c>
-      <c r="B89" s="59"/>
-      <c r="C89" s="33"/>
+      <c r="B89" s="34"/>
+      <c r="C89" s="32"/>
       <c r="D89" s="13">
         <v>43931</v>
       </c>
-      <c r="E89" s="32"/>
-      <c r="F89" s="60"/>
+      <c r="E89" s="29"/>
+      <c r="F89" s="30"/>
       <c r="H89" s="20"/>
       <c r="I89" s="20"/>
       <c r="J89" s="22">
         <f t="shared" si="0"/>
         <v>43931</v>
       </c>
-      <c r="K89" s="26" t="s">
+      <c r="K89" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="L89" s="26" t="s">
+      <c r="L89" s="25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12">
       <c r="A90" s="21">
         <v>43932</v>
       </c>
-      <c r="B90" s="59"/>
-      <c r="C90" s="33"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="32"/>
       <c r="D90" s="13">
         <v>43932</v>
       </c>
-      <c r="E90" s="32"/>
-      <c r="F90" s="60"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="30"/>
       <c r="H90" s="20"/>
       <c r="I90" s="20"/>
       <c r="J90" s="22">
         <f t="shared" si="0"/>
         <v>43932</v>
       </c>
-      <c r="K90" s="26" t="s">
+      <c r="K90" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="L90" s="26" t="s">
+      <c r="L90" s="25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12">
       <c r="A91" s="13">
         <v>43933</v>
       </c>
@@ -2906,25 +2917,25 @@
         <f t="shared" si="0"/>
         <v>43933</v>
       </c>
-      <c r="K91" s="61" t="s">
+      <c r="K91" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="L91" s="61"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L91" s="31"/>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" s="13">
         <v>43934</v>
       </c>
-      <c r="B92" s="32" t="s">
+      <c r="B92" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C92" s="33">
+      <c r="C92" s="32">
         <v>4</v>
       </c>
       <c r="D92" s="13">
         <v>43934</v>
       </c>
-      <c r="E92" s="32" t="s">
+      <c r="E92" s="29" t="s">
         <v>65</v>
       </c>
       <c r="H92" s="20"/>
@@ -2933,86 +2944,86 @@
         <f t="shared" si="0"/>
         <v>43934</v>
       </c>
-      <c r="K92" s="61"/>
-      <c r="L92" s="61"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K92" s="31"/>
+      <c r="L92" s="31"/>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" s="13">
         <v>43935</v>
       </c>
-      <c r="B93" s="32"/>
-      <c r="C93" s="33"/>
+      <c r="B93" s="29"/>
+      <c r="C93" s="32"/>
       <c r="D93" s="13">
         <v>43935</v>
       </c>
-      <c r="E93" s="62"/>
+      <c r="E93" s="33"/>
       <c r="H93" s="20"/>
       <c r="I93" s="20"/>
       <c r="J93" s="22">
         <f t="shared" si="0"/>
         <v>43935</v>
       </c>
-      <c r="K93" s="61"/>
-      <c r="L93" s="61"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K93" s="31"/>
+      <c r="L93" s="31"/>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" s="13">
         <v>43936</v>
       </c>
-      <c r="B94" s="32"/>
-      <c r="C94" s="33"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="32"/>
       <c r="D94" s="13">
         <v>43936</v>
       </c>
-      <c r="E94" s="62"/>
+      <c r="E94" s="33"/>
       <c r="H94" s="20"/>
       <c r="I94" s="20"/>
       <c r="J94" s="22">
         <f t="shared" si="0"/>
         <v>43936</v>
       </c>
-      <c r="K94" s="61"/>
-      <c r="L94" s="61"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K94" s="31"/>
+      <c r="L94" s="31"/>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" s="13">
         <v>43937</v>
       </c>
-      <c r="B95" s="32"/>
-      <c r="C95" s="33"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="32"/>
       <c r="D95" s="13">
         <v>43937</v>
       </c>
-      <c r="E95" s="62"/>
+      <c r="E95" s="33"/>
       <c r="H95" s="20"/>
       <c r="I95" s="20"/>
       <c r="J95" s="22">
         <f t="shared" si="0"/>
         <v>43937</v>
       </c>
-      <c r="K95" s="61"/>
-      <c r="L95" s="61"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K95" s="31"/>
+      <c r="L95" s="31"/>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" s="13">
         <v>43938</v>
       </c>
-      <c r="B96" s="32"/>
-      <c r="C96" s="33"/>
+      <c r="B96" s="29"/>
+      <c r="C96" s="32"/>
       <c r="D96" s="13">
         <v>43938</v>
       </c>
-      <c r="E96" s="62"/>
+      <c r="E96" s="33"/>
       <c r="H96" s="20"/>
       <c r="I96" s="20"/>
       <c r="J96" s="22">
         <f t="shared" si="0"/>
         <v>43938</v>
       </c>
-      <c r="K96" s="61"/>
-      <c r="L96" s="61"/>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K96" s="31"/>
+      <c r="L96" s="31"/>
+    </row>
+    <row r="97" spans="1:12">
       <c r="A97" s="13">
         <v>43939</v>
       </c>
@@ -3021,17 +3032,17 @@
       <c r="D97" s="13">
         <v>43939</v>
       </c>
-      <c r="E97" s="62"/>
+      <c r="E97" s="33"/>
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
       <c r="J97" s="22">
         <f t="shared" si="0"/>
         <v>43939</v>
       </c>
-      <c r="K97" s="61"/>
-      <c r="L97" s="61"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K97" s="31"/>
+      <c r="L97" s="31"/>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" s="13">
         <v>43940</v>
       </c>
@@ -3040,146 +3051,146 @@
       <c r="D98" s="13">
         <v>43940</v>
       </c>
-      <c r="E98" s="62"/>
+      <c r="E98" s="33"/>
       <c r="H98" s="20"/>
       <c r="I98" s="20"/>
       <c r="J98" s="22">
         <f t="shared" si="0"/>
         <v>43940</v>
       </c>
-      <c r="K98" s="61"/>
-      <c r="L98" s="61"/>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K98" s="31"/>
+      <c r="L98" s="31"/>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99" s="13">
         <v>43941</v>
       </c>
-      <c r="B99" s="32" t="s">
+      <c r="B99" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C99" s="33">
+      <c r="C99" s="32">
         <v>4</v>
       </c>
       <c r="D99" s="13">
         <v>43941</v>
       </c>
-      <c r="E99" s="62"/>
+      <c r="E99" s="33"/>
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
       <c r="J99" s="22">
         <f t="shared" si="0"/>
         <v>43941</v>
       </c>
-      <c r="K99" s="61"/>
-      <c r="L99" s="61"/>
-    </row>
-    <row r="100" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K99" s="31"/>
+      <c r="L99" s="31"/>
+    </row>
+    <row r="100" spans="1:12" ht="30" customHeight="1">
       <c r="A100" s="13">
         <v>43942</v>
       </c>
-      <c r="B100" s="32"/>
-      <c r="C100" s="33"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="32"/>
       <c r="D100" s="13">
         <v>43942</v>
       </c>
-      <c r="E100" s="62"/>
+      <c r="E100" s="33"/>
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
       <c r="J100" s="22">
         <f t="shared" si="0"/>
         <v>43942</v>
       </c>
-      <c r="K100" s="61"/>
-      <c r="L100" s="61"/>
-    </row>
-    <row r="101" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K100" s="31"/>
+      <c r="L100" s="31"/>
+    </row>
+    <row r="101" spans="1:12" ht="15" customHeight="1">
       <c r="A101" s="13">
         <v>43943</v>
       </c>
-      <c r="B101" s="32"/>
-      <c r="C101" s="33"/>
+      <c r="B101" s="29"/>
+      <c r="C101" s="32"/>
       <c r="D101" s="13">
         <v>43943</v>
       </c>
-      <c r="E101" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="F101" s="60">
+      <c r="E101" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F101" s="30">
         <v>3</v>
       </c>
       <c r="G101" s="13">
         <v>43943</v>
       </c>
-      <c r="H101" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="I101" s="28"/>
+      <c r="H101" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="I101" s="26"/>
       <c r="J101" s="22">
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="K101" s="61"/>
-      <c r="L101" s="61"/>
-    </row>
-    <row r="102" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K101" s="31"/>
+      <c r="L101" s="31"/>
+    </row>
+    <row r="102" spans="1:12" ht="27.75" customHeight="1">
       <c r="A102" s="13">
         <v>43944</v>
       </c>
-      <c r="B102" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C102" s="33">
+      <c r="B102" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C102" s="32">
         <v>2</v>
       </c>
       <c r="D102" s="13">
         <v>43944</v>
       </c>
-      <c r="E102" s="32"/>
-      <c r="F102" s="60"/>
+      <c r="E102" s="29"/>
+      <c r="F102" s="30"/>
       <c r="G102" s="13">
         <v>43944</v>
       </c>
-      <c r="H102" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="I102" s="28"/>
+      <c r="H102" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I102" s="26"/>
       <c r="J102" s="22">
         <f t="shared" si="0"/>
         <v>43944</v>
       </c>
-      <c r="K102" s="61"/>
-      <c r="L102" s="61"/>
-    </row>
-    <row r="103" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K102" s="31"/>
+      <c r="L102" s="31"/>
+    </row>
+    <row r="103" spans="1:12" ht="41.25" customHeight="1">
       <c r="A103" s="13">
         <v>43945</v>
       </c>
-      <c r="B103" s="32"/>
-      <c r="C103" s="33"/>
+      <c r="B103" s="29"/>
+      <c r="C103" s="32"/>
       <c r="D103" s="13">
         <v>43945</v>
       </c>
-      <c r="E103" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F103" s="31">
+      <c r="E103" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F103" s="28">
         <v>2</v>
       </c>
       <c r="G103" s="13">
         <v>43945</v>
       </c>
-      <c r="H103" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="I103" s="28"/>
+      <c r="H103" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I103" s="26"/>
       <c r="J103" s="22">
         <f t="shared" si="0"/>
         <v>43945</v>
       </c>
-      <c r="K103" s="61"/>
-      <c r="L103" s="61"/>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K103" s="31"/>
+      <c r="L103" s="31"/>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104" s="13">
         <v>43946</v>
       </c>
@@ -3193,16 +3204,16 @@
       <c r="G104" s="13">
         <v>43946</v>
       </c>
-      <c r="H104" s="28"/>
-      <c r="I104" s="28"/>
+      <c r="H104" s="26"/>
+      <c r="I104" s="26"/>
       <c r="J104" s="22">
         <f t="shared" si="0"/>
         <v>43946</v>
       </c>
-      <c r="K104" s="61"/>
-      <c r="L104" s="61"/>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K104" s="31"/>
+      <c r="L104" s="31"/>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105" s="13">
         <v>43947</v>
       </c>
@@ -3216,195 +3227,197 @@
       <c r="G105" s="13">
         <v>43947</v>
       </c>
-      <c r="H105" s="28"/>
-      <c r="I105" s="28"/>
+      <c r="H105" s="26"/>
+      <c r="I105" s="26"/>
       <c r="J105" s="22">
         <f t="shared" si="0"/>
         <v>43947</v>
       </c>
-      <c r="K105" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="L105" s="33" t="s">
+      <c r="K105" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="L105" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="60">
       <c r="A106" s="13">
         <v>43948</v>
       </c>
-      <c r="B106" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C106" s="26">
+      <c r="B106" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C106" s="25">
         <v>4</v>
       </c>
       <c r="D106" s="13">
         <v>43948</v>
       </c>
-      <c r="E106" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="F106" s="60">
+      <c r="E106" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F106" s="30">
         <v>3</v>
       </c>
       <c r="G106" s="13">
         <v>43948</v>
       </c>
-      <c r="H106" s="28"/>
-      <c r="I106" s="28"/>
+      <c r="H106" s="26"/>
+      <c r="I106" s="26"/>
       <c r="J106" s="22">
         <f t="shared" si="0"/>
         <v>43948</v>
       </c>
-      <c r="K106" s="60"/>
-      <c r="L106" s="33"/>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K106" s="30"/>
+      <c r="L106" s="32"/>
+    </row>
+    <row r="107" spans="1:12">
       <c r="A107" s="13">
         <v>43949</v>
       </c>
-      <c r="B107" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="C107" s="33">
+      <c r="B107" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C107" s="32">
         <v>3</v>
       </c>
       <c r="D107" s="13">
         <v>43949</v>
       </c>
-      <c r="E107" s="32"/>
-      <c r="F107" s="60"/>
+      <c r="E107" s="29"/>
+      <c r="F107" s="30"/>
       <c r="G107" s="13">
         <v>43949</v>
       </c>
-      <c r="H107" s="28"/>
-      <c r="I107" s="28"/>
+      <c r="H107" s="26"/>
+      <c r="I107" s="26"/>
       <c r="J107" s="22">
         <f t="shared" si="0"/>
         <v>43949</v>
       </c>
-      <c r="K107" s="26" t="s">
+      <c r="K107" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="L107" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L107" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="30">
       <c r="A108" s="13">
         <v>43950</v>
       </c>
-      <c r="B108" s="32"/>
-      <c r="C108" s="33"/>
+      <c r="B108" s="29"/>
+      <c r="C108" s="32"/>
       <c r="D108" s="13">
         <v>43950</v>
       </c>
-      <c r="E108" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="F108" s="60">
+      <c r="E108" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F108" s="30">
         <v>3</v>
       </c>
       <c r="G108" s="13">
         <v>43950</v>
       </c>
-      <c r="H108" s="30"/>
-      <c r="I108" s="28"/>
+      <c r="H108" s="26"/>
+      <c r="I108" s="26"/>
       <c r="J108" s="22">
         <f t="shared" si="0"/>
         <v>43950</v>
       </c>
-      <c r="K108" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="L108" s="26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K108" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="L108" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109" s="13">
         <v>43951</v>
       </c>
-      <c r="B109" s="25"/>
-      <c r="C109" s="26"/>
+      <c r="B109" s="28"/>
+      <c r="C109" s="25"/>
       <c r="D109" s="13">
         <v>43951</v>
       </c>
-      <c r="E109" s="32"/>
-      <c r="F109" s="60"/>
+      <c r="E109" s="29"/>
+      <c r="F109" s="30"/>
       <c r="G109" s="13">
         <v>43951</v>
       </c>
-      <c r="H109" s="29"/>
-      <c r="I109" s="28"/>
+      <c r="H109" s="25"/>
+      <c r="I109" s="26"/>
       <c r="J109" s="22">
         <f t="shared" si="0"/>
         <v>43951</v>
       </c>
-      <c r="K109" s="28"/>
-      <c r="L109" s="28"/>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K109" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="L109" s="60"/>
+    </row>
+    <row r="110" spans="1:12">
       <c r="A110" s="13">
         <v>43952</v>
       </c>
-      <c r="B110" s="25"/>
-      <c r="C110" s="26"/>
+      <c r="B110" s="28"/>
+      <c r="C110" s="25"/>
       <c r="D110" s="13">
         <v>43952</v>
       </c>
-      <c r="E110" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="F110" s="60">
+      <c r="E110" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F110" s="30">
         <v>2</v>
       </c>
       <c r="G110" s="13">
         <v>43952</v>
       </c>
-      <c r="H110" s="29"/>
-      <c r="I110" s="28"/>
+      <c r="H110" s="25"/>
+      <c r="I110" s="26"/>
       <c r="J110" s="22">
         <f t="shared" si="0"/>
         <v>43952</v>
       </c>
-      <c r="K110" s="28"/>
-      <c r="L110" s="28"/>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K110" s="60"/>
+      <c r="L110" s="60"/>
+    </row>
+    <row r="111" spans="1:12">
       <c r="A111" s="13">
         <v>43953</v>
       </c>
-      <c r="B111" s="25"/>
-      <c r="C111" s="26"/>
+      <c r="B111" s="28"/>
+      <c r="C111" s="25"/>
       <c r="D111" s="13">
         <v>43953</v>
       </c>
-      <c r="E111" s="32"/>
-      <c r="F111" s="60"/>
+      <c r="E111" s="29"/>
+      <c r="F111" s="30"/>
       <c r="G111" s="13">
         <v>43953</v>
       </c>
-      <c r="H111" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="I111" s="28">
+      <c r="H111" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="I111" s="26">
         <v>6</v>
       </c>
       <c r="J111" s="22">
         <f t="shared" si="0"/>
         <v>43953</v>
       </c>
-      <c r="K111" s="28"/>
-      <c r="L111" s="28"/>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K111" s="60"/>
+      <c r="L111" s="60"/>
+    </row>
+    <row r="112" spans="1:12">
       <c r="A112" s="13">
         <v>43954</v>
       </c>
-      <c r="B112" s="25"/>
-      <c r="C112" s="26"/>
+      <c r="B112" s="28"/>
+      <c r="C112" s="25"/>
       <c r="D112" s="13">
         <v>43954</v>
       </c>
@@ -3413,915 +3426,955 @@
       <c r="G112" s="13">
         <v>43954</v>
       </c>
-      <c r="H112" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="I112" s="28"/>
+      <c r="H112" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="I112" s="26"/>
       <c r="J112" s="22">
         <f t="shared" si="0"/>
         <v>43954</v>
       </c>
-      <c r="K112" s="28"/>
-      <c r="L112" s="28"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K112" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="L112" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
       <c r="A113" s="13">
         <v>43955</v>
       </c>
-      <c r="B113" s="25"/>
-      <c r="C113" s="26"/>
+      <c r="B113" s="28"/>
+      <c r="C113" s="25"/>
       <c r="D113" s="13">
         <v>43955</v>
       </c>
       <c r="G113" s="13">
         <v>43955</v>
       </c>
-      <c r="H113" s="28"/>
-      <c r="I113" s="28"/>
+      <c r="H113" s="26"/>
+      <c r="I113" s="26"/>
       <c r="J113" s="22">
         <f t="shared" si="0"/>
         <v>43955</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K113" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="L113" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
       <c r="A114" s="13">
         <v>43956</v>
       </c>
-      <c r="B114" s="25"/>
-      <c r="C114" s="26"/>
+      <c r="B114" s="28"/>
+      <c r="C114" s="25"/>
       <c r="D114" s="13">
         <v>43956</v>
       </c>
       <c r="G114" s="13">
         <v>43956</v>
       </c>
-      <c r="H114" s="28"/>
-      <c r="I114" s="28"/>
+      <c r="H114" s="26"/>
+      <c r="I114" s="26"/>
       <c r="J114" s="22">
         <f t="shared" si="0"/>
         <v>43956</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K114" s="26"/>
+      <c r="L114" s="26"/>
+    </row>
+    <row r="115" spans="1:12">
       <c r="A115" s="13">
         <v>43957</v>
       </c>
-      <c r="B115" s="25"/>
-      <c r="C115" s="26"/>
+      <c r="B115" s="28"/>
+      <c r="C115" s="25"/>
       <c r="D115" s="13">
         <v>43957</v>
       </c>
       <c r="G115" s="13">
         <v>43957</v>
       </c>
-      <c r="H115" s="28"/>
-      <c r="I115" s="28"/>
+      <c r="H115" s="26"/>
+      <c r="I115" s="26"/>
       <c r="J115" s="22">
         <f>J114+1</f>
         <v>43957</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K115" s="26"/>
+      <c r="L115" s="26"/>
+    </row>
+    <row r="116" spans="1:12">
       <c r="A116" s="13">
         <v>43958</v>
       </c>
-      <c r="B116" s="25"/>
-      <c r="C116" s="26"/>
+      <c r="B116" s="28"/>
+      <c r="C116" s="25"/>
       <c r="D116" s="13">
         <v>43958</v>
       </c>
       <c r="G116" s="13">
         <v>43958</v>
       </c>
-      <c r="H116" s="28"/>
-      <c r="I116" s="28"/>
+      <c r="H116" s="26"/>
+      <c r="I116" s="26"/>
       <c r="J116" s="22">
         <f t="shared" si="0"/>
         <v>43958</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K116" s="26"/>
+      <c r="L116" s="26"/>
+    </row>
+    <row r="117" spans="1:12">
       <c r="A117" s="13">
         <v>43959</v>
       </c>
-      <c r="B117" s="25"/>
-      <c r="C117" s="26"/>
+      <c r="B117" s="28"/>
+      <c r="C117" s="25"/>
       <c r="D117" s="13">
         <v>43959</v>
       </c>
       <c r="G117" s="13">
         <v>43959</v>
       </c>
-      <c r="H117" s="28"/>
-      <c r="I117" s="28"/>
+      <c r="H117" s="26"/>
+      <c r="I117" s="26"/>
       <c r="J117" s="22">
         <f t="shared" si="0"/>
         <v>43959</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K117" s="26"/>
+      <c r="L117" s="26"/>
+    </row>
+    <row r="118" spans="1:12">
       <c r="A118" s="13">
         <v>43960</v>
       </c>
-      <c r="B118" s="25"/>
-      <c r="C118" s="26"/>
+      <c r="B118" s="28"/>
+      <c r="C118" s="25"/>
       <c r="D118" s="13">
         <v>43960</v>
       </c>
       <c r="G118" s="13">
         <v>43960</v>
       </c>
-      <c r="H118" s="28"/>
-      <c r="I118" s="28"/>
+      <c r="H118" s="26"/>
+      <c r="I118" s="26"/>
       <c r="J118" s="22">
         <f t="shared" si="0"/>
         <v>43960</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K118" s="26"/>
+      <c r="L118" s="26"/>
+    </row>
+    <row r="119" spans="1:12">
       <c r="A119" s="13">
         <v>43961</v>
       </c>
-      <c r="B119" s="25"/>
-      <c r="C119" s="26"/>
+      <c r="B119" s="28"/>
+      <c r="C119" s="25"/>
       <c r="D119" s="13">
         <v>43961</v>
       </c>
       <c r="G119" s="13">
         <v>43961</v>
       </c>
-      <c r="H119" s="28"/>
-      <c r="I119" s="28"/>
+      <c r="H119" s="26"/>
+      <c r="I119" s="26"/>
       <c r="J119" s="22">
         <f t="shared" si="0"/>
         <v>43961</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K119" s="26"/>
+      <c r="L119" s="26"/>
+    </row>
+    <row r="120" spans="1:12">
       <c r="A120" s="13">
         <v>43962</v>
       </c>
-      <c r="B120" s="25"/>
-      <c r="C120" s="26"/>
+      <c r="B120" s="28"/>
+      <c r="C120" s="25"/>
       <c r="D120" s="13">
         <v>43962</v>
       </c>
       <c r="G120" s="13">
         <v>43962</v>
       </c>
-      <c r="H120" s="28"/>
-      <c r="I120" s="28"/>
+      <c r="H120" s="26"/>
+      <c r="I120" s="26"/>
       <c r="J120" s="22">
         <f t="shared" si="0"/>
         <v>43962</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K120" s="26"/>
+      <c r="L120" s="26"/>
+    </row>
+    <row r="121" spans="1:12">
       <c r="A121" s="13">
         <v>43963</v>
       </c>
-      <c r="B121" s="25"/>
-      <c r="C121" s="26"/>
+      <c r="B121" s="28"/>
+      <c r="C121" s="25"/>
       <c r="D121" s="13">
         <v>43963</v>
       </c>
       <c r="G121" s="13">
         <v>43963</v>
       </c>
-      <c r="H121" s="28"/>
-      <c r="I121" s="28"/>
+      <c r="H121" s="26"/>
+      <c r="I121" s="26"/>
       <c r="J121" s="22">
         <f t="shared" si="0"/>
         <v>43963</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K121" s="26"/>
+      <c r="L121" s="26"/>
+    </row>
+    <row r="122" spans="1:12">
       <c r="A122" s="13">
         <v>43964</v>
       </c>
-      <c r="B122" s="25"/>
-      <c r="C122" s="26"/>
+      <c r="B122" s="28"/>
+      <c r="C122" s="25"/>
       <c r="D122" s="13">
         <v>43964</v>
       </c>
       <c r="G122" s="13">
         <v>43964</v>
       </c>
-      <c r="H122" s="28"/>
-      <c r="I122" s="28"/>
+      <c r="H122" s="26"/>
+      <c r="I122" s="26"/>
       <c r="J122" s="22">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K122" s="26"/>
+      <c r="L122" s="26"/>
+    </row>
+    <row r="123" spans="1:12">
       <c r="A123" s="13">
         <v>43965</v>
       </c>
-      <c r="B123" s="25"/>
-      <c r="C123" s="26"/>
+      <c r="B123" s="28"/>
+      <c r="C123" s="25"/>
       <c r="D123" s="13">
         <v>43965</v>
       </c>
       <c r="G123" s="13">
         <v>43965</v>
       </c>
-      <c r="H123" s="28"/>
-      <c r="I123" s="28"/>
+      <c r="H123" s="26"/>
+      <c r="I123" s="26"/>
       <c r="J123" s="22">
         <f>J122+1</f>
         <v>43965</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K123" s="26"/>
+      <c r="L123" s="26"/>
+    </row>
+    <row r="124" spans="1:12">
       <c r="A124" s="13">
         <v>43966</v>
       </c>
-      <c r="B124" s="25"/>
-      <c r="C124" s="26"/>
+      <c r="B124" s="28"/>
+      <c r="C124" s="25"/>
       <c r="D124" s="13">
         <v>43966</v>
       </c>
       <c r="G124" s="13">
         <v>43966</v>
       </c>
-      <c r="H124" s="28"/>
-      <c r="I124" s="28"/>
+      <c r="H124" s="26"/>
+      <c r="I124" s="26"/>
       <c r="J124" s="22">
         <f t="shared" si="0"/>
         <v>43966</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K124" s="26"/>
+      <c r="L124" s="26"/>
+    </row>
+    <row r="125" spans="1:12">
       <c r="A125" s="13">
         <v>43967</v>
       </c>
-      <c r="B125" s="25"/>
-      <c r="C125" s="26"/>
+      <c r="B125" s="28"/>
+      <c r="C125" s="25"/>
       <c r="D125" s="13">
         <v>43967</v>
       </c>
       <c r="G125" s="13">
         <v>43967</v>
       </c>
-      <c r="H125" s="28"/>
-      <c r="I125" s="28"/>
+      <c r="H125" s="26"/>
+      <c r="I125" s="26"/>
       <c r="J125" s="22">
         <f t="shared" si="0"/>
         <v>43967</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K125" s="26"/>
+      <c r="L125" s="26"/>
+    </row>
+    <row r="126" spans="1:12">
       <c r="A126" s="13">
         <v>43968</v>
       </c>
-      <c r="B126" s="25"/>
-      <c r="C126" s="26"/>
+      <c r="B126" s="28"/>
+      <c r="C126" s="25"/>
       <c r="D126" s="13">
         <v>43968</v>
       </c>
       <c r="G126" s="13">
         <v>43968</v>
       </c>
-      <c r="H126" s="28"/>
-      <c r="I126" s="28"/>
+      <c r="H126" s="26"/>
+      <c r="I126" s="26"/>
       <c r="J126" s="22">
         <f t="shared" si="0"/>
         <v>43968</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K126" s="26"/>
+      <c r="L126" s="26"/>
+    </row>
+    <row r="127" spans="1:12">
       <c r="A127" s="13">
         <v>43969</v>
       </c>
-      <c r="B127" s="25"/>
-      <c r="C127" s="26"/>
+      <c r="B127" s="28"/>
+      <c r="C127" s="25"/>
       <c r="D127" s="13">
         <v>43969</v>
       </c>
       <c r="G127" s="13">
         <v>43969</v>
       </c>
-      <c r="H127" s="28"/>
-      <c r="I127" s="28"/>
+      <c r="H127" s="26"/>
+      <c r="I127" s="26"/>
       <c r="J127" s="22">
         <f t="shared" si="0"/>
         <v>43969</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K127" s="26"/>
+      <c r="L127" s="26"/>
+    </row>
+    <row r="128" spans="1:12">
       <c r="A128" s="13">
         <v>43970</v>
       </c>
-      <c r="B128" s="25"/>
-      <c r="C128" s="26"/>
+      <c r="B128" s="28"/>
+      <c r="C128" s="25"/>
       <c r="D128" s="13">
         <v>43970</v>
       </c>
       <c r="G128" s="13">
         <v>43970</v>
       </c>
-      <c r="H128" s="28"/>
-      <c r="I128" s="28"/>
+      <c r="H128" s="26"/>
+      <c r="I128" s="26"/>
       <c r="J128" s="22">
         <f t="shared" si="0"/>
         <v>43970</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K128" s="26"/>
+      <c r="L128" s="26"/>
+    </row>
+    <row r="129" spans="1:10">
       <c r="A129" s="13">
         <v>43971</v>
       </c>
-      <c r="B129" s="25"/>
-      <c r="C129" s="26"/>
+      <c r="B129" s="28"/>
+      <c r="C129" s="25"/>
       <c r="D129" s="13">
         <v>43971</v>
       </c>
       <c r="G129" s="13">
         <v>43971</v>
       </c>
-      <c r="H129" s="28"/>
-      <c r="I129" s="28"/>
+      <c r="H129" s="26"/>
+      <c r="I129" s="26"/>
       <c r="J129" s="22">
         <f t="shared" si="0"/>
         <v>43971</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="13">
         <v>43972</v>
       </c>
-      <c r="B130" s="25"/>
-      <c r="C130" s="26"/>
+      <c r="B130" s="28"/>
+      <c r="C130" s="25"/>
       <c r="D130" s="13">
         <v>43972</v>
       </c>
       <c r="G130" s="13">
         <v>43972</v>
       </c>
-      <c r="H130" s="28"/>
-      <c r="I130" s="28"/>
+      <c r="H130" s="26"/>
+      <c r="I130" s="26"/>
       <c r="J130" s="22">
         <f t="shared" ref="J130:J160" si="1">J129+1</f>
         <v>43972</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="13">
         <v>43973</v>
       </c>
-      <c r="B131" s="25"/>
-      <c r="C131" s="26"/>
+      <c r="B131" s="28"/>
+      <c r="C131" s="25"/>
       <c r="D131" s="13">
         <v>43973</v>
       </c>
       <c r="G131" s="13">
         <v>43973</v>
       </c>
-      <c r="H131" s="28"/>
-      <c r="I131" s="28"/>
+      <c r="H131" s="26"/>
+      <c r="I131" s="26"/>
       <c r="J131" s="22">
         <f t="shared" si="1"/>
         <v>43973</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="13">
         <v>43974</v>
       </c>
-      <c r="B132" s="25"/>
-      <c r="C132" s="26"/>
+      <c r="B132" s="28"/>
+      <c r="C132" s="25"/>
       <c r="D132" s="13">
         <v>43974</v>
       </c>
       <c r="G132" s="13">
         <v>43974</v>
       </c>
-      <c r="H132" s="28"/>
-      <c r="I132" s="28"/>
+      <c r="H132" s="26"/>
+      <c r="I132" s="26"/>
       <c r="J132" s="22">
         <f t="shared" si="1"/>
         <v>43974</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="13">
         <v>43975</v>
       </c>
-      <c r="B133" s="25"/>
-      <c r="C133" s="26"/>
+      <c r="B133" s="28"/>
+      <c r="C133" s="25"/>
       <c r="D133" s="13">
         <v>43975</v>
       </c>
       <c r="G133" s="13">
         <v>43975</v>
       </c>
-      <c r="H133" s="28"/>
-      <c r="I133" s="28"/>
+      <c r="H133" s="26"/>
+      <c r="I133" s="26"/>
       <c r="J133" s="22">
         <f t="shared" si="1"/>
         <v>43975</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="13">
         <v>43976</v>
       </c>
-      <c r="B134" s="25"/>
-      <c r="C134" s="26"/>
+      <c r="B134" s="28"/>
+      <c r="C134" s="25"/>
       <c r="D134" s="13">
         <v>43976</v>
       </c>
       <c r="G134" s="13">
         <v>43976</v>
       </c>
-      <c r="H134" s="28"/>
-      <c r="I134" s="28"/>
+      <c r="H134" s="26"/>
+      <c r="I134" s="26"/>
       <c r="J134" s="22">
         <f t="shared" si="1"/>
         <v>43976</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="13">
         <v>43977</v>
       </c>
-      <c r="B135" s="25"/>
-      <c r="C135" s="26"/>
+      <c r="B135" s="28"/>
+      <c r="C135" s="25"/>
       <c r="D135" s="13">
         <v>43977</v>
       </c>
       <c r="G135" s="13">
         <v>43977</v>
       </c>
-      <c r="H135" s="28"/>
-      <c r="I135" s="28"/>
+      <c r="H135" s="26"/>
+      <c r="I135" s="26"/>
       <c r="J135" s="22">
         <f t="shared" si="1"/>
         <v>43977</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="13">
         <v>43978</v>
       </c>
-      <c r="B136" s="25"/>
-      <c r="C136" s="26"/>
+      <c r="B136" s="28"/>
+      <c r="C136" s="25"/>
       <c r="D136" s="13">
         <v>43978</v>
       </c>
       <c r="G136" s="13">
         <v>43978</v>
       </c>
-      <c r="H136" s="28"/>
-      <c r="I136" s="28"/>
+      <c r="H136" s="26"/>
+      <c r="I136" s="26"/>
       <c r="J136" s="22">
         <f t="shared" si="1"/>
         <v>43978</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="13">
         <v>43979</v>
       </c>
-      <c r="B137" s="25"/>
-      <c r="C137" s="26"/>
+      <c r="B137" s="28"/>
+      <c r="C137" s="25"/>
       <c r="D137" s="13">
         <v>43979</v>
       </c>
       <c r="G137" s="13">
         <v>43979</v>
       </c>
-      <c r="H137" s="28"/>
-      <c r="I137" s="28"/>
+      <c r="H137" s="26"/>
+      <c r="I137" s="26"/>
       <c r="J137" s="22">
         <f t="shared" si="1"/>
         <v>43979</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="13">
         <v>43980</v>
       </c>
-      <c r="B138" s="25"/>
-      <c r="C138" s="26"/>
+      <c r="B138" s="28"/>
+      <c r="C138" s="25"/>
       <c r="D138" s="13">
         <v>43980</v>
       </c>
       <c r="G138" s="13">
         <v>43980</v>
       </c>
-      <c r="H138" s="28"/>
-      <c r="I138" s="28"/>
+      <c r="H138" s="26"/>
+      <c r="I138" s="26"/>
       <c r="J138" s="22">
         <f t="shared" si="1"/>
         <v>43980</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="13">
         <v>43981</v>
       </c>
-      <c r="B139" s="25"/>
-      <c r="C139" s="26"/>
+      <c r="B139" s="28"/>
+      <c r="C139" s="25"/>
       <c r="D139" s="13">
         <v>43981</v>
       </c>
       <c r="G139" s="13">
         <v>43981</v>
       </c>
-      <c r="H139" s="28"/>
-      <c r="I139" s="28"/>
+      <c r="H139" s="26"/>
+      <c r="I139" s="26"/>
       <c r="J139" s="22">
         <f t="shared" si="1"/>
         <v>43981</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="13">
         <v>43982</v>
       </c>
-      <c r="B140" s="25"/>
-      <c r="C140" s="26"/>
+      <c r="B140" s="28"/>
+      <c r="C140" s="25"/>
       <c r="D140" s="13">
         <v>43982</v>
       </c>
       <c r="G140" s="13">
         <v>43982</v>
       </c>
-      <c r="H140" s="28"/>
-      <c r="I140" s="28"/>
+      <c r="H140" s="26"/>
+      <c r="I140" s="26"/>
       <c r="J140" s="22">
         <f t="shared" si="1"/>
         <v>43982</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="13">
         <v>43983</v>
       </c>
-      <c r="B141" s="25"/>
-      <c r="C141" s="26"/>
+      <c r="B141" s="28"/>
+      <c r="C141" s="25"/>
       <c r="D141" s="13">
         <v>43983</v>
       </c>
       <c r="G141" s="13">
         <v>43983</v>
       </c>
-      <c r="H141" s="28"/>
-      <c r="I141" s="28"/>
+      <c r="H141" s="26"/>
+      <c r="I141" s="26"/>
       <c r="J141" s="22">
         <f t="shared" si="1"/>
         <v>43983</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="13">
         <v>43984</v>
       </c>
-      <c r="B142" s="25"/>
-      <c r="C142" s="26"/>
+      <c r="B142" s="28"/>
+      <c r="C142" s="25"/>
       <c r="D142" s="13">
         <v>43984</v>
       </c>
       <c r="G142" s="13">
         <v>43984</v>
       </c>
-      <c r="H142" s="28"/>
-      <c r="I142" s="28"/>
+      <c r="H142" s="26"/>
+      <c r="I142" s="26"/>
       <c r="J142" s="22">
         <f t="shared" si="1"/>
         <v>43984</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="13">
         <v>43985</v>
       </c>
-      <c r="B143" s="25"/>
-      <c r="C143" s="26"/>
+      <c r="B143" s="28"/>
+      <c r="C143" s="25"/>
       <c r="D143" s="13">
         <v>43985</v>
       </c>
       <c r="G143" s="13">
         <v>43985</v>
       </c>
-      <c r="H143" s="28"/>
-      <c r="I143" s="28"/>
+      <c r="H143" s="26"/>
+      <c r="I143" s="26"/>
       <c r="J143" s="22">
         <f t="shared" si="1"/>
         <v>43985</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="13">
         <v>43986</v>
       </c>
-      <c r="B144" s="25"/>
-      <c r="C144" s="26"/>
+      <c r="B144" s="28"/>
+      <c r="C144" s="25"/>
       <c r="D144" s="13">
         <v>43986</v>
       </c>
       <c r="G144" s="13">
         <v>43986</v>
       </c>
-      <c r="H144" s="28"/>
-      <c r="I144" s="28"/>
+      <c r="H144" s="26"/>
+      <c r="I144" s="26"/>
       <c r="J144" s="22">
         <f t="shared" si="1"/>
         <v>43986</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12">
       <c r="A145" s="13">
         <v>43987</v>
       </c>
-      <c r="B145" s="25"/>
-      <c r="C145" s="26"/>
+      <c r="B145" s="28"/>
+      <c r="C145" s="25"/>
       <c r="D145" s="13">
         <v>43987</v>
       </c>
       <c r="G145" s="13">
         <v>43987</v>
       </c>
-      <c r="H145" s="28"/>
-      <c r="I145" s="28"/>
+      <c r="H145" s="26"/>
+      <c r="I145" s="26"/>
       <c r="J145" s="22">
         <f t="shared" si="1"/>
         <v>43987</v>
       </c>
-      <c r="K145" s="28"/>
-      <c r="L145" s="28"/>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K145" s="26"/>
+      <c r="L145" s="26"/>
+    </row>
+    <row r="146" spans="1:12">
       <c r="A146" s="13">
         <v>43988</v>
       </c>
-      <c r="B146" s="25"/>
-      <c r="C146" s="26"/>
+      <c r="B146" s="28"/>
+      <c r="C146" s="25"/>
       <c r="D146" s="13">
         <v>43988</v>
       </c>
       <c r="G146" s="13">
         <v>43988</v>
       </c>
-      <c r="H146" s="28"/>
-      <c r="I146" s="28"/>
+      <c r="H146" s="26"/>
+      <c r="I146" s="26"/>
       <c r="J146" s="22">
         <f t="shared" si="1"/>
         <v>43988</v>
       </c>
-      <c r="K146" s="28"/>
-      <c r="L146" s="28"/>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K146" s="26"/>
+      <c r="L146" s="26"/>
+    </row>
+    <row r="147" spans="1:12">
       <c r="A147" s="13">
         <v>43989</v>
       </c>
-      <c r="B147" s="25"/>
-      <c r="C147" s="26"/>
+      <c r="B147" s="28"/>
+      <c r="C147" s="25"/>
       <c r="D147" s="13">
         <v>43989</v>
       </c>
       <c r="G147" s="13">
         <v>43989</v>
       </c>
-      <c r="H147" s="28"/>
-      <c r="I147" s="28"/>
+      <c r="H147" s="26"/>
+      <c r="I147" s="26"/>
       <c r="J147" s="22">
         <f t="shared" si="1"/>
         <v>43989</v>
       </c>
-      <c r="K147" s="28"/>
-      <c r="L147" s="28"/>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K147" s="26"/>
+      <c r="L147" s="26"/>
+    </row>
+    <row r="148" spans="1:12">
       <c r="A148" s="13">
         <v>43990</v>
       </c>
-      <c r="B148" s="25"/>
-      <c r="C148" s="26"/>
+      <c r="B148" s="28"/>
+      <c r="C148" s="25"/>
       <c r="D148" s="13">
         <v>43990</v>
       </c>
       <c r="G148" s="13">
         <v>43990</v>
       </c>
-      <c r="H148" s="28"/>
-      <c r="I148" s="28"/>
+      <c r="H148" s="26"/>
+      <c r="I148" s="26"/>
       <c r="J148" s="22">
         <f t="shared" si="1"/>
         <v>43990</v>
       </c>
-      <c r="K148" s="28"/>
-      <c r="L148" s="28"/>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K148" s="26"/>
+      <c r="L148" s="26"/>
+    </row>
+    <row r="149" spans="1:12">
       <c r="A149" s="13">
         <v>43991</v>
       </c>
-      <c r="B149" s="25"/>
-      <c r="C149" s="26"/>
+      <c r="B149" s="28"/>
+      <c r="C149" s="25"/>
       <c r="D149" s="13">
         <v>43991</v>
       </c>
       <c r="G149" s="13">
         <v>43991</v>
       </c>
-      <c r="H149" s="28"/>
-      <c r="I149" s="28"/>
+      <c r="H149" s="26"/>
+      <c r="I149" s="26"/>
       <c r="J149" s="22">
         <f t="shared" si="1"/>
         <v>43991</v>
       </c>
-      <c r="K149" s="28"/>
-      <c r="L149" s="28"/>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K149" s="26"/>
+      <c r="L149" s="26"/>
+    </row>
+    <row r="150" spans="1:12">
       <c r="A150" s="13">
         <v>43992</v>
       </c>
-      <c r="B150" s="25"/>
-      <c r="C150" s="26"/>
+      <c r="B150" s="28"/>
+      <c r="C150" s="25"/>
       <c r="D150" s="13">
         <v>43992</v>
       </c>
       <c r="G150" s="13">
         <v>43992</v>
       </c>
-      <c r="H150" s="28"/>
-      <c r="I150" s="28"/>
+      <c r="H150" s="26"/>
+      <c r="I150" s="26"/>
       <c r="J150" s="22">
         <f t="shared" si="1"/>
         <v>43992</v>
       </c>
-      <c r="K150" s="28"/>
-      <c r="L150" s="28"/>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K150" s="26"/>
+      <c r="L150" s="26"/>
+    </row>
+    <row r="151" spans="1:12">
       <c r="A151" s="13">
         <v>43993</v>
       </c>
-      <c r="B151" s="25"/>
-      <c r="C151" s="26"/>
+      <c r="B151" s="28"/>
+      <c r="C151" s="25"/>
       <c r="D151" s="13">
         <v>43993</v>
       </c>
       <c r="G151" s="13">
         <v>43993</v>
       </c>
-      <c r="H151" s="28"/>
-      <c r="I151" s="28"/>
+      <c r="H151" s="26"/>
+      <c r="I151" s="26"/>
       <c r="J151" s="22">
         <f t="shared" si="1"/>
         <v>43993</v>
       </c>
-      <c r="K151" s="28"/>
-      <c r="L151" s="28"/>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K151" s="26"/>
+      <c r="L151" s="26"/>
+    </row>
+    <row r="152" spans="1:12">
       <c r="A152" s="13">
         <v>43994</v>
       </c>
-      <c r="B152" s="25"/>
-      <c r="C152" s="26"/>
+      <c r="B152" s="28"/>
+      <c r="C152" s="25"/>
       <c r="D152" s="13">
         <v>43994</v>
       </c>
       <c r="G152" s="13">
         <v>43994</v>
       </c>
-      <c r="H152" s="28"/>
-      <c r="I152" s="28"/>
+      <c r="H152" s="26"/>
+      <c r="I152" s="26"/>
       <c r="J152" s="22">
         <f t="shared" si="1"/>
         <v>43994</v>
       </c>
-      <c r="K152" s="28"/>
-      <c r="L152" s="28"/>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K152" s="26"/>
+      <c r="L152" s="26"/>
+    </row>
+    <row r="153" spans="1:12">
       <c r="A153" s="13">
         <v>43995</v>
       </c>
-      <c r="B153" s="25"/>
-      <c r="C153" s="26"/>
+      <c r="B153" s="28"/>
+      <c r="C153" s="25"/>
       <c r="D153" s="13">
         <v>43995</v>
       </c>
       <c r="G153" s="13">
         <v>43995</v>
       </c>
-      <c r="H153" s="28"/>
-      <c r="I153" s="28"/>
+      <c r="H153" s="26"/>
+      <c r="I153" s="26"/>
       <c r="J153" s="22">
         <f t="shared" si="1"/>
         <v>43995</v>
       </c>
-      <c r="K153" s="28"/>
-      <c r="L153" s="28"/>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K153" s="26"/>
+      <c r="L153" s="26"/>
+    </row>
+    <row r="154" spans="1:12">
       <c r="A154" s="13">
         <v>43996</v>
       </c>
-      <c r="B154" s="25"/>
-      <c r="C154" s="26"/>
+      <c r="B154" s="28"/>
+      <c r="C154" s="25"/>
       <c r="D154" s="13">
         <v>43996</v>
       </c>
       <c r="G154" s="13">
         <v>43996</v>
       </c>
-      <c r="H154" s="28"/>
-      <c r="I154" s="28"/>
+      <c r="H154" s="26"/>
+      <c r="I154" s="26"/>
       <c r="J154" s="22">
         <f t="shared" si="1"/>
         <v>43996</v>
       </c>
-      <c r="K154" s="28"/>
-      <c r="L154" s="28"/>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K154" s="26"/>
+      <c r="L154" s="26"/>
+    </row>
+    <row r="155" spans="1:12">
       <c r="A155" s="13">
         <v>43997</v>
       </c>
-      <c r="B155" s="25"/>
-      <c r="C155" s="26"/>
+      <c r="B155" s="28"/>
+      <c r="C155" s="25"/>
       <c r="D155" s="13">
         <v>43997</v>
       </c>
       <c r="G155" s="13">
         <v>43997</v>
       </c>
-      <c r="H155" s="28"/>
-      <c r="I155" s="28"/>
+      <c r="H155" s="26"/>
+      <c r="I155" s="26"/>
       <c r="J155" s="22">
         <f t="shared" si="1"/>
         <v>43997</v>
       </c>
-      <c r="K155" s="28"/>
-      <c r="L155" s="28"/>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K155" s="26"/>
+      <c r="L155" s="26"/>
+    </row>
+    <row r="156" spans="1:12">
       <c r="A156" s="14"/>
-      <c r="B156" s="28"/>
-      <c r="C156" s="28"/>
+      <c r="B156" s="26"/>
+      <c r="C156" s="26"/>
       <c r="D156" s="13"/>
-      <c r="H156" s="28"/>
-      <c r="I156" s="28"/>
+      <c r="H156" s="26"/>
+      <c r="I156" s="26"/>
       <c r="J156" s="22">
         <f t="shared" si="1"/>
         <v>43998</v>
       </c>
-      <c r="K156" s="28"/>
-      <c r="L156" s="28"/>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K156" s="26"/>
+      <c r="L156" s="26"/>
+    </row>
+    <row r="157" spans="1:12">
       <c r="A157" s="14"/>
-      <c r="B157" s="28"/>
-      <c r="C157" s="28"/>
+      <c r="B157" s="26"/>
+      <c r="C157" s="26"/>
       <c r="D157" s="14"/>
-      <c r="H157" s="28"/>
-      <c r="I157" s="28"/>
+      <c r="H157" s="26"/>
+      <c r="I157" s="26"/>
       <c r="J157" s="22">
         <f t="shared" si="1"/>
         <v>43999</v>
       </c>
-      <c r="K157" s="28"/>
-      <c r="L157" s="28"/>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K157" s="26"/>
+      <c r="L157" s="26"/>
+    </row>
+    <row r="158" spans="1:12">
       <c r="A158" s="14"/>
-      <c r="B158" s="28"/>
-      <c r="C158" s="28"/>
+      <c r="B158" s="26"/>
+      <c r="C158" s="26"/>
       <c r="D158" s="14"/>
-      <c r="H158" s="28"/>
-      <c r="I158" s="28"/>
+      <c r="H158" s="26"/>
+      <c r="I158" s="26"/>
       <c r="J158" s="22">
         <f t="shared" si="1"/>
         <v>44000</v>
       </c>
-      <c r="K158" s="28"/>
-      <c r="L158" s="28"/>
-    </row>
-    <row r="159" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K158" s="26"/>
+      <c r="L158" s="26"/>
+    </row>
+    <row r="159" spans="1:12" ht="30.75" thickBot="1">
       <c r="A159" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B159" s="28"/>
+        <v>87</v>
+      </c>
+      <c r="B159" s="26"/>
       <c r="C159" s="8">
         <f>SUM(C64:C155)</f>
         <v>67</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F159" s="8">
         <f>SUM(F64:F156)</f>
         <v>60</v>
       </c>
-      <c r="H159" s="28"/>
+      <c r="H159" s="26"/>
       <c r="I159" s="17">
         <f>SUM(I2:I155)</f>
         <v>53</v>
@@ -4330,135 +4383,135 @@
         <f t="shared" si="1"/>
         <v>44001</v>
       </c>
-      <c r="K159" s="28"/>
+      <c r="K159" s="26"/>
       <c r="L159" s="17">
         <f>SUM(L64:L155)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="28"/>
-      <c r="C160" s="28"/>
+    <row r="160" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B160" s="26"/>
+      <c r="C160" s="26"/>
       <c r="D160" s="6"/>
-      <c r="H160" s="28"/>
-      <c r="I160" s="28"/>
+      <c r="H160" s="26"/>
+      <c r="I160" s="26"/>
       <c r="J160" s="22">
         <f t="shared" si="1"/>
         <v>44002</v>
       </c>
-      <c r="K160" s="28"/>
-      <c r="L160" s="28"/>
-    </row>
-    <row r="161" spans="10:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K160" s="26"/>
+      <c r="L160" s="26"/>
+    </row>
+    <row r="161" spans="10:10" ht="15.75" thickTop="1">
       <c r="J161" s="22">
         <f>J160+1</f>
         <v>44003</v>
       </c>
     </row>
-    <row r="162" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="10:10">
       <c r="J162" s="22">
         <f t="shared" ref="J162:J168" si="2">J161+1</f>
         <v>44004</v>
       </c>
     </row>
-    <row r="163" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="10:10">
       <c r="J163" s="22">
         <f t="shared" si="2"/>
         <v>44005</v>
       </c>
     </row>
-    <row r="164" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="10:10">
       <c r="J164" s="22">
         <f t="shared" si="2"/>
         <v>44006</v>
       </c>
     </row>
-    <row r="165" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="10:10">
       <c r="J165" s="22">
         <f t="shared" si="2"/>
         <v>44007</v>
       </c>
     </row>
-    <row r="166" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="10:10">
       <c r="J166" s="22">
         <f t="shared" si="2"/>
         <v>44008</v>
       </c>
     </row>
-    <row r="167" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="10:10">
       <c r="J167" s="22">
         <f t="shared" si="2"/>
         <v>44009</v>
       </c>
     </row>
-    <row r="168" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="10:10">
       <c r="J168" s="22">
         <f t="shared" si="2"/>
         <v>44010</v>
       </c>
     </row>
-    <row r="169" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="10:10">
       <c r="J169" s="22">
         <f>J168+1</f>
         <v>44011</v>
       </c>
     </row>
-    <row r="170" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="10:10">
       <c r="J170" s="22">
         <f t="shared" ref="J170:J171" si="3">J169+1</f>
         <v>44012</v>
       </c>
     </row>
-    <row r="171" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="10:10">
       <c r="J171" s="22">
         <f t="shared" si="3"/>
         <v>44013</v>
       </c>
     </row>
-    <row r="172" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="10:10">
       <c r="J172" s="22">
         <f>J171+1</f>
         <v>44014</v>
       </c>
     </row>
-    <row r="173" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="10:10">
       <c r="J173" s="22">
         <f t="shared" ref="J173:J174" si="4">J172+1</f>
         <v>44015</v>
       </c>
     </row>
-    <row r="174" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="10:10">
       <c r="J174" s="22">
         <f t="shared" si="4"/>
         <v>44016</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="E110:E111"/>
-    <mergeCell ref="F110:F111"/>
-    <mergeCell ref="K91:L104"/>
-    <mergeCell ref="K105:K106"/>
-    <mergeCell ref="L105:L106"/>
-    <mergeCell ref="C92:C96"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="E88:E90"/>
-    <mergeCell ref="E92:E100"/>
-    <mergeCell ref="F88:F90"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="E101:E102"/>
-    <mergeCell ref="F101:F102"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="B92:B96"/>
+  <mergeCells count="65">
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="K83:L84"/>
+    <mergeCell ref="H3:I64"/>
+    <mergeCell ref="H73:H74"/>
+    <mergeCell ref="I73:I74"/>
+    <mergeCell ref="B2:C63"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="H65:H71"/>
+    <mergeCell ref="I65:I71"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="K2:L63"/>
+    <mergeCell ref="L81:L82"/>
+    <mergeCell ref="K65:K68"/>
+    <mergeCell ref="L65:L68"/>
+    <mergeCell ref="K69:L70"/>
+    <mergeCell ref="K76:L77"/>
+    <mergeCell ref="K81:K82"/>
     <mergeCell ref="B85:B90"/>
     <mergeCell ref="C85:C90"/>
     <mergeCell ref="E71:E72"/>
@@ -4475,30 +4528,31 @@
     <mergeCell ref="F78:F81"/>
     <mergeCell ref="E73:E76"/>
     <mergeCell ref="F73:F76"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="K2:L63"/>
-    <mergeCell ref="L81:L82"/>
-    <mergeCell ref="K65:K68"/>
-    <mergeCell ref="L65:L68"/>
-    <mergeCell ref="K69:L70"/>
-    <mergeCell ref="K76:L77"/>
-    <mergeCell ref="K81:K82"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="K83:L84"/>
-    <mergeCell ref="H3:I64"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="I73:I74"/>
-    <mergeCell ref="B2:C63"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="C65:C68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="H65:H71"/>
-    <mergeCell ref="I65:I71"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="C92:C96"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="E92:E100"/>
+    <mergeCell ref="F88:F90"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="F85:F87"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="E110:E111"/>
+    <mergeCell ref="F110:F111"/>
+    <mergeCell ref="K91:L104"/>
+    <mergeCell ref="K105:K106"/>
+    <mergeCell ref="L105:L106"/>
+    <mergeCell ref="E101:E102"/>
+    <mergeCell ref="F101:F102"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="K109:L111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
code mecanisme air+ up JA
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\totok\Documents\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C130FDB-ED4F-41DC-9D86-62B939951EA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{85EA7BD6-8542-41D4-BE5D-E369CA3A1C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t xml:space="preserve">fusionner les rapports + physique </t>
+  </si>
+  <si>
+    <t>code mécanisme air</t>
   </si>
   <si>
     <t>Total heures</t>
@@ -665,108 +668,108 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1094,7 +1097,7 @@
   <dimension ref="A1:M174"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L114" sqref="L114"/>
+      <selection activeCell="K118" sqref="K118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1125,7 +1128,7 @@
       <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
@@ -1134,1046 +1137,1046 @@
       <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="55"/>
+      <c r="G1" s="40"/>
       <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="57"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="40"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1">
       <c r="A2" s="13">
         <v>43844</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="54"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="27"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="56"/>
+      <c r="G2" s="41"/>
       <c r="H2" s="27"/>
       <c r="I2" s="11"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="41"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1">
       <c r="A3" s="13">
         <v>43845</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="38"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="13">
         <v>43845</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="36"/>
-      <c r="H3" s="35" t="s">
+      <c r="F3" s="33"/>
+      <c r="H3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="45"/>
+      <c r="I3" s="33"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="50"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1">
       <c r="A4" s="13">
         <v>43846</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="13">
         <v>43846</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="38"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="45"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="35"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="35"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="50"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1">
       <c r="A5" s="13">
         <v>43847</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="13">
         <v>43847</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="38"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="38"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="45"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="35"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="35"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="50"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
       <c r="A6" s="13">
         <v>43848</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="13">
         <v>43848</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="38"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="45"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="35"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="50"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
       <c r="A7" s="13">
         <v>43849</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="13">
         <v>43849</v>
       </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="38"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="45"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="35"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="50"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1">
       <c r="A8" s="13">
         <v>43850</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="13">
         <v>43850</v>
       </c>
-      <c r="E8" s="37"/>
-      <c r="F8" s="38"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="38"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="45"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="35"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="50"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1">
       <c r="A9" s="13">
         <v>43851</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="38"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="13">
         <v>43851</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="38"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="45"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="35"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="50"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1">
       <c r="A10" s="13">
         <v>43852</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="13">
         <v>43852</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="38"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="45"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="35"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="50"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1">
       <c r="A11" s="13">
         <v>43853</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="13">
         <v>43853</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="38"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="45"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="35"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="35"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="50"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1">
       <c r="A12" s="13">
         <v>43854</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="13">
         <v>43854</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="38"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="38"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="45"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="50"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1">
       <c r="A13" s="13">
         <v>43855</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="13">
         <v>43855</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="38"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="45"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="35"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="50"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1">
       <c r="A14" s="13">
         <v>43856</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="13">
         <v>43856</v>
       </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="38"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="38"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="45"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="35"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="50"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1">
       <c r="A15" s="13">
         <v>43857</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="13">
         <v>43857</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="45"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="35"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="50"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1">
       <c r="A16" s="13">
         <v>43858</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="13">
         <v>43858</v>
       </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="38"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="45"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="35"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="50"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1">
       <c r="A17" s="13">
         <v>43859</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="13">
         <v>43859</v>
       </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="38"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="38"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="45"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="35"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="50"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1">
       <c r="A18" s="13">
         <v>43860</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="38"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="13">
         <v>43860</v>
       </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="38"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="38"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="45"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="35"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="50"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1">
       <c r="A19" s="13">
         <v>43861</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="13">
         <v>43861</v>
       </c>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="38"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="45"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="35"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="50"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="A20" s="13">
         <v>43862</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="13">
         <v>43862</v>
       </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="45"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="35"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="50"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1">
       <c r="A21" s="13">
         <v>43863</v>
       </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="38"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="13">
         <v>43863</v>
       </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="38"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="45"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="35"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="50"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="A22" s="13">
         <v>43864</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="38"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="13">
         <v>43864</v>
       </c>
-      <c r="E22" s="37"/>
-      <c r="F22" s="38"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="38"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="45"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="35"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="50"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1">
       <c r="A23" s="13">
         <v>43865</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="38"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="13">
         <v>43865</v>
       </c>
-      <c r="E23" s="37"/>
-      <c r="F23" s="38"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="38"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="45"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="35"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="35"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="50"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1">
       <c r="A24" s="13">
         <v>43866</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="38"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
       <c r="D24" s="13">
         <v>43866</v>
       </c>
-      <c r="E24" s="37"/>
-      <c r="F24" s="38"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="38"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="45"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="35"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="35"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="50"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1">
       <c r="A25" s="13">
         <v>43867</v>
       </c>
-      <c r="B25" s="37"/>
-      <c r="C25" s="38"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="13">
         <v>43867</v>
       </c>
-      <c r="E25" s="37"/>
-      <c r="F25" s="38"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="38"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="45"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="35"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="50"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1">
       <c r="A26" s="13">
         <v>43868</v>
       </c>
-      <c r="B26" s="37"/>
-      <c r="C26" s="38"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="13">
         <v>43868</v>
       </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="38"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="38"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="45"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="35"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="50"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1">
       <c r="A27" s="13">
         <v>43869</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
       <c r="D27" s="13">
         <v>43869</v>
       </c>
-      <c r="E27" s="37"/>
-      <c r="F27" s="38"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="38"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="45"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="35"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="50"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1">
       <c r="A28" s="13">
         <v>43870</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="38"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="35"/>
       <c r="D28" s="13">
         <v>43870</v>
       </c>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="38"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="45"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="35"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="50"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="A29" s="13">
         <v>43871</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="38"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
       <c r="D29" s="13">
         <v>43871</v>
       </c>
-      <c r="E29" s="37"/>
-      <c r="F29" s="38"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="38"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="45"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="35"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="50"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1">
       <c r="A30" s="13">
         <v>43872</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="38"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
       <c r="D30" s="13">
         <v>43872</v>
       </c>
-      <c r="E30" s="37"/>
-      <c r="F30" s="38"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="38"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="45"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="35"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="35"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="50"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1">
       <c r="A31" s="13">
         <v>43873</v>
       </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
       <c r="D31" s="13">
         <v>43873</v>
       </c>
-      <c r="E31" s="37"/>
-      <c r="F31" s="38"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="38"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="45"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="35"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="35"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="50"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1">
       <c r="A32" s="13">
         <v>43874</v>
       </c>
-      <c r="B32" s="37"/>
-      <c r="C32" s="38"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="35"/>
       <c r="D32" s="13">
         <v>43874</v>
       </c>
-      <c r="E32" s="37"/>
-      <c r="F32" s="38"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="38"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="45"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="35"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="35"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="50"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1">
       <c r="A33" s="13">
         <v>43875</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="35"/>
       <c r="D33" s="13">
         <v>43875</v>
       </c>
-      <c r="E33" s="37"/>
-      <c r="F33" s="38"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="38"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="45"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="35"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="35"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="50"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1">
       <c r="A34" s="13">
         <v>43876</v>
       </c>
-      <c r="B34" s="37"/>
-      <c r="C34" s="38"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
       <c r="D34" s="13">
         <v>43876</v>
       </c>
-      <c r="E34" s="37"/>
-      <c r="F34" s="38"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="38"/>
-      <c r="K34" s="44"/>
-      <c r="L34" s="45"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="35"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="35"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="50"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1">
       <c r="A35" s="13">
         <v>43877</v>
       </c>
-      <c r="B35" s="37"/>
-      <c r="C35" s="38"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="35"/>
       <c r="D35" s="13">
         <v>43877</v>
       </c>
-      <c r="E35" s="37"/>
-      <c r="F35" s="38"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="38"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="45"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="35"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="35"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="50"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1">
       <c r="A36" s="13">
         <v>43878</v>
       </c>
-      <c r="B36" s="37"/>
-      <c r="C36" s="38"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="35"/>
       <c r="D36" s="13">
         <v>43878</v>
       </c>
-      <c r="E36" s="37"/>
-      <c r="F36" s="38"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="38"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="45"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="35"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="35"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="50"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1">
       <c r="A37" s="13">
         <v>43879</v>
       </c>
-      <c r="B37" s="37"/>
-      <c r="C37" s="38"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="35"/>
       <c r="D37" s="13">
         <v>43879</v>
       </c>
-      <c r="E37" s="37"/>
-      <c r="F37" s="38"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="38"/>
-      <c r="K37" s="44"/>
-      <c r="L37" s="45"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="35"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="35"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="50"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1">
       <c r="A38" s="13">
         <v>43880</v>
       </c>
-      <c r="B38" s="37"/>
-      <c r="C38" s="38"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
       <c r="D38" s="13">
         <v>43880</v>
       </c>
-      <c r="E38" s="37"/>
-      <c r="F38" s="38"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="38"/>
-      <c r="K38" s="44"/>
-      <c r="L38" s="45"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="35"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="35"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="50"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1">
       <c r="A39" s="13">
         <v>43881</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="38"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="35"/>
       <c r="D39" s="13">
         <v>43881</v>
       </c>
-      <c r="E39" s="37"/>
-      <c r="F39" s="38"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="38"/>
-      <c r="K39" s="44"/>
-      <c r="L39" s="45"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="35"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="35"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="50"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1">
       <c r="A40" s="13">
         <v>43882</v>
       </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="38"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="35"/>
       <c r="D40" s="13">
         <v>43882</v>
       </c>
-      <c r="E40" s="37"/>
-      <c r="F40" s="38"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="38"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="45"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="35"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="35"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="50"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1">
       <c r="A41" s="13">
         <v>43883</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="38"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="35"/>
       <c r="D41" s="13">
         <v>43883</v>
       </c>
-      <c r="E41" s="37"/>
-      <c r="F41" s="38"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="38"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="45"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="35"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="35"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="50"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1">
       <c r="A42" s="13">
         <v>43884</v>
       </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="38"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="35"/>
       <c r="D42" s="13">
         <v>43884</v>
       </c>
-      <c r="E42" s="37"/>
-      <c r="F42" s="38"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="38"/>
-      <c r="K42" s="44"/>
-      <c r="L42" s="45"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="35"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="35"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="50"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1">
       <c r="A43" s="13">
         <v>43885</v>
       </c>
-      <c r="B43" s="37"/>
-      <c r="C43" s="38"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="35"/>
       <c r="D43" s="13">
         <v>43885</v>
       </c>
-      <c r="E43" s="37"/>
-      <c r="F43" s="38"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="38"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="45"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="35"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="35"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="50"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1">
       <c r="A44" s="13">
         <v>43886</v>
       </c>
-      <c r="B44" s="37"/>
-      <c r="C44" s="38"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="35"/>
       <c r="D44" s="13">
         <v>43886</v>
       </c>
-      <c r="E44" s="37"/>
-      <c r="F44" s="38"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="38"/>
-      <c r="K44" s="44"/>
-      <c r="L44" s="45"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="35"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="35"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="50"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1">
       <c r="A45" s="13">
         <v>43887</v>
       </c>
-      <c r="B45" s="37"/>
-      <c r="C45" s="38"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="35"/>
       <c r="D45" s="13">
         <v>43887</v>
       </c>
-      <c r="E45" s="37"/>
-      <c r="F45" s="38"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="38"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="45"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="35"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="35"/>
+      <c r="K45" s="49"/>
+      <c r="L45" s="50"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1">
       <c r="A46" s="13">
         <v>43888</v>
       </c>
-      <c r="B46" s="37"/>
-      <c r="C46" s="38"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="35"/>
       <c r="D46" s="13">
         <v>43888</v>
       </c>
-      <c r="E46" s="37"/>
-      <c r="F46" s="38"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="38"/>
-      <c r="K46" s="44"/>
-      <c r="L46" s="45"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="35"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="35"/>
+      <c r="K46" s="49"/>
+      <c r="L46" s="50"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1">
       <c r="A47" s="13">
         <v>43889</v>
       </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="38"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="35"/>
       <c r="D47" s="13">
         <v>43889</v>
       </c>
-      <c r="E47" s="37"/>
-      <c r="F47" s="38"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="38"/>
-      <c r="K47" s="44"/>
-      <c r="L47" s="45"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="35"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="35"/>
+      <c r="K47" s="49"/>
+      <c r="L47" s="50"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1">
       <c r="A48" s="13">
         <v>43890</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="38"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="35"/>
       <c r="D48" s="13">
         <v>43890</v>
       </c>
-      <c r="E48" s="37"/>
-      <c r="F48" s="38"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="38"/>
-      <c r="K48" s="44"/>
-      <c r="L48" s="45"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="35"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="35"/>
+      <c r="K48" s="49"/>
+      <c r="L48" s="50"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1">
       <c r="A49" s="13">
         <v>43891</v>
       </c>
-      <c r="B49" s="37"/>
-      <c r="C49" s="38"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="35"/>
       <c r="D49" s="13">
         <v>43891</v>
       </c>
-      <c r="E49" s="37"/>
-      <c r="F49" s="38"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="38"/>
-      <c r="K49" s="44"/>
-      <c r="L49" s="45"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="35"/>
+      <c r="H49" s="34"/>
+      <c r="I49" s="35"/>
+      <c r="K49" s="49"/>
+      <c r="L49" s="50"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1">
       <c r="A50" s="13">
         <v>43892</v>
       </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="38"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="35"/>
       <c r="D50" s="13">
         <v>43892</v>
       </c>
-      <c r="E50" s="37"/>
-      <c r="F50" s="38"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="38"/>
-      <c r="K50" s="44"/>
-      <c r="L50" s="45"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="35"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="35"/>
+      <c r="K50" s="49"/>
+      <c r="L50" s="50"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1">
       <c r="A51" s="13">
         <v>43893</v>
       </c>
-      <c r="B51" s="37"/>
-      <c r="C51" s="38"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="35"/>
       <c r="D51" s="13">
         <v>43893</v>
       </c>
-      <c r="E51" s="37"/>
-      <c r="F51" s="38"/>
-      <c r="H51" s="37"/>
-      <c r="I51" s="38"/>
-      <c r="K51" s="44"/>
-      <c r="L51" s="45"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="35"/>
+      <c r="H51" s="34"/>
+      <c r="I51" s="35"/>
+      <c r="K51" s="49"/>
+      <c r="L51" s="50"/>
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1">
       <c r="A52" s="13">
         <v>43894</v>
       </c>
-      <c r="B52" s="37"/>
-      <c r="C52" s="38"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="35"/>
       <c r="D52" s="13">
         <v>43894</v>
       </c>
-      <c r="E52" s="37"/>
-      <c r="F52" s="38"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="38"/>
-      <c r="K52" s="44"/>
-      <c r="L52" s="45"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="35"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="35"/>
+      <c r="K52" s="49"/>
+      <c r="L52" s="50"/>
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1">
       <c r="A53" s="13">
         <v>43895</v>
       </c>
-      <c r="B53" s="37"/>
-      <c r="C53" s="38"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="35"/>
       <c r="D53" s="13">
         <v>43895</v>
       </c>
-      <c r="E53" s="37"/>
-      <c r="F53" s="38"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="38"/>
-      <c r="K53" s="44"/>
-      <c r="L53" s="45"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="35"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="35"/>
+      <c r="K53" s="49"/>
+      <c r="L53" s="50"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1">
       <c r="A54" s="13">
         <v>43896</v>
       </c>
-      <c r="B54" s="37"/>
-      <c r="C54" s="38"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="35"/>
       <c r="D54" s="13">
         <v>43896</v>
       </c>
-      <c r="E54" s="37"/>
-      <c r="F54" s="38"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="38"/>
-      <c r="K54" s="44"/>
-      <c r="L54" s="45"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="35"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="35"/>
+      <c r="K54" s="49"/>
+      <c r="L54" s="50"/>
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1">
       <c r="A55" s="13">
         <v>43897</v>
       </c>
-      <c r="B55" s="37"/>
-      <c r="C55" s="38"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="35"/>
       <c r="D55" s="13">
         <v>43897</v>
       </c>
-      <c r="E55" s="37"/>
-      <c r="F55" s="38"/>
-      <c r="H55" s="37"/>
-      <c r="I55" s="38"/>
-      <c r="K55" s="44"/>
-      <c r="L55" s="45"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="35"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="35"/>
+      <c r="K55" s="49"/>
+      <c r="L55" s="50"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1">
       <c r="A56" s="13">
         <v>43898</v>
       </c>
-      <c r="B56" s="37"/>
-      <c r="C56" s="38"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="35"/>
       <c r="D56" s="13">
         <v>43898</v>
       </c>
-      <c r="E56" s="37"/>
-      <c r="F56" s="38"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="38"/>
-      <c r="K56" s="44"/>
-      <c r="L56" s="45"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="35"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="35"/>
+      <c r="K56" s="49"/>
+      <c r="L56" s="50"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1">
       <c r="A57" s="13">
         <v>43899</v>
       </c>
-      <c r="B57" s="37"/>
-      <c r="C57" s="38"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="35"/>
       <c r="D57" s="13">
         <v>43899</v>
       </c>
-      <c r="E57" s="37"/>
-      <c r="F57" s="38"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="38"/>
-      <c r="K57" s="44"/>
-      <c r="L57" s="45"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="35"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="35"/>
+      <c r="K57" s="49"/>
+      <c r="L57" s="50"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1">
       <c r="A58" s="13">
         <v>43900</v>
       </c>
-      <c r="B58" s="37"/>
-      <c r="C58" s="38"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="35"/>
       <c r="D58" s="13">
         <v>43900</v>
       </c>
-      <c r="E58" s="37"/>
-      <c r="F58" s="38"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="38"/>
-      <c r="K58" s="44"/>
-      <c r="L58" s="45"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="35"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="35"/>
+      <c r="K58" s="49"/>
+      <c r="L58" s="50"/>
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1">
       <c r="A59" s="13">
         <v>43901</v>
       </c>
-      <c r="B59" s="37"/>
-      <c r="C59" s="38"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="35"/>
       <c r="D59" s="13">
         <v>43901</v>
       </c>
-      <c r="E59" s="37"/>
-      <c r="F59" s="38"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="38"/>
-      <c r="K59" s="44"/>
-      <c r="L59" s="45"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="35"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="35"/>
+      <c r="K59" s="49"/>
+      <c r="L59" s="50"/>
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1">
       <c r="A60" s="13">
         <v>43902</v>
       </c>
-      <c r="B60" s="37"/>
-      <c r="C60" s="38"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="35"/>
       <c r="D60" s="13">
         <v>43902</v>
       </c>
-      <c r="E60" s="37"/>
-      <c r="F60" s="38"/>
-      <c r="H60" s="37"/>
-      <c r="I60" s="38"/>
-      <c r="K60" s="44"/>
-      <c r="L60" s="45"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="35"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="35"/>
+      <c r="K60" s="49"/>
+      <c r="L60" s="50"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1">
       <c r="A61" s="13">
         <v>43903</v>
       </c>
-      <c r="B61" s="37"/>
-      <c r="C61" s="38"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="35"/>
       <c r="D61" s="13">
         <v>43903</v>
       </c>
-      <c r="E61" s="37"/>
-      <c r="F61" s="38"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="38"/>
-      <c r="K61" s="44"/>
-      <c r="L61" s="45"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="35"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="35"/>
+      <c r="K61" s="49"/>
+      <c r="L61" s="50"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1">
       <c r="A62" s="13">
         <v>43904</v>
       </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="38"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="35"/>
       <c r="D62" s="13">
         <v>43904</v>
       </c>
-      <c r="E62" s="37"/>
-      <c r="F62" s="38"/>
-      <c r="H62" s="37"/>
-      <c r="I62" s="38"/>
-      <c r="K62" s="44"/>
-      <c r="L62" s="45"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="35"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="35"/>
+      <c r="K62" s="49"/>
+      <c r="L62" s="50"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1">
       <c r="A63" s="13">
         <v>43905</v>
       </c>
-      <c r="B63" s="37"/>
-      <c r="C63" s="38"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="35"/>
       <c r="D63" s="13">
         <v>43905</v>
       </c>
-      <c r="E63" s="37"/>
-      <c r="F63" s="38"/>
-      <c r="H63" s="37"/>
-      <c r="I63" s="38"/>
-      <c r="K63" s="44"/>
-      <c r="L63" s="45"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="35"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="35"/>
+      <c r="K63" s="49"/>
+      <c r="L63" s="50"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1">
       <c r="A64" s="13">
         <v>43906</v>
       </c>
-      <c r="B64" s="28" t="s">
+      <c r="B64" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C64" s="25">
+      <c r="C64" s="26">
         <v>2</v>
       </c>
       <c r="D64" s="13">
         <v>43906</v>
       </c>
-      <c r="E64" s="28" t="s">
+      <c r="E64" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F64" s="25">
+      <c r="F64" s="26">
         <v>2</v>
       </c>
-      <c r="H64" s="37"/>
-      <c r="I64" s="38"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="35"/>
       <c r="J64" s="22">
         <v>43906</v>
       </c>
-      <c r="K64" s="28" t="s">
+      <c r="K64" s="25" t="s">
         <v>11</v>
       </c>
       <c r="L64" s="18" t="s">
@@ -2187,7 +2190,7 @@
       <c r="B65" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="39">
+      <c r="C65" s="37">
         <v>10</v>
       </c>
       <c r="D65" s="13">
@@ -2196,13 +2199,13 @@
       <c r="E65" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="39">
+      <c r="F65" s="37">
         <v>12</v>
       </c>
       <c r="H65" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I65" s="59"/>
+      <c r="I65" s="44"/>
       <c r="J65" s="22">
         <f>J64+1</f>
         <v>43907</v>
@@ -2210,7 +2213,7 @@
       <c r="K65" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="L65" s="46" t="s">
+      <c r="L65" s="51" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2219,60 +2222,60 @@
         <v>43908</v>
       </c>
       <c r="B66" s="29"/>
-      <c r="C66" s="39"/>
+      <c r="C66" s="37"/>
       <c r="D66" s="13">
         <v>43908</v>
       </c>
       <c r="E66" s="29"/>
-      <c r="F66" s="39"/>
+      <c r="F66" s="37"/>
       <c r="H66" s="29"/>
-      <c r="I66" s="59"/>
+      <c r="I66" s="44"/>
       <c r="J66" s="22">
         <f t="shared" ref="J66:J129" si="0">J65+1</f>
         <v>43908</v>
       </c>
       <c r="K66" s="29"/>
-      <c r="L66" s="46"/>
+      <c r="L66" s="51"/>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="13">
         <v>43909</v>
       </c>
       <c r="B67" s="29"/>
-      <c r="C67" s="39"/>
+      <c r="C67" s="37"/>
       <c r="D67" s="13">
         <v>43909</v>
       </c>
       <c r="E67" s="29"/>
-      <c r="F67" s="39"/>
+      <c r="F67" s="37"/>
       <c r="H67" s="29"/>
-      <c r="I67" s="59"/>
+      <c r="I67" s="44"/>
       <c r="J67" s="22">
         <f t="shared" si="0"/>
         <v>43909</v>
       </c>
       <c r="K67" s="29"/>
-      <c r="L67" s="46"/>
+      <c r="L67" s="51"/>
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="13">
         <v>43910</v>
       </c>
       <c r="B68" s="29"/>
-      <c r="C68" s="39"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="13">
         <v>43910</v>
       </c>
       <c r="E68" s="29"/>
-      <c r="F68" s="39"/>
+      <c r="F68" s="37"/>
       <c r="H68" s="29"/>
-      <c r="I68" s="59"/>
+      <c r="I68" s="44"/>
       <c r="J68" s="22">
         <f t="shared" si="0"/>
         <v>43910</v>
       </c>
       <c r="K68" s="29"/>
-      <c r="L68" s="46"/>
+      <c r="L68" s="51"/>
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="13">
@@ -2281,7 +2284,7 @@
       <c r="B69" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C69" s="32">
+      <c r="C69" s="30">
         <v>4</v>
       </c>
       <c r="D69" s="13">
@@ -2290,48 +2293,48 @@
       <c r="E69" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F69" s="30">
+      <c r="F69" s="57">
         <v>6</v>
       </c>
       <c r="H69" s="29"/>
-      <c r="I69" s="59"/>
+      <c r="I69" s="44"/>
       <c r="J69" s="22">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="K69" s="47" t="s">
+      <c r="K69" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="L69" s="48"/>
+      <c r="L69" s="53"/>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1">
       <c r="A70" s="13">
         <v>43912</v>
       </c>
       <c r="B70" s="29"/>
-      <c r="C70" s="32"/>
+      <c r="C70" s="30"/>
       <c r="D70" s="13">
         <v>43912</v>
       </c>
       <c r="E70" s="29"/>
-      <c r="F70" s="30"/>
+      <c r="F70" s="57"/>
       <c r="H70" s="29"/>
-      <c r="I70" s="59"/>
+      <c r="I70" s="44"/>
       <c r="J70" s="22">
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
-      <c r="K70" s="47"/>
-      <c r="L70" s="48"/>
+      <c r="K70" s="52"/>
+      <c r="L70" s="53"/>
     </row>
     <row r="71" spans="1:12" ht="60">
       <c r="A71" s="13">
         <v>43913</v>
       </c>
-      <c r="B71" s="28" t="s">
+      <c r="B71" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C71" s="25">
+      <c r="C71" s="26">
         <v>2</v>
       </c>
       <c r="D71" s="13">
@@ -2340,19 +2343,19 @@
       <c r="E71" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F71" s="30">
+      <c r="F71" s="57">
         <v>4</v>
       </c>
       <c r="H71" s="29"/>
-      <c r="I71" s="59"/>
+      <c r="I71" s="44"/>
       <c r="J71" s="22">
         <f t="shared" si="0"/>
         <v>43913</v>
       </c>
-      <c r="K71" s="28" t="s">
+      <c r="K71" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="L71" s="28" t="s">
+      <c r="L71" s="25" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2360,34 +2363,34 @@
       <c r="A72" s="13">
         <v>43914</v>
       </c>
-      <c r="B72" s="28" t="s">
+      <c r="B72" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C72" s="25">
+      <c r="C72" s="26">
         <v>3</v>
       </c>
       <c r="D72" s="13">
         <v>43914</v>
       </c>
       <c r="E72" s="29"/>
-      <c r="F72" s="30"/>
+      <c r="F72" s="57"/>
       <c r="G72" s="13">
         <v>43913</v>
       </c>
-      <c r="H72" s="28" t="s">
+      <c r="H72" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I72" s="25">
+      <c r="I72" s="26">
         <v>6</v>
       </c>
       <c r="J72" s="22">
         <f t="shared" si="0"/>
         <v>43914</v>
       </c>
-      <c r="K72" s="28" t="s">
+      <c r="K72" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="L72" s="28" t="s">
+      <c r="L72" s="25" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2395,10 +2398,10 @@
       <c r="A73" s="13">
         <v>43915</v>
       </c>
-      <c r="B73" s="28" t="s">
+      <c r="B73" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C73" s="25">
+      <c r="C73" s="26">
         <v>2</v>
       </c>
       <c r="D73" s="13">
@@ -2407,7 +2410,7 @@
       <c r="E73" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F73" s="30">
+      <c r="F73" s="57">
         <v>6</v>
       </c>
       <c r="G73" s="13">
@@ -2416,15 +2419,15 @@
       <c r="H73" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="I73" s="52"/>
+      <c r="I73" s="36"/>
       <c r="J73" s="22">
         <f t="shared" si="0"/>
         <v>43915</v>
       </c>
-      <c r="K73" s="28" t="s">
+      <c r="K73" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="L73" s="28" t="s">
+      <c r="L73" s="25" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2435,14 +2438,14 @@
       <c r="B74" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="30"/>
+      <c r="C74" s="57"/>
       <c r="D74" s="13">
         <v>43916</v>
       </c>
       <c r="E74" s="29"/>
-      <c r="F74" s="30"/>
+      <c r="F74" s="57"/>
       <c r="H74" s="29"/>
-      <c r="I74" s="52"/>
+      <c r="I74" s="36"/>
       <c r="J74" s="22">
         <f t="shared" si="0"/>
         <v>43916</v>
@@ -2454,31 +2457,31 @@
       <c r="A75" s="13">
         <v>43917</v>
       </c>
-      <c r="B75" s="28" t="s">
+      <c r="B75" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C75" s="25">
+      <c r="C75" s="26">
         <v>2</v>
       </c>
       <c r="D75" s="13">
         <v>43917</v>
       </c>
       <c r="E75" s="29"/>
-      <c r="F75" s="30"/>
+      <c r="F75" s="57"/>
       <c r="G75" s="13">
         <v>43915</v>
       </c>
-      <c r="H75" s="28" t="s">
+      <c r="H75" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="I75" s="25">
+      <c r="I75" s="26">
         <v>3</v>
       </c>
       <c r="J75" s="22">
         <f t="shared" si="0"/>
         <v>43917</v>
       </c>
-      <c r="K75" s="28" t="s">
+      <c r="K75" s="25" t="s">
         <v>36</v>
       </c>
       <c r="L75" s="2"/>
@@ -2487,34 +2490,34 @@
       <c r="A76" s="13">
         <v>43918</v>
       </c>
-      <c r="B76" s="28" t="s">
+      <c r="B76" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="25">
+      <c r="C76" s="26">
         <v>2</v>
       </c>
       <c r="D76" s="13">
         <v>43918</v>
       </c>
       <c r="E76" s="29"/>
-      <c r="F76" s="30"/>
+      <c r="F76" s="57"/>
       <c r="G76" s="13">
         <v>43916</v>
       </c>
-      <c r="H76" s="28" t="s">
+      <c r="H76" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="I76" s="25">
+      <c r="I76" s="26">
         <v>8</v>
       </c>
       <c r="J76" s="22">
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
-      <c r="K76" s="47" t="s">
+      <c r="K76" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="L76" s="49"/>
+      <c r="L76" s="54"/>
     </row>
     <row r="77" spans="1:12" ht="30">
       <c r="A77" s="13">
@@ -2530,27 +2533,27 @@
       <c r="G77" s="13">
         <v>43917</v>
       </c>
-      <c r="H77" s="28" t="s">
+      <c r="H77" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="I77" s="25">
+      <c r="I77" s="26">
         <v>8</v>
       </c>
       <c r="J77" s="22">
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="K77" s="50"/>
-      <c r="L77" s="49"/>
+      <c r="K77" s="55"/>
+      <c r="L77" s="54"/>
     </row>
     <row r="78" spans="1:12" ht="30">
       <c r="A78" s="13">
         <v>43920</v>
       </c>
-      <c r="B78" s="28" t="s">
+      <c r="B78" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C78" s="25">
+      <c r="C78" s="26">
         <v>2</v>
       </c>
       <c r="D78" s="13">
@@ -2559,26 +2562,26 @@
       <c r="E78" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F78" s="30">
+      <c r="F78" s="57">
         <v>4</v>
       </c>
       <c r="G78" s="13">
         <v>43918</v>
       </c>
-      <c r="H78" s="28" t="s">
+      <c r="H78" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I78" s="25">
+      <c r="I78" s="26">
         <v>8</v>
       </c>
       <c r="J78" s="22">
         <f t="shared" si="0"/>
         <v>43920</v>
       </c>
-      <c r="K78" s="28" t="s">
+      <c r="K78" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="L78" s="28" t="s">
+      <c r="L78" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2589,31 +2592,31 @@
       <c r="B79" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C79" s="32">
+      <c r="C79" s="30">
         <v>4</v>
       </c>
       <c r="D79" s="13">
         <v>43921</v>
       </c>
       <c r="E79" s="29"/>
-      <c r="F79" s="30"/>
+      <c r="F79" s="57"/>
       <c r="G79" s="13">
         <v>43919</v>
       </c>
-      <c r="H79" s="28" t="s">
+      <c r="H79" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I79" s="25">
+      <c r="I79" s="26">
         <v>8</v>
       </c>
       <c r="J79" s="22">
         <f t="shared" si="0"/>
         <v>43921</v>
       </c>
-      <c r="K79" s="28" t="s">
+      <c r="K79" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="L79" s="28" t="s">
+      <c r="L79" s="25" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2622,51 +2625,51 @@
         <v>43922</v>
       </c>
       <c r="B80" s="29"/>
-      <c r="C80" s="32"/>
+      <c r="C80" s="30"/>
       <c r="D80" s="13">
         <v>43922</v>
       </c>
       <c r="E80" s="29"/>
-      <c r="F80" s="30"/>
+      <c r="F80" s="57"/>
       <c r="G80" s="13">
         <v>43920</v>
       </c>
-      <c r="H80" s="28" t="s">
+      <c r="H80" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="I80" s="25">
+      <c r="I80" s="26">
         <v>6</v>
       </c>
       <c r="J80" s="22">
         <f t="shared" si="0"/>
         <v>43922</v>
       </c>
-      <c r="K80" s="26" t="s">
+      <c r="K80" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="L80" s="26"/>
+      <c r="L80" s="28"/>
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="13">
         <v>43923</v>
       </c>
       <c r="B81" s="29"/>
-      <c r="C81" s="32"/>
+      <c r="C81" s="30"/>
       <c r="D81" s="13">
         <v>43923</v>
       </c>
       <c r="E81" s="29"/>
-      <c r="F81" s="30"/>
+      <c r="F81" s="57"/>
       <c r="H81" s="20"/>
       <c r="I81" s="20"/>
       <c r="J81" s="22">
         <f t="shared" si="0"/>
         <v>43923</v>
       </c>
-      <c r="K81" s="32" t="s">
+      <c r="K81" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="L81" s="32" t="s">
+      <c r="L81" s="30" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2674,10 +2677,10 @@
       <c r="A82" s="13">
         <v>43924</v>
       </c>
-      <c r="B82" s="28" t="s">
+      <c r="B82" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C82" s="25">
+      <c r="C82" s="26">
         <v>3</v>
       </c>
       <c r="D82" s="13">
@@ -2686,7 +2689,7 @@
       <c r="E82" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F82" s="30">
+      <c r="F82" s="57">
         <v>3</v>
       </c>
       <c r="H82" s="20"/>
@@ -2695,8 +2698,8 @@
         <f t="shared" si="0"/>
         <v>43924</v>
       </c>
-      <c r="K82" s="32"/>
-      <c r="L82" s="32"/>
+      <c r="K82" s="30"/>
+      <c r="L82" s="30"/>
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="13">
@@ -2708,17 +2711,17 @@
         <v>43925</v>
       </c>
       <c r="E83" s="29"/>
-      <c r="F83" s="30"/>
+      <c r="F83" s="57"/>
       <c r="H83" s="20"/>
       <c r="I83" s="20"/>
       <c r="J83" s="22">
         <f t="shared" si="0"/>
         <v>43925</v>
       </c>
-      <c r="K83" s="51" t="s">
+      <c r="K83" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="L83" s="51"/>
+      <c r="L83" s="31"/>
     </row>
     <row r="84" spans="1:12" ht="30" customHeight="1">
       <c r="A84" s="13">
@@ -2741,17 +2744,17 @@
         <f t="shared" si="0"/>
         <v>43926</v>
       </c>
-      <c r="K84" s="51"/>
-      <c r="L84" s="51"/>
+      <c r="K84" s="31"/>
+      <c r="L84" s="31"/>
     </row>
     <row r="85" spans="1:12" ht="53.25" customHeight="1">
       <c r="A85" s="13">
         <v>43927</v>
       </c>
-      <c r="B85" s="34" t="s">
+      <c r="B85" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="C85" s="32">
+      <c r="C85" s="30">
         <v>12</v>
       </c>
       <c r="D85" s="13">
@@ -2760,7 +2763,7 @@
       <c r="E85" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F85" s="30">
+      <c r="F85" s="57">
         <v>6</v>
       </c>
       <c r="H85" s="20"/>
@@ -2769,10 +2772,10 @@
         <f t="shared" si="0"/>
         <v>43927</v>
       </c>
-      <c r="K85" s="28" t="s">
+      <c r="K85" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="L85" s="25" t="s">
+      <c r="L85" s="26" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2780,23 +2783,23 @@
       <c r="A86" s="13">
         <v>43928</v>
       </c>
-      <c r="B86" s="34"/>
-      <c r="C86" s="32"/>
+      <c r="B86" s="56"/>
+      <c r="C86" s="30"/>
       <c r="D86" s="13">
         <v>43928</v>
       </c>
       <c r="E86" s="29"/>
-      <c r="F86" s="30"/>
+      <c r="F86" s="57"/>
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
       <c r="J86" s="22">
         <f>J85+1</f>
         <v>43928</v>
       </c>
-      <c r="K86" s="28" t="s">
+      <c r="K86" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="L86" s="25" t="s">
+      <c r="L86" s="26" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2804,23 +2807,23 @@
       <c r="A87" s="13">
         <v>43929</v>
       </c>
-      <c r="B87" s="34"/>
-      <c r="C87" s="32"/>
+      <c r="B87" s="56"/>
+      <c r="C87" s="30"/>
       <c r="D87" s="13">
         <v>43929</v>
       </c>
       <c r="E87" s="29"/>
-      <c r="F87" s="30"/>
+      <c r="F87" s="57"/>
       <c r="H87" s="20"/>
       <c r="I87" s="20"/>
       <c r="J87" s="22">
         <f t="shared" si="0"/>
         <v>43929</v>
       </c>
-      <c r="K87" s="28" t="s">
+      <c r="K87" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="L87" s="25" t="s">
+      <c r="L87" s="26" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2828,15 +2831,15 @@
       <c r="A88" s="21">
         <v>43930</v>
       </c>
-      <c r="B88" s="34"/>
-      <c r="C88" s="32"/>
+      <c r="B88" s="56"/>
+      <c r="C88" s="30"/>
       <c r="D88" s="13">
         <v>43930</v>
       </c>
       <c r="E88" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F88" s="30">
+      <c r="F88" s="57">
         <v>4</v>
       </c>
       <c r="H88" s="20"/>
@@ -2845,10 +2848,10 @@
         <f t="shared" si="0"/>
         <v>43930</v>
       </c>
-      <c r="K88" s="28" t="s">
+      <c r="K88" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="L88" s="25" t="s">
+      <c r="L88" s="26" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2856,23 +2859,23 @@
       <c r="A89" s="21">
         <v>43931</v>
       </c>
-      <c r="B89" s="34"/>
-      <c r="C89" s="32"/>
+      <c r="B89" s="56"/>
+      <c r="C89" s="30"/>
       <c r="D89" s="13">
         <v>43931</v>
       </c>
       <c r="E89" s="29"/>
-      <c r="F89" s="30"/>
+      <c r="F89" s="57"/>
       <c r="H89" s="20"/>
       <c r="I89" s="20"/>
       <c r="J89" s="22">
         <f t="shared" si="0"/>
         <v>43931</v>
       </c>
-      <c r="K89" s="25" t="s">
+      <c r="K89" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="L89" s="25" t="s">
+      <c r="L89" s="26" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2880,23 +2883,23 @@
       <c r="A90" s="21">
         <v>43932</v>
       </c>
-      <c r="B90" s="34"/>
-      <c r="C90" s="32"/>
+      <c r="B90" s="56"/>
+      <c r="C90" s="30"/>
       <c r="D90" s="13">
         <v>43932</v>
       </c>
       <c r="E90" s="29"/>
-      <c r="F90" s="30"/>
+      <c r="F90" s="57"/>
       <c r="H90" s="20"/>
       <c r="I90" s="20"/>
       <c r="J90" s="22">
         <f t="shared" si="0"/>
         <v>43932</v>
       </c>
-      <c r="K90" s="25" t="s">
+      <c r="K90" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="L90" s="25" t="s">
+      <c r="L90" s="26" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2917,10 +2920,10 @@
         <f t="shared" si="0"/>
         <v>43933</v>
       </c>
-      <c r="K91" s="31" t="s">
+      <c r="K91" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="L91" s="31"/>
+      <c r="L91" s="59"/>
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="13">
@@ -2929,7 +2932,7 @@
       <c r="B92" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C92" s="32">
+      <c r="C92" s="30">
         <v>4</v>
       </c>
       <c r="D92" s="13">
@@ -2944,84 +2947,84 @@
         <f t="shared" si="0"/>
         <v>43934</v>
       </c>
-      <c r="K92" s="31"/>
-      <c r="L92" s="31"/>
+      <c r="K92" s="59"/>
+      <c r="L92" s="59"/>
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="13">
         <v>43935</v>
       </c>
       <c r="B93" s="29"/>
-      <c r="C93" s="32"/>
+      <c r="C93" s="30"/>
       <c r="D93" s="13">
         <v>43935</v>
       </c>
-      <c r="E93" s="33"/>
+      <c r="E93" s="58"/>
       <c r="H93" s="20"/>
       <c r="I93" s="20"/>
       <c r="J93" s="22">
         <f t="shared" si="0"/>
         <v>43935</v>
       </c>
-      <c r="K93" s="31"/>
-      <c r="L93" s="31"/>
+      <c r="K93" s="59"/>
+      <c r="L93" s="59"/>
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="13">
         <v>43936</v>
       </c>
       <c r="B94" s="29"/>
-      <c r="C94" s="32"/>
+      <c r="C94" s="30"/>
       <c r="D94" s="13">
         <v>43936</v>
       </c>
-      <c r="E94" s="33"/>
+      <c r="E94" s="58"/>
       <c r="H94" s="20"/>
       <c r="I94" s="20"/>
       <c r="J94" s="22">
         <f t="shared" si="0"/>
         <v>43936</v>
       </c>
-      <c r="K94" s="31"/>
-      <c r="L94" s="31"/>
+      <c r="K94" s="59"/>
+      <c r="L94" s="59"/>
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="13">
         <v>43937</v>
       </c>
       <c r="B95" s="29"/>
-      <c r="C95" s="32"/>
+      <c r="C95" s="30"/>
       <c r="D95" s="13">
         <v>43937</v>
       </c>
-      <c r="E95" s="33"/>
+      <c r="E95" s="58"/>
       <c r="H95" s="20"/>
       <c r="I95" s="20"/>
       <c r="J95" s="22">
         <f t="shared" si="0"/>
         <v>43937</v>
       </c>
-      <c r="K95" s="31"/>
-      <c r="L95" s="31"/>
+      <c r="K95" s="59"/>
+      <c r="L95" s="59"/>
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="13">
         <v>43938</v>
       </c>
       <c r="B96" s="29"/>
-      <c r="C96" s="32"/>
+      <c r="C96" s="30"/>
       <c r="D96" s="13">
         <v>43938</v>
       </c>
-      <c r="E96" s="33"/>
+      <c r="E96" s="58"/>
       <c r="H96" s="20"/>
       <c r="I96" s="20"/>
       <c r="J96" s="22">
         <f t="shared" si="0"/>
         <v>43938</v>
       </c>
-      <c r="K96" s="31"/>
-      <c r="L96" s="31"/>
+      <c r="K96" s="59"/>
+      <c r="L96" s="59"/>
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="13">
@@ -3032,15 +3035,15 @@
       <c r="D97" s="13">
         <v>43939</v>
       </c>
-      <c r="E97" s="33"/>
+      <c r="E97" s="58"/>
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
       <c r="J97" s="22">
         <f t="shared" si="0"/>
         <v>43939</v>
       </c>
-      <c r="K97" s="31"/>
-      <c r="L97" s="31"/>
+      <c r="K97" s="59"/>
+      <c r="L97" s="59"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="13">
@@ -3051,15 +3054,15 @@
       <c r="D98" s="13">
         <v>43940</v>
       </c>
-      <c r="E98" s="33"/>
+      <c r="E98" s="58"/>
       <c r="H98" s="20"/>
       <c r="I98" s="20"/>
       <c r="J98" s="22">
         <f t="shared" si="0"/>
         <v>43940</v>
       </c>
-      <c r="K98" s="31"/>
-      <c r="L98" s="31"/>
+      <c r="K98" s="59"/>
+      <c r="L98" s="59"/>
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="13">
@@ -3068,69 +3071,69 @@
       <c r="B99" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C99" s="32">
+      <c r="C99" s="30">
         <v>4</v>
       </c>
       <c r="D99" s="13">
         <v>43941</v>
       </c>
-      <c r="E99" s="33"/>
+      <c r="E99" s="58"/>
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
       <c r="J99" s="22">
         <f t="shared" si="0"/>
         <v>43941</v>
       </c>
-      <c r="K99" s="31"/>
-      <c r="L99" s="31"/>
+      <c r="K99" s="59"/>
+      <c r="L99" s="59"/>
     </row>
     <row r="100" spans="1:12" ht="30" customHeight="1">
       <c r="A100" s="13">
         <v>43942</v>
       </c>
       <c r="B100" s="29"/>
-      <c r="C100" s="32"/>
+      <c r="C100" s="30"/>
       <c r="D100" s="13">
         <v>43942</v>
       </c>
-      <c r="E100" s="33"/>
+      <c r="E100" s="58"/>
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
       <c r="J100" s="22">
         <f t="shared" si="0"/>
         <v>43942</v>
       </c>
-      <c r="K100" s="31"/>
-      <c r="L100" s="31"/>
+      <c r="K100" s="59"/>
+      <c r="L100" s="59"/>
     </row>
     <row r="101" spans="1:12" ht="15" customHeight="1">
       <c r="A101" s="13">
         <v>43943</v>
       </c>
       <c r="B101" s="29"/>
-      <c r="C101" s="32"/>
+      <c r="C101" s="30"/>
       <c r="D101" s="13">
         <v>43943</v>
       </c>
       <c r="E101" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="F101" s="30">
+      <c r="F101" s="57">
         <v>3</v>
       </c>
       <c r="G101" s="13">
         <v>43943</v>
       </c>
-      <c r="H101" s="25" t="s">
+      <c r="H101" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="I101" s="26"/>
+      <c r="I101" s="28"/>
       <c r="J101" s="22">
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="K101" s="31"/>
-      <c r="L101" s="31"/>
+      <c r="K101" s="59"/>
+      <c r="L101" s="59"/>
     </row>
     <row r="102" spans="1:12" ht="27.75" customHeight="1">
       <c r="A102" s="13">
@@ -3139,56 +3142,56 @@
       <c r="B102" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C102" s="32">
+      <c r="C102" s="30">
         <v>2</v>
       </c>
       <c r="D102" s="13">
         <v>43944</v>
       </c>
       <c r="E102" s="29"/>
-      <c r="F102" s="30"/>
+      <c r="F102" s="57"/>
       <c r="G102" s="13">
         <v>43944</v>
       </c>
-      <c r="H102" s="25" t="s">
+      <c r="H102" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="I102" s="26"/>
+      <c r="I102" s="28"/>
       <c r="J102" s="22">
         <f t="shared" si="0"/>
         <v>43944</v>
       </c>
-      <c r="K102" s="31"/>
-      <c r="L102" s="31"/>
+      <c r="K102" s="59"/>
+      <c r="L102" s="59"/>
     </row>
     <row r="103" spans="1:12" ht="41.25" customHeight="1">
       <c r="A103" s="13">
         <v>43945</v>
       </c>
       <c r="B103" s="29"/>
-      <c r="C103" s="32"/>
+      <c r="C103" s="30"/>
       <c r="D103" s="13">
         <v>43945</v>
       </c>
-      <c r="E103" s="28" t="s">
+      <c r="E103" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="F103" s="28">
+      <c r="F103" s="25">
         <v>2</v>
       </c>
       <c r="G103" s="13">
         <v>43945</v>
       </c>
-      <c r="H103" s="25" t="s">
+      <c r="H103" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="I103" s="26"/>
+      <c r="I103" s="28"/>
       <c r="J103" s="22">
         <f t="shared" si="0"/>
         <v>43945</v>
       </c>
-      <c r="K103" s="31"/>
-      <c r="L103" s="31"/>
+      <c r="K103" s="59"/>
+      <c r="L103" s="59"/>
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="13">
@@ -3204,14 +3207,14 @@
       <c r="G104" s="13">
         <v>43946</v>
       </c>
-      <c r="H104" s="26"/>
-      <c r="I104" s="26"/>
+      <c r="H104" s="28"/>
+      <c r="I104" s="28"/>
       <c r="J104" s="22">
         <f t="shared" si="0"/>
         <v>43946</v>
       </c>
-      <c r="K104" s="31"/>
-      <c r="L104" s="31"/>
+      <c r="K104" s="59"/>
+      <c r="L104" s="59"/>
     </row>
     <row r="105" spans="1:12">
       <c r="A105" s="13">
@@ -3227,16 +3230,16 @@
       <c r="G105" s="13">
         <v>43947</v>
       </c>
-      <c r="H105" s="26"/>
-      <c r="I105" s="26"/>
+      <c r="H105" s="28"/>
+      <c r="I105" s="28"/>
       <c r="J105" s="22">
         <f t="shared" si="0"/>
         <v>43947</v>
       </c>
-      <c r="K105" s="30" t="s">
+      <c r="K105" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="L105" s="32" t="s">
+      <c r="L105" s="30" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3244,10 +3247,10 @@
       <c r="A106" s="13">
         <v>43948</v>
       </c>
-      <c r="B106" s="28" t="s">
+      <c r="B106" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C106" s="25">
+      <c r="C106" s="26">
         <v>4</v>
       </c>
       <c r="D106" s="13">
@@ -3256,20 +3259,20 @@
       <c r="E106" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="F106" s="30">
+      <c r="F106" s="57">
         <v>3</v>
       </c>
       <c r="G106" s="13">
         <v>43948</v>
       </c>
-      <c r="H106" s="26"/>
-      <c r="I106" s="26"/>
+      <c r="H106" s="28"/>
+      <c r="I106" s="28"/>
       <c r="J106" s="22">
         <f t="shared" si="0"/>
         <v>43948</v>
       </c>
-      <c r="K106" s="30"/>
-      <c r="L106" s="32"/>
+      <c r="K106" s="57"/>
+      <c r="L106" s="30"/>
     </row>
     <row r="107" spans="1:12">
       <c r="A107" s="13">
@@ -3278,27 +3281,27 @@
       <c r="B107" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C107" s="32">
+      <c r="C107" s="30">
         <v>3</v>
       </c>
       <c r="D107" s="13">
         <v>43949</v>
       </c>
       <c r="E107" s="29"/>
-      <c r="F107" s="30"/>
+      <c r="F107" s="57"/>
       <c r="G107" s="13">
         <v>43949</v>
       </c>
-      <c r="H107" s="26"/>
-      <c r="I107" s="26"/>
+      <c r="H107" s="28"/>
+      <c r="I107" s="28"/>
       <c r="J107" s="22">
         <f t="shared" si="0"/>
         <v>43949</v>
       </c>
-      <c r="K107" s="25" t="s">
+      <c r="K107" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="L107" s="25" t="s">
+      <c r="L107" s="26" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3307,29 +3310,29 @@
         <v>43950</v>
       </c>
       <c r="B108" s="29"/>
-      <c r="C108" s="32"/>
+      <c r="C108" s="30"/>
       <c r="D108" s="13">
         <v>43950</v>
       </c>
       <c r="E108" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="F108" s="30">
+      <c r="F108" s="57">
         <v>3</v>
       </c>
       <c r="G108" s="13">
         <v>43950</v>
       </c>
-      <c r="H108" s="26"/>
-      <c r="I108" s="26"/>
+      <c r="H108" s="28"/>
+      <c r="I108" s="28"/>
       <c r="J108" s="22">
         <f t="shared" si="0"/>
         <v>43950</v>
       </c>
-      <c r="K108" s="28" t="s">
+      <c r="K108" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="L108" s="25" t="s">
+      <c r="L108" s="26" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3337,18 +3340,18 @@
       <c r="A109" s="13">
         <v>43951</v>
       </c>
-      <c r="B109" s="28"/>
-      <c r="C109" s="25"/>
+      <c r="B109" s="25"/>
+      <c r="C109" s="26"/>
       <c r="D109" s="13">
         <v>43951</v>
       </c>
       <c r="E109" s="29"/>
-      <c r="F109" s="30"/>
+      <c r="F109" s="57"/>
       <c r="G109" s="13">
         <v>43951</v>
       </c>
-      <c r="H109" s="25"/>
-      <c r="I109" s="26"/>
+      <c r="H109" s="26"/>
+      <c r="I109" s="28"/>
       <c r="J109" s="22">
         <f t="shared" si="0"/>
         <v>43951</v>
@@ -3362,22 +3365,22 @@
       <c r="A110" s="13">
         <v>43952</v>
       </c>
-      <c r="B110" s="28"/>
-      <c r="C110" s="25"/>
+      <c r="B110" s="25"/>
+      <c r="C110" s="26"/>
       <c r="D110" s="13">
         <v>43952</v>
       </c>
       <c r="E110" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="F110" s="30">
+      <c r="F110" s="57">
         <v>2</v>
       </c>
       <c r="G110" s="13">
         <v>43952</v>
       </c>
-      <c r="H110" s="25"/>
-      <c r="I110" s="26"/>
+      <c r="H110" s="26"/>
+      <c r="I110" s="28"/>
       <c r="J110" s="22">
         <f t="shared" si="0"/>
         <v>43952</v>
@@ -3389,20 +3392,20 @@
       <c r="A111" s="13">
         <v>43953</v>
       </c>
-      <c r="B111" s="28"/>
-      <c r="C111" s="25"/>
+      <c r="B111" s="25"/>
+      <c r="C111" s="26"/>
       <c r="D111" s="13">
         <v>43953</v>
       </c>
       <c r="E111" s="29"/>
-      <c r="F111" s="30"/>
+      <c r="F111" s="57"/>
       <c r="G111" s="13">
         <v>43953</v>
       </c>
-      <c r="H111" s="25" t="s">
+      <c r="H111" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="I111" s="26">
+      <c r="I111" s="28">
         <v>6</v>
       </c>
       <c r="J111" s="22">
@@ -3416,8 +3419,8 @@
       <c r="A112" s="13">
         <v>43954</v>
       </c>
-      <c r="B112" s="28"/>
-      <c r="C112" s="25"/>
+      <c r="B112" s="25"/>
+      <c r="C112" s="26"/>
       <c r="D112" s="13">
         <v>43954</v>
       </c>
@@ -3426,18 +3429,18 @@
       <c r="G112" s="13">
         <v>43954</v>
       </c>
-      <c r="H112" s="25" t="s">
+      <c r="H112" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="I112" s="26"/>
+      <c r="I112" s="28"/>
       <c r="J112" s="22">
         <f t="shared" si="0"/>
         <v>43954</v>
       </c>
-      <c r="K112" s="25" t="s">
+      <c r="K112" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="L112" s="25" t="s">
+      <c r="L112" s="26" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3445,24 +3448,24 @@
       <c r="A113" s="13">
         <v>43955</v>
       </c>
-      <c r="B113" s="28"/>
-      <c r="C113" s="25"/>
+      <c r="B113" s="25"/>
+      <c r="C113" s="26"/>
       <c r="D113" s="13">
         <v>43955</v>
       </c>
       <c r="G113" s="13">
         <v>43955</v>
       </c>
-      <c r="H113" s="26"/>
-      <c r="I113" s="26"/>
+      <c r="H113" s="28"/>
+      <c r="I113" s="28"/>
       <c r="J113" s="22">
         <f t="shared" si="0"/>
         <v>43955</v>
       </c>
-      <c r="K113" s="25" t="s">
+      <c r="K113" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="L113" s="25" t="s">
+      <c r="L113" s="26" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3470,331 +3473,335 @@
       <c r="A114" s="13">
         <v>43956</v>
       </c>
-      <c r="B114" s="28"/>
-      <c r="C114" s="25"/>
+      <c r="B114" s="25"/>
+      <c r="C114" s="26"/>
       <c r="D114" s="13">
         <v>43956</v>
       </c>
       <c r="G114" s="13">
         <v>43956</v>
       </c>
-      <c r="H114" s="26"/>
-      <c r="I114" s="26"/>
+      <c r="H114" s="28"/>
+      <c r="I114" s="28"/>
       <c r="J114" s="22">
         <f t="shared" si="0"/>
         <v>43956</v>
       </c>
-      <c r="K114" s="26"/>
-      <c r="L114" s="26"/>
+      <c r="K114" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="L114" s="26" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="115" spans="1:12">
       <c r="A115" s="13">
         <v>43957</v>
       </c>
-      <c r="B115" s="28"/>
-      <c r="C115" s="25"/>
+      <c r="B115" s="25"/>
+      <c r="C115" s="26"/>
       <c r="D115" s="13">
         <v>43957</v>
       </c>
       <c r="G115" s="13">
         <v>43957</v>
       </c>
-      <c r="H115" s="26"/>
-      <c r="I115" s="26"/>
+      <c r="H115" s="28"/>
+      <c r="I115" s="28"/>
       <c r="J115" s="22">
         <f>J114+1</f>
         <v>43957</v>
       </c>
-      <c r="K115" s="26"/>
-      <c r="L115" s="26"/>
+      <c r="K115" s="28"/>
+      <c r="L115" s="28"/>
     </row>
     <row r="116" spans="1:12">
       <c r="A116" s="13">
         <v>43958</v>
       </c>
-      <c r="B116" s="28"/>
-      <c r="C116" s="25"/>
+      <c r="B116" s="25"/>
+      <c r="C116" s="26"/>
       <c r="D116" s="13">
         <v>43958</v>
       </c>
       <c r="G116" s="13">
         <v>43958</v>
       </c>
-      <c r="H116" s="26"/>
-      <c r="I116" s="26"/>
+      <c r="H116" s="28"/>
+      <c r="I116" s="28"/>
       <c r="J116" s="22">
         <f t="shared" si="0"/>
         <v>43958</v>
       </c>
-      <c r="K116" s="26"/>
-      <c r="L116" s="26"/>
+      <c r="K116" s="28"/>
+      <c r="L116" s="28"/>
     </row>
     <row r="117" spans="1:12">
       <c r="A117" s="13">
         <v>43959</v>
       </c>
-      <c r="B117" s="28"/>
-      <c r="C117" s="25"/>
+      <c r="B117" s="25"/>
+      <c r="C117" s="26"/>
       <c r="D117" s="13">
         <v>43959</v>
       </c>
       <c r="G117" s="13">
         <v>43959</v>
       </c>
-      <c r="H117" s="26"/>
-      <c r="I117" s="26"/>
+      <c r="H117" s="28"/>
+      <c r="I117" s="28"/>
       <c r="J117" s="22">
         <f t="shared" si="0"/>
         <v>43959</v>
       </c>
-      <c r="K117" s="26"/>
-      <c r="L117" s="26"/>
+      <c r="K117" s="28"/>
+      <c r="L117" s="28"/>
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="13">
         <v>43960</v>
       </c>
-      <c r="B118" s="28"/>
-      <c r="C118" s="25"/>
+      <c r="B118" s="25"/>
+      <c r="C118" s="26"/>
       <c r="D118" s="13">
         <v>43960</v>
       </c>
       <c r="G118" s="13">
         <v>43960</v>
       </c>
-      <c r="H118" s="26"/>
-      <c r="I118" s="26"/>
+      <c r="H118" s="28"/>
+      <c r="I118" s="28"/>
       <c r="J118" s="22">
         <f t="shared" si="0"/>
         <v>43960</v>
       </c>
-      <c r="K118" s="26"/>
-      <c r="L118" s="26"/>
+      <c r="K118" s="28"/>
+      <c r="L118" s="28"/>
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="13">
         <v>43961</v>
       </c>
-      <c r="B119" s="28"/>
-      <c r="C119" s="25"/>
+      <c r="B119" s="25"/>
+      <c r="C119" s="26"/>
       <c r="D119" s="13">
         <v>43961</v>
       </c>
       <c r="G119" s="13">
         <v>43961</v>
       </c>
-      <c r="H119" s="26"/>
-      <c r="I119" s="26"/>
+      <c r="H119" s="28"/>
+      <c r="I119" s="28"/>
       <c r="J119" s="22">
         <f t="shared" si="0"/>
         <v>43961</v>
       </c>
-      <c r="K119" s="26"/>
-      <c r="L119" s="26"/>
+      <c r="K119" s="28"/>
+      <c r="L119" s="28"/>
     </row>
     <row r="120" spans="1:12">
       <c r="A120" s="13">
         <v>43962</v>
       </c>
-      <c r="B120" s="28"/>
-      <c r="C120" s="25"/>
+      <c r="B120" s="25"/>
+      <c r="C120" s="26"/>
       <c r="D120" s="13">
         <v>43962</v>
       </c>
       <c r="G120" s="13">
         <v>43962</v>
       </c>
-      <c r="H120" s="26"/>
-      <c r="I120" s="26"/>
+      <c r="H120" s="28"/>
+      <c r="I120" s="28"/>
       <c r="J120" s="22">
         <f t="shared" si="0"/>
         <v>43962</v>
       </c>
-      <c r="K120" s="26"/>
-      <c r="L120" s="26"/>
+      <c r="K120" s="28"/>
+      <c r="L120" s="28"/>
     </row>
     <row r="121" spans="1:12">
       <c r="A121" s="13">
         <v>43963</v>
       </c>
-      <c r="B121" s="28"/>
-      <c r="C121" s="25"/>
+      <c r="B121" s="25"/>
+      <c r="C121" s="26"/>
       <c r="D121" s="13">
         <v>43963</v>
       </c>
       <c r="G121" s="13">
         <v>43963</v>
       </c>
-      <c r="H121" s="26"/>
-      <c r="I121" s="26"/>
+      <c r="H121" s="28"/>
+      <c r="I121" s="28"/>
       <c r="J121" s="22">
         <f t="shared" si="0"/>
         <v>43963</v>
       </c>
-      <c r="K121" s="26"/>
-      <c r="L121" s="26"/>
+      <c r="K121" s="28"/>
+      <c r="L121" s="28"/>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="13">
         <v>43964</v>
       </c>
-      <c r="B122" s="28"/>
-      <c r="C122" s="25"/>
+      <c r="B122" s="25"/>
+      <c r="C122" s="26"/>
       <c r="D122" s="13">
         <v>43964</v>
       </c>
       <c r="G122" s="13">
         <v>43964</v>
       </c>
-      <c r="H122" s="26"/>
-      <c r="I122" s="26"/>
+      <c r="H122" s="28"/>
+      <c r="I122" s="28"/>
       <c r="J122" s="22">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-      <c r="K122" s="26"/>
-      <c r="L122" s="26"/>
+      <c r="K122" s="28"/>
+      <c r="L122" s="28"/>
     </row>
     <row r="123" spans="1:12">
       <c r="A123" s="13">
         <v>43965</v>
       </c>
-      <c r="B123" s="28"/>
-      <c r="C123" s="25"/>
+      <c r="B123" s="25"/>
+      <c r="C123" s="26"/>
       <c r="D123" s="13">
         <v>43965</v>
       </c>
       <c r="G123" s="13">
         <v>43965</v>
       </c>
-      <c r="H123" s="26"/>
-      <c r="I123" s="26"/>
+      <c r="H123" s="28"/>
+      <c r="I123" s="28"/>
       <c r="J123" s="22">
         <f>J122+1</f>
         <v>43965</v>
       </c>
-      <c r="K123" s="26"/>
-      <c r="L123" s="26"/>
+      <c r="K123" s="28"/>
+      <c r="L123" s="28"/>
     </row>
     <row r="124" spans="1:12">
       <c r="A124" s="13">
         <v>43966</v>
       </c>
-      <c r="B124" s="28"/>
-      <c r="C124" s="25"/>
+      <c r="B124" s="25"/>
+      <c r="C124" s="26"/>
       <c r="D124" s="13">
         <v>43966</v>
       </c>
       <c r="G124" s="13">
         <v>43966</v>
       </c>
-      <c r="H124" s="26"/>
-      <c r="I124" s="26"/>
+      <c r="H124" s="28"/>
+      <c r="I124" s="28"/>
       <c r="J124" s="22">
         <f t="shared" si="0"/>
         <v>43966</v>
       </c>
-      <c r="K124" s="26"/>
-      <c r="L124" s="26"/>
+      <c r="K124" s="28"/>
+      <c r="L124" s="28"/>
     </row>
     <row r="125" spans="1:12">
       <c r="A125" s="13">
         <v>43967</v>
       </c>
-      <c r="B125" s="28"/>
-      <c r="C125" s="25"/>
+      <c r="B125" s="25"/>
+      <c r="C125" s="26"/>
       <c r="D125" s="13">
         <v>43967</v>
       </c>
       <c r="G125" s="13">
         <v>43967</v>
       </c>
-      <c r="H125" s="26"/>
-      <c r="I125" s="26"/>
+      <c r="H125" s="28"/>
+      <c r="I125" s="28"/>
       <c r="J125" s="22">
         <f t="shared" si="0"/>
         <v>43967</v>
       </c>
-      <c r="K125" s="26"/>
-      <c r="L125" s="26"/>
+      <c r="K125" s="28"/>
+      <c r="L125" s="28"/>
     </row>
     <row r="126" spans="1:12">
       <c r="A126" s="13">
         <v>43968</v>
       </c>
-      <c r="B126" s="28"/>
-      <c r="C126" s="25"/>
+      <c r="B126" s="25"/>
+      <c r="C126" s="26"/>
       <c r="D126" s="13">
         <v>43968</v>
       </c>
       <c r="G126" s="13">
         <v>43968</v>
       </c>
-      <c r="H126" s="26"/>
-      <c r="I126" s="26"/>
+      <c r="H126" s="28"/>
+      <c r="I126" s="28"/>
       <c r="J126" s="22">
         <f t="shared" si="0"/>
         <v>43968</v>
       </c>
-      <c r="K126" s="26"/>
-      <c r="L126" s="26"/>
+      <c r="K126" s="28"/>
+      <c r="L126" s="28"/>
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="13">
         <v>43969</v>
       </c>
-      <c r="B127" s="28"/>
-      <c r="C127" s="25"/>
+      <c r="B127" s="25"/>
+      <c r="C127" s="26"/>
       <c r="D127" s="13">
         <v>43969</v>
       </c>
       <c r="G127" s="13">
         <v>43969</v>
       </c>
-      <c r="H127" s="26"/>
-      <c r="I127" s="26"/>
+      <c r="H127" s="28"/>
+      <c r="I127" s="28"/>
       <c r="J127" s="22">
         <f t="shared" si="0"/>
         <v>43969</v>
       </c>
-      <c r="K127" s="26"/>
-      <c r="L127" s="26"/>
+      <c r="K127" s="28"/>
+      <c r="L127" s="28"/>
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="13">
         <v>43970</v>
       </c>
-      <c r="B128" s="28"/>
-      <c r="C128" s="25"/>
+      <c r="B128" s="25"/>
+      <c r="C128" s="26"/>
       <c r="D128" s="13">
         <v>43970</v>
       </c>
       <c r="G128" s="13">
         <v>43970</v>
       </c>
-      <c r="H128" s="26"/>
-      <c r="I128" s="26"/>
+      <c r="H128" s="28"/>
+      <c r="I128" s="28"/>
       <c r="J128" s="22">
         <f t="shared" si="0"/>
         <v>43970</v>
       </c>
-      <c r="K128" s="26"/>
-      <c r="L128" s="26"/>
+      <c r="K128" s="28"/>
+      <c r="L128" s="28"/>
     </row>
     <row r="129" spans="1:10">
       <c r="A129" s="13">
         <v>43971</v>
       </c>
-      <c r="B129" s="28"/>
-      <c r="C129" s="25"/>
+      <c r="B129" s="25"/>
+      <c r="C129" s="26"/>
       <c r="D129" s="13">
         <v>43971</v>
       </c>
       <c r="G129" s="13">
         <v>43971</v>
       </c>
-      <c r="H129" s="26"/>
-      <c r="I129" s="26"/>
+      <c r="H129" s="28"/>
+      <c r="I129" s="28"/>
       <c r="J129" s="22">
         <f t="shared" si="0"/>
         <v>43971</v>
@@ -3804,16 +3811,16 @@
       <c r="A130" s="13">
         <v>43972</v>
       </c>
-      <c r="B130" s="28"/>
-      <c r="C130" s="25"/>
+      <c r="B130" s="25"/>
+      <c r="C130" s="26"/>
       <c r="D130" s="13">
         <v>43972</v>
       </c>
       <c r="G130" s="13">
         <v>43972</v>
       </c>
-      <c r="H130" s="26"/>
-      <c r="I130" s="26"/>
+      <c r="H130" s="28"/>
+      <c r="I130" s="28"/>
       <c r="J130" s="22">
         <f t="shared" ref="J130:J160" si="1">J129+1</f>
         <v>43972</v>
@@ -3823,16 +3830,16 @@
       <c r="A131" s="13">
         <v>43973</v>
       </c>
-      <c r="B131" s="28"/>
-      <c r="C131" s="25"/>
+      <c r="B131" s="25"/>
+      <c r="C131" s="26"/>
       <c r="D131" s="13">
         <v>43973</v>
       </c>
       <c r="G131" s="13">
         <v>43973</v>
       </c>
-      <c r="H131" s="26"/>
-      <c r="I131" s="26"/>
+      <c r="H131" s="28"/>
+      <c r="I131" s="28"/>
       <c r="J131" s="22">
         <f t="shared" si="1"/>
         <v>43973</v>
@@ -3842,16 +3849,16 @@
       <c r="A132" s="13">
         <v>43974</v>
       </c>
-      <c r="B132" s="28"/>
-      <c r="C132" s="25"/>
+      <c r="B132" s="25"/>
+      <c r="C132" s="26"/>
       <c r="D132" s="13">
         <v>43974</v>
       </c>
       <c r="G132" s="13">
         <v>43974</v>
       </c>
-      <c r="H132" s="26"/>
-      <c r="I132" s="26"/>
+      <c r="H132" s="28"/>
+      <c r="I132" s="28"/>
       <c r="J132" s="22">
         <f t="shared" si="1"/>
         <v>43974</v>
@@ -3861,16 +3868,16 @@
       <c r="A133" s="13">
         <v>43975</v>
       </c>
-      <c r="B133" s="28"/>
-      <c r="C133" s="25"/>
+      <c r="B133" s="25"/>
+      <c r="C133" s="26"/>
       <c r="D133" s="13">
         <v>43975</v>
       </c>
       <c r="G133" s="13">
         <v>43975</v>
       </c>
-      <c r="H133" s="26"/>
-      <c r="I133" s="26"/>
+      <c r="H133" s="28"/>
+      <c r="I133" s="28"/>
       <c r="J133" s="22">
         <f t="shared" si="1"/>
         <v>43975</v>
@@ -3880,16 +3887,16 @@
       <c r="A134" s="13">
         <v>43976</v>
       </c>
-      <c r="B134" s="28"/>
-      <c r="C134" s="25"/>
+      <c r="B134" s="25"/>
+      <c r="C134" s="26"/>
       <c r="D134" s="13">
         <v>43976</v>
       </c>
       <c r="G134" s="13">
         <v>43976</v>
       </c>
-      <c r="H134" s="26"/>
-      <c r="I134" s="26"/>
+      <c r="H134" s="28"/>
+      <c r="I134" s="28"/>
       <c r="J134" s="22">
         <f t="shared" si="1"/>
         <v>43976</v>
@@ -3899,16 +3906,16 @@
       <c r="A135" s="13">
         <v>43977</v>
       </c>
-      <c r="B135" s="28"/>
-      <c r="C135" s="25"/>
+      <c r="B135" s="25"/>
+      <c r="C135" s="26"/>
       <c r="D135" s="13">
         <v>43977</v>
       </c>
       <c r="G135" s="13">
         <v>43977</v>
       </c>
-      <c r="H135" s="26"/>
-      <c r="I135" s="26"/>
+      <c r="H135" s="28"/>
+      <c r="I135" s="28"/>
       <c r="J135" s="22">
         <f t="shared" si="1"/>
         <v>43977</v>
@@ -3918,16 +3925,16 @@
       <c r="A136" s="13">
         <v>43978</v>
       </c>
-      <c r="B136" s="28"/>
-      <c r="C136" s="25"/>
+      <c r="B136" s="25"/>
+      <c r="C136" s="26"/>
       <c r="D136" s="13">
         <v>43978</v>
       </c>
       <c r="G136" s="13">
         <v>43978</v>
       </c>
-      <c r="H136" s="26"/>
-      <c r="I136" s="26"/>
+      <c r="H136" s="28"/>
+      <c r="I136" s="28"/>
       <c r="J136" s="22">
         <f t="shared" si="1"/>
         <v>43978</v>
@@ -3937,16 +3944,16 @@
       <c r="A137" s="13">
         <v>43979</v>
       </c>
-      <c r="B137" s="28"/>
-      <c r="C137" s="25"/>
+      <c r="B137" s="25"/>
+      <c r="C137" s="26"/>
       <c r="D137" s="13">
         <v>43979</v>
       </c>
       <c r="G137" s="13">
         <v>43979</v>
       </c>
-      <c r="H137" s="26"/>
-      <c r="I137" s="26"/>
+      <c r="H137" s="28"/>
+      <c r="I137" s="28"/>
       <c r="J137" s="22">
         <f t="shared" si="1"/>
         <v>43979</v>
@@ -3956,16 +3963,16 @@
       <c r="A138" s="13">
         <v>43980</v>
       </c>
-      <c r="B138" s="28"/>
-      <c r="C138" s="25"/>
+      <c r="B138" s="25"/>
+      <c r="C138" s="26"/>
       <c r="D138" s="13">
         <v>43980</v>
       </c>
       <c r="G138" s="13">
         <v>43980</v>
       </c>
-      <c r="H138" s="26"/>
-      <c r="I138" s="26"/>
+      <c r="H138" s="28"/>
+      <c r="I138" s="28"/>
       <c r="J138" s="22">
         <f t="shared" si="1"/>
         <v>43980</v>
@@ -3975,16 +3982,16 @@
       <c r="A139" s="13">
         <v>43981</v>
       </c>
-      <c r="B139" s="28"/>
-      <c r="C139" s="25"/>
+      <c r="B139" s="25"/>
+      <c r="C139" s="26"/>
       <c r="D139" s="13">
         <v>43981</v>
       </c>
       <c r="G139" s="13">
         <v>43981</v>
       </c>
-      <c r="H139" s="26"/>
-      <c r="I139" s="26"/>
+      <c r="H139" s="28"/>
+      <c r="I139" s="28"/>
       <c r="J139" s="22">
         <f t="shared" si="1"/>
         <v>43981</v>
@@ -3994,16 +4001,16 @@
       <c r="A140" s="13">
         <v>43982</v>
       </c>
-      <c r="B140" s="28"/>
-      <c r="C140" s="25"/>
+      <c r="B140" s="25"/>
+      <c r="C140" s="26"/>
       <c r="D140" s="13">
         <v>43982</v>
       </c>
       <c r="G140" s="13">
         <v>43982</v>
       </c>
-      <c r="H140" s="26"/>
-      <c r="I140" s="26"/>
+      <c r="H140" s="28"/>
+      <c r="I140" s="28"/>
       <c r="J140" s="22">
         <f t="shared" si="1"/>
         <v>43982</v>
@@ -4013,16 +4020,16 @@
       <c r="A141" s="13">
         <v>43983</v>
       </c>
-      <c r="B141" s="28"/>
-      <c r="C141" s="25"/>
+      <c r="B141" s="25"/>
+      <c r="C141" s="26"/>
       <c r="D141" s="13">
         <v>43983</v>
       </c>
       <c r="G141" s="13">
         <v>43983</v>
       </c>
-      <c r="H141" s="26"/>
-      <c r="I141" s="26"/>
+      <c r="H141" s="28"/>
+      <c r="I141" s="28"/>
       <c r="J141" s="22">
         <f t="shared" si="1"/>
         <v>43983</v>
@@ -4032,16 +4039,16 @@
       <c r="A142" s="13">
         <v>43984</v>
       </c>
-      <c r="B142" s="28"/>
-      <c r="C142" s="25"/>
+      <c r="B142" s="25"/>
+      <c r="C142" s="26"/>
       <c r="D142" s="13">
         <v>43984</v>
       </c>
       <c r="G142" s="13">
         <v>43984</v>
       </c>
-      <c r="H142" s="26"/>
-      <c r="I142" s="26"/>
+      <c r="H142" s="28"/>
+      <c r="I142" s="28"/>
       <c r="J142" s="22">
         <f t="shared" si="1"/>
         <v>43984</v>
@@ -4051,16 +4058,16 @@
       <c r="A143" s="13">
         <v>43985</v>
       </c>
-      <c r="B143" s="28"/>
-      <c r="C143" s="25"/>
+      <c r="B143" s="25"/>
+      <c r="C143" s="26"/>
       <c r="D143" s="13">
         <v>43985</v>
       </c>
       <c r="G143" s="13">
         <v>43985</v>
       </c>
-      <c r="H143" s="26"/>
-      <c r="I143" s="26"/>
+      <c r="H143" s="28"/>
+      <c r="I143" s="28"/>
       <c r="J143" s="22">
         <f t="shared" si="1"/>
         <v>43985</v>
@@ -4070,16 +4077,16 @@
       <c r="A144" s="13">
         <v>43986</v>
       </c>
-      <c r="B144" s="28"/>
-      <c r="C144" s="25"/>
+      <c r="B144" s="25"/>
+      <c r="C144" s="26"/>
       <c r="D144" s="13">
         <v>43986</v>
       </c>
       <c r="G144" s="13">
         <v>43986</v>
       </c>
-      <c r="H144" s="26"/>
-      <c r="I144" s="26"/>
+      <c r="H144" s="28"/>
+      <c r="I144" s="28"/>
       <c r="J144" s="22">
         <f t="shared" si="1"/>
         <v>43986</v>
@@ -4089,292 +4096,292 @@
       <c r="A145" s="13">
         <v>43987</v>
       </c>
-      <c r="B145" s="28"/>
-      <c r="C145" s="25"/>
+      <c r="B145" s="25"/>
+      <c r="C145" s="26"/>
       <c r="D145" s="13">
         <v>43987</v>
       </c>
       <c r="G145" s="13">
         <v>43987</v>
       </c>
-      <c r="H145" s="26"/>
-      <c r="I145" s="26"/>
+      <c r="H145" s="28"/>
+      <c r="I145" s="28"/>
       <c r="J145" s="22">
         <f t="shared" si="1"/>
         <v>43987</v>
       </c>
-      <c r="K145" s="26"/>
-      <c r="L145" s="26"/>
+      <c r="K145" s="28"/>
+      <c r="L145" s="28"/>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="13">
         <v>43988</v>
       </c>
-      <c r="B146" s="28"/>
-      <c r="C146" s="25"/>
+      <c r="B146" s="25"/>
+      <c r="C146" s="26"/>
       <c r="D146" s="13">
         <v>43988</v>
       </c>
       <c r="G146" s="13">
         <v>43988</v>
       </c>
-      <c r="H146" s="26"/>
-      <c r="I146" s="26"/>
+      <c r="H146" s="28"/>
+      <c r="I146" s="28"/>
       <c r="J146" s="22">
         <f t="shared" si="1"/>
         <v>43988</v>
       </c>
-      <c r="K146" s="26"/>
-      <c r="L146" s="26"/>
+      <c r="K146" s="28"/>
+      <c r="L146" s="28"/>
     </row>
     <row r="147" spans="1:12">
       <c r="A147" s="13">
         <v>43989</v>
       </c>
-      <c r="B147" s="28"/>
-      <c r="C147" s="25"/>
+      <c r="B147" s="25"/>
+      <c r="C147" s="26"/>
       <c r="D147" s="13">
         <v>43989</v>
       </c>
       <c r="G147" s="13">
         <v>43989</v>
       </c>
-      <c r="H147" s="26"/>
-      <c r="I147" s="26"/>
+      <c r="H147" s="28"/>
+      <c r="I147" s="28"/>
       <c r="J147" s="22">
         <f t="shared" si="1"/>
         <v>43989</v>
       </c>
-      <c r="K147" s="26"/>
-      <c r="L147" s="26"/>
+      <c r="K147" s="28"/>
+      <c r="L147" s="28"/>
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="13">
         <v>43990</v>
       </c>
-      <c r="B148" s="28"/>
-      <c r="C148" s="25"/>
+      <c r="B148" s="25"/>
+      <c r="C148" s="26"/>
       <c r="D148" s="13">
         <v>43990</v>
       </c>
       <c r="G148" s="13">
         <v>43990</v>
       </c>
-      <c r="H148" s="26"/>
-      <c r="I148" s="26"/>
+      <c r="H148" s="28"/>
+      <c r="I148" s="28"/>
       <c r="J148" s="22">
         <f t="shared" si="1"/>
         <v>43990</v>
       </c>
-      <c r="K148" s="26"/>
-      <c r="L148" s="26"/>
+      <c r="K148" s="28"/>
+      <c r="L148" s="28"/>
     </row>
     <row r="149" spans="1:12">
       <c r="A149" s="13">
         <v>43991</v>
       </c>
-      <c r="B149" s="28"/>
-      <c r="C149" s="25"/>
+      <c r="B149" s="25"/>
+      <c r="C149" s="26"/>
       <c r="D149" s="13">
         <v>43991</v>
       </c>
       <c r="G149" s="13">
         <v>43991</v>
       </c>
-      <c r="H149" s="26"/>
-      <c r="I149" s="26"/>
+      <c r="H149" s="28"/>
+      <c r="I149" s="28"/>
       <c r="J149" s="22">
         <f t="shared" si="1"/>
         <v>43991</v>
       </c>
-      <c r="K149" s="26"/>
-      <c r="L149" s="26"/>
+      <c r="K149" s="28"/>
+      <c r="L149" s="28"/>
     </row>
     <row r="150" spans="1:12">
       <c r="A150" s="13">
         <v>43992</v>
       </c>
-      <c r="B150" s="28"/>
-      <c r="C150" s="25"/>
+      <c r="B150" s="25"/>
+      <c r="C150" s="26"/>
       <c r="D150" s="13">
         <v>43992</v>
       </c>
       <c r="G150" s="13">
         <v>43992</v>
       </c>
-      <c r="H150" s="26"/>
-      <c r="I150" s="26"/>
+      <c r="H150" s="28"/>
+      <c r="I150" s="28"/>
       <c r="J150" s="22">
         <f t="shared" si="1"/>
         <v>43992</v>
       </c>
-      <c r="K150" s="26"/>
-      <c r="L150" s="26"/>
+      <c r="K150" s="28"/>
+      <c r="L150" s="28"/>
     </row>
     <row r="151" spans="1:12">
       <c r="A151" s="13">
         <v>43993</v>
       </c>
-      <c r="B151" s="28"/>
-      <c r="C151" s="25"/>
+      <c r="B151" s="25"/>
+      <c r="C151" s="26"/>
       <c r="D151" s="13">
         <v>43993</v>
       </c>
       <c r="G151" s="13">
         <v>43993</v>
       </c>
-      <c r="H151" s="26"/>
-      <c r="I151" s="26"/>
+      <c r="H151" s="28"/>
+      <c r="I151" s="28"/>
       <c r="J151" s="22">
         <f t="shared" si="1"/>
         <v>43993</v>
       </c>
-      <c r="K151" s="26"/>
-      <c r="L151" s="26"/>
+      <c r="K151" s="28"/>
+      <c r="L151" s="28"/>
     </row>
     <row r="152" spans="1:12">
       <c r="A152" s="13">
         <v>43994</v>
       </c>
-      <c r="B152" s="28"/>
-      <c r="C152" s="25"/>
+      <c r="B152" s="25"/>
+      <c r="C152" s="26"/>
       <c r="D152" s="13">
         <v>43994</v>
       </c>
       <c r="G152" s="13">
         <v>43994</v>
       </c>
-      <c r="H152" s="26"/>
-      <c r="I152" s="26"/>
+      <c r="H152" s="28"/>
+      <c r="I152" s="28"/>
       <c r="J152" s="22">
         <f t="shared" si="1"/>
         <v>43994</v>
       </c>
-      <c r="K152" s="26"/>
-      <c r="L152" s="26"/>
+      <c r="K152" s="28"/>
+      <c r="L152" s="28"/>
     </row>
     <row r="153" spans="1:12">
       <c r="A153" s="13">
         <v>43995</v>
       </c>
-      <c r="B153" s="28"/>
-      <c r="C153" s="25"/>
+      <c r="B153" s="25"/>
+      <c r="C153" s="26"/>
       <c r="D153" s="13">
         <v>43995</v>
       </c>
       <c r="G153" s="13">
         <v>43995</v>
       </c>
-      <c r="H153" s="26"/>
-      <c r="I153" s="26"/>
+      <c r="H153" s="28"/>
+      <c r="I153" s="28"/>
       <c r="J153" s="22">
         <f t="shared" si="1"/>
         <v>43995</v>
       </c>
-      <c r="K153" s="26"/>
-      <c r="L153" s="26"/>
+      <c r="K153" s="28"/>
+      <c r="L153" s="28"/>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="13">
         <v>43996</v>
       </c>
-      <c r="B154" s="28"/>
-      <c r="C154" s="25"/>
+      <c r="B154" s="25"/>
+      <c r="C154" s="26"/>
       <c r="D154" s="13">
         <v>43996</v>
       </c>
       <c r="G154" s="13">
         <v>43996</v>
       </c>
-      <c r="H154" s="26"/>
-      <c r="I154" s="26"/>
+      <c r="H154" s="28"/>
+      <c r="I154" s="28"/>
       <c r="J154" s="22">
         <f t="shared" si="1"/>
         <v>43996</v>
       </c>
-      <c r="K154" s="26"/>
-      <c r="L154" s="26"/>
+      <c r="K154" s="28"/>
+      <c r="L154" s="28"/>
     </row>
     <row r="155" spans="1:12">
       <c r="A155" s="13">
         <v>43997</v>
       </c>
-      <c r="B155" s="28"/>
-      <c r="C155" s="25"/>
+      <c r="B155" s="25"/>
+      <c r="C155" s="26"/>
       <c r="D155" s="13">
         <v>43997</v>
       </c>
       <c r="G155" s="13">
         <v>43997</v>
       </c>
-      <c r="H155" s="26"/>
-      <c r="I155" s="26"/>
+      <c r="H155" s="28"/>
+      <c r="I155" s="28"/>
       <c r="J155" s="22">
         <f t="shared" si="1"/>
         <v>43997</v>
       </c>
-      <c r="K155" s="26"/>
-      <c r="L155" s="26"/>
+      <c r="K155" s="28"/>
+      <c r="L155" s="28"/>
     </row>
     <row r="156" spans="1:12">
       <c r="A156" s="14"/>
-      <c r="B156" s="26"/>
-      <c r="C156" s="26"/>
+      <c r="B156" s="28"/>
+      <c r="C156" s="28"/>
       <c r="D156" s="13"/>
-      <c r="H156" s="26"/>
-      <c r="I156" s="26"/>
+      <c r="H156" s="28"/>
+      <c r="I156" s="28"/>
       <c r="J156" s="22">
         <f t="shared" si="1"/>
         <v>43998</v>
       </c>
-      <c r="K156" s="26"/>
-      <c r="L156" s="26"/>
+      <c r="K156" s="28"/>
+      <c r="L156" s="28"/>
     </row>
     <row r="157" spans="1:12">
       <c r="A157" s="14"/>
-      <c r="B157" s="26"/>
-      <c r="C157" s="26"/>
+      <c r="B157" s="28"/>
+      <c r="C157" s="28"/>
       <c r="D157" s="14"/>
-      <c r="H157" s="26"/>
-      <c r="I157" s="26"/>
+      <c r="H157" s="28"/>
+      <c r="I157" s="28"/>
       <c r="J157" s="22">
         <f t="shared" si="1"/>
         <v>43999</v>
       </c>
-      <c r="K157" s="26"/>
-      <c r="L157" s="26"/>
+      <c r="K157" s="28"/>
+      <c r="L157" s="28"/>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" s="14"/>
-      <c r="B158" s="26"/>
-      <c r="C158" s="26"/>
+      <c r="B158" s="28"/>
+      <c r="C158" s="28"/>
       <c r="D158" s="14"/>
-      <c r="H158" s="26"/>
-      <c r="I158" s="26"/>
+      <c r="H158" s="28"/>
+      <c r="I158" s="28"/>
       <c r="J158" s="22">
         <f t="shared" si="1"/>
         <v>44000</v>
       </c>
-      <c r="K158" s="26"/>
-      <c r="L158" s="26"/>
+      <c r="K158" s="28"/>
+      <c r="L158" s="28"/>
     </row>
     <row r="159" spans="1:12" ht="30.75" thickBot="1">
       <c r="A159" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B159" s="26"/>
+        <v>88</v>
+      </c>
+      <c r="B159" s="28"/>
       <c r="C159" s="8">
         <f>SUM(C64:C155)</f>
         <v>67</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F159" s="8">
         <f>SUM(F64:F156)</f>
         <v>60</v>
       </c>
-      <c r="H159" s="26"/>
+      <c r="H159" s="28"/>
       <c r="I159" s="17">
         <f>SUM(I2:I155)</f>
         <v>53</v>
@@ -4383,24 +4390,24 @@
         <f t="shared" si="1"/>
         <v>44001</v>
       </c>
-      <c r="K159" s="26"/>
+      <c r="K159" s="28"/>
       <c r="L159" s="17">
         <f>SUM(L64:L155)</f>
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B160" s="26"/>
-      <c r="C160" s="26"/>
+      <c r="B160" s="28"/>
+      <c r="C160" s="28"/>
       <c r="D160" s="6"/>
-      <c r="H160" s="26"/>
-      <c r="I160" s="26"/>
+      <c r="H160" s="28"/>
+      <c r="I160" s="28"/>
       <c r="J160" s="22">
         <f t="shared" si="1"/>
         <v>44002</v>
       </c>
-      <c r="K160" s="26"/>
-      <c r="L160" s="26"/>
+      <c r="K160" s="28"/>
+      <c r="L160" s="28"/>
     </row>
     <row r="161" spans="10:10" ht="15.75" thickTop="1">
       <c r="J161" s="22">
@@ -4488,6 +4495,55 @@
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="E110:E111"/>
+    <mergeCell ref="F110:F111"/>
+    <mergeCell ref="K91:L104"/>
+    <mergeCell ref="K105:K106"/>
+    <mergeCell ref="L105:L106"/>
+    <mergeCell ref="E101:E102"/>
+    <mergeCell ref="F101:F102"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="K109:L111"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="E92:E100"/>
+    <mergeCell ref="F88:F90"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="F85:F87"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="C92:C96"/>
+    <mergeCell ref="B85:B90"/>
+    <mergeCell ref="C85:C90"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="E3:F63"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="E73:E76"/>
+    <mergeCell ref="F73:F76"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="K2:L63"/>
+    <mergeCell ref="L81:L82"/>
+    <mergeCell ref="K65:K68"/>
+    <mergeCell ref="L65:L68"/>
+    <mergeCell ref="K69:L70"/>
+    <mergeCell ref="K76:L77"/>
+    <mergeCell ref="K81:K82"/>
     <mergeCell ref="B107:B108"/>
     <mergeCell ref="C107:C108"/>
     <mergeCell ref="K83:L84"/>
@@ -4504,55 +4560,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="H65:H71"/>
     <mergeCell ref="I65:I71"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="K2:L63"/>
-    <mergeCell ref="L81:L82"/>
-    <mergeCell ref="K65:K68"/>
-    <mergeCell ref="L65:L68"/>
-    <mergeCell ref="K69:L70"/>
-    <mergeCell ref="K76:L77"/>
-    <mergeCell ref="K81:K82"/>
-    <mergeCell ref="B85:B90"/>
-    <mergeCell ref="C85:C90"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="E3:F63"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="F78:F81"/>
-    <mergeCell ref="E73:E76"/>
-    <mergeCell ref="F73:F76"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="C92:C96"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="E88:E90"/>
-    <mergeCell ref="E92:E100"/>
-    <mergeCell ref="F88:F90"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="E110:E111"/>
-    <mergeCell ref="F110:F111"/>
-    <mergeCell ref="K91:L104"/>
-    <mergeCell ref="K105:K106"/>
-    <mergeCell ref="L105:L106"/>
-    <mergeCell ref="E101:E102"/>
-    <mergeCell ref="F101:F102"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="K109:L111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
commentaire des mécanismes et UP JA
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UTILISATEUR 1\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9602B2A9-463F-4AE5-B8BF-E36FC8CC0674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1302B061-6349-4E97-9BAA-D7EF93D257EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="100">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -324,6 +324,15 @@
   </si>
   <si>
     <t>Travail sur les mécanismes en ajoutant la partie I2C fournie par Constantin</t>
+  </si>
+  <si>
+    <t>Correction Rapport et améliorations</t>
+  </si>
+  <si>
+    <t>Commenter code mécanisme air pour rapport + infos sur fonctions arduino</t>
+  </si>
+  <si>
+    <t>Commenter code mécanisme katana pour rapport</t>
   </si>
 </sst>
 </file>
@@ -617,7 +626,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -709,6 +718,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -718,6 +733,21 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -730,12 +760,45 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -755,54 +818,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1126,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView tabSelected="1" topLeftCell="E108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K118" sqref="K118:L119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,7 +1173,7 @@
       <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="58" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
@@ -1167,1020 +1182,1020 @@
       <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="42"/>
+      <c r="G1" s="60"/>
       <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="44"/>
+      <c r="J1" s="62"/>
       <c r="K1" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="47"/>
+      <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>43844</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="27"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="43"/>
+      <c r="G2" s="61"/>
       <c r="H2" s="27"/>
       <c r="I2" s="11"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="48"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="47"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>43845</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="13">
         <v>43845</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="H3" s="34" t="s">
+      <c r="F3" s="42"/>
+      <c r="H3" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="35"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="52"/>
+      <c r="I3" s="42"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="51"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>43846</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="13">
         <v>43846</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="52"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="51"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>43847</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="13">
         <v>43847</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="37"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="52"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="44"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="51"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>43848</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="13">
         <v>43848</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="52"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="44"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="44"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="51"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>43849</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="13">
         <v>43849</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="37"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="52"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="44"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="44"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="51"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>43850</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="13">
         <v>43850</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="37"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="52"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="44"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="51"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>43851</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="13">
         <v>43851</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="52"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="44"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="44"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="51"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>43852</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="13">
         <v>43852</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="52"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="44"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="44"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="51"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>43853</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="13">
         <v>43853</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="37"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="52"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="44"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="44"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="51"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>43854</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="13">
         <v>43854</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="52"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="44"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="44"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="51"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>43855</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="13">
         <v>43855</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="52"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="44"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="44"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="51"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>43856</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="13">
         <v>43856</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="52"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="44"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="44"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="51"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>43857</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="13">
         <v>43857</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="37"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="52"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="44"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="44"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="51"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>43858</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="13">
         <v>43858</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="52"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="44"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="44"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="51"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>43859</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="13">
         <v>43859</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="37"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="52"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="44"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="44"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="51"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>43860</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="13">
         <v>43860</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="37"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="52"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="44"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="44"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="51"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>43861</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="13">
         <v>43861</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="37"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="52"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="44"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="44"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="51"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>43862</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="13">
         <v>43862</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="52"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="51"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>43863</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="13">
         <v>43863</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="37"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="52"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="44"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="44"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="51"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>43864</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="13">
         <v>43864</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="37"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="52"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="44"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="51"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>43865</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="13">
         <v>43865</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="37"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="37"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="52"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="44"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="44"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="51"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>43866</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="13">
         <v>43866</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="37"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="52"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="44"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="51"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>43867</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="37"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="13">
         <v>43867</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="37"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="52"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="44"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="44"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="51"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>43868</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="13">
         <v>43868</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="37"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="52"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="44"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="44"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="51"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>43869</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="37"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="13">
         <v>43869</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="37"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="52"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="44"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="44"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="51"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>43870</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="13">
         <v>43870</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="37"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="52"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="44"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="51"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>43871</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="37"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="13">
         <v>43871</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="37"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="37"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="52"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="44"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="51"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>43872</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="37"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
       <c r="D30" s="13">
         <v>43872</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="37"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="52"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="44"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="51"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>43873</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="37"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="44"/>
       <c r="D31" s="13">
         <v>43873</v>
       </c>
-      <c r="E31" s="36"/>
-      <c r="F31" s="37"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="37"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="52"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="44"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="44"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="51"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>43874</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="37"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
       <c r="D32" s="13">
         <v>43874</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="37"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="52"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="44"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="K32" s="50"/>
+      <c r="L32" s="51"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>43875</v>
       </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="37"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
       <c r="D33" s="13">
         <v>43875</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="37"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="52"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="44"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="44"/>
+      <c r="K33" s="50"/>
+      <c r="L33" s="51"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>43876</v>
       </c>
-      <c r="B34" s="36"/>
-      <c r="C34" s="37"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
       <c r="D34" s="13">
         <v>43876</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="37"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="37"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="52"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="44"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="K34" s="50"/>
+      <c r="L34" s="51"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>43877</v>
       </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="37"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="13">
         <v>43877</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="37"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="37"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="52"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="44"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="44"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="51"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>43878</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="37"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="44"/>
       <c r="D36" s="13">
         <v>43878</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="37"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="37"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="52"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="44"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="44"/>
+      <c r="K36" s="50"/>
+      <c r="L36" s="51"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>43879</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="37"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="44"/>
       <c r="D37" s="13">
         <v>43879</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="37"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="37"/>
-      <c r="K37" s="51"/>
-      <c r="L37" s="52"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="44"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="44"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="51"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>43880</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="37"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="44"/>
       <c r="D38" s="13">
         <v>43880</v>
       </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="37"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="37"/>
-      <c r="K38" s="51"/>
-      <c r="L38" s="52"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="44"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="44"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="51"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>43881</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="37"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="44"/>
       <c r="D39" s="13">
         <v>43881</v>
       </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="37"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="37"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="52"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="44"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="44"/>
+      <c r="K39" s="50"/>
+      <c r="L39" s="51"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>43882</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="37"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="44"/>
       <c r="D40" s="13">
         <v>43882</v>
       </c>
-      <c r="E40" s="36"/>
-      <c r="F40" s="37"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="37"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="52"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="44"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="44"/>
+      <c r="K40" s="50"/>
+      <c r="L40" s="51"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>43883</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="37"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="44"/>
       <c r="D41" s="13">
         <v>43883</v>
       </c>
-      <c r="E41" s="36"/>
-      <c r="F41" s="37"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="37"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="52"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="44"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="44"/>
+      <c r="K41" s="50"/>
+      <c r="L41" s="51"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>43884</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="37"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="44"/>
       <c r="D42" s="13">
         <v>43884</v>
       </c>
-      <c r="E42" s="36"/>
-      <c r="F42" s="37"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="37"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="52"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="44"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="44"/>
+      <c r="K42" s="50"/>
+      <c r="L42" s="51"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>43885</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="37"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="44"/>
       <c r="D43" s="13">
         <v>43885</v>
       </c>
-      <c r="E43" s="36"/>
-      <c r="F43" s="37"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="37"/>
-      <c r="K43" s="51"/>
-      <c r="L43" s="52"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="44"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="44"/>
+      <c r="K43" s="50"/>
+      <c r="L43" s="51"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>43886</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="37"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="44"/>
       <c r="D44" s="13">
         <v>43886</v>
       </c>
-      <c r="E44" s="36"/>
-      <c r="F44" s="37"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="52"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="44"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="44"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="51"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>43887</v>
       </c>
-      <c r="B45" s="36"/>
-      <c r="C45" s="37"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="44"/>
       <c r="D45" s="13">
         <v>43887</v>
       </c>
-      <c r="E45" s="36"/>
-      <c r="F45" s="37"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="37"/>
-      <c r="K45" s="51"/>
-      <c r="L45" s="52"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="44"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="44"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="51"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>43888</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="37"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="44"/>
       <c r="D46" s="13">
         <v>43888</v>
       </c>
-      <c r="E46" s="36"/>
-      <c r="F46" s="37"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="37"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="52"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="44"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="44"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="51"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>43889</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="37"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="44"/>
       <c r="D47" s="13">
         <v>43889</v>
       </c>
-      <c r="E47" s="36"/>
-      <c r="F47" s="37"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="37"/>
-      <c r="K47" s="51"/>
-      <c r="L47" s="52"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="44"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="51"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>43890</v>
       </c>
-      <c r="B48" s="36"/>
-      <c r="C48" s="37"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="44"/>
       <c r="D48" s="13">
         <v>43890</v>
       </c>
-      <c r="E48" s="36"/>
-      <c r="F48" s="37"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="37"/>
-      <c r="K48" s="51"/>
-      <c r="L48" s="52"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="44"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="44"/>
+      <c r="K48" s="50"/>
+      <c r="L48" s="51"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>43891</v>
       </c>
-      <c r="B49" s="36"/>
-      <c r="C49" s="37"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="44"/>
       <c r="D49" s="13">
         <v>43891</v>
       </c>
-      <c r="E49" s="36"/>
-      <c r="F49" s="37"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="37"/>
-      <c r="K49" s="51"/>
-      <c r="L49" s="52"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="44"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="44"/>
+      <c r="K49" s="50"/>
+      <c r="L49" s="51"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>43892</v>
       </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="37"/>
+      <c r="B50" s="43"/>
+      <c r="C50" s="44"/>
       <c r="D50" s="13">
         <v>43892</v>
       </c>
-      <c r="E50" s="36"/>
-      <c r="F50" s="37"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="37"/>
-      <c r="K50" s="51"/>
-      <c r="L50" s="52"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="44"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="44"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="51"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>43893</v>
       </c>
-      <c r="B51" s="36"/>
-      <c r="C51" s="37"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="44"/>
       <c r="D51" s="13">
         <v>43893</v>
       </c>
-      <c r="E51" s="36"/>
-      <c r="F51" s="37"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="37"/>
-      <c r="K51" s="51"/>
-      <c r="L51" s="52"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="44"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="44"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="51"/>
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>43894</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="37"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="44"/>
       <c r="D52" s="13">
         <v>43894</v>
       </c>
-      <c r="E52" s="36"/>
-      <c r="F52" s="37"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="37"/>
-      <c r="K52" s="51"/>
-      <c r="L52" s="52"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="44"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="44"/>
+      <c r="K52" s="50"/>
+      <c r="L52" s="51"/>
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
         <v>43895</v>
       </c>
-      <c r="B53" s="36"/>
-      <c r="C53" s="37"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="13">
         <v>43895</v>
       </c>
-      <c r="E53" s="36"/>
-      <c r="F53" s="37"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="37"/>
-      <c r="K53" s="51"/>
-      <c r="L53" s="52"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="44"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="44"/>
+      <c r="K53" s="50"/>
+      <c r="L53" s="51"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>43896</v>
       </c>
-      <c r="B54" s="36"/>
-      <c r="C54" s="37"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="44"/>
       <c r="D54" s="13">
         <v>43896</v>
       </c>
-      <c r="E54" s="36"/>
-      <c r="F54" s="37"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="37"/>
-      <c r="K54" s="51"/>
-      <c r="L54" s="52"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="44"/>
+      <c r="H54" s="43"/>
+      <c r="I54" s="44"/>
+      <c r="K54" s="50"/>
+      <c r="L54" s="51"/>
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>43897</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="37"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="44"/>
       <c r="D55" s="13">
         <v>43897</v>
       </c>
-      <c r="E55" s="36"/>
-      <c r="F55" s="37"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="37"/>
-      <c r="K55" s="51"/>
-      <c r="L55" s="52"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="44"/>
+      <c r="H55" s="43"/>
+      <c r="I55" s="44"/>
+      <c r="K55" s="50"/>
+      <c r="L55" s="51"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>43898</v>
       </c>
-      <c r="B56" s="36"/>
-      <c r="C56" s="37"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="44"/>
       <c r="D56" s="13">
         <v>43898</v>
       </c>
-      <c r="E56" s="36"/>
-      <c r="F56" s="37"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="37"/>
-      <c r="K56" s="51"/>
-      <c r="L56" s="52"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="44"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="44"/>
+      <c r="K56" s="50"/>
+      <c r="L56" s="51"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>43899</v>
       </c>
-      <c r="B57" s="36"/>
-      <c r="C57" s="37"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="44"/>
       <c r="D57" s="13">
         <v>43899</v>
       </c>
-      <c r="E57" s="36"/>
-      <c r="F57" s="37"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="37"/>
-      <c r="K57" s="51"/>
-      <c r="L57" s="52"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="44"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="44"/>
+      <c r="K57" s="50"/>
+      <c r="L57" s="51"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>43900</v>
       </c>
-      <c r="B58" s="36"/>
-      <c r="C58" s="37"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="44"/>
       <c r="D58" s="13">
         <v>43900</v>
       </c>
-      <c r="E58" s="36"/>
-      <c r="F58" s="37"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="37"/>
-      <c r="K58" s="51"/>
-      <c r="L58" s="52"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="44"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="44"/>
+      <c r="K58" s="50"/>
+      <c r="L58" s="51"/>
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>43901</v>
       </c>
-      <c r="B59" s="36"/>
-      <c r="C59" s="37"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="44"/>
       <c r="D59" s="13">
         <v>43901</v>
       </c>
-      <c r="E59" s="36"/>
-      <c r="F59" s="37"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="37"/>
-      <c r="K59" s="51"/>
-      <c r="L59" s="52"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="44"/>
+      <c r="H59" s="43"/>
+      <c r="I59" s="44"/>
+      <c r="K59" s="50"/>
+      <c r="L59" s="51"/>
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>43902</v>
       </c>
-      <c r="B60" s="36"/>
-      <c r="C60" s="37"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="44"/>
       <c r="D60" s="13">
         <v>43902</v>
       </c>
-      <c r="E60" s="36"/>
-      <c r="F60" s="37"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="37"/>
-      <c r="K60" s="51"/>
-      <c r="L60" s="52"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="44"/>
+      <c r="H60" s="43"/>
+      <c r="I60" s="44"/>
+      <c r="K60" s="50"/>
+      <c r="L60" s="51"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>43903</v>
       </c>
-      <c r="B61" s="36"/>
-      <c r="C61" s="37"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="44"/>
       <c r="D61" s="13">
         <v>43903</v>
       </c>
-      <c r="E61" s="36"/>
-      <c r="F61" s="37"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="37"/>
-      <c r="K61" s="51"/>
-      <c r="L61" s="52"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="44"/>
+      <c r="H61" s="43"/>
+      <c r="I61" s="44"/>
+      <c r="K61" s="50"/>
+      <c r="L61" s="51"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>43904</v>
       </c>
-      <c r="B62" s="36"/>
-      <c r="C62" s="37"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="44"/>
       <c r="D62" s="13">
         <v>43904</v>
       </c>
-      <c r="E62" s="36"/>
-      <c r="F62" s="37"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="37"/>
-      <c r="K62" s="51"/>
-      <c r="L62" s="52"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="44"/>
+      <c r="H62" s="43"/>
+      <c r="I62" s="44"/>
+      <c r="K62" s="50"/>
+      <c r="L62" s="51"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>43905</v>
       </c>
-      <c r="B63" s="36"/>
-      <c r="C63" s="37"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="44"/>
       <c r="D63" s="13">
         <v>43905</v>
       </c>
-      <c r="E63" s="36"/>
-      <c r="F63" s="37"/>
-      <c r="H63" s="36"/>
-      <c r="I63" s="37"/>
-      <c r="K63" s="51"/>
-      <c r="L63" s="52"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="44"/>
+      <c r="H63" s="43"/>
+      <c r="I63" s="44"/>
+      <c r="K63" s="50"/>
+      <c r="L63" s="51"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
@@ -2201,8 +2216,8 @@
       <c r="F64" s="26">
         <v>2</v>
       </c>
-      <c r="H64" s="36"/>
-      <c r="I64" s="37"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="44"/>
       <c r="J64" s="22">
         <v>43906</v>
       </c>
@@ -2217,33 +2232,33 @@
       <c r="A65" s="13">
         <v>43907</v>
       </c>
-      <c r="B65" s="31" t="s">
+      <c r="B65" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="39">
+      <c r="C65" s="45">
         <v>10</v>
       </c>
       <c r="D65" s="13">
         <v>43907</v>
       </c>
-      <c r="E65" s="31" t="s">
+      <c r="E65" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="39">
+      <c r="F65" s="45">
         <v>12</v>
       </c>
-      <c r="H65" s="31" t="s">
+      <c r="H65" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="I65" s="46"/>
+      <c r="I65" s="64"/>
       <c r="J65" s="22">
         <f>J64+1</f>
         <v>43907</v>
       </c>
-      <c r="K65" s="31" t="s">
+      <c r="K65" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="L65" s="53" t="s">
+      <c r="L65" s="52" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2251,111 +2266,111 @@
       <c r="A66" s="13">
         <v>43908</v>
       </c>
-      <c r="B66" s="31"/>
-      <c r="C66" s="39"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="45"/>
       <c r="D66" s="13">
         <v>43908</v>
       </c>
-      <c r="E66" s="31"/>
-      <c r="F66" s="39"/>
-      <c r="H66" s="31"/>
-      <c r="I66" s="46"/>
+      <c r="E66" s="33"/>
+      <c r="F66" s="45"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="64"/>
       <c r="J66" s="22">
         <f t="shared" ref="J66:J129" si="0">J65+1</f>
         <v>43908</v>
       </c>
-      <c r="K66" s="31"/>
-      <c r="L66" s="53"/>
+      <c r="K66" s="33"/>
+      <c r="L66" s="52"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
         <v>43909</v>
       </c>
-      <c r="B67" s="31"/>
-      <c r="C67" s="39"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="45"/>
       <c r="D67" s="13">
         <v>43909</v>
       </c>
-      <c r="E67" s="31"/>
-      <c r="F67" s="39"/>
-      <c r="H67" s="31"/>
-      <c r="I67" s="46"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="45"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="64"/>
       <c r="J67" s="22">
         <f t="shared" si="0"/>
         <v>43909</v>
       </c>
-      <c r="K67" s="31"/>
-      <c r="L67" s="53"/>
+      <c r="K67" s="33"/>
+      <c r="L67" s="52"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
         <v>43910</v>
       </c>
-      <c r="B68" s="31"/>
-      <c r="C68" s="39"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="45"/>
       <c r="D68" s="13">
         <v>43910</v>
       </c>
-      <c r="E68" s="31"/>
-      <c r="F68" s="39"/>
-      <c r="H68" s="31"/>
-      <c r="I68" s="46"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="45"/>
+      <c r="H68" s="33"/>
+      <c r="I68" s="64"/>
       <c r="J68" s="22">
         <f t="shared" si="0"/>
         <v>43910</v>
       </c>
-      <c r="K68" s="31"/>
-      <c r="L68" s="53"/>
+      <c r="K68" s="33"/>
+      <c r="L68" s="52"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
         <v>43911</v>
       </c>
-      <c r="B69" s="31" t="s">
+      <c r="B69" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C69" s="32">
+      <c r="C69" s="34">
         <v>4</v>
       </c>
       <c r="D69" s="13">
         <v>43911</v>
       </c>
-      <c r="E69" s="31" t="s">
+      <c r="E69" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="F69" s="59">
+      <c r="F69" s="36">
         <v>6</v>
       </c>
-      <c r="H69" s="31"/>
-      <c r="I69" s="46"/>
+      <c r="H69" s="33"/>
+      <c r="I69" s="64"/>
       <c r="J69" s="22">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="K69" s="54" t="s">
+      <c r="K69" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="L69" s="55"/>
+      <c r="L69" s="54"/>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
         <v>43912</v>
       </c>
-      <c r="B70" s="31"/>
-      <c r="C70" s="32"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="34"/>
       <c r="D70" s="13">
         <v>43912</v>
       </c>
-      <c r="E70" s="31"/>
-      <c r="F70" s="59"/>
-      <c r="H70" s="31"/>
-      <c r="I70" s="46"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="36"/>
+      <c r="H70" s="33"/>
+      <c r="I70" s="64"/>
       <c r="J70" s="22">
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
-      <c r="K70" s="54"/>
-      <c r="L70" s="55"/>
+      <c r="K70" s="53"/>
+      <c r="L70" s="54"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
@@ -2370,14 +2385,14 @@
       <c r="D71" s="13">
         <v>43913</v>
       </c>
-      <c r="E71" s="31" t="s">
+      <c r="E71" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="F71" s="59">
+      <c r="F71" s="36">
         <v>4</v>
       </c>
-      <c r="H71" s="31"/>
-      <c r="I71" s="46"/>
+      <c r="H71" s="33"/>
+      <c r="I71" s="64"/>
       <c r="J71" s="22">
         <f t="shared" si="0"/>
         <v>43913</v>
@@ -2402,8 +2417,8 @@
       <c r="D72" s="13">
         <v>43914</v>
       </c>
-      <c r="E72" s="31"/>
-      <c r="F72" s="59"/>
+      <c r="E72" s="33"/>
+      <c r="F72" s="36"/>
       <c r="G72" s="13">
         <v>43913</v>
       </c>
@@ -2437,19 +2452,19 @@
       <c r="D73" s="13">
         <v>43915</v>
       </c>
-      <c r="E73" s="31" t="s">
+      <c r="E73" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F73" s="59">
+      <c r="F73" s="36">
         <v>6</v>
       </c>
       <c r="G73" s="13">
         <v>43914</v>
       </c>
-      <c r="H73" s="31" t="s">
+      <c r="H73" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="I73" s="38"/>
+      <c r="I73" s="57"/>
       <c r="J73" s="22">
         <f t="shared" si="0"/>
         <v>43915</v>
@@ -2465,17 +2480,17 @@
       <c r="A74" s="13">
         <v>43916</v>
       </c>
-      <c r="B74" s="31" t="s">
+      <c r="B74" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="59"/>
+      <c r="C74" s="36"/>
       <c r="D74" s="13">
         <v>43916</v>
       </c>
-      <c r="E74" s="31"/>
-      <c r="F74" s="59"/>
-      <c r="H74" s="31"/>
-      <c r="I74" s="38"/>
+      <c r="E74" s="33"/>
+      <c r="F74" s="36"/>
+      <c r="H74" s="33"/>
+      <c r="I74" s="57"/>
       <c r="J74" s="22">
         <f t="shared" si="0"/>
         <v>43916</v>
@@ -2496,8 +2511,8 @@
       <c r="D75" s="13">
         <v>43917</v>
       </c>
-      <c r="E75" s="31"/>
-      <c r="F75" s="59"/>
+      <c r="E75" s="33"/>
+      <c r="F75" s="36"/>
       <c r="G75" s="13">
         <v>43915</v>
       </c>
@@ -2529,8 +2544,8 @@
       <c r="D76" s="13">
         <v>43918</v>
       </c>
-      <c r="E76" s="31"/>
-      <c r="F76" s="59"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="36"/>
       <c r="G76" s="13">
         <v>43916</v>
       </c>
@@ -2544,10 +2559,10 @@
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
-      <c r="K76" s="54" t="s">
+      <c r="K76" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="L76" s="56"/>
+      <c r="L76" s="55"/>
     </row>
     <row r="77" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="13">
@@ -2573,8 +2588,8 @@
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="K77" s="57"/>
-      <c r="L77" s="56"/>
+      <c r="K77" s="56"/>
+      <c r="L77" s="55"/>
     </row>
     <row r="78" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="13">
@@ -2589,10 +2604,10 @@
       <c r="D78" s="13">
         <v>43920</v>
       </c>
-      <c r="E78" s="31" t="s">
+      <c r="E78" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F78" s="59">
+      <c r="F78" s="36">
         <v>4</v>
       </c>
       <c r="G78" s="13">
@@ -2619,17 +2634,17 @@
       <c r="A79" s="13">
         <v>43921</v>
       </c>
-      <c r="B79" s="31" t="s">
+      <c r="B79" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C79" s="32">
+      <c r="C79" s="34">
         <v>4</v>
       </c>
       <c r="D79" s="13">
         <v>43921</v>
       </c>
-      <c r="E79" s="31"/>
-      <c r="F79" s="59"/>
+      <c r="E79" s="33"/>
+      <c r="F79" s="36"/>
       <c r="G79" s="13">
         <v>43919</v>
       </c>
@@ -2654,13 +2669,13 @@
       <c r="A80" s="13">
         <v>43922</v>
       </c>
-      <c r="B80" s="31"/>
-      <c r="C80" s="32"/>
+      <c r="B80" s="33"/>
+      <c r="C80" s="34"/>
       <c r="D80" s="13">
         <v>43922</v>
       </c>
-      <c r="E80" s="31"/>
-      <c r="F80" s="59"/>
+      <c r="E80" s="33"/>
+      <c r="F80" s="36"/>
       <c r="G80" s="13">
         <v>43920</v>
       </c>
@@ -2683,23 +2698,23 @@
       <c r="A81" s="13">
         <v>43923</v>
       </c>
-      <c r="B81" s="31"/>
-      <c r="C81" s="32"/>
+      <c r="B81" s="33"/>
+      <c r="C81" s="34"/>
       <c r="D81" s="13">
         <v>43923</v>
       </c>
-      <c r="E81" s="31"/>
-      <c r="F81" s="59"/>
+      <c r="E81" s="33"/>
+      <c r="F81" s="36"/>
       <c r="H81" s="20"/>
       <c r="I81" s="20"/>
       <c r="J81" s="22">
         <f t="shared" si="0"/>
         <v>43923</v>
       </c>
-      <c r="K81" s="32" t="s">
+      <c r="K81" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="L81" s="32" t="s">
+      <c r="L81" s="34" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2716,10 +2731,10 @@
       <c r="D82" s="13">
         <v>43924</v>
       </c>
-      <c r="E82" s="31" t="s">
+      <c r="E82" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="F82" s="59">
+      <c r="F82" s="36">
         <v>3</v>
       </c>
       <c r="H82" s="20"/>
@@ -2728,8 +2743,8 @@
         <f t="shared" si="0"/>
         <v>43924</v>
       </c>
-      <c r="K82" s="32"/>
-      <c r="L82" s="32"/>
+      <c r="K82" s="34"/>
+      <c r="L82" s="34"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="13">
@@ -2740,18 +2755,18 @@
       <c r="D83" s="13">
         <v>43925</v>
       </c>
-      <c r="E83" s="31"/>
-      <c r="F83" s="59"/>
+      <c r="E83" s="33"/>
+      <c r="F83" s="36"/>
       <c r="H83" s="20"/>
       <c r="I83" s="20"/>
       <c r="J83" s="22">
         <f t="shared" si="0"/>
         <v>43925</v>
       </c>
-      <c r="K83" s="33" t="s">
+      <c r="K83" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="L83" s="33"/>
+      <c r="L83" s="35"/>
     </row>
     <row r="84" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13">
@@ -2774,26 +2789,26 @@
         <f t="shared" si="0"/>
         <v>43926</v>
       </c>
-      <c r="K84" s="33"/>
-      <c r="L84" s="33"/>
+      <c r="K84" s="35"/>
+      <c r="L84" s="35"/>
     </row>
     <row r="85" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13">
         <v>43927</v>
       </c>
-      <c r="B85" s="58" t="s">
+      <c r="B85" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="C85" s="32">
+      <c r="C85" s="34">
         <v>12</v>
       </c>
       <c r="D85" s="13">
         <v>43927</v>
       </c>
-      <c r="E85" s="31" t="s">
+      <c r="E85" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="F85" s="59">
+      <c r="F85" s="36">
         <v>6</v>
       </c>
       <c r="H85" s="20"/>
@@ -2813,13 +2828,13 @@
       <c r="A86" s="13">
         <v>43928</v>
       </c>
-      <c r="B86" s="58"/>
-      <c r="C86" s="32"/>
+      <c r="B86" s="40"/>
+      <c r="C86" s="34"/>
       <c r="D86" s="13">
         <v>43928</v>
       </c>
-      <c r="E86" s="31"/>
-      <c r="F86" s="59"/>
+      <c r="E86" s="33"/>
+      <c r="F86" s="36"/>
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
       <c r="J86" s="22">
@@ -2837,13 +2852,13 @@
       <c r="A87" s="13">
         <v>43929</v>
       </c>
-      <c r="B87" s="58"/>
-      <c r="C87" s="32"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="34"/>
       <c r="D87" s="13">
         <v>43929</v>
       </c>
-      <c r="E87" s="31"/>
-      <c r="F87" s="59"/>
+      <c r="E87" s="33"/>
+      <c r="F87" s="36"/>
       <c r="H87" s="20"/>
       <c r="I87" s="20"/>
       <c r="J87" s="22">
@@ -2861,15 +2876,15 @@
       <c r="A88" s="21">
         <v>43930</v>
       </c>
-      <c r="B88" s="58"/>
-      <c r="C88" s="32"/>
+      <c r="B88" s="40"/>
+      <c r="C88" s="34"/>
       <c r="D88" s="13">
         <v>43930</v>
       </c>
-      <c r="E88" s="31" t="s">
+      <c r="E88" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="F88" s="59">
+      <c r="F88" s="36">
         <v>4</v>
       </c>
       <c r="H88" s="20"/>
@@ -2889,13 +2904,13 @@
       <c r="A89" s="21">
         <v>43931</v>
       </c>
-      <c r="B89" s="58"/>
-      <c r="C89" s="32"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="34"/>
       <c r="D89" s="13">
         <v>43931</v>
       </c>
-      <c r="E89" s="31"/>
-      <c r="F89" s="59"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="36"/>
       <c r="H89" s="20"/>
       <c r="I89" s="20"/>
       <c r="J89" s="22">
@@ -2913,13 +2928,13 @@
       <c r="A90" s="21">
         <v>43932</v>
       </c>
-      <c r="B90" s="58"/>
-      <c r="C90" s="32"/>
+      <c r="B90" s="40"/>
+      <c r="C90" s="34"/>
       <c r="D90" s="13">
         <v>43932</v>
       </c>
-      <c r="E90" s="31"/>
-      <c r="F90" s="59"/>
+      <c r="E90" s="33"/>
+      <c r="F90" s="36"/>
       <c r="H90" s="20"/>
       <c r="I90" s="20"/>
       <c r="J90" s="22">
@@ -2950,25 +2965,25 @@
         <f t="shared" si="0"/>
         <v>43933</v>
       </c>
-      <c r="K91" s="61" t="s">
+      <c r="K91" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="L91" s="61"/>
+      <c r="L91" s="38"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="13">
         <v>43934</v>
       </c>
-      <c r="B92" s="31" t="s">
+      <c r="B92" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="C92" s="32">
+      <c r="C92" s="34">
         <v>4</v>
       </c>
       <c r="D92" s="13">
         <v>43934</v>
       </c>
-      <c r="E92" s="31" t="s">
+      <c r="E92" s="33" t="s">
         <v>65</v>
       </c>
       <c r="H92" s="20"/>
@@ -2977,84 +2992,84 @@
         <f t="shared" si="0"/>
         <v>43934</v>
       </c>
-      <c r="K92" s="61"/>
-      <c r="L92" s="61"/>
+      <c r="K92" s="38"/>
+      <c r="L92" s="38"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="13">
         <v>43935</v>
       </c>
-      <c r="B93" s="31"/>
-      <c r="C93" s="32"/>
+      <c r="B93" s="33"/>
+      <c r="C93" s="34"/>
       <c r="D93" s="13">
         <v>43935</v>
       </c>
-      <c r="E93" s="60"/>
+      <c r="E93" s="39"/>
       <c r="H93" s="20"/>
       <c r="I93" s="20"/>
       <c r="J93" s="22">
         <f t="shared" si="0"/>
         <v>43935</v>
       </c>
-      <c r="K93" s="61"/>
-      <c r="L93" s="61"/>
+      <c r="K93" s="38"/>
+      <c r="L93" s="38"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="13">
         <v>43936</v>
       </c>
-      <c r="B94" s="31"/>
-      <c r="C94" s="32"/>
+      <c r="B94" s="33"/>
+      <c r="C94" s="34"/>
       <c r="D94" s="13">
         <v>43936</v>
       </c>
-      <c r="E94" s="60"/>
+      <c r="E94" s="39"/>
       <c r="H94" s="20"/>
       <c r="I94" s="20"/>
       <c r="J94" s="22">
         <f t="shared" si="0"/>
         <v>43936</v>
       </c>
-      <c r="K94" s="61"/>
-      <c r="L94" s="61"/>
+      <c r="K94" s="38"/>
+      <c r="L94" s="38"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="13">
         <v>43937</v>
       </c>
-      <c r="B95" s="31"/>
-      <c r="C95" s="32"/>
+      <c r="B95" s="33"/>
+      <c r="C95" s="34"/>
       <c r="D95" s="13">
         <v>43937</v>
       </c>
-      <c r="E95" s="60"/>
+      <c r="E95" s="39"/>
       <c r="H95" s="20"/>
       <c r="I95" s="20"/>
       <c r="J95" s="22">
         <f t="shared" si="0"/>
         <v>43937</v>
       </c>
-      <c r="K95" s="61"/>
-      <c r="L95" s="61"/>
+      <c r="K95" s="38"/>
+      <c r="L95" s="38"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="13">
         <v>43938</v>
       </c>
-      <c r="B96" s="31"/>
-      <c r="C96" s="32"/>
+      <c r="B96" s="33"/>
+      <c r="C96" s="34"/>
       <c r="D96" s="13">
         <v>43938</v>
       </c>
-      <c r="E96" s="60"/>
+      <c r="E96" s="39"/>
       <c r="H96" s="20"/>
       <c r="I96" s="20"/>
       <c r="J96" s="22">
         <f t="shared" si="0"/>
         <v>43938</v>
       </c>
-      <c r="K96" s="61"/>
-      <c r="L96" s="61"/>
+      <c r="K96" s="38"/>
+      <c r="L96" s="38"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="13">
@@ -3065,15 +3080,15 @@
       <c r="D97" s="13">
         <v>43939</v>
       </c>
-      <c r="E97" s="60"/>
+      <c r="E97" s="39"/>
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
       <c r="J97" s="22">
         <f t="shared" si="0"/>
         <v>43939</v>
       </c>
-      <c r="K97" s="61"/>
-      <c r="L97" s="61"/>
+      <c r="K97" s="38"/>
+      <c r="L97" s="38"/>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="13">
@@ -3084,71 +3099,71 @@
       <c r="D98" s="13">
         <v>43940</v>
       </c>
-      <c r="E98" s="60"/>
+      <c r="E98" s="39"/>
       <c r="H98" s="20"/>
       <c r="I98" s="20"/>
       <c r="J98" s="22">
         <f t="shared" si="0"/>
         <v>43940</v>
       </c>
-      <c r="K98" s="61"/>
-      <c r="L98" s="61"/>
+      <c r="K98" s="38"/>
+      <c r="L98" s="38"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="13">
         <v>43941</v>
       </c>
-      <c r="B99" s="31" t="s">
+      <c r="B99" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="C99" s="32">
+      <c r="C99" s="34">
         <v>4</v>
       </c>
       <c r="D99" s="13">
         <v>43941</v>
       </c>
-      <c r="E99" s="60"/>
+      <c r="E99" s="39"/>
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
       <c r="J99" s="22">
         <f t="shared" si="0"/>
         <v>43941</v>
       </c>
-      <c r="K99" s="61"/>
-      <c r="L99" s="61"/>
+      <c r="K99" s="38"/>
+      <c r="L99" s="38"/>
     </row>
     <row r="100" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13">
         <v>43942</v>
       </c>
-      <c r="B100" s="31"/>
-      <c r="C100" s="32"/>
+      <c r="B100" s="33"/>
+      <c r="C100" s="34"/>
       <c r="D100" s="13">
         <v>43942</v>
       </c>
-      <c r="E100" s="60"/>
+      <c r="E100" s="39"/>
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
       <c r="J100" s="22">
         <f t="shared" si="0"/>
         <v>43942</v>
       </c>
-      <c r="K100" s="61"/>
-      <c r="L100" s="61"/>
+      <c r="K100" s="38"/>
+      <c r="L100" s="38"/>
     </row>
     <row r="101" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13">
         <v>43943</v>
       </c>
-      <c r="B101" s="31"/>
-      <c r="C101" s="32"/>
+      <c r="B101" s="33"/>
+      <c r="C101" s="34"/>
       <c r="D101" s="13">
         <v>43943</v>
       </c>
-      <c r="E101" s="31" t="s">
+      <c r="E101" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F101" s="59">
+      <c r="F101" s="36">
         <v>3</v>
       </c>
       <c r="G101" s="13">
@@ -3162,24 +3177,24 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="K101" s="61"/>
-      <c r="L101" s="61"/>
+      <c r="K101" s="38"/>
+      <c r="L101" s="38"/>
     </row>
     <row r="102" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13">
         <v>43944</v>
       </c>
-      <c r="B102" s="31" t="s">
+      <c r="B102" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C102" s="32">
+      <c r="C102" s="34">
         <v>2</v>
       </c>
       <c r="D102" s="13">
         <v>43944</v>
       </c>
-      <c r="E102" s="31"/>
-      <c r="F102" s="59"/>
+      <c r="E102" s="33"/>
+      <c r="F102" s="36"/>
       <c r="G102" s="13">
         <v>43944</v>
       </c>
@@ -3191,15 +3206,15 @@
         <f t="shared" si="0"/>
         <v>43944</v>
       </c>
-      <c r="K102" s="61"/>
-      <c r="L102" s="61"/>
+      <c r="K102" s="38"/>
+      <c r="L102" s="38"/>
     </row>
     <row r="103" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13">
         <v>43945</v>
       </c>
-      <c r="B103" s="31"/>
-      <c r="C103" s="32"/>
+      <c r="B103" s="33"/>
+      <c r="C103" s="34"/>
       <c r="D103" s="13">
         <v>43945</v>
       </c>
@@ -3220,8 +3235,8 @@
         <f t="shared" si="0"/>
         <v>43945</v>
       </c>
-      <c r="K103" s="61"/>
-      <c r="L103" s="61"/>
+      <c r="K103" s="38"/>
+      <c r="L103" s="38"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="13">
@@ -3243,8 +3258,8 @@
         <f t="shared" si="0"/>
         <v>43946</v>
       </c>
-      <c r="K104" s="61"/>
-      <c r="L104" s="61"/>
+      <c r="K104" s="38"/>
+      <c r="L104" s="38"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="13">
@@ -3266,10 +3281,10 @@
         <f t="shared" si="0"/>
         <v>43947</v>
       </c>
-      <c r="K105" s="59" t="s">
+      <c r="K105" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="L105" s="32" t="s">
+      <c r="L105" s="34" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3286,10 +3301,10 @@
       <c r="D106" s="13">
         <v>43948</v>
       </c>
-      <c r="E106" s="31" t="s">
+      <c r="E106" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F106" s="59">
+      <c r="F106" s="36">
         <v>3</v>
       </c>
       <c r="G106" s="13">
@@ -3301,24 +3316,24 @@
         <f t="shared" si="0"/>
         <v>43948</v>
       </c>
-      <c r="K106" s="59"/>
-      <c r="L106" s="32"/>
+      <c r="K106" s="36"/>
+      <c r="L106" s="34"/>
     </row>
     <row r="107" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="13">
         <v>43949</v>
       </c>
-      <c r="B107" s="31" t="s">
+      <c r="B107" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="C107" s="32">
+      <c r="C107" s="34">
         <v>4</v>
       </c>
       <c r="D107" s="13">
         <v>43949</v>
       </c>
-      <c r="E107" s="31"/>
-      <c r="F107" s="59"/>
+      <c r="E107" s="33"/>
+      <c r="F107" s="36"/>
       <c r="G107" s="13">
         <v>43949</v>
       </c>
@@ -3339,15 +3354,15 @@
       <c r="A108" s="13">
         <v>43950</v>
       </c>
-      <c r="B108" s="31"/>
-      <c r="C108" s="32"/>
+      <c r="B108" s="33"/>
+      <c r="C108" s="34"/>
       <c r="D108" s="13">
         <v>43950</v>
       </c>
-      <c r="E108" s="31" t="s">
+      <c r="E108" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="F108" s="59">
+      <c r="F108" s="36">
         <v>3</v>
       </c>
       <c r="G108" s="13">
@@ -3370,13 +3385,13 @@
       <c r="A109" s="13">
         <v>43951</v>
       </c>
-      <c r="B109" s="31"/>
-      <c r="C109" s="32"/>
+      <c r="B109" s="33"/>
+      <c r="C109" s="34"/>
       <c r="D109" s="13">
         <v>43951</v>
       </c>
-      <c r="E109" s="31"/>
-      <c r="F109" s="59"/>
+      <c r="E109" s="33"/>
+      <c r="F109" s="36"/>
       <c r="G109" s="13">
         <v>43951</v>
       </c>
@@ -3386,24 +3401,24 @@
         <f t="shared" si="0"/>
         <v>43951</v>
       </c>
-      <c r="K109" s="62" t="s">
+      <c r="K109" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="L109" s="62"/>
+      <c r="L109" s="37"/>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="13">
         <v>43952</v>
       </c>
-      <c r="B110" s="31"/>
-      <c r="C110" s="32"/>
+      <c r="B110" s="33"/>
+      <c r="C110" s="34"/>
       <c r="D110" s="13">
         <v>43952</v>
       </c>
-      <c r="E110" s="31" t="s">
+      <c r="E110" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="F110" s="59">
+      <c r="F110" s="36">
         <v>2</v>
       </c>
       <c r="G110" s="13">
@@ -3415,8 +3430,8 @@
         <f t="shared" si="0"/>
         <v>43952</v>
       </c>
-      <c r="K110" s="62"/>
-      <c r="L110" s="62"/>
+      <c r="K110" s="37"/>
+      <c r="L110" s="37"/>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="13">
@@ -3427,8 +3442,8 @@
       <c r="D111" s="13">
         <v>43953</v>
       </c>
-      <c r="E111" s="31"/>
-      <c r="F111" s="59"/>
+      <c r="E111" s="33"/>
+      <c r="F111" s="36"/>
       <c r="G111" s="13">
         <v>43953</v>
       </c>
@@ -3442,8 +3457,8 @@
         <f t="shared" si="0"/>
         <v>43953</v>
       </c>
-      <c r="K111" s="62"/>
-      <c r="L111" s="62"/>
+      <c r="K111" s="37"/>
+      <c r="L111" s="37"/>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="13">
@@ -3478,19 +3493,19 @@
       <c r="A113" s="13">
         <v>43955</v>
       </c>
-      <c r="B113" s="31" t="s">
+      <c r="B113" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C113" s="32">
+      <c r="C113" s="34">
         <v>5</v>
       </c>
       <c r="D113" s="13">
         <v>43955</v>
       </c>
-      <c r="E113" s="31" t="s">
+      <c r="E113" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="F113" s="59">
+      <c r="F113" s="36">
         <v>3</v>
       </c>
       <c r="G113" s="13">
@@ -3513,13 +3528,13 @@
       <c r="A114" s="13">
         <v>43956</v>
       </c>
-      <c r="B114" s="31"/>
-      <c r="C114" s="32"/>
+      <c r="B114" s="33"/>
+      <c r="C114" s="34"/>
       <c r="D114" s="13">
         <v>43956</v>
       </c>
-      <c r="E114" s="31"/>
-      <c r="F114" s="59"/>
+      <c r="E114" s="33"/>
+      <c r="F114" s="36"/>
       <c r="G114" s="13">
         <v>43956</v>
       </c>
@@ -3540,17 +3555,17 @@
       <c r="A115" s="13">
         <v>43957</v>
       </c>
-      <c r="B115" s="31" t="s">
+      <c r="B115" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="C115" s="32">
+      <c r="C115" s="34">
         <v>4</v>
       </c>
       <c r="D115" s="13">
         <v>43957</v>
       </c>
-      <c r="E115" s="31"/>
-      <c r="F115" s="59"/>
+      <c r="E115" s="33"/>
+      <c r="F115" s="36"/>
       <c r="G115" s="13">
         <v>43957</v>
       </c>
@@ -3571,15 +3586,15 @@
       <c r="A116" s="13">
         <v>43958</v>
       </c>
-      <c r="B116" s="31"/>
-      <c r="C116" s="32"/>
+      <c r="B116" s="33"/>
+      <c r="C116" s="34"/>
       <c r="D116" s="13">
         <v>43958</v>
       </c>
-      <c r="E116" s="31" t="s">
+      <c r="E116" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="F116" s="59">
+      <c r="F116" s="36">
         <v>3</v>
       </c>
       <c r="G116" s="13">
@@ -3602,13 +3617,13 @@
       <c r="A117" s="13">
         <v>43959</v>
       </c>
-      <c r="B117" s="31"/>
-      <c r="C117" s="32"/>
+      <c r="B117" s="33"/>
+      <c r="C117" s="34"/>
       <c r="D117" s="13">
         <v>43959</v>
       </c>
-      <c r="E117" s="31"/>
-      <c r="F117" s="59"/>
+      <c r="E117" s="33"/>
+      <c r="F117" s="36"/>
       <c r="G117" s="13">
         <v>43959</v>
       </c>
@@ -3643,10 +3658,10 @@
         <f t="shared" si="0"/>
         <v>43960</v>
       </c>
-      <c r="K118" s="33" t="s">
+      <c r="K118" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="L118" s="33"/>
+      <c r="L118" s="35"/>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="13">
@@ -3666,8 +3681,8 @@
         <f t="shared" si="0"/>
         <v>43961</v>
       </c>
-      <c r="K119" s="28"/>
-      <c r="L119" s="28"/>
+      <c r="K119" s="35"/>
+      <c r="L119" s="35"/>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="13">
@@ -3691,10 +3706,14 @@
         <f t="shared" si="0"/>
         <v>43962</v>
       </c>
-      <c r="K120" s="28"/>
-      <c r="L120" s="28"/>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K120" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="L120" s="31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="13">
         <v>43963</v>
       </c>
@@ -3712,8 +3731,12 @@
         <f t="shared" si="0"/>
         <v>43963</v>
       </c>
-      <c r="K121" s="28"/>
-      <c r="L121" s="28"/>
+      <c r="K121" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="L121" s="31" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="13">
@@ -3733,10 +3756,10 @@
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-      <c r="K122" s="28"/>
-      <c r="L122" s="28"/>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K122" s="31"/>
+      <c r="L122" s="31"/>
+    </row>
+    <row r="123" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="13">
         <v>43965</v>
       </c>
@@ -3754,8 +3777,12 @@
         <f>J122+1</f>
         <v>43965</v>
       </c>
-      <c r="K123" s="28"/>
-      <c r="L123" s="28"/>
+      <c r="K123" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="L123" s="31" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="13">
@@ -4569,42 +4596,28 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B107:B110"/>
-    <mergeCell ref="C107:C110"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="B115:B117"/>
-    <mergeCell ref="C115:C117"/>
-    <mergeCell ref="K118:L118"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="E110:E111"/>
-    <mergeCell ref="F110:F111"/>
-    <mergeCell ref="K109:L111"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="K91:L104"/>
-    <mergeCell ref="K105:K106"/>
-    <mergeCell ref="L105:L106"/>
-    <mergeCell ref="E101:E102"/>
-    <mergeCell ref="F101:F102"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="E88:E90"/>
-    <mergeCell ref="E92:E100"/>
-    <mergeCell ref="F88:F90"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="C92:C96"/>
+    <mergeCell ref="K83:L84"/>
+    <mergeCell ref="H3:I64"/>
+    <mergeCell ref="H73:H74"/>
+    <mergeCell ref="I73:I74"/>
+    <mergeCell ref="B2:C63"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="H65:H71"/>
+    <mergeCell ref="I65:I71"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="K2:L63"/>
+    <mergeCell ref="L81:L82"/>
+    <mergeCell ref="K65:K68"/>
+    <mergeCell ref="L65:L68"/>
+    <mergeCell ref="K69:L70"/>
+    <mergeCell ref="K76:L77"/>
+    <mergeCell ref="K81:K82"/>
     <mergeCell ref="B85:B90"/>
     <mergeCell ref="C85:C90"/>
     <mergeCell ref="E71:E72"/>
@@ -4621,28 +4634,42 @@
     <mergeCell ref="F78:F81"/>
     <mergeCell ref="E73:E76"/>
     <mergeCell ref="F73:F76"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="K2:L63"/>
-    <mergeCell ref="L81:L82"/>
-    <mergeCell ref="K65:K68"/>
-    <mergeCell ref="L65:L68"/>
-    <mergeCell ref="K69:L70"/>
-    <mergeCell ref="K76:L77"/>
-    <mergeCell ref="K81:K82"/>
-    <mergeCell ref="K83:L84"/>
-    <mergeCell ref="H3:I64"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="I73:I74"/>
-    <mergeCell ref="B2:C63"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="C65:C68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="H65:H71"/>
-    <mergeCell ref="I65:I71"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="C92:C96"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="E92:E100"/>
+    <mergeCell ref="F88:F90"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="F85:F87"/>
+    <mergeCell ref="K91:L104"/>
+    <mergeCell ref="K105:K106"/>
+    <mergeCell ref="L105:L106"/>
+    <mergeCell ref="E101:E102"/>
+    <mergeCell ref="F101:F102"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="E110:E111"/>
+    <mergeCell ref="F110:F111"/>
+    <mergeCell ref="K109:L111"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="K118:L119"/>
+    <mergeCell ref="B107:B110"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="B115:B117"/>
+    <mergeCell ref="C115:C117"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
schemas + bdd + JA
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal-dactivité.xlsx
+++ b/Journal d'activité/Journal-dactivité.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UTILISATEUR 1\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B422B791-057F-4C1B-8AF7-6552D07548FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F159FC-282C-49D4-80D4-6384DDCB1F9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="104">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>Travail sur le dossier à rendre pour la mardi 19/05. J'ai complété le fichier Analyse et Spécification, notamment en modifiant mes diagrammes de classes et en ajoutant un schéma fonctionnel de chaque mécanisme afin qu'il soit mieux comprit + Mise en commun avec Constantin des fonctions I2C</t>
+  </si>
+  <si>
+    <t>Amelioration bdd+ schémas mécanismes pour rapport</t>
+  </si>
+  <si>
+    <t>4h</t>
   </si>
 </sst>
 </file>
@@ -632,7 +638,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -742,9 +748,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -757,18 +790,45 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -788,54 +848,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1159,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G127" sqref="G127"/>
+    <sheetView tabSelected="1" topLeftCell="E119" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K132" sqref="K132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1203,7 @@
       <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="64" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
@@ -1200,1020 +1212,1020 @@
       <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="48"/>
+      <c r="G1" s="66"/>
       <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="50"/>
+      <c r="J1" s="68"/>
       <c r="K1" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="53"/>
+      <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>43844</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="27"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="49"/>
+      <c r="G2" s="67"/>
       <c r="H2" s="27"/>
       <c r="I2" s="11"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="54"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="53"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>43845</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="13">
         <v>43845</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="H3" s="38" t="s">
+      <c r="F3" s="48"/>
+      <c r="H3" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="58"/>
+      <c r="I3" s="48"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="57"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>43846</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="13">
         <v>43846</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="41"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="41"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="58"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="50"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>43847</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="41"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="13">
         <v>43847</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="41"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="58"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="57"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>43848</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="13">
         <v>43848</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="41"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="58"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="50"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="57"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>43849</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="41"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="13">
         <v>43849</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="41"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="58"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="57"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>43850</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="41"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="13">
         <v>43850</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="41"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="58"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="50"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="57"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>43851</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="41"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="13">
         <v>43851</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="41"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="58"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="50"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="57"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>43852</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="13">
         <v>43852</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="41"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="58"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="50"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="57"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>43853</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="13">
         <v>43853</v>
       </c>
-      <c r="E11" s="40"/>
-      <c r="F11" s="41"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="41"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="58"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="50"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="57"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>43854</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="41"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="13">
         <v>43854</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="41"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="58"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="50"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="57"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>43855</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="13">
         <v>43855</v>
       </c>
-      <c r="E13" s="40"/>
-      <c r="F13" s="41"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="41"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="58"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="57"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>43856</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="13">
         <v>43856</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="41"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="58"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="50"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="57"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>43857</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="13">
         <v>43857</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="41"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="58"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="50"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="50"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="57"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>43858</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="13">
         <v>43858</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="58"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="50"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="57"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>43859</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="41"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="13">
         <v>43859</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="41"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="41"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="58"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="50"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="50"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="57"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>43860</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="13">
         <v>43860</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="41"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="58"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="50"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="50"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="57"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>43861</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="41"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="13">
         <v>43861</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="41"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="58"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="50"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="57"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>43862</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="13">
         <v>43862</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="41"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="58"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="57"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>43863</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
       <c r="D21" s="13">
         <v>43863</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="41"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="58"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="50"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="57"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>43864</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="13">
         <v>43864</v>
       </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="41"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="58"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="50"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="50"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="57"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>43865</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="13">
         <v>43865</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="41"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="58"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="50"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="57"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>43866</v>
       </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="13">
         <v>43866</v>
       </c>
-      <c r="E24" s="40"/>
-      <c r="F24" s="41"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="41"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="58"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="50"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="50"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="57"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>43867</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="13">
         <v>43867</v>
       </c>
-      <c r="E25" s="40"/>
-      <c r="F25" s="41"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="41"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="58"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="57"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>43868</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="41"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="13">
         <v>43868</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="41"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="41"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="58"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="50"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="50"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="57"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>43869</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="41"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="13">
         <v>43869</v>
       </c>
-      <c r="E27" s="40"/>
-      <c r="F27" s="41"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="41"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="58"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="50"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="57"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>43870</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="41"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="13">
         <v>43870</v>
       </c>
-      <c r="E28" s="40"/>
-      <c r="F28" s="41"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="41"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="58"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="50"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="57"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>43871</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="41"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="50"/>
       <c r="D29" s="13">
         <v>43871</v>
       </c>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="41"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="58"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="50"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="50"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="57"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>43872</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="13">
         <v>43872</v>
       </c>
-      <c r="E30" s="40"/>
-      <c r="F30" s="41"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="41"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="58"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="50"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="57"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>43873</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
       <c r="D31" s="13">
         <v>43873</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="41"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="41"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="58"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="50"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="50"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="57"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>43874</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="41"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="50"/>
       <c r="D32" s="13">
         <v>43874</v>
       </c>
-      <c r="E32" s="40"/>
-      <c r="F32" s="41"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="41"/>
-      <c r="K32" s="57"/>
-      <c r="L32" s="58"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="50"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="50"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="57"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>43875</v>
       </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="41"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="50"/>
       <c r="D33" s="13">
         <v>43875</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="41"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="41"/>
-      <c r="K33" s="57"/>
-      <c r="L33" s="58"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="50"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="50"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="57"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>43876</v>
       </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="41"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="50"/>
       <c r="D34" s="13">
         <v>43876</v>
       </c>
-      <c r="E34" s="40"/>
-      <c r="F34" s="41"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="41"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="58"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="50"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="50"/>
+      <c r="K34" s="56"/>
+      <c r="L34" s="57"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>43877</v>
       </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="13">
         <v>43877</v>
       </c>
-      <c r="E35" s="40"/>
-      <c r="F35" s="41"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="41"/>
-      <c r="K35" s="57"/>
-      <c r="L35" s="58"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="50"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="50"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="57"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>43878</v>
       </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="41"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
       <c r="D36" s="13">
         <v>43878</v>
       </c>
-      <c r="E36" s="40"/>
-      <c r="F36" s="41"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="41"/>
-      <c r="K36" s="57"/>
-      <c r="L36" s="58"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="50"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="50"/>
+      <c r="K36" s="56"/>
+      <c r="L36" s="57"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>43879</v>
       </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="41"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
       <c r="D37" s="13">
         <v>43879</v>
       </c>
-      <c r="E37" s="40"/>
-      <c r="F37" s="41"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="41"/>
-      <c r="K37" s="57"/>
-      <c r="L37" s="58"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="50"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="50"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="57"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>43880</v>
       </c>
-      <c r="B38" s="40"/>
-      <c r="C38" s="41"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
       <c r="D38" s="13">
         <v>43880</v>
       </c>
-      <c r="E38" s="40"/>
-      <c r="F38" s="41"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="41"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="58"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="50"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="50"/>
+      <c r="K38" s="56"/>
+      <c r="L38" s="57"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>43881</v>
       </c>
-      <c r="B39" s="40"/>
-      <c r="C39" s="41"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
       <c r="D39" s="13">
         <v>43881</v>
       </c>
-      <c r="E39" s="40"/>
-      <c r="F39" s="41"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="41"/>
-      <c r="K39" s="57"/>
-      <c r="L39" s="58"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="50"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="50"/>
+      <c r="K39" s="56"/>
+      <c r="L39" s="57"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>43882</v>
       </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="41"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="50"/>
       <c r="D40" s="13">
         <v>43882</v>
       </c>
-      <c r="E40" s="40"/>
-      <c r="F40" s="41"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="41"/>
-      <c r="K40" s="57"/>
-      <c r="L40" s="58"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="50"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="50"/>
+      <c r="K40" s="56"/>
+      <c r="L40" s="57"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>43883</v>
       </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="41"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="50"/>
       <c r="D41" s="13">
         <v>43883</v>
       </c>
-      <c r="E41" s="40"/>
-      <c r="F41" s="41"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="41"/>
-      <c r="K41" s="57"/>
-      <c r="L41" s="58"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="50"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="50"/>
+      <c r="K41" s="56"/>
+      <c r="L41" s="57"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>43884</v>
       </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="41"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="50"/>
       <c r="D42" s="13">
         <v>43884</v>
       </c>
-      <c r="E42" s="40"/>
-      <c r="F42" s="41"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="41"/>
-      <c r="K42" s="57"/>
-      <c r="L42" s="58"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="50"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="50"/>
+      <c r="K42" s="56"/>
+      <c r="L42" s="57"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>43885</v>
       </c>
-      <c r="B43" s="40"/>
-      <c r="C43" s="41"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="50"/>
       <c r="D43" s="13">
         <v>43885</v>
       </c>
-      <c r="E43" s="40"/>
-      <c r="F43" s="41"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="41"/>
-      <c r="K43" s="57"/>
-      <c r="L43" s="58"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="50"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="50"/>
+      <c r="K43" s="56"/>
+      <c r="L43" s="57"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>43886</v>
       </c>
-      <c r="B44" s="40"/>
-      <c r="C44" s="41"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="50"/>
       <c r="D44" s="13">
         <v>43886</v>
       </c>
-      <c r="E44" s="40"/>
-      <c r="F44" s="41"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="41"/>
-      <c r="K44" s="57"/>
-      <c r="L44" s="58"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="50"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="50"/>
+      <c r="K44" s="56"/>
+      <c r="L44" s="57"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>43887</v>
       </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="41"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="50"/>
       <c r="D45" s="13">
         <v>43887</v>
       </c>
-      <c r="E45" s="40"/>
-      <c r="F45" s="41"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="41"/>
-      <c r="K45" s="57"/>
-      <c r="L45" s="58"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="50"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="50"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="57"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>43888</v>
       </c>
-      <c r="B46" s="40"/>
-      <c r="C46" s="41"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="50"/>
       <c r="D46" s="13">
         <v>43888</v>
       </c>
-      <c r="E46" s="40"/>
-      <c r="F46" s="41"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="41"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="58"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="50"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="50"/>
+      <c r="K46" s="56"/>
+      <c r="L46" s="57"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>43889</v>
       </c>
-      <c r="B47" s="40"/>
-      <c r="C47" s="41"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="50"/>
       <c r="D47" s="13">
         <v>43889</v>
       </c>
-      <c r="E47" s="40"/>
-      <c r="F47" s="41"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="41"/>
-      <c r="K47" s="57"/>
-      <c r="L47" s="58"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="50"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="50"/>
+      <c r="K47" s="56"/>
+      <c r="L47" s="57"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>43890</v>
       </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="41"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="13">
         <v>43890</v>
       </c>
-      <c r="E48" s="40"/>
-      <c r="F48" s="41"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="41"/>
-      <c r="K48" s="57"/>
-      <c r="L48" s="58"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="50"/>
+      <c r="H48" s="49"/>
+      <c r="I48" s="50"/>
+      <c r="K48" s="56"/>
+      <c r="L48" s="57"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>43891</v>
       </c>
-      <c r="B49" s="40"/>
-      <c r="C49" s="41"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="50"/>
       <c r="D49" s="13">
         <v>43891</v>
       </c>
-      <c r="E49" s="40"/>
-      <c r="F49" s="41"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="41"/>
-      <c r="K49" s="57"/>
-      <c r="L49" s="58"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="50"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="50"/>
+      <c r="K49" s="56"/>
+      <c r="L49" s="57"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>43892</v>
       </c>
-      <c r="B50" s="40"/>
-      <c r="C50" s="41"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="50"/>
       <c r="D50" s="13">
         <v>43892</v>
       </c>
-      <c r="E50" s="40"/>
-      <c r="F50" s="41"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="41"/>
-      <c r="K50" s="57"/>
-      <c r="L50" s="58"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="50"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="50"/>
+      <c r="K50" s="56"/>
+      <c r="L50" s="57"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>43893</v>
       </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="41"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="50"/>
       <c r="D51" s="13">
         <v>43893</v>
       </c>
-      <c r="E51" s="40"/>
-      <c r="F51" s="41"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="41"/>
-      <c r="K51" s="57"/>
-      <c r="L51" s="58"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="50"/>
+      <c r="H51" s="49"/>
+      <c r="I51" s="50"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="57"/>
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>43894</v>
       </c>
-      <c r="B52" s="40"/>
-      <c r="C52" s="41"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="50"/>
       <c r="D52" s="13">
         <v>43894</v>
       </c>
-      <c r="E52" s="40"/>
-      <c r="F52" s="41"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="41"/>
-      <c r="K52" s="57"/>
-      <c r="L52" s="58"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="50"/>
+      <c r="H52" s="49"/>
+      <c r="I52" s="50"/>
+      <c r="K52" s="56"/>
+      <c r="L52" s="57"/>
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
         <v>43895</v>
       </c>
-      <c r="B53" s="40"/>
-      <c r="C53" s="41"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="50"/>
       <c r="D53" s="13">
         <v>43895</v>
       </c>
-      <c r="E53" s="40"/>
-      <c r="F53" s="41"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="41"/>
-      <c r="K53" s="57"/>
-      <c r="L53" s="58"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="50"/>
+      <c r="H53" s="49"/>
+      <c r="I53" s="50"/>
+      <c r="K53" s="56"/>
+      <c r="L53" s="57"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>43896</v>
       </c>
-      <c r="B54" s="40"/>
-      <c r="C54" s="41"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="50"/>
       <c r="D54" s="13">
         <v>43896</v>
       </c>
-      <c r="E54" s="40"/>
-      <c r="F54" s="41"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="41"/>
-      <c r="K54" s="57"/>
-      <c r="L54" s="58"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="50"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="50"/>
+      <c r="K54" s="56"/>
+      <c r="L54" s="57"/>
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>43897</v>
       </c>
-      <c r="B55" s="40"/>
-      <c r="C55" s="41"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="50"/>
       <c r="D55" s="13">
         <v>43897</v>
       </c>
-      <c r="E55" s="40"/>
-      <c r="F55" s="41"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="41"/>
-      <c r="K55" s="57"/>
-      <c r="L55" s="58"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="50"/>
+      <c r="H55" s="49"/>
+      <c r="I55" s="50"/>
+      <c r="K55" s="56"/>
+      <c r="L55" s="57"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>43898</v>
       </c>
-      <c r="B56" s="40"/>
-      <c r="C56" s="41"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="50"/>
       <c r="D56" s="13">
         <v>43898</v>
       </c>
-      <c r="E56" s="40"/>
-      <c r="F56" s="41"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="41"/>
-      <c r="K56" s="57"/>
-      <c r="L56" s="58"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="50"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="50"/>
+      <c r="K56" s="56"/>
+      <c r="L56" s="57"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>43899</v>
       </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="41"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="50"/>
       <c r="D57" s="13">
         <v>43899</v>
       </c>
-      <c r="E57" s="40"/>
-      <c r="F57" s="41"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="41"/>
-      <c r="K57" s="57"/>
-      <c r="L57" s="58"/>
+      <c r="E57" s="49"/>
+      <c r="F57" s="50"/>
+      <c r="H57" s="49"/>
+      <c r="I57" s="50"/>
+      <c r="K57" s="56"/>
+      <c r="L57" s="57"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>43900</v>
       </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="41"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="50"/>
       <c r="D58" s="13">
         <v>43900</v>
       </c>
-      <c r="E58" s="40"/>
-      <c r="F58" s="41"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="41"/>
-      <c r="K58" s="57"/>
-      <c r="L58" s="58"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="50"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="50"/>
+      <c r="K58" s="56"/>
+      <c r="L58" s="57"/>
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>43901</v>
       </c>
-      <c r="B59" s="40"/>
-      <c r="C59" s="41"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="50"/>
       <c r="D59" s="13">
         <v>43901</v>
       </c>
-      <c r="E59" s="40"/>
-      <c r="F59" s="41"/>
-      <c r="H59" s="40"/>
-      <c r="I59" s="41"/>
-      <c r="K59" s="57"/>
-      <c r="L59" s="58"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="50"/>
+      <c r="H59" s="49"/>
+      <c r="I59" s="50"/>
+      <c r="K59" s="56"/>
+      <c r="L59" s="57"/>
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>43902</v>
       </c>
-      <c r="B60" s="40"/>
-      <c r="C60" s="41"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="50"/>
       <c r="D60" s="13">
         <v>43902</v>
       </c>
-      <c r="E60" s="40"/>
-      <c r="F60" s="41"/>
-      <c r="H60" s="40"/>
-      <c r="I60" s="41"/>
-      <c r="K60" s="57"/>
-      <c r="L60" s="58"/>
+      <c r="E60" s="49"/>
+      <c r="F60" s="50"/>
+      <c r="H60" s="49"/>
+      <c r="I60" s="50"/>
+      <c r="K60" s="56"/>
+      <c r="L60" s="57"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>43903</v>
       </c>
-      <c r="B61" s="40"/>
-      <c r="C61" s="41"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="50"/>
       <c r="D61" s="13">
         <v>43903</v>
       </c>
-      <c r="E61" s="40"/>
-      <c r="F61" s="41"/>
-      <c r="H61" s="40"/>
-      <c r="I61" s="41"/>
-      <c r="K61" s="57"/>
-      <c r="L61" s="58"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="50"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="50"/>
+      <c r="K61" s="56"/>
+      <c r="L61" s="57"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>43904</v>
       </c>
-      <c r="B62" s="40"/>
-      <c r="C62" s="41"/>
+      <c r="B62" s="49"/>
+      <c r="C62" s="50"/>
       <c r="D62" s="13">
         <v>43904</v>
       </c>
-      <c r="E62" s="40"/>
-      <c r="F62" s="41"/>
-      <c r="H62" s="40"/>
-      <c r="I62" s="41"/>
-      <c r="K62" s="57"/>
-      <c r="L62" s="58"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="50"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="50"/>
+      <c r="K62" s="56"/>
+      <c r="L62" s="57"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>43905</v>
       </c>
-      <c r="B63" s="40"/>
-      <c r="C63" s="41"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="50"/>
       <c r="D63" s="13">
         <v>43905</v>
       </c>
-      <c r="E63" s="40"/>
-      <c r="F63" s="41"/>
-      <c r="H63" s="40"/>
-      <c r="I63" s="41"/>
-      <c r="K63" s="57"/>
-      <c r="L63" s="58"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="50"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="50"/>
+      <c r="K63" s="56"/>
+      <c r="L63" s="57"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
@@ -2234,8 +2246,8 @@
       <c r="F64" s="26">
         <v>2</v>
       </c>
-      <c r="H64" s="40"/>
-      <c r="I64" s="41"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="50"/>
       <c r="J64" s="22">
         <v>43906</v>
       </c>
@@ -2250,33 +2262,33 @@
       <c r="A65" s="13">
         <v>43907</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="44">
+      <c r="C65" s="51">
         <v>10</v>
       </c>
       <c r="D65" s="13">
         <v>43907</v>
       </c>
-      <c r="E65" s="42" t="s">
+      <c r="E65" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="44">
+      <c r="F65" s="51">
         <v>12</v>
       </c>
-      <c r="H65" s="42" t="s">
+      <c r="H65" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="I65" s="52"/>
+      <c r="I65" s="70"/>
       <c r="J65" s="22">
         <f>J64+1</f>
         <v>43907</v>
       </c>
-      <c r="K65" s="42" t="s">
+      <c r="K65" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="L65" s="59" t="s">
+      <c r="L65" s="58" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2284,111 +2296,111 @@
       <c r="A66" s="13">
         <v>43908</v>
       </c>
-      <c r="B66" s="42"/>
-      <c r="C66" s="44"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="51"/>
       <c r="D66" s="13">
         <v>43908</v>
       </c>
-      <c r="E66" s="42"/>
-      <c r="F66" s="44"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="52"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="51"/>
+      <c r="H66" s="39"/>
+      <c r="I66" s="70"/>
       <c r="J66" s="22">
         <f t="shared" ref="J66:J129" si="0">J65+1</f>
         <v>43908</v>
       </c>
-      <c r="K66" s="42"/>
-      <c r="L66" s="59"/>
+      <c r="K66" s="39"/>
+      <c r="L66" s="58"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
         <v>43909</v>
       </c>
-      <c r="B67" s="42"/>
-      <c r="C67" s="44"/>
+      <c r="B67" s="39"/>
+      <c r="C67" s="51"/>
       <c r="D67" s="13">
         <v>43909</v>
       </c>
-      <c r="E67" s="42"/>
-      <c r="F67" s="44"/>
-      <c r="H67" s="42"/>
-      <c r="I67" s="52"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="51"/>
+      <c r="H67" s="39"/>
+      <c r="I67" s="70"/>
       <c r="J67" s="22">
         <f t="shared" si="0"/>
         <v>43909</v>
       </c>
-      <c r="K67" s="42"/>
-      <c r="L67" s="59"/>
+      <c r="K67" s="39"/>
+      <c r="L67" s="58"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
         <v>43910</v>
       </c>
-      <c r="B68" s="42"/>
-      <c r="C68" s="44"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="51"/>
       <c r="D68" s="13">
         <v>43910</v>
       </c>
-      <c r="E68" s="42"/>
-      <c r="F68" s="44"/>
-      <c r="H68" s="42"/>
-      <c r="I68" s="52"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="51"/>
+      <c r="H68" s="39"/>
+      <c r="I68" s="70"/>
       <c r="J68" s="22">
         <f t="shared" si="0"/>
         <v>43910</v>
       </c>
-      <c r="K68" s="42"/>
-      <c r="L68" s="59"/>
+      <c r="K68" s="39"/>
+      <c r="L68" s="58"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
         <v>43911</v>
       </c>
-      <c r="B69" s="42" t="s">
+      <c r="B69" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C69" s="45">
+      <c r="C69" s="40">
         <v>4</v>
       </c>
       <c r="D69" s="13">
         <v>43911</v>
       </c>
-      <c r="E69" s="42" t="s">
+      <c r="E69" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="F69" s="65">
+      <c r="F69" s="41">
         <v>6</v>
       </c>
-      <c r="H69" s="42"/>
-      <c r="I69" s="52"/>
+      <c r="H69" s="39"/>
+      <c r="I69" s="70"/>
       <c r="J69" s="22">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="K69" s="60" t="s">
+      <c r="K69" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="L69" s="61"/>
+      <c r="L69" s="60"/>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
         <v>43912</v>
       </c>
-      <c r="B70" s="42"/>
-      <c r="C70" s="45"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="40"/>
       <c r="D70" s="13">
         <v>43912</v>
       </c>
-      <c r="E70" s="42"/>
-      <c r="F70" s="65"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="52"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="41"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="70"/>
       <c r="J70" s="22">
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
-      <c r="K70" s="60"/>
-      <c r="L70" s="61"/>
+      <c r="K70" s="59"/>
+      <c r="L70" s="60"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
@@ -2403,14 +2415,14 @@
       <c r="D71" s="13">
         <v>43913</v>
       </c>
-      <c r="E71" s="42" t="s">
+      <c r="E71" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F71" s="65">
+      <c r="F71" s="41">
         <v>4</v>
       </c>
-      <c r="H71" s="42"/>
-      <c r="I71" s="52"/>
+      <c r="H71" s="39"/>
+      <c r="I71" s="70"/>
       <c r="J71" s="22">
         <f t="shared" si="0"/>
         <v>43913</v>
@@ -2435,8 +2447,8 @@
       <c r="D72" s="13">
         <v>43914</v>
       </c>
-      <c r="E72" s="42"/>
-      <c r="F72" s="65"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="41"/>
       <c r="G72" s="13">
         <v>43913</v>
       </c>
@@ -2470,19 +2482,19 @@
       <c r="D73" s="13">
         <v>43915</v>
       </c>
-      <c r="E73" s="42" t="s">
+      <c r="E73" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="F73" s="65">
+      <c r="F73" s="41">
         <v>6</v>
       </c>
       <c r="G73" s="13">
         <v>43914</v>
       </c>
-      <c r="H73" s="42" t="s">
+      <c r="H73" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="I73" s="43"/>
+      <c r="I73" s="63"/>
       <c r="J73" s="22">
         <f t="shared" si="0"/>
         <v>43915</v>
@@ -2498,17 +2510,17 @@
       <c r="A74" s="13">
         <v>43916</v>
       </c>
-      <c r="B74" s="42" t="s">
+      <c r="B74" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="65"/>
+      <c r="C74" s="41"/>
       <c r="D74" s="13">
         <v>43916</v>
       </c>
-      <c r="E74" s="42"/>
-      <c r="F74" s="65"/>
-      <c r="H74" s="42"/>
-      <c r="I74" s="43"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="41"/>
+      <c r="H74" s="39"/>
+      <c r="I74" s="63"/>
       <c r="J74" s="22">
         <f t="shared" si="0"/>
         <v>43916</v>
@@ -2529,8 +2541,8 @@
       <c r="D75" s="13">
         <v>43917</v>
       </c>
-      <c r="E75" s="42"/>
-      <c r="F75" s="65"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="41"/>
       <c r="G75" s="13">
         <v>43915</v>
       </c>
@@ -2562,8 +2574,8 @@
       <c r="D76" s="13">
         <v>43918</v>
       </c>
-      <c r="E76" s="42"/>
-      <c r="F76" s="65"/>
+      <c r="E76" s="39"/>
+      <c r="F76" s="41"/>
       <c r="G76" s="13">
         <v>43916</v>
       </c>
@@ -2577,10 +2589,10 @@
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
-      <c r="K76" s="60" t="s">
+      <c r="K76" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="L76" s="62"/>
+      <c r="L76" s="61"/>
     </row>
     <row r="77" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="13">
@@ -2606,8 +2618,8 @@
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="K77" s="63"/>
-      <c r="L77" s="62"/>
+      <c r="K77" s="62"/>
+      <c r="L77" s="61"/>
     </row>
     <row r="78" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="13">
@@ -2622,10 +2634,10 @@
       <c r="D78" s="13">
         <v>43920</v>
       </c>
-      <c r="E78" s="42" t="s">
+      <c r="E78" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F78" s="65">
+      <c r="F78" s="41">
         <v>4</v>
       </c>
       <c r="G78" s="13">
@@ -2652,17 +2664,17 @@
       <c r="A79" s="13">
         <v>43921</v>
       </c>
-      <c r="B79" s="42" t="s">
+      <c r="B79" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C79" s="45">
+      <c r="C79" s="40">
         <v>4</v>
       </c>
       <c r="D79" s="13">
         <v>43921</v>
       </c>
-      <c r="E79" s="42"/>
-      <c r="F79" s="65"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="41"/>
       <c r="G79" s="13">
         <v>43919</v>
       </c>
@@ -2687,13 +2699,13 @@
       <c r="A80" s="13">
         <v>43922</v>
       </c>
-      <c r="B80" s="42"/>
-      <c r="C80" s="45"/>
+      <c r="B80" s="39"/>
+      <c r="C80" s="40"/>
       <c r="D80" s="13">
         <v>43922</v>
       </c>
-      <c r="E80" s="42"/>
-      <c r="F80" s="65"/>
+      <c r="E80" s="39"/>
+      <c r="F80" s="41"/>
       <c r="G80" s="13">
         <v>43920</v>
       </c>
@@ -2716,23 +2728,23 @@
       <c r="A81" s="13">
         <v>43923</v>
       </c>
-      <c r="B81" s="42"/>
-      <c r="C81" s="45"/>
+      <c r="B81" s="39"/>
+      <c r="C81" s="40"/>
       <c r="D81" s="13">
         <v>43923</v>
       </c>
-      <c r="E81" s="42"/>
-      <c r="F81" s="65"/>
+      <c r="E81" s="39"/>
+      <c r="F81" s="41"/>
       <c r="H81" s="20"/>
       <c r="I81" s="20"/>
       <c r="J81" s="22">
         <f t="shared" si="0"/>
         <v>43923</v>
       </c>
-      <c r="K81" s="45" t="s">
+      <c r="K81" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="L81" s="45" t="s">
+      <c r="L81" s="40" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2749,10 +2761,10 @@
       <c r="D82" s="13">
         <v>43924</v>
       </c>
-      <c r="E82" s="42" t="s">
+      <c r="E82" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="F82" s="65">
+      <c r="F82" s="41">
         <v>3</v>
       </c>
       <c r="H82" s="20"/>
@@ -2761,8 +2773,8 @@
         <f t="shared" si="0"/>
         <v>43924</v>
       </c>
-      <c r="K82" s="45"/>
-      <c r="L82" s="45"/>
+      <c r="K82" s="40"/>
+      <c r="L82" s="40"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="13">
@@ -2773,18 +2785,18 @@
       <c r="D83" s="13">
         <v>43925</v>
       </c>
-      <c r="E83" s="42"/>
-      <c r="F83" s="65"/>
+      <c r="E83" s="39"/>
+      <c r="F83" s="41"/>
       <c r="H83" s="20"/>
       <c r="I83" s="20"/>
       <c r="J83" s="22">
         <f t="shared" si="0"/>
         <v>43925</v>
       </c>
-      <c r="K83" s="37" t="s">
+      <c r="K83" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L83" s="37"/>
+      <c r="L83" s="42"/>
     </row>
     <row r="84" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13">
@@ -2807,26 +2819,26 @@
         <f t="shared" si="0"/>
         <v>43926</v>
       </c>
-      <c r="K84" s="37"/>
-      <c r="L84" s="37"/>
+      <c r="K84" s="42"/>
+      <c r="L84" s="42"/>
     </row>
     <row r="85" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13">
         <v>43927</v>
       </c>
-      <c r="B85" s="64" t="s">
+      <c r="B85" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C85" s="45">
+      <c r="C85" s="40">
         <v>12</v>
       </c>
       <c r="D85" s="13">
         <v>43927</v>
       </c>
-      <c r="E85" s="42" t="s">
+      <c r="E85" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="F85" s="65">
+      <c r="F85" s="41">
         <v>6</v>
       </c>
       <c r="H85" s="20"/>
@@ -2846,13 +2858,13 @@
       <c r="A86" s="13">
         <v>43928</v>
       </c>
-      <c r="B86" s="64"/>
-      <c r="C86" s="45"/>
+      <c r="B86" s="46"/>
+      <c r="C86" s="40"/>
       <c r="D86" s="13">
         <v>43928</v>
       </c>
-      <c r="E86" s="42"/>
-      <c r="F86" s="65"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="41"/>
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
       <c r="J86" s="22">
@@ -2870,13 +2882,13 @@
       <c r="A87" s="13">
         <v>43929</v>
       </c>
-      <c r="B87" s="64"/>
-      <c r="C87" s="45"/>
+      <c r="B87" s="46"/>
+      <c r="C87" s="40"/>
       <c r="D87" s="13">
         <v>43929</v>
       </c>
-      <c r="E87" s="42"/>
-      <c r="F87" s="65"/>
+      <c r="E87" s="39"/>
+      <c r="F87" s="41"/>
       <c r="H87" s="20"/>
       <c r="I87" s="20"/>
       <c r="J87" s="22">
@@ -2894,15 +2906,15 @@
       <c r="A88" s="21">
         <v>43930</v>
       </c>
-      <c r="B88" s="64"/>
-      <c r="C88" s="45"/>
+      <c r="B88" s="46"/>
+      <c r="C88" s="40"/>
       <c r="D88" s="13">
         <v>43930</v>
       </c>
-      <c r="E88" s="42" t="s">
+      <c r="E88" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="F88" s="65">
+      <c r="F88" s="41">
         <v>4</v>
       </c>
       <c r="H88" s="20"/>
@@ -2922,13 +2934,13 @@
       <c r="A89" s="21">
         <v>43931</v>
       </c>
-      <c r="B89" s="64"/>
-      <c r="C89" s="45"/>
+      <c r="B89" s="46"/>
+      <c r="C89" s="40"/>
       <c r="D89" s="13">
         <v>43931</v>
       </c>
-      <c r="E89" s="42"/>
-      <c r="F89" s="65"/>
+      <c r="E89" s="39"/>
+      <c r="F89" s="41"/>
       <c r="H89" s="20"/>
       <c r="I89" s="20"/>
       <c r="J89" s="22">
@@ -2946,13 +2958,13 @@
       <c r="A90" s="21">
         <v>43932</v>
       </c>
-      <c r="B90" s="64"/>
-      <c r="C90" s="45"/>
+      <c r="B90" s="46"/>
+      <c r="C90" s="40"/>
       <c r="D90" s="13">
         <v>43932</v>
       </c>
-      <c r="E90" s="42"/>
-      <c r="F90" s="65"/>
+      <c r="E90" s="39"/>
+      <c r="F90" s="41"/>
       <c r="H90" s="20"/>
       <c r="I90" s="20"/>
       <c r="J90" s="22">
@@ -2983,25 +2995,25 @@
         <f t="shared" si="0"/>
         <v>43933</v>
       </c>
-      <c r="K91" s="67" t="s">
+      <c r="K91" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="L91" s="67"/>
+      <c r="L91" s="44"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="13">
         <v>43934</v>
       </c>
-      <c r="B92" s="42" t="s">
+      <c r="B92" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="C92" s="45">
+      <c r="C92" s="40">
         <v>4</v>
       </c>
       <c r="D92" s="13">
         <v>43934</v>
       </c>
-      <c r="E92" s="42" t="s">
+      <c r="E92" s="39" t="s">
         <v>65</v>
       </c>
       <c r="H92" s="20"/>
@@ -3010,84 +3022,84 @@
         <f t="shared" si="0"/>
         <v>43934</v>
       </c>
-      <c r="K92" s="67"/>
-      <c r="L92" s="67"/>
+      <c r="K92" s="44"/>
+      <c r="L92" s="44"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="13">
         <v>43935</v>
       </c>
-      <c r="B93" s="42"/>
-      <c r="C93" s="45"/>
+      <c r="B93" s="39"/>
+      <c r="C93" s="40"/>
       <c r="D93" s="13">
         <v>43935</v>
       </c>
-      <c r="E93" s="66"/>
+      <c r="E93" s="45"/>
       <c r="H93" s="20"/>
       <c r="I93" s="20"/>
       <c r="J93" s="22">
         <f t="shared" si="0"/>
         <v>43935</v>
       </c>
-      <c r="K93" s="67"/>
-      <c r="L93" s="67"/>
+      <c r="K93" s="44"/>
+      <c r="L93" s="44"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="13">
         <v>43936</v>
       </c>
-      <c r="B94" s="42"/>
-      <c r="C94" s="45"/>
+      <c r="B94" s="39"/>
+      <c r="C94" s="40"/>
       <c r="D94" s="13">
         <v>43936</v>
       </c>
-      <c r="E94" s="66"/>
+      <c r="E94" s="45"/>
       <c r="H94" s="20"/>
       <c r="I94" s="20"/>
       <c r="J94" s="22">
         <f t="shared" si="0"/>
         <v>43936</v>
       </c>
-      <c r="K94" s="67"/>
-      <c r="L94" s="67"/>
+      <c r="K94" s="44"/>
+      <c r="L94" s="44"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="13">
         <v>43937</v>
       </c>
-      <c r="B95" s="42"/>
-      <c r="C95" s="45"/>
+      <c r="B95" s="39"/>
+      <c r="C95" s="40"/>
       <c r="D95" s="13">
         <v>43937</v>
       </c>
-      <c r="E95" s="66"/>
+      <c r="E95" s="45"/>
       <c r="H95" s="20"/>
       <c r="I95" s="20"/>
       <c r="J95" s="22">
         <f t="shared" si="0"/>
         <v>43937</v>
       </c>
-      <c r="K95" s="67"/>
-      <c r="L95" s="67"/>
+      <c r="K95" s="44"/>
+      <c r="L95" s="44"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="13">
         <v>43938</v>
       </c>
-      <c r="B96" s="42"/>
-      <c r="C96" s="45"/>
+      <c r="B96" s="39"/>
+      <c r="C96" s="40"/>
       <c r="D96" s="13">
         <v>43938</v>
       </c>
-      <c r="E96" s="66"/>
+      <c r="E96" s="45"/>
       <c r="H96" s="20"/>
       <c r="I96" s="20"/>
       <c r="J96" s="22">
         <f t="shared" si="0"/>
         <v>43938</v>
       </c>
-      <c r="K96" s="67"/>
-      <c r="L96" s="67"/>
+      <c r="K96" s="44"/>
+      <c r="L96" s="44"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="13">
@@ -3098,15 +3110,15 @@
       <c r="D97" s="13">
         <v>43939</v>
       </c>
-      <c r="E97" s="66"/>
+      <c r="E97" s="45"/>
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
       <c r="J97" s="22">
         <f t="shared" si="0"/>
         <v>43939</v>
       </c>
-      <c r="K97" s="67"/>
-      <c r="L97" s="67"/>
+      <c r="K97" s="44"/>
+      <c r="L97" s="44"/>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="13">
@@ -3117,71 +3129,71 @@
       <c r="D98" s="13">
         <v>43940</v>
       </c>
-      <c r="E98" s="66"/>
+      <c r="E98" s="45"/>
       <c r="H98" s="20"/>
       <c r="I98" s="20"/>
       <c r="J98" s="22">
         <f t="shared" si="0"/>
         <v>43940</v>
       </c>
-      <c r="K98" s="67"/>
-      <c r="L98" s="67"/>
+      <c r="K98" s="44"/>
+      <c r="L98" s="44"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="13">
         <v>43941</v>
       </c>
-      <c r="B99" s="42" t="s">
+      <c r="B99" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C99" s="45">
+      <c r="C99" s="40">
         <v>4</v>
       </c>
       <c r="D99" s="13">
         <v>43941</v>
       </c>
-      <c r="E99" s="66"/>
+      <c r="E99" s="45"/>
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
       <c r="J99" s="22">
         <f t="shared" si="0"/>
         <v>43941</v>
       </c>
-      <c r="K99" s="67"/>
-      <c r="L99" s="67"/>
+      <c r="K99" s="44"/>
+      <c r="L99" s="44"/>
     </row>
     <row r="100" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13">
         <v>43942</v>
       </c>
-      <c r="B100" s="42"/>
-      <c r="C100" s="45"/>
+      <c r="B100" s="39"/>
+      <c r="C100" s="40"/>
       <c r="D100" s="13">
         <v>43942</v>
       </c>
-      <c r="E100" s="66"/>
+      <c r="E100" s="45"/>
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
       <c r="J100" s="22">
         <f t="shared" si="0"/>
         <v>43942</v>
       </c>
-      <c r="K100" s="67"/>
-      <c r="L100" s="67"/>
+      <c r="K100" s="44"/>
+      <c r="L100" s="44"/>
     </row>
     <row r="101" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13">
         <v>43943</v>
       </c>
-      <c r="B101" s="42"/>
-      <c r="C101" s="45"/>
+      <c r="B101" s="39"/>
+      <c r="C101" s="40"/>
       <c r="D101" s="13">
         <v>43943</v>
       </c>
-      <c r="E101" s="42" t="s">
+      <c r="E101" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="F101" s="65">
+      <c r="F101" s="41">
         <v>3</v>
       </c>
       <c r="G101" s="13">
@@ -3195,24 +3207,24 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="K101" s="67"/>
-      <c r="L101" s="67"/>
+      <c r="K101" s="44"/>
+      <c r="L101" s="44"/>
     </row>
     <row r="102" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13">
         <v>43944</v>
       </c>
-      <c r="B102" s="42" t="s">
+      <c r="B102" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C102" s="45">
+      <c r="C102" s="40">
         <v>2</v>
       </c>
       <c r="D102" s="13">
         <v>43944</v>
       </c>
-      <c r="E102" s="42"/>
-      <c r="F102" s="65"/>
+      <c r="E102" s="39"/>
+      <c r="F102" s="41"/>
       <c r="G102" s="13">
         <v>43944</v>
       </c>
@@ -3224,15 +3236,15 @@
         <f t="shared" si="0"/>
         <v>43944</v>
       </c>
-      <c r="K102" s="67"/>
-      <c r="L102" s="67"/>
+      <c r="K102" s="44"/>
+      <c r="L102" s="44"/>
     </row>
     <row r="103" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13">
         <v>43945</v>
       </c>
-      <c r="B103" s="42"/>
-      <c r="C103" s="45"/>
+      <c r="B103" s="39"/>
+      <c r="C103" s="40"/>
       <c r="D103" s="13">
         <v>43945</v>
       </c>
@@ -3253,8 +3265,8 @@
         <f t="shared" si="0"/>
         <v>43945</v>
       </c>
-      <c r="K103" s="67"/>
-      <c r="L103" s="67"/>
+      <c r="K103" s="44"/>
+      <c r="L103" s="44"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="13">
@@ -3276,8 +3288,8 @@
         <f t="shared" si="0"/>
         <v>43946</v>
       </c>
-      <c r="K104" s="67"/>
-      <c r="L104" s="67"/>
+      <c r="K104" s="44"/>
+      <c r="L104" s="44"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="13">
@@ -3299,10 +3311,10 @@
         <f t="shared" si="0"/>
         <v>43947</v>
       </c>
-      <c r="K105" s="65" t="s">
+      <c r="K105" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="L105" s="45" t="s">
+      <c r="L105" s="40" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3319,10 +3331,10 @@
       <c r="D106" s="13">
         <v>43948</v>
       </c>
-      <c r="E106" s="42" t="s">
+      <c r="E106" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="F106" s="65">
+      <c r="F106" s="41">
         <v>3</v>
       </c>
       <c r="G106" s="13">
@@ -3334,24 +3346,24 @@
         <f t="shared" si="0"/>
         <v>43948</v>
       </c>
-      <c r="K106" s="65"/>
-      <c r="L106" s="45"/>
+      <c r="K106" s="41"/>
+      <c r="L106" s="40"/>
     </row>
     <row r="107" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="13">
         <v>43949</v>
       </c>
-      <c r="B107" s="42" t="s">
+      <c r="B107" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C107" s="45">
+      <c r="C107" s="40">
         <v>4</v>
       </c>
       <c r="D107" s="13">
         <v>43949</v>
       </c>
-      <c r="E107" s="42"/>
-      <c r="F107" s="65"/>
+      <c r="E107" s="39"/>
+      <c r="F107" s="41"/>
       <c r="G107" s="13">
         <v>43949</v>
       </c>
@@ -3372,15 +3384,15 @@
       <c r="A108" s="13">
         <v>43950</v>
       </c>
-      <c r="B108" s="42"/>
-      <c r="C108" s="45"/>
+      <c r="B108" s="39"/>
+      <c r="C108" s="40"/>
       <c r="D108" s="13">
         <v>43950</v>
       </c>
-      <c r="E108" s="42" t="s">
+      <c r="E108" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="F108" s="65">
+      <c r="F108" s="41">
         <v>3</v>
       </c>
       <c r="G108" s="13">
@@ -3403,13 +3415,13 @@
       <c r="A109" s="13">
         <v>43951</v>
       </c>
-      <c r="B109" s="42"/>
-      <c r="C109" s="45"/>
+      <c r="B109" s="39"/>
+      <c r="C109" s="40"/>
       <c r="D109" s="13">
         <v>43951</v>
       </c>
-      <c r="E109" s="42"/>
-      <c r="F109" s="65"/>
+      <c r="E109" s="39"/>
+      <c r="F109" s="41"/>
       <c r="G109" s="13">
         <v>43951</v>
       </c>
@@ -3419,24 +3431,24 @@
         <f t="shared" si="0"/>
         <v>43951</v>
       </c>
-      <c r="K109" s="68" t="s">
+      <c r="K109" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="L109" s="68"/>
+      <c r="L109" s="43"/>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="13">
         <v>43952</v>
       </c>
-      <c r="B110" s="42"/>
-      <c r="C110" s="45"/>
+      <c r="B110" s="39"/>
+      <c r="C110" s="40"/>
       <c r="D110" s="13">
         <v>43952</v>
       </c>
-      <c r="E110" s="42" t="s">
+      <c r="E110" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="F110" s="65">
+      <c r="F110" s="41">
         <v>2</v>
       </c>
       <c r="G110" s="13">
@@ -3448,8 +3460,8 @@
         <f t="shared" si="0"/>
         <v>43952</v>
       </c>
-      <c r="K110" s="68"/>
-      <c r="L110" s="68"/>
+      <c r="K110" s="43"/>
+      <c r="L110" s="43"/>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="13">
@@ -3460,8 +3472,8 @@
       <c r="D111" s="13">
         <v>43953</v>
       </c>
-      <c r="E111" s="42"/>
-      <c r="F111" s="65"/>
+      <c r="E111" s="39"/>
+      <c r="F111" s="41"/>
       <c r="G111" s="13">
         <v>43953</v>
       </c>
@@ -3475,8 +3487,8 @@
         <f t="shared" si="0"/>
         <v>43953</v>
       </c>
-      <c r="K111" s="68"/>
-      <c r="L111" s="68"/>
+      <c r="K111" s="43"/>
+      <c r="L111" s="43"/>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="13">
@@ -3511,19 +3523,19 @@
       <c r="A113" s="13">
         <v>43955</v>
       </c>
-      <c r="B113" s="42" t="s">
+      <c r="B113" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="C113" s="45">
+      <c r="C113" s="40">
         <v>5</v>
       </c>
       <c r="D113" s="13">
         <v>43955</v>
       </c>
-      <c r="E113" s="42" t="s">
+      <c r="E113" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="F113" s="65">
+      <c r="F113" s="41">
         <v>3</v>
       </c>
       <c r="G113" s="13">
@@ -3546,13 +3558,13 @@
       <c r="A114" s="13">
         <v>43956</v>
       </c>
-      <c r="B114" s="42"/>
-      <c r="C114" s="45"/>
+      <c r="B114" s="39"/>
+      <c r="C114" s="40"/>
       <c r="D114" s="13">
         <v>43956</v>
       </c>
-      <c r="E114" s="42"/>
-      <c r="F114" s="65"/>
+      <c r="E114" s="39"/>
+      <c r="F114" s="41"/>
       <c r="G114" s="13">
         <v>43956</v>
       </c>
@@ -3573,17 +3585,17 @@
       <c r="A115" s="13">
         <v>43957</v>
       </c>
-      <c r="B115" s="42" t="s">
+      <c r="B115" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C115" s="45">
+      <c r="C115" s="40">
         <v>4</v>
       </c>
       <c r="D115" s="13">
         <v>43957</v>
       </c>
-      <c r="E115" s="42"/>
-      <c r="F115" s="65"/>
+      <c r="E115" s="39"/>
+      <c r="F115" s="41"/>
       <c r="G115" s="13">
         <v>43957</v>
       </c>
@@ -3604,15 +3616,15 @@
       <c r="A116" s="13">
         <v>43958</v>
       </c>
-      <c r="B116" s="42"/>
-      <c r="C116" s="45"/>
+      <c r="B116" s="39"/>
+      <c r="C116" s="40"/>
       <c r="D116" s="13">
         <v>43958</v>
       </c>
-      <c r="E116" s="42" t="s">
+      <c r="E116" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="F116" s="65">
+      <c r="F116" s="41">
         <v>3</v>
       </c>
       <c r="G116" s="13">
@@ -3635,13 +3647,13 @@
       <c r="A117" s="13">
         <v>43959</v>
       </c>
-      <c r="B117" s="42"/>
-      <c r="C117" s="45"/>
+      <c r="B117" s="39"/>
+      <c r="C117" s="40"/>
       <c r="D117" s="13">
         <v>43959</v>
       </c>
-      <c r="E117" s="42"/>
-      <c r="F117" s="65"/>
+      <c r="E117" s="39"/>
+      <c r="F117" s="41"/>
       <c r="G117" s="13">
         <v>43959</v>
       </c>
@@ -3676,10 +3688,10 @@
         <f t="shared" si="0"/>
         <v>43960</v>
       </c>
-      <c r="K118" s="37" t="s">
+      <c r="K118" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L118" s="37"/>
+      <c r="L118" s="42"/>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="13">
@@ -3699,8 +3711,8 @@
         <f t="shared" si="0"/>
         <v>43961</v>
       </c>
-      <c r="K119" s="37"/>
-      <c r="L119" s="37"/>
+      <c r="K119" s="42"/>
+      <c r="L119" s="42"/>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="13">
@@ -3735,10 +3747,10 @@
       <c r="A121" s="13">
         <v>43963</v>
       </c>
-      <c r="B121" s="42" t="s">
+      <c r="B121" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="C121" s="45">
+      <c r="C121" s="40">
         <v>5</v>
       </c>
       <c r="D121" s="13">
@@ -3764,8 +3776,8 @@
       <c r="A122" s="13">
         <v>43964</v>
       </c>
-      <c r="B122" s="42"/>
-      <c r="C122" s="45"/>
+      <c r="B122" s="39"/>
+      <c r="C122" s="40"/>
       <c r="D122" s="13">
         <v>43964</v>
       </c>
@@ -3785,8 +3797,8 @@
       <c r="A123" s="13">
         <v>43965</v>
       </c>
-      <c r="B123" s="42"/>
-      <c r="C123" s="45"/>
+      <c r="B123" s="39"/>
+      <c r="C123" s="40"/>
       <c r="D123" s="13">
         <v>43965</v>
       </c>
@@ -3824,8 +3836,10 @@
         <f t="shared" si="0"/>
         <v>43966</v>
       </c>
-      <c r="K124" s="28"/>
-      <c r="L124" s="28"/>
+      <c r="K124" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="L124" s="42"/>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="13">
@@ -3845,8 +3859,8 @@
         <f t="shared" si="0"/>
         <v>43967</v>
       </c>
-      <c r="K125" s="28"/>
-      <c r="L125" s="28"/>
+      <c r="K125" s="42"/>
+      <c r="L125" s="42"/>
     </row>
     <row r="126" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A126" s="13">
@@ -3870,8 +3884,12 @@
         <f t="shared" si="0"/>
         <v>43968</v>
       </c>
-      <c r="K126" s="28"/>
-      <c r="L126" s="28"/>
+      <c r="K126" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="L126" s="37" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="13">
@@ -4621,44 +4639,31 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="B121:B123"/>
-    <mergeCell ref="C121:C123"/>
-    <mergeCell ref="B107:B110"/>
-    <mergeCell ref="C107:C110"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="B115:B117"/>
-    <mergeCell ref="C115:C117"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="K118:L119"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="E110:E111"/>
-    <mergeCell ref="F110:F111"/>
-    <mergeCell ref="K109:L111"/>
-    <mergeCell ref="K91:L104"/>
-    <mergeCell ref="K105:K106"/>
-    <mergeCell ref="L105:L106"/>
-    <mergeCell ref="E101:E102"/>
-    <mergeCell ref="F101:F102"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="E88:E90"/>
-    <mergeCell ref="E92:E100"/>
-    <mergeCell ref="F88:F90"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="C92:C96"/>
+  <mergeCells count="77">
+    <mergeCell ref="K124:L125"/>
+    <mergeCell ref="K83:L84"/>
+    <mergeCell ref="H3:I64"/>
+    <mergeCell ref="H73:H74"/>
+    <mergeCell ref="I73:I74"/>
+    <mergeCell ref="B2:C63"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="H65:H71"/>
+    <mergeCell ref="I65:I71"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="K2:L63"/>
+    <mergeCell ref="L81:L82"/>
+    <mergeCell ref="K65:K68"/>
+    <mergeCell ref="L65:L68"/>
+    <mergeCell ref="K69:L70"/>
+    <mergeCell ref="K76:L77"/>
+    <mergeCell ref="K81:K82"/>
     <mergeCell ref="B85:B90"/>
     <mergeCell ref="C85:C90"/>
     <mergeCell ref="E71:E72"/>
@@ -4675,29 +4680,43 @@
     <mergeCell ref="F78:F81"/>
     <mergeCell ref="E73:E76"/>
     <mergeCell ref="F73:F76"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="K2:L63"/>
-    <mergeCell ref="L81:L82"/>
-    <mergeCell ref="K65:K68"/>
-    <mergeCell ref="L65:L68"/>
-    <mergeCell ref="K69:L70"/>
-    <mergeCell ref="K76:L77"/>
-    <mergeCell ref="K81:K82"/>
-    <mergeCell ref="K83:L84"/>
-    <mergeCell ref="H3:I64"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="I73:I74"/>
-    <mergeCell ref="B2:C63"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="C65:C68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="H65:H71"/>
-    <mergeCell ref="I65:I71"/>
-    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="C92:C96"/>
+    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="E92:E100"/>
+    <mergeCell ref="F88:F90"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="F85:F87"/>
+    <mergeCell ref="K91:L104"/>
+    <mergeCell ref="K105:K106"/>
+    <mergeCell ref="L105:L106"/>
+    <mergeCell ref="E101:E102"/>
+    <mergeCell ref="F101:F102"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="E110:E111"/>
+    <mergeCell ref="F110:F111"/>
+    <mergeCell ref="K109:L111"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="K118:L119"/>
+    <mergeCell ref="B121:B123"/>
+    <mergeCell ref="C121:C123"/>
+    <mergeCell ref="B107:B110"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="B115:B117"/>
+    <mergeCell ref="C115:C117"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>